<commit_message>
- Import new plugin to show the data on table, we made it :D
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
   <si>
     <t>PATIENT</t>
   </si>
@@ -200,6 +200,18 @@
   </si>
   <si>
     <t>order</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>user_update</t>
+  </si>
+  <si>
+    <t>sex</t>
   </si>
 </sst>
 </file>
@@ -274,21 +286,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -305,6 +320,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.59999389629810485"/>
@@ -325,6 +341,85 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -367,9 +462,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -381,7 +473,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="3" tint="-0.499984740745262"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
@@ -395,16 +487,19 @@
         <left style="thin">
           <color theme="0"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
         <top style="thin">
           <color theme="0"/>
         </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -443,6 +538,9 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -457,14 +555,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D49" totalsRowShown="0">
-  <autoFilter ref="A4:D49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D51" totalsRowShown="0">
+  <autoFilter ref="A4:D51"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated">
-      <calculatedColumnFormula>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');")) )))</calculatedColumnFormula>
+    <tableColumn id="4" name="Code generated" dataDxfId="3">
+      <calculatedColumnFormula>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"')-&gt;unsigned()-&gt;default(0);"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5),"('",Table1[[#This Row],[Column name]],"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -472,14 +570,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A53:D57" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A53:D57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A55:D59" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A55:D59"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="5"/>
+    <tableColumn id="2" name="Type" dataDxfId="8"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="4">
-      <calculatedColumnFormula>IF(B54="String", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"', ",C54,");"), IF(B54="Integer", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"');"), IF(B54="Text", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"');"), IF(B54="Date", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"');")) )))</calculatedColumnFormula>
+    <tableColumn id="4" name="Code generated" dataDxfId="1">
+      <calculatedColumnFormula>IF(B56="String", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"', ",C56,");"), IF(B56="Integer", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"')-&gt;unsigned()-&gt;default(0);"), IF(B56="Text", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');"), IF(B56="Date", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -487,14 +585,29 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A61:D65" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A61:D65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A63:D67" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A63:D67"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="1"/>
+    <tableColumn id="2" name="Type" dataDxfId="6"/>
+    <tableColumn id="3" name="Length"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="2">
+      <calculatedColumnFormula>IF(B64="String", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"', ",C64,");"), IF(B64="Integer", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"')-&gt;unsigned()-&gt;default(0);"), IF(B64="Text", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');"), IF(B64="Date", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');")) )))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A71:D75" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A71:D75"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Column name"/>
+    <tableColumn id="2" name="Type" dataDxfId="4"/>
     <tableColumn id="3" name="Length"/>
     <tableColumn id="4" name="Code generated" dataDxfId="0">
-      <calculatedColumnFormula>IF(B62="String", CONCATENATE("$table-&gt;",LOWER(B62),"('",A62,"', ",C62,");"), IF(B62="Integer", CONCATENATE("$table-&gt;",LOWER(B62),"('",A62,"');"), IF(B62="Text", CONCATENATE("$table-&gt;",LOWER(B62),"('",A62,"');"), IF(B62="Date", CONCATENATE("$table-&gt;",LOWER(B62),"('",A62,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B72="String", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"', ",C72,");"), IF(B72="Integer", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"')-&gt;unsigned()-&gt;default(0);"), IF(B72="Text", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');"), IF(B72="Date", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -788,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62:D65"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,26 +912,26 @@
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -845,7 +958,7 @@
         <v>50</v>
       </c>
       <c r="D5" t="str">
-        <f>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5))) )))</f>
+        <f>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"')-&gt;unsigned()-&gt;default(0);"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('id_patient', 50);</v>
       </c>
     </row>
@@ -860,7 +973,7 @@
         <v>50</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" ref="D6:D48" si="0">IF(B6="String", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"', ",C6,");"), IF(B6="Integer", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"');"), IF(B6="Text", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"');"), IF(B6="Date", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"');")) )))</f>
+        <f>IF(B6="String", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"', ",C6,");"), IF(B6="Integer", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"')-&gt;unsigned()-&gt;default(0);"), IF(B6="Text", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"');"), IF(B6="Date", CONCATENATE("$table-&gt;",LOWER(B6),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('id_dentist', 50);</v>
       </c>
     </row>
@@ -875,7 +988,7 @@
         <v>50</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B7="String", CONCATENATE("$table-&gt;",LOWER(B7),"('",A7,"', ",C7,");"), IF(B7="Integer", CONCATENATE("$table-&gt;",LOWER(B7),"('",A7,"')-&gt;unsigned()-&gt;default(0);"), IF(B7="Text", CONCATENATE("$table-&gt;",LOWER(B7),"('",A7,"');"), IF(B7="Date", CONCATENATE("$table-&gt;",LOWER(B7),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('proffession', 50);</v>
       </c>
     </row>
@@ -890,7 +1003,7 @@
         <v>255</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B8="String", CONCATENATE("$table-&gt;",LOWER(B8),"('",A8,"', ",C8,");"), IF(B8="Integer", CONCATENATE("$table-&gt;",LOWER(B8),"('",A8,"')-&gt;unsigned()-&gt;default(0);"), IF(B8="Text", CONCATENATE("$table-&gt;",LOWER(B8),"('",A8,"');"), IF(B8="Date", CONCATENATE("$table-&gt;",LOWER(B8),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('company_name', 255);</v>
       </c>
     </row>
@@ -905,7 +1018,7 @@
         <v>255</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B9="String", CONCATENATE("$table-&gt;",LOWER(B9),"('",A9,"', ",C9,");"), IF(B9="Integer", CONCATENATE("$table-&gt;",LOWER(B9),"('",A9,"')-&gt;unsigned()-&gt;default(0);"), IF(B9="Text", CONCATENATE("$table-&gt;",LOWER(B9),"('",A9,"');"), IF(B9="Date", CONCATENATE("$table-&gt;",LOWER(B9),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('last_name', 255);</v>
       </c>
     </row>
@@ -920,7 +1033,7 @@
         <v>255</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B10="String", CONCATENATE("$table-&gt;",LOWER(B10),"('",A10,"', ",C10,");"), IF(B10="Integer", CONCATENATE("$table-&gt;",LOWER(B10),"('",A10,"')-&gt;unsigned()-&gt;default(0);"), IF(B10="Text", CONCATENATE("$table-&gt;",LOWER(B10),"('",A10,"');"), IF(B10="Date", CONCATENATE("$table-&gt;",LOWER(B10),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('first_name', 255);</v>
       </c>
     </row>
@@ -935,7 +1048,7 @@
         <v>255</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B11="String", CONCATENATE("$table-&gt;",LOWER(B11),"('",A11,"', ",C11,");"), IF(B11="Integer", CONCATENATE("$table-&gt;",LOWER(B11),"('",A11,"')-&gt;unsigned()-&gt;default(0);"), IF(B11="Text", CONCATENATE("$table-&gt;",LOWER(B11),"('",A11,"');"), IF(B11="Date", CONCATENATE("$table-&gt;",LOWER(B11),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('address', 255);</v>
       </c>
     </row>
@@ -950,7 +1063,7 @@
         <v>100</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B12="String", CONCATENATE("$table-&gt;",LOWER(B12),"('",A12,"', ",C12,");"), IF(B12="Integer", CONCATENATE("$table-&gt;",LOWER(B12),"('",A12,"')-&gt;unsigned()-&gt;default(0);"), IF(B12="Text", CONCATENATE("$table-&gt;",LOWER(B12),"('",A12,"');"), IF(B12="Date", CONCATENATE("$table-&gt;",LOWER(B12),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('city', 100);</v>
       </c>
     </row>
@@ -962,7 +1075,7 @@
         <v>15</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B13="String", CONCATENATE("$table-&gt;",LOWER(B13),"('",A13,"', ",C13,");"), IF(B13="Integer", CONCATENATE("$table-&gt;",LOWER(B13),"('",A13,"')-&gt;unsigned()-&gt;default(0);"), IF(B13="Text", CONCATENATE("$table-&gt;",LOWER(B13),"('",A13,"');"), IF(B13="Date", CONCATENATE("$table-&gt;",LOWER(B13),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;date('date_birth');</v>
       </c>
     </row>
@@ -977,7 +1090,7 @@
         <v>20</v>
       </c>
       <c r="D14" t="str">
-        <f>IF(B14="String", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"', ",C14,");"), IF(B14="Integer", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"');"), IF(B14="Text", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"');"), IF(B14="Date", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"');")) )))</f>
+        <f>IF(B14="String", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"', ",C14,");"), IF(B14="Integer", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"')-&gt;unsigned()-&gt;default(0);"), IF(B14="Text", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"');"), IF(B14="Date", CONCATENATE("$table-&gt;",LOWER(B14),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('marital_status', 20);</v>
       </c>
     </row>
@@ -992,73 +1105,73 @@
         <v>100</v>
       </c>
       <c r="D15" t="str">
-        <f>IF(B15="String", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"', ",C15,");"), IF(B15="Integer", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"');"), IF(B15="Text", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"');"), IF(B15="Date", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"');")) )))</f>
+        <f>IF(B15="String", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"', ",C15,");"), IF(B15="Integer", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"')-&gt;unsigned()-&gt;default(0);"), IF(B15="Text", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"');"), IF(B15="Date", CONCATENATE("$table-&gt;",LOWER(B15),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('language', 100);</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16">
-        <v>255</v>
+        <v>50</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('email', 255);</v>
+        <f>IF(B16="String", CONCATENATE("$table-&gt;",LOWER(B16),"('",A16,"', ",C16,");"), IF(B16="Integer", CONCATENATE("$table-&gt;",LOWER(B16),"('",A16,"')-&gt;unsigned()-&gt;default(0);"), IF(B16="Text", CONCATENATE("$table-&gt;",LOWER(B16),"('",A16,"');"), IF(B16="Date", CONCATENATE("$table-&gt;",LOWER(B16),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('sex', 50);</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17">
-        <v>100</v>
+        <v>255</v>
       </c>
       <c r="D17" t="str">
-        <f>IF(B17="String", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"', ",C17,");"), IF(B17="Integer", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"');"), IF(B17="Text", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"');"), IF(B17="Date", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"');")) )))</f>
-        <v>$table-&gt;string('zip_code', 100);</v>
+        <f>IF(B17="String", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"', ",C17,");"), IF(B17="Integer", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"')-&gt;unsigned()-&gt;default(0);"), IF(B17="Text", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"');"), IF(B17="Date", CONCATENATE("$table-&gt;",LOWER(B17),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('email', 255);</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('birth_place', 200);</v>
+        <f>IF(B18="String", CONCATENATE("$table-&gt;",LOWER(B18),"('",A18,"', ",C18,");"), IF(B18="Integer", CONCATENATE("$table-&gt;",LOWER(B18),"('",A18,"')-&gt;unsigned()-&gt;default(0);"), IF(B18="Text", CONCATENATE("$table-&gt;",LOWER(B18),"('",A18,"');"), IF(B18="Date", CONCATENATE("$table-&gt;",LOWER(B18),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('zip_code', 100);</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('personal_phone', 30);</v>
+        <f>IF(B19="String", CONCATENATE("$table-&gt;",LOWER(B19),"('",A19,"', ",C19,");"), IF(B19="Integer", CONCATENATE("$table-&gt;",LOWER(B19),"('",A19,"')-&gt;unsigned()-&gt;default(0);"), IF(B19="Text", CONCATENATE("$table-&gt;",LOWER(B19),"('",A19,"');"), IF(B19="Date", CONCATENATE("$table-&gt;",LOWER(B19),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('birth_place', 200);</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1067,13 +1180,13 @@
         <v>30</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('office_phone', 30);</v>
+        <f>IF(B20="String", CONCATENATE("$table-&gt;",LOWER(B20),"('",A20,"', ",C20,");"), IF(B20="Integer", CONCATENATE("$table-&gt;",LOWER(B20),"('",A20,"')-&gt;unsigned()-&gt;default(0);"), IF(B20="Text", CONCATENATE("$table-&gt;",LOWER(B20),"('",A20,"');"), IF(B20="Date", CONCATENATE("$table-&gt;",LOWER(B20),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('personal_phone', 30);</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1082,28 +1195,28 @@
         <v>30</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('fax', 30);</v>
+        <f>IF(B21="String", CONCATENATE("$table-&gt;",LOWER(B21),"('",A21,"', ",C21,");"), IF(B21="Integer", CONCATENATE("$table-&gt;",LOWER(B21),"('",A21,"')-&gt;unsigned()-&gt;default(0);"), IF(B21="Text", CONCATENATE("$table-&gt;",LOWER(B21),"('",A21,"');"), IF(B21="Date", CONCATENATE("$table-&gt;",LOWER(B21),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('office_phone', 30);</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22">
-        <v>255</v>
+        <v>30</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('tax_code', 255);</v>
+        <f>IF(B22="String", CONCATENATE("$table-&gt;",LOWER(B22),"('",A22,"', ",C22,");"), IF(B22="Integer", CONCATENATE("$table-&gt;",LOWER(B22),"('",A22,"')-&gt;unsigned()-&gt;default(0);"), IF(B22="Text", CONCATENATE("$table-&gt;",LOWER(B22),"('",A22,"');"), IF(B22="Date", CONCATENATE("$table-&gt;",LOWER(B22),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('fax', 30);</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -1112,112 +1225,112 @@
         <v>255</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('photo', 255);</v>
+        <f>IF(B23="String", CONCATENATE("$table-&gt;",LOWER(B23),"('",A23,"', ",C23,");"), IF(B23="Integer", CONCATENATE("$table-&gt;",LOWER(B23),"('",A23,"')-&gt;unsigned()-&gt;default(0);"), IF(B23="Text", CONCATENATE("$table-&gt;",LOWER(B23),"('",A23,"');"), IF(B23="Date", CONCATENATE("$table-&gt;",LOWER(B23),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('tax_code', 255);</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>255</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;integer('type_photo');</v>
+        <f>IF(B24="String", CONCATENATE("$table-&gt;",LOWER(B24),"('",A24,"', ",C24,");"), IF(B24="Integer", CONCATENATE("$table-&gt;",LOWER(B24),"('",A24,"')-&gt;unsigned()-&gt;default(0);"), IF(B24="Text", CONCATENATE("$table-&gt;",LOWER(B24),"('",A24,"');"), IF(B24="Date", CONCATENATE("$table-&gt;",LOWER(B24),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('photo', 255);</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;date('date_last_visit');</v>
+        <f>IF(B25="String", CONCATENATE("$table-&gt;",LOWER(B25),"('",A25,"', ",C25,");"), IF(B25="Integer", CONCATENATE("$table-&gt;",LOWER(B25),"('",A25,"')-&gt;unsigned()-&gt;default(0);"), IF(B25="Text", CONCATENATE("$table-&gt;",LOWER(B25),"('",A25,"');"), IF(B25="Date", CONCATENATE("$table-&gt;",LOWER(B25),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;integer('type_photo')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;date('date_next_visit');</v>
+        <f>IF(B26="String", CONCATENATE("$table-&gt;",LOWER(B26),"('",A26,"', ",C26,");"), IF(B26="Integer", CONCATENATE("$table-&gt;",LOWER(B26),"('",A26,"')-&gt;unsigned()-&gt;default(0);"), IF(B26="Text", CONCATENATE("$table-&gt;",LOWER(B26),"('",A26,"');"), IF(B26="Date", CONCATENATE("$table-&gt;",LOWER(B26),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;date('date_last_visit');</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;date('date_first_visit');</v>
+        <f>IF(B27="String", CONCATENATE("$table-&gt;",LOWER(B27),"('",A27,"', ",C27,");"), IF(B27="Integer", CONCATENATE("$table-&gt;",LOWER(B27),"('",A27,"')-&gt;unsigned()-&gt;default(0);"), IF(B27="Text", CONCATENATE("$table-&gt;",LOWER(B27),"('",A27,"');"), IF(B27="Date", CONCATENATE("$table-&gt;",LOWER(B27),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;date('date_next_visit');</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>15</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;date('date_last_pay');</v>
+        <f>IF(B28="String", CONCATENATE("$table-&gt;",LOWER(B28),"('",A28,"', ",C28,");"), IF(B28="Integer", CONCATENATE("$table-&gt;",LOWER(B28),"('",A28,"')-&gt;unsigned()-&gt;default(0);"), IF(B28="Text", CONCATENATE("$table-&gt;",LOWER(B28),"('",A28,"');"), IF(B28="Date", CONCATENATE("$table-&gt;",LOWER(B28),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;date('date_first_visit');</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;text('note');</v>
+        <f>IF(B29="String", CONCATENATE("$table-&gt;",LOWER(B29),"('",A29,"', ",C29,");"), IF(B29="Integer", CONCATENATE("$table-&gt;",LOWER(B29),"('",A29,"')-&gt;unsigned()-&gt;default(0);"), IF(B29="Text", CONCATENATE("$table-&gt;",LOWER(B29),"('",A29,"');"), IF(B29="Date", CONCATENATE("$table-&gt;",LOWER(B29),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;date('date_last_pay');</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;integer('discount');</v>
+        <f>IF(B30="String", CONCATENATE("$table-&gt;",LOWER(B30),"('",A30,"', ",C30,");"), IF(B30="Integer", CONCATENATE("$table-&gt;",LOWER(B30),"('",A30,"')-&gt;unsigned()-&gt;default(0);"), IF(B30="Text", CONCATENATE("$table-&gt;",LOWER(B30),"('",A30,"');"), IF(B30="Date", CONCATENATE("$table-&gt;",LOWER(B30),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note');</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('insurance', 100);</v>
+        <f>IF(B31="String", CONCATENATE("$table-&gt;",LOWER(B31),"('",A31,"', ",C31,");"), IF(B31="Integer", CONCATENATE("$table-&gt;",LOWER(B31),"('",A31,"')-&gt;unsigned()-&gt;default(0);"), IF(B31="Text", CONCATENATE("$table-&gt;",LOWER(B31),"('",A31,"');"), IF(B31="Date", CONCATENATE("$table-&gt;",LOWER(B31),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;integer('discount')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -1226,232 +1339,229 @@
         <v>100</v>
       </c>
       <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('doctor_name', 100);</v>
+        <f>IF(B32="String", CONCATENATE("$table-&gt;",LOWER(B32),"('",A32,"', ",C32,");"), IF(B32="Integer", CONCATENATE("$table-&gt;",LOWER(B32),"('",A32,"')-&gt;unsigned()-&gt;default(0);"), IF(B32="Text", CONCATENATE("$table-&gt;",LOWER(B32),"('",A32,"');"), IF(B32="Date", CONCATENATE("$table-&gt;",LOWER(B32),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('insurance', 100);</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('phone_doctor', 50);</v>
+        <f>IF(B33="String", CONCATENATE("$table-&gt;",LOWER(B33),"('",A33,"', ",C33,");"), IF(B33="Integer", CONCATENATE("$table-&gt;",LOWER(B33),"('",A33,"')-&gt;unsigned()-&gt;default(0);"), IF(B33="Text", CONCATENATE("$table-&gt;",LOWER(B33),"('",A33,"');"), IF(B33="Date", CONCATENATE("$table-&gt;",LOWER(B33),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;integer('user_update')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
       </c>
       <c r="C34">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('adult_child', 10);</v>
+        <f>IF(B34="String", CONCATENATE("$table-&gt;",LOWER(B34),"('",A34,"', ",C34,");"), IF(B34="Integer", CONCATENATE("$table-&gt;",LOWER(B34),"('",A34,"')-&gt;unsigned()-&gt;default(0);"), IF(B34="Text", CONCATENATE("$table-&gt;",LOWER(B34),"('",A34,"');"), IF(B34="Date", CONCATENATE("$table-&gt;",LOWER(B34),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('doctor_name', 100);</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>50</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;integer('age');</v>
+        <f>IF(B35="String", CONCATENATE("$table-&gt;",LOWER(B35),"('",A35,"', ",C35,");"), IF(B35="Integer", CONCATENATE("$table-&gt;",LOWER(B35),"('",A35,"')-&gt;unsigned()-&gt;default(0);"), IF(B35="Text", CONCATENATE("$table-&gt;",LOWER(B35),"('",A35,"');"), IF(B35="Date", CONCATENATE("$table-&gt;",LOWER(B35),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('phone_doctor', 50);</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
       </c>
       <c r="C36">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('barcode', 20);</v>
+        <f>IF(B36="String", CONCATENATE("$table-&gt;",LOWER(B36),"('",A36,"', ",C36,");"), IF(B36="Integer", CONCATENATE("$table-&gt;",LOWER(B36),"('",A36,"')-&gt;unsigned()-&gt;default(0);"), IF(B36="Text", CONCATENATE("$table-&gt;",LOWER(B36),"('",A36,"');"), IF(B36="Date", CONCATENATE("$table-&gt;",LOWER(B36),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('adult_child', 10);</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('province', 50);</v>
+        <f>IF(B37="String", CONCATENATE("$table-&gt;",LOWER(B37),"('",A37,"', ",C37,");"), IF(B37="Integer", CONCATENATE("$table-&gt;",LOWER(B37),"('",A37,"')-&gt;unsigned()-&gt;default(0);"), IF(B37="Text", CONCATENATE("$table-&gt;",LOWER(B37),"('",A37,"');"), IF(B37="Date", CONCATENATE("$table-&gt;",LOWER(B37),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;integer('age')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
       </c>
       <c r="C38">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('id_family', 50);</v>
+        <f>IF(B38="String", CONCATENATE("$table-&gt;",LOWER(B38),"('",A38,"', ",C38,");"), IF(B38="Integer", CONCATENATE("$table-&gt;",LOWER(B38),"('",A38,"')-&gt;unsigned()-&gt;default(0);"), IF(B38="Text", CONCATENATE("$table-&gt;",LOWER(B38),"('",A38,"');"), IF(B38="Date", CONCATENATE("$table-&gt;",LOWER(B38),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('barcode', 20);</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <v>50</v>
       </c>
       <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;integer('family_type');</v>
+        <f>IF(B39="String", CONCATENATE("$table-&gt;",LOWER(B39),"('",A39,"', ",C39,");"), IF(B39="Integer", CONCATENATE("$table-&gt;",LOWER(B39),"('",A39,"')-&gt;unsigned()-&gt;default(0);"), IF(B39="Text", CONCATENATE("$table-&gt;",LOWER(B39),"('",A39,"');"), IF(B39="Date", CONCATENATE("$table-&gt;",LOWER(B39),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('province', 50);</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
       </c>
       <c r="C40">
-        <v>255</v>
+        <v>50</v>
       </c>
       <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('nation', 255);</v>
+        <f>IF(B40="String", CONCATENATE("$table-&gt;",LOWER(B40),"('",A40,"', ",C40,");"), IF(B40="Integer", CONCATENATE("$table-&gt;",LOWER(B40),"('",A40,"')-&gt;unsigned()-&gt;default(0);"), IF(B40="Text", CONCATENATE("$table-&gt;",LOWER(B40),"('",A40,"');"), IF(B40="Date", CONCATENATE("$table-&gt;",LOWER(B40),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('id_family', 50);</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41">
-        <v>255</v>
+        <v>25</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('site', 255);</v>
+        <f>IF(B41="String", CONCATENATE("$table-&gt;",LOWER(B41),"('",A41,"', ",C41,");"), IF(B41="Integer", CONCATENATE("$table-&gt;",LOWER(B41),"('",A41,"')-&gt;unsigned()-&gt;default(0);"), IF(B41="Text", CONCATENATE("$table-&gt;",LOWER(B41),"('",A41,"');"), IF(B41="Date", CONCATENATE("$table-&gt;",LOWER(B41),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;integer('family_type')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <v>255</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;text('note1');</v>
+        <f>IF(B42="String", CONCATENATE("$table-&gt;",LOWER(B42),"('",A42,"', ",C42,");"), IF(B42="Integer", CONCATENATE("$table-&gt;",LOWER(B42),"('",A42,"')-&gt;unsigned()-&gt;default(0);"), IF(B42="Text", CONCATENATE("$table-&gt;",LOWER(B42),"('",A42,"');"), IF(B42="Date", CONCATENATE("$table-&gt;",LOWER(B42),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('nation', 255);</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>6</v>
+      </c>
+      <c r="C43">
+        <v>255</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;text('note2');</v>
+        <f>IF(B43="String", CONCATENATE("$table-&gt;",LOWER(B43),"('",A43,"', ",C43,");"), IF(B43="Integer", CONCATENATE("$table-&gt;",LOWER(B43),"('",A43,"')-&gt;unsigned()-&gt;default(0);"), IF(B43="Text", CONCATENATE("$table-&gt;",LOWER(B43),"('",A43,"');"), IF(B43="Date", CONCATENATE("$table-&gt;",LOWER(B43),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('site', 255);</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>31</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;text('note3');</v>
+        <f>IF(B44="String", CONCATENATE("$table-&gt;",LOWER(B44),"('",A44,"', ",C44,");"), IF(B44="Integer", CONCATENATE("$table-&gt;",LOWER(B44),"('",A44,"')-&gt;unsigned()-&gt;default(0);"), IF(B44="Text", CONCATENATE("$table-&gt;",LOWER(B44),"('",A44,"');"), IF(B44="Date", CONCATENATE("$table-&gt;",LOWER(B44),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note1');</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>31</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;text('note4');</v>
+        <f>IF(B45="String", CONCATENATE("$table-&gt;",LOWER(B45),"('",A45,"', ",C45,");"), IF(B45="Integer", CONCATENATE("$table-&gt;",LOWER(B45),"('",A45,"')-&gt;unsigned()-&gt;default(0);"), IF(B45="Text", CONCATENATE("$table-&gt;",LOWER(B45),"('",A45,"');"), IF(B45="Date", CONCATENATE("$table-&gt;",LOWER(B45),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note2');</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
         <v>31</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;text('note5');</v>
+        <f>IF(B46="String", CONCATENATE("$table-&gt;",LOWER(B46),"('",A46,"', ",C46,");"), IF(B46="Integer", CONCATENATE("$table-&gt;",LOWER(B46),"('",A46,"')-&gt;unsigned()-&gt;default(0);"), IF(B46="Text", CONCATENATE("$table-&gt;",LOWER(B46),"('",A46,"');"), IF(B46="Date", CONCATENATE("$table-&gt;",LOWER(B46),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note3');</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('sms_notify_news', 1);</v>
+        <f>IF(B47="String", CONCATENATE("$table-&gt;",LOWER(B47),"('",A47,"', ",C47,");"), IF(B47="Integer", CONCATENATE("$table-&gt;",LOWER(B47),"('",A47,"')-&gt;unsigned()-&gt;default(0);"), IF(B47="Text", CONCATENATE("$table-&gt;",LOWER(B47),"('",A47,"');"), IF(B47="Date", CONCATENATE("$table-&gt;",LOWER(B47),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note4');</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('patient_status', 30);</v>
+        <f>IF(B48="String", CONCATENATE("$table-&gt;",LOWER(B48),"('",A48,"', ",C48,");"), IF(B48="Integer", CONCATENATE("$table-&gt;",LOWER(B48),"('",A48,"')-&gt;unsigned()-&gt;default(0);"), IF(B48="Text", CONCATENATE("$table-&gt;",LOWER(B48),"('",A48,"');"), IF(B48="Date", CONCATENATE("$table-&gt;",LOWER(B48),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note5');</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>6</v>
@@ -1460,198 +1570,294 @@
         <v>1</v>
       </c>
       <c r="D49" t="str">
-        <f>IF(B54="String", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"', ",C54,");"), IF(B54="Integer", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"');"), IF(B54="Text", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"');"), IF(B54="Date", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"');")) )))</f>
-        <v>$table-&gt;string('option', 100);</v>
+        <f>IF(B49="String", CONCATENATE("$table-&gt;",LOWER(B49),"('",A49,"', ",C49,");"), IF(B49="Integer", CONCATENATE("$table-&gt;",LOWER(B49),"('",A49,"')-&gt;unsigned()-&gt;default(0);"), IF(B49="Text", CONCATENATE("$table-&gt;",LOWER(B49),"('",A49,"');"), IF(B49="Date", CONCATENATE("$table-&gt;",LOWER(B49),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('sms_notify_news', 1);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50">
+        <v>30</v>
+      </c>
+      <c r="D50" t="str">
+        <f>IF(B50="String", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"', ",C50,");"), IF(B50="Integer", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"')-&gt;unsigned()-&gt;default(0);"), IF(B50="Text", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"');"), IF(B50="Date", CONCATENATE("$table-&gt;",LOWER(B50),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('patient_status', 30);</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="str">
+        <f>IF(B51="String", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"', ",C51,");"), IF(B51="Integer", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"')-&gt;unsigned()-&gt;default(0);"), IF(B51="Text", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"');"), IF(B51="Date", CONCATENATE("$table-&gt;",LOWER(B51),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('head_household', 1);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54">
-        <v>100</v>
-      </c>
-      <c r="D54" s="4" t="str">
-        <f>IF(B54="String", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"', ",C54,");"), IF(B54="Integer", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"');"), IF(B54="Text", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"');"), IF(B54="Date", CONCATENATE("$table-&gt;",LOWER(B54),"('",A54,"');")) )))</f>
-        <v>$table-&gt;string('option', 100);</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55">
-        <v>100</v>
-      </c>
-      <c r="D55" s="4" t="str">
-        <f t="shared" ref="D55:D57" si="1">IF(B55="String", CONCATENATE("$table-&gt;",LOWER(B55),"('",A55,"', ",C55,");"), IF(B55="Integer", CONCATENATE("$table-&gt;",LOWER(B55),"('",A55,"');"), IF(B55="Text", CONCATENATE("$table-&gt;",LOWER(B55),"('",A55,"');"), IF(B55="Date", CONCATENATE("$table-&gt;",LOWER(B55),"('",A55,"');")) )))</f>
-        <v>$table-&gt;string('section', 100);</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>57</v>
-      </c>
-      <c r="B56" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C56">
         <v>100</v>
       </c>
-      <c r="D56" s="4" t="str">
+      <c r="D56" s="3" t="str">
+        <f t="shared" ref="D56:D59" si="0">IF(B56="String", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"', ",C56,");"), IF(B56="Integer", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"')-&gt;unsigned()-&gt;default(0);"), IF(B56="Text", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');"), IF(B56="Date", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');")) )))</f>
+        <v>$table-&gt;string('option', 100);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57">
+        <v>100</v>
+      </c>
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>$table-&gt;string('section', 100);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58">
+        <v>100</v>
+      </c>
+      <c r="D58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>$table-&gt;string('description', 100);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59">
+        <v>100</v>
+      </c>
+      <c r="D59" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>$table-&gt;string('value', 100);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64">
+        <v>100</v>
+      </c>
+      <c r="D64" s="3" t="str">
+        <f t="shared" ref="D64:D67" si="1">IF(B64="String", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"', ",C64,");"), IF(B64="Integer", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"')-&gt;unsigned()-&gt;default(0);"), IF(B64="Text", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');"), IF(B64="Date", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');")) )))</f>
+        <v>$table-&gt;string('des_dom', 100);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65">
+        <v>100</v>
+      </c>
+      <c r="D65" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>$table-&gt;integer('order')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66">
+        <v>100</v>
+      </c>
+      <c r="D66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>$table-&gt;string('description', 100);</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57">
+      <c r="B67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67">
         <v>100</v>
       </c>
-      <c r="D57" s="4" t="str">
+      <c r="D67" s="3" t="str">
         <f t="shared" si="1"/>
         <v>$table-&gt;string('value', 100);</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B71" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C71" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D71" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62">
-        <v>100</v>
-      </c>
-      <c r="D62" s="4" t="str">
-        <f>IF(B62="String", CONCATENATE("$table-&gt;",LOWER(B62),"('",A62,"', ",C62,");"), IF(B62="Integer", CONCATENATE("$table-&gt;",LOWER(B62),"('",A62,"');"), IF(B62="Text", CONCATENATE("$table-&gt;",LOWER(B62),"('",A62,"');"), IF(B62="Date", CONCATENATE("$table-&gt;",LOWER(B62),"('",A62,"');")) )))</f>
-        <v>$table-&gt;string('des_dom', 100);</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>61</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63">
-        <v>100</v>
-      </c>
-      <c r="D63" s="4" t="str">
-        <f t="shared" ref="D63:D65" si="2">IF(B63="String", CONCATENATE("$table-&gt;",LOWER(B63),"('",A63,"', ",C63,");"), IF(B63="Integer", CONCATENATE("$table-&gt;",LOWER(B63),"('",A63,"');"), IF(B63="Text", CONCATENATE("$table-&gt;",LOWER(B63),"('",A63,"');"), IF(B63="Date", CONCATENATE("$table-&gt;",LOWER(B63),"('",A63,"');")) )))</f>
-        <v>$table-&gt;integer('order');</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>57</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64">
-        <v>100</v>
-      </c>
-      <c r="D64" s="4" t="str">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72">
+        <v>255</v>
+      </c>
+      <c r="D72" s="3" t="str">
+        <f t="shared" ref="D72:D75" si="2">IF(B72="String", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"', ",C72,");"), IF(B72="Integer", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"')-&gt;unsigned()-&gt;default(0);"), IF(B72="Text", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');"), IF(B72="Date", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');")) )))</f>
+        <v>$table-&gt;string('path', 255);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+      <c r="D73" s="3" t="b">
         <f t="shared" si="2"/>
-        <v>$table-&gt;string('description', 100);</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>58</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65">
-        <v>100</v>
-      </c>
-      <c r="D65" s="4" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+      <c r="D74" s="3" t="b">
         <f t="shared" si="2"/>
-        <v>$table-&gt;string('value', 100);</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="2"/>
+      <c r="D75" s="3" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A51:D52"/>
-    <mergeCell ref="A59:D60"/>
+    <mergeCell ref="A53:D54"/>
+    <mergeCell ref="A61:D62"/>
+    <mergeCell ref="A69:D70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Created Calendar, next step is to render the create new event with AJAX
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tables" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -354,11 +354,10 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="3" tint="-0.499984740745262"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.59999389629810485"/>
@@ -369,16 +368,19 @@
         <left style="thin">
           <color theme="0"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
         <top style="thin">
           <color theme="0"/>
         </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -417,9 +419,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -473,10 +472,11 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="3" tint="-0.499984740745262"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.59999389629810485"/>
@@ -487,19 +487,16 @@
         <left style="thin">
           <color theme="0"/>
         </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
+        <right/>
         <top style="thin">
           <color theme="0"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -541,6 +538,9 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -561,7 +561,7 @@
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="3">
+    <tableColumn id="4" name="Code generated" dataDxfId="9">
       <calculatedColumnFormula>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"')-&gt;unsigned()-&gt;default(0);"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5),"('",Table1[[#This Row],[Column name]],"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -570,13 +570,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A55:D59" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A55:D59" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A55:D59"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="8"/>
+    <tableColumn id="2" name="Type" dataDxfId="7"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="1">
+    <tableColumn id="4" name="Code generated" dataDxfId="6">
       <calculatedColumnFormula>IF(B56="String", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"', ",C56,");"), IF(B56="Integer", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"')-&gt;unsigned()-&gt;default(0);"), IF(B56="Text", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');"), IF(B56="Date", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -585,13 +585,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A63:D67" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A63:D67" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A63:D67"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="6"/>
+    <tableColumn id="2" name="Type" dataDxfId="4"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="2">
+    <tableColumn id="4" name="Code generated" dataDxfId="3">
       <calculatedColumnFormula>IF(B64="String", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"', ",C64,");"), IF(B64="Integer", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"')-&gt;unsigned()-&gt;default(0);"), IF(B64="Text", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');"), IF(B64="Date", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -600,11 +600,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A71:D75" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A71:D75" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A71:D75"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="4"/>
+    <tableColumn id="2" name="Type" dataDxfId="1"/>
     <tableColumn id="3" name="Length"/>
     <tableColumn id="4" name="Code generated" dataDxfId="0">
       <calculatedColumnFormula>IF(B72="String", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"', ",C72,");"), IF(B72="Integer", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"')-&gt;unsigned()-&gt;default(0);"), IF(B72="Text", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');"), IF(B72="Date", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');")) )))</calculatedColumnFormula>
@@ -657,7 +657,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -692,7 +692,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>

</xml_diff>

<commit_message>
- Calendar: CRUD operations woks well
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
   <si>
     <t>PATIENT</t>
   </si>
@@ -212,13 +212,28 @@
   </si>
   <si>
     <t>sex</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>end_time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +244,13 @@
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -286,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,11 +321,136 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -561,7 +708,7 @@
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="9">
+    <tableColumn id="4" name="Code generated" dataDxfId="15">
       <calculatedColumnFormula>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"')-&gt;unsigned()-&gt;default(0);"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5),"('",Table1[[#This Row],[Column name]],"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -570,13 +717,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A55:D59" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A55:D59" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A55:D59"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="7"/>
+    <tableColumn id="2" name="Type" dataDxfId="13"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="6">
+    <tableColumn id="4" name="Code generated" dataDxfId="12">
       <calculatedColumnFormula>IF(B56="String", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"', ",C56,");"), IF(B56="Integer", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"')-&gt;unsigned()-&gt;default(0);"), IF(B56="Text", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');"), IF(B56="Date", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -585,13 +732,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A63:D67" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A63:D67" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A63:D67"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="4"/>
+    <tableColumn id="2" name="Type" dataDxfId="10"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="3">
+    <tableColumn id="4" name="Code generated" dataDxfId="9">
       <calculatedColumnFormula>IF(B64="String", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"', ",C64,");"), IF(B64="Integer", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"')-&gt;unsigned()-&gt;default(0);"), IF(B64="Text", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');"), IF(B64="Date", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -600,14 +747,29 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A71:D75" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A71:D75" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A71:D75"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="1"/>
+    <tableColumn id="2" name="Type" dataDxfId="7"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="0">
+    <tableColumn id="4" name="Code generated" dataDxfId="6">
       <calculatedColumnFormula>IF(B72="String", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"', ",C72,");"), IF(B72="Integer", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"')-&gt;unsigned()-&gt;default(0);"), IF(B72="Text", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');"), IF(B72="Date", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');")) )))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A81:D85" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0">
+  <autoFilter ref="A81:D85"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Column name" dataDxfId="4"/>
+    <tableColumn id="2" name="Type" dataDxfId="3"/>
+    <tableColumn id="3" name="Length" dataDxfId="2"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="1">
+      <calculatedColumnFormula>IF(B82="String", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"', ",C82,");"), IF(B82="Integer", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"')-&gt;unsigned()-&gt;default(0);"), IF(B82="Text", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"');"), IF(B82="Date", CONCATENATE("$table-&gt;","timestamp","('",A82,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -657,7 +819,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -692,7 +854,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -901,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,22 +1078,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1605,18 +1767,18 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -1693,18 +1855,18 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -1781,18 +1943,18 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
@@ -1844,20 +2006,104 @@
         <v>0</v>
       </c>
     </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" s="8">
+        <v>250</v>
+      </c>
+      <c r="D82" s="9" t="str">
+        <f t="shared" ref="D82:D85" si="3">IF(B82="String", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"', ",C82,");"), IF(B82="Integer", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"')-&gt;unsigned()-&gt;default(0);"), IF(B82="Text", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"');"), IF(B82="Date", CONCATENATE("$table-&gt;","timestamp","('",A82,"');")) )))</f>
+        <v>$table-&gt;string('name', 250);</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>$table-&gt;text('title');</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="8"/>
+      <c r="D84" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>$table-&gt;timestamp('start_time');</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="8"/>
+      <c r="D85" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>$table-&gt;timestamp('end_time');</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A53:D54"/>
     <mergeCell ref="A61:D62"/>
     <mergeCell ref="A69:D70"/>
+    <mergeCell ref="A79:D80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- My Account panel: 1- My profile 2- Contacts 3- Mailbox
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="83">
   <si>
     <t>PATIENT</t>
   </si>
@@ -227,13 +227,49 @@
   </si>
   <si>
     <t>end_time</t>
+  </si>
+  <si>
+    <t>role_id</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>$table-&gt;integer('role_id')-&gt;index()-&gt;unsigned()-&gt;nullable();</t>
+  </si>
+  <si>
+    <t>$table-&gt;integer('is_active')-&gt;default(0);</t>
+  </si>
+  <si>
+    <t>$table-&gt;string('email', 200)-&gt;unique();</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>image_id</t>
+  </si>
+  <si>
+    <t>$table-&gt;integer('image_id');</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,8 +291,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF808080"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF660000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,8 +330,14 @@
         <bgColor theme="4" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -304,11 +371,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -330,11 +408,73 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -348,6 +488,189 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -449,6 +772,20 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -708,7 +1045,7 @@
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="15">
+    <tableColumn id="4" name="Code generated" dataDxfId="27">
       <calculatedColumnFormula>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"')-&gt;unsigned()-&gt;default(0);"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5),"('",Table1[[#This Row],[Column name]],"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -717,13 +1054,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A55:D59" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A55:D59" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A55:D59"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="13"/>
+    <tableColumn id="2" name="Type" dataDxfId="25"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="12">
+    <tableColumn id="4" name="Code generated" dataDxfId="24">
       <calculatedColumnFormula>IF(B56="String", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"', ",C56,");"), IF(B56="Integer", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"')-&gt;unsigned()-&gt;default(0);"), IF(B56="Text", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');"), IF(B56="Date", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -732,13 +1069,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A63:D67" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A63:D67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A63:D68" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A63:D68"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="10"/>
+    <tableColumn id="2" name="Type" dataDxfId="22"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="9">
+    <tableColumn id="4" name="Code generated" dataDxfId="21">
       <calculatedColumnFormula>IF(B64="String", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"', ",C64,");"), IF(B64="Integer", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"')-&gt;unsigned()-&gt;default(0);"), IF(B64="Text", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');"), IF(B64="Date", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -747,14 +1084,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A71:D75" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A71:D75"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A72:D74" totalsRowShown="0" headerRowDxfId="20">
+  <autoFilter ref="A72:D74"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="7"/>
+    <tableColumn id="2" name="Type" dataDxfId="19"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="6">
-      <calculatedColumnFormula>IF(B72="String", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"', ",C72,");"), IF(B72="Integer", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"')-&gt;unsigned()-&gt;default(0);"), IF(B72="Text", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');"), IF(B72="Date", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');")) )))</calculatedColumnFormula>
+    <tableColumn id="4" name="Code generated" dataDxfId="18">
+      <calculatedColumnFormula>IF(B73="String", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"', ",C73,");"), IF(B73="Integer", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"')-&gt;unsigned()-&gt;default(0);"), IF(B73="Text", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"');"), IF(B73="Date", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -762,15 +1099,41 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A81:D85" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0">
-  <autoFilter ref="A81:D85"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A80:D84" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A80:D84"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Column name" dataDxfId="4"/>
-    <tableColumn id="2" name="Type" dataDxfId="3"/>
-    <tableColumn id="3" name="Length" dataDxfId="2"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="1">
-      <calculatedColumnFormula>IF(B82="String", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"', ",C82,");"), IF(B82="Integer", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"')-&gt;unsigned()-&gt;default(0);"), IF(B82="Text", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"');"), IF(B82="Date", CONCATENATE("$table-&gt;","timestamp","('",A82,"');")) )))</calculatedColumnFormula>
+    <tableColumn id="1" name="Column name" dataDxfId="15"/>
+    <tableColumn id="2" name="Type" dataDxfId="14"/>
+    <tableColumn id="3" name="Length" dataDxfId="13"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="12">
+      <calculatedColumnFormula>IF(B81="String", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"', ",C81,");"), IF(B81="Integer", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"')-&gt;unsigned()-&gt;default(0);"), IF(B81="Text", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"');"), IF(B81="Date", CONCATENATE("$table-&gt;","timestamp","('",A81,"');")) )))</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A89:D98" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A89:D98"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Column name" dataDxfId="9"/>
+    <tableColumn id="2" name="Type" dataDxfId="8"/>
+    <tableColumn id="3" name="Length" dataDxfId="7"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A103:D105" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A103:D105"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Column name" dataDxfId="3"/>
+    <tableColumn id="2" name="Type" dataDxfId="2"/>
+    <tableColumn id="3" name="Length" dataDxfId="1"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1063,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,26 +1437,26 @@
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1767,18 +2130,18 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -1855,18 +2218,18 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -1893,7 +2256,7 @@
         <v>100</v>
       </c>
       <c r="D64" s="3" t="str">
-        <f t="shared" ref="D64:D67" si="1">IF(B64="String", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"', ",C64,");"), IF(B64="Integer", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"')-&gt;unsigned()-&gt;default(0);"), IF(B64="Text", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');"), IF(B64="Date", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');")) )))</f>
+        <f t="shared" ref="D64:D66" si="1">IF(B64="String", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"', ",C64,");"), IF(B64="Integer", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"')-&gt;unsigned()-&gt;default(0);"), IF(B64="Text", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');"), IF(B64="Date", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');")) )))</f>
         <v>$table-&gt;string('des_dom', 100);</v>
       </c>
     </row>
@@ -1938,58 +2301,60 @@
         <v>100</v>
       </c>
       <c r="D67" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(B67="String", CONCATENATE("$table-&gt;",LOWER(B67),"('",A67,"', ",C67,");"), IF(B67="Integer", CONCATENATE("$table-&gt;",LOWER(B67),"('",A67,"')-&gt;unsigned()-&gt;default(0);"), IF(B67="Text", CONCATENATE("$table-&gt;",LOWER(B67),"('",A67,"');"), IF(B67="Date", CONCATENATE("$table-&gt;",LOWER(B67),"('",A67,"');")) )))</f>
         <v>$table-&gt;string('value', 100);</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="19"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="20" t="b">
+        <f>IF(B68="String", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"', ",C68,");"), IF(B68="Integer", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"')-&gt;unsigned()-&gt;default(0);"), IF(B68="Text", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"');"), IF(B68="Date", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"');")) )))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="21"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D72" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>63</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C72">
+      <c r="B73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73">
         <v>255</v>
       </c>
-      <c r="D72" s="3" t="str">
-        <f t="shared" ref="D72:D75" si="2">IF(B72="String", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"', ",C72,");"), IF(B72="Integer", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"')-&gt;unsigned()-&gt;default(0);"), IF(B72="Text", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');"), IF(B72="Date", CONCATENATE("$table-&gt;",LOWER(B72),"('",A72,"');")) )))</f>
+      <c r="D73" s="3" t="str">
+        <f t="shared" ref="D73:D74" si="2">IF(B73="String", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"', ",C73,");"), IF(B73="Integer", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"')-&gt;unsigned()-&gt;default(0);"), IF(B73="Text", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"');"), IF(B73="Date", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"');")) )))</f>
         <v>$table-&gt;string('path', 255);</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="2"/>
-      <c r="D73" s="3" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1999,111 +2364,309 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="2"/>
-      <c r="D75" s="3" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B78" s="21"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
+      <c r="A79" s="21"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+      <c r="A80" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B80" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D80" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" s="8">
+        <v>250</v>
+      </c>
+      <c r="D81" s="9" t="str">
+        <f t="shared" ref="D81:D83" si="3">IF(B81="String", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"', ",C81,");"), IF(B81="Integer", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"')-&gt;unsigned()-&gt;default(0);"), IF(B81="Text", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"');"), IF(B81="Date", CONCATENATE("$table-&gt;","timestamp","('",A81,"');")) )))</f>
+        <v>$table-&gt;string('name', 250);</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" s="8">
-        <v>250</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C82" s="8"/>
       <c r="D82" s="9" t="str">
-        <f t="shared" ref="D82:D85" si="3">IF(B82="String", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"', ",C82,");"), IF(B82="Integer", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"')-&gt;unsigned()-&gt;default(0);"), IF(B82="Text", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"');"), IF(B82="Date", CONCATENATE("$table-&gt;","timestamp","('",A82,"');")) )))</f>
-        <v>$table-&gt;string('name', 250);</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>$table-&gt;text('title');</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>31</v>
+        <v>69</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>$table-&gt;text('title');</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="10" t="s">
-        <v>69</v>
+        <v>$table-&gt;timestamp('start_time');</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="B84" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v>$table-&gt;timestamp('start_time');</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B85" s="10" t="s">
+        <f>IF(B84="String", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"', ",C84,");"), IF(B84="Integer", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"')-&gt;unsigned()-&gt;default(0);"), IF(B84="Text", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"');"), IF(B84="Date", CONCATENATE("$table-&gt;","timestamp","('",A84,"');")) )))</f>
+        <v>$table-&gt;timestamp('end_time');</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B87" s="21"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="21"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="21"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="21"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G89" s="12"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C90" s="8">
+        <v>250</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" s="8"/>
+      <c r="D91" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C92" s="8"/>
+      <c r="D92" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G92" s="13"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" s="10">
+        <v>255</v>
+      </c>
+      <c r="D93" s="14" t="str">
+        <f>IF(B93="String", CONCATENATE("$table-&gt;",LOWER(B93),"('",A93,"', ",C93,");"), IF(B93="Integer", CONCATENATE("$table-&gt;",LOWER(B93),"('",A93,"')-&gt;unsigned()-&gt;default(0);"), IF(B93="Text", CONCATENATE("$table-&gt;",LOWER(B93),"('",A93,"');"), IF(B93="Date", CONCATENATE("$table-&gt;","timestamp","('",A93,"');")) )))</f>
+        <v>$table-&gt;string('first_name', 255);</v>
+      </c>
+      <c r="G93" s="13"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" s="10">
+        <v>255</v>
+      </c>
+      <c r="D94" s="14" t="str">
+        <f>IF(B94="String", CONCATENATE("$table-&gt;",LOWER(B94),"('",A94,"', ",C94,");"), IF(B94="Integer", CONCATENATE("$table-&gt;",LOWER(B94),"('",A94,"')-&gt;unsigned()-&gt;default(0);"), IF(B94="Text", CONCATENATE("$table-&gt;",LOWER(B94),"('",A94,"');"), IF(B94="Date", CONCATENATE("$table-&gt;","timestamp","('",A94,"');")) )))</f>
+        <v>$table-&gt;string('last_name', 255);</v>
+      </c>
+      <c r="G94" s="13"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B95" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C85" s="8"/>
-      <c r="D85" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v>$table-&gt;timestamp('end_time');</v>
-      </c>
+      <c r="C95" s="8"/>
+      <c r="D95" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G95" s="13"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B96" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" s="8">
+        <v>50</v>
+      </c>
+      <c r="D96" s="14" t="str">
+        <f>IF(B96="String", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"', ",C96,");"), IF(B96="Integer", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"')-&gt;unsigned()-&gt;default(0);"), IF(B96="Text", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"');"), IF(B96="Date", CONCATENATE("$table-&gt;","timestamp","('",A96,"');")) )))</f>
+        <v>$table-&gt;string('phone', 50);</v>
+      </c>
+      <c r="G96" s="13"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" s="8">
+        <v>255</v>
+      </c>
+      <c r="D97" s="14" t="str">
+        <f>IF(B97="String", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"', ",C97,");"), IF(B97="Integer", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"')-&gt;unsigned()-&gt;default(0);"), IF(B97="Text", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"');"), IF(B97="Date", CONCATENATE("$table-&gt;","timestamp","('",A97,"');")) )))</f>
+        <v>$table-&gt;string('password', 255);</v>
+      </c>
+      <c r="G97" s="13"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="15"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="16"/>
+      <c r="G98" s="13"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="21"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="21"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="21"/>
+      <c r="D102" s="21"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B103" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C103" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D103" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104" s="8">
+        <v>255</v>
+      </c>
+      <c r="D104" s="14" t="str">
+        <f>IF(B104="String", CONCATENATE("$table-&gt;",LOWER(B104),"('",A104,"', ",C104,");"), IF(B104="Integer", CONCATENATE("$table-&gt;",LOWER(B104),"('",A104,"')-&gt;unsigned()-&gt;default(0);"), IF(B104="Text", CONCATENATE("$table-&gt;",LOWER(B104),"('",A104,"');"), IF(B104="Date", CONCATENATE("$table-&gt;","timestamp","('",A104,"');")) )))</f>
+        <v>$table-&gt;string('status', 255);</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="15"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="15"/>
+      <c r="D105" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A101:D102"/>
+    <mergeCell ref="A87:D88"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A53:D54"/>
     <mergeCell ref="A61:D62"/>
-    <mergeCell ref="A69:D70"/>
-    <mergeCell ref="A79:D80"/>
+    <mergeCell ref="A70:D71"/>
+    <mergeCell ref="A78:D79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <tableParts count="5">
+  <tableParts count="7">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Most of work dedicated to validation forms (jQuery Validation)
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="84">
   <si>
     <t>PATIENT</t>
   </si>
@@ -262,14 +262,17 @@
     <t>image_id</t>
   </si>
   <si>
-    <t>$table-&gt;integer('image_id');</t>
+    <t>$table-&gt;integer('image_id')-&gt;index()-&gt;unsigned()-&gt;nullable();</t>
+  </si>
+  <si>
+    <t>$table-&gt;integer('user_update')-&gt;unsigned()-&gt;default(0);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,6 +317,13 @@
       <sz val="11"/>
       <color theme="3" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -386,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -432,6 +442,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1428,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93:D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1450,7 @@
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2497,7 +2510,7 @@
         <v>25</v>
       </c>
       <c r="C91" s="8"/>
-      <c r="D91" s="14" t="s">
+      <c r="D91" s="10" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2553,7 +2566,9 @@
       <c r="B95" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C95" s="8"/>
+      <c r="C95" s="8">
+        <v>200</v>
+      </c>
       <c r="D95" s="14" t="s">
         <v>76</v>
       </c>
@@ -2592,10 +2607,16 @@
       <c r="G97" s="13"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="15"/>
-      <c r="B98" s="7"/>
+      <c r="A98" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="C98" s="15"/>
-      <c r="D98" s="16"/>
+      <c r="D98" s="22" t="s">
+        <v>83</v>
+      </c>
       <c r="G98" s="13"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Making the app better and better
PS: Don't give up!
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="84">
   <si>
     <t>PATIENT</t>
   </si>
@@ -272,7 +272,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +324,12 @@
       <color theme="2" tint="-0.89999084444715716"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -396,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -440,10 +446,14 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1127,8 +1137,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A89:D98" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A89:D98"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A89:D99" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A89:D99"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="9"/>
     <tableColumn id="2" name="Type" dataDxfId="8"/>
@@ -1140,8 +1150,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A103:D105" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A103:D105"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A104:D106" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A104:D106"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="3"/>
     <tableColumn id="2" name="Type" dataDxfId="2"/>
@@ -1439,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93:D98"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,22 +1464,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2143,18 +2153,18 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="21"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -2231,18 +2241,18 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="21" t="s">
+      <c r="A61" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="21"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
+      <c r="A62" s="22"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -2328,18 +2338,18 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="21" t="s">
+      <c r="A70" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="21"/>
-      <c r="B71" s="21"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
+      <c r="A71" s="22"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
@@ -2378,18 +2388,18 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="21" t="s">
+      <c r="A78" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B78" s="21"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="21"/>
-      <c r="B79" s="21"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
+      <c r="A79" s="22"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
@@ -2460,18 +2470,18 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="21" t="s">
+      <c r="A87" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B87" s="21"/>
-      <c r="C87" s="21"/>
-      <c r="D87" s="21"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="21"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="21"/>
+      <c r="A88" s="22"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
@@ -2575,102 +2585,118 @@
       <c r="G95" s="13"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B96" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C96" s="8">
-        <v>50</v>
+      <c r="A96" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" s="23">
+        <v>255</v>
       </c>
       <c r="D96" s="14" t="str">
         <f>IF(B96="String", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"', ",C96,");"), IF(B96="Integer", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"')-&gt;unsigned()-&gt;default(0);"), IF(B96="Text", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"');"), IF(B96="Date", CONCATENATE("$table-&gt;","timestamp","('",A96,"');")) )))</f>
-        <v>$table-&gt;string('phone', 50);</v>
+        <v>$table-&gt;string('address', 255);</v>
       </c>
       <c r="G96" s="13"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B97" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B97" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C97" s="8">
-        <v>255</v>
+        <v>50</v>
       </c>
       <c r="D97" s="14" t="str">
         <f>IF(B97="String", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"', ",C97,");"), IF(B97="Integer", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"')-&gt;unsigned()-&gt;default(0);"), IF(B97="Text", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"');"), IF(B97="Date", CONCATENATE("$table-&gt;","timestamp","('",A97,"');")) )))</f>
+        <v>$table-&gt;string('phone', 50);</v>
+      </c>
+      <c r="G97" s="13"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98" s="8">
+        <v>255</v>
+      </c>
+      <c r="D98" s="14" t="str">
+        <f>IF(B98="String", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"', ",C98,");"), IF(B98="Integer", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"')-&gt;unsigned()-&gt;default(0);"), IF(B98="Text", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"');"), IF(B98="Date", CONCATENATE("$table-&gt;","timestamp","('",A98,"');")) )))</f>
         <v>$table-&gt;string('password', 255);</v>
       </c>
-      <c r="G97" s="13"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="15" t="s">
+      <c r="G98" s="13"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B99" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C98" s="15"/>
-      <c r="D98" s="22" t="s">
+      <c r="C99" s="15"/>
+      <c r="D99" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="G98" s="13"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="21" t="s">
+      <c r="G99" s="13"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B101" s="21"/>
-      <c r="C101" s="21"/>
-      <c r="D101" s="21"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="21"/>
-      <c r="B102" s="21"/>
-      <c r="C102" s="21"/>
-      <c r="D102" s="21"/>
+      <c r="B102" s="22"/>
+      <c r="C102" s="22"/>
+      <c r="D102" s="22"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="11" t="s">
+      <c r="A103" s="22"/>
+      <c r="B103" s="22"/>
+      <c r="C103" s="22"/>
+      <c r="D103" s="22"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B103" s="11" t="s">
+      <c r="B104" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C103" s="11" t="s">
+      <c r="C104" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D103" s="11" t="s">
+      <c r="D104" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="8" t="s">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B104" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C104" s="8">
+      <c r="B105" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C105" s="8">
         <v>255</v>
       </c>
-      <c r="D104" s="14" t="str">
-        <f>IF(B104="String", CONCATENATE("$table-&gt;",LOWER(B104),"('",A104,"', ",C104,");"), IF(B104="Integer", CONCATENATE("$table-&gt;",LOWER(B104),"('",A104,"')-&gt;unsigned()-&gt;default(0);"), IF(B104="Text", CONCATENATE("$table-&gt;",LOWER(B104),"('",A104,"');"), IF(B104="Date", CONCATENATE("$table-&gt;","timestamp","('",A104,"');")) )))</f>
+      <c r="D105" s="14" t="str">
+        <f>IF(B105="String", CONCATENATE("$table-&gt;",LOWER(B105),"('",A105,"', ",C105,");"), IF(B105="Integer", CONCATENATE("$table-&gt;",LOWER(B105),"('",A105,"')-&gt;unsigned()-&gt;default(0);"), IF(B105="Text", CONCATENATE("$table-&gt;",LOWER(B105),"('",A105,"');"), IF(B105="Date", CONCATENATE("$table-&gt;","timestamp","('",A105,"');")) )))</f>
         <v>$table-&gt;string('status', 255);</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="15"/>
-      <c r="B105" s="7"/>
-      <c r="C105" s="15"/>
-      <c r="D105" s="16"/>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="15"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A101:D102"/>
+    <mergeCell ref="A102:D103"/>
     <mergeCell ref="A87:D88"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A53:D54"/>
@@ -2679,15 +2705,15 @@
     <mergeCell ref="A78:D79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="7">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added patient at event modal
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="89">
   <si>
     <t>PATIENT</t>
   </si>
@@ -217,9 +217,6 @@
     <t>Events</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -266,13 +263,55 @@
   </si>
   <si>
     <t>$table-&gt;integer('user_update')-&gt;unsigned()-&gt;default(0);</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>foreign key</t>
+  </si>
+  <si>
+    <t>Type Column</t>
+  </si>
+  <si>
+    <t>$table-&gt;primary('id_patient');</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-&gt;string('id_patient');</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-&gt;foreign('id_patient')-&gt;references('id_patient')-&gt;on('patients');</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +371,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -353,7 +399,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -398,11 +444,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -420,7 +488,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -456,11 +523,59 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="30">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -581,6 +696,20 @@
     <dxf>
       <font>
         <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -698,6 +827,21 @@
     <dxf>
       <font>
         <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -718,10 +862,9 @@
           <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
+        <left/>
         <right/>
         <top style="thin">
           <color theme="0"/>
@@ -744,6 +887,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -767,13 +911,12 @@
           <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="0"/>
         </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
+        <right/>
         <top style="thin">
           <color theme="0"/>
         </top>
@@ -793,6 +936,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -807,6 +951,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1045,9 +1190,6 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1062,28 +1204,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D51" totalsRowShown="0">
-  <autoFilter ref="A4:D51"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E51" totalsRowShown="0">
+  <autoFilter ref="A4:E51"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="27">
+    <tableColumn id="4" name="Code generated" dataDxfId="0">
       <calculatedColumnFormula>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"')-&gt;unsigned()-&gt;default(0);"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5),"('",Table1[[#This Row],[Column name]],"');")) )))</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="5" name="Type Column"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A55:D59" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A55:D59" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A55:D59"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="25"/>
+    <tableColumn id="2" name="Type" dataDxfId="28"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="24">
+    <tableColumn id="4" name="Code generated" dataDxfId="27">
       <calculatedColumnFormula>IF(B56="String", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"', ",C56,");"), IF(B56="Integer", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"')-&gt;unsigned()-&gt;default(0);"), IF(B56="Text", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');"), IF(B56="Date", CONCATENATE("$table-&gt;",LOWER(B56),"('",A56,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1092,13 +1235,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A63:D68" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A63:D68" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A63:D68"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="22"/>
+    <tableColumn id="2" name="Type" dataDxfId="25"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="21">
+    <tableColumn id="4" name="Code generated" dataDxfId="24">
       <calculatedColumnFormula>IF(B64="String", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"', ",C64,");"), IF(B64="Integer", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"')-&gt;unsigned()-&gt;default(0);"), IF(B64="Text", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');"), IF(B64="Date", CONCATENATE("$table-&gt;",LOWER(B64),"('",A64,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1107,13 +1250,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A72:D74" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A72:D74" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A72:D74"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="19"/>
+    <tableColumn id="2" name="Type" dataDxfId="22"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="18">
+    <tableColumn id="4" name="Code generated" dataDxfId="21">
       <calculatedColumnFormula>IF(B73="String", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"', ",C73,");"), IF(B73="Integer", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"')-&gt;unsigned()-&gt;default(0);"), IF(B73="Text", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"');"), IF(B73="Date", CONCATENATE("$table-&gt;",LOWER(B73),"('",A73,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1122,41 +1265,43 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A80:D84" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A80:D84"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Column name" dataDxfId="15"/>
-    <tableColumn id="2" name="Type" dataDxfId="14"/>
-    <tableColumn id="3" name="Length" dataDxfId="13"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A80:E86" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A80:E86"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Column name" dataDxfId="18"/>
+    <tableColumn id="2" name="Type" dataDxfId="17"/>
+    <tableColumn id="3" name="Length" dataDxfId="16"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="15">
       <calculatedColumnFormula>IF(B81="String", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"', ",C81,");"), IF(B81="Integer", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"')-&gt;unsigned()-&gt;default(0);"), IF(B81="Text", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"');"), IF(B81="Date", CONCATENATE("$table-&gt;","timestamp","('",A81,"');")) )))</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="5" name="Type Column" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A89:D99" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A89:D99"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Column name" dataDxfId="9"/>
-    <tableColumn id="2" name="Type" dataDxfId="8"/>
-    <tableColumn id="3" name="Length" dataDxfId="7"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A90:E100" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A90:E100"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Column name" dataDxfId="11"/>
+    <tableColumn id="2" name="Type" dataDxfId="10"/>
+    <tableColumn id="3" name="Length" dataDxfId="9"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="8"/>
+    <tableColumn id="5" name="Type Column" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A104:D106" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A104:D106"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A105:D107" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A105:D107"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Column name" dataDxfId="3"/>
-    <tableColumn id="2" name="Type" dataDxfId="2"/>
-    <tableColumn id="3" name="Length" dataDxfId="1"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="0"/>
+    <tableColumn id="1" name="Column name" dataDxfId="4"/>
+    <tableColumn id="2" name="Type" dataDxfId="3"/>
+    <tableColumn id="3" name="Length" dataDxfId="2"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1205,7 +1350,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1240,7 +1385,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1449,10 +1594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,25 +1606,26 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1494,6 +1640,9 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1509,6 +1658,9 @@
         <f>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"')-&gt;unsigned()-&gt;default(0);"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('id_patient', 50);</v>
       </c>
+      <c r="E5" s="33" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2153,18 +2305,18 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
+      <c r="A53" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
+      <c r="A54" s="32"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -2241,18 +2393,18 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="22" t="s">
+      <c r="A61" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="22"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
-      <c r="B62" s="22"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="22"/>
+      <c r="A62" s="32"/>
+      <c r="B62" s="32"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="32"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -2283,7 +2435,7 @@
         <v>$table-&gt;string('des_dom', 100);</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -2298,7 +2450,7 @@
         <v>$table-&gt;integer('order')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>57</v>
       </c>
@@ -2313,7 +2465,7 @@
         <v>$table-&gt;string('description', 100);</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -2328,30 +2480,30 @@
         <v>$table-&gt;string('value', 100);</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="19"/>
-      <c r="B68" s="18"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="20" t="b">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="18"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="19" t="b">
         <f>IF(B68="String", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"', ",C68,");"), IF(B68="Integer", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"')-&gt;unsigned()-&gt;default(0);"), IF(B68="Text", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"');"), IF(B68="Date", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"');")) )))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="22" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="22"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="22"/>
-      <c r="B71" s="22"/>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="32"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="32"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="32"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>1</v>
       </c>
@@ -2365,7 +2517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>63</v>
       </c>
@@ -2380,28 +2532,28 @@
         <v>$table-&gt;string('path', 255);</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="D74" s="3" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="22" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B78" s="22"/>
-      <c r="C78" s="22"/>
-      <c r="D78" s="22"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="22"/>
-      <c r="B79" s="22"/>
-      <c r="C79" s="22"/>
-      <c r="D79" s="22"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="32"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>1</v>
       </c>
@@ -2414,290 +2566,340 @@
       <c r="D80" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="E80" s="21" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="10" t="s">
+      <c r="A81" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" s="29">
+        <v>255</v>
+      </c>
+      <c r="D81" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E81" s="25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B81" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" s="8">
+      <c r="B82" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" s="30">
         <v>250</v>
       </c>
-      <c r="D81" s="9" t="str">
-        <f t="shared" ref="D81:D83" si="3">IF(B81="String", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"', ",C81,");"), IF(B81="Integer", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"')-&gt;unsigned()-&gt;default(0);"), IF(B81="Text", CONCATENATE("$table-&gt;",LOWER(B81),"('",A81,"');"), IF(B81="Date", CONCATENATE("$table-&gt;","timestamp","('",A81,"');")) )))</f>
-        <v>$table-&gt;string('name', 250);</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="10" t="s">
+      <c r="D82" s="28" t="str">
+        <f t="shared" ref="D82:D84" si="3">IF(B82="String", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"', ",C82,");"), IF(B82="Integer", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"')-&gt;unsigned()-&gt;default(0);"), IF(B82="Text", CONCATENATE("$table-&gt;",LOWER(B82),"('",A82,"');"), IF(B82="Date", CONCATENATE("$table-&gt;","timestamp","('",A82,"');")) )))</f>
+        <v>$table-&gt;string('title', 250);</v>
+      </c>
+      <c r="E82" s="25"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C83" s="30"/>
+      <c r="D83" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>$table-&gt;text('content');</v>
+      </c>
+      <c r="E83" s="25"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B82" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C82" s="8"/>
-      <c r="D82" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v>$table-&gt;text('title');</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B83" s="10" t="s">
+      <c r="B84" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="9" t="str">
+      <c r="C84" s="30"/>
+      <c r="D84" s="28" t="str">
         <f t="shared" si="3"/>
         <v>$table-&gt;timestamp('start_time');</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
+      <c r="E84" s="25"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="30"/>
+      <c r="D85" s="31" t="str">
+        <f>IF(B85="String", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"', ",C85,");"), IF(B85="Integer", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"')-&gt;unsigned()-&gt;default(0);"), IF(B85="Text", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"');"), IF(B85="Date", CONCATENATE("$table-&gt;","timestamp","('",A85,"');")) )))</f>
+        <v>$table-&gt;timestamp('end_time');</v>
+      </c>
+      <c r="E85" s="25"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="35"/>
+      <c r="B86" s="34"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B88" s="32"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="32"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="32"/>
+      <c r="B89" s="32"/>
+      <c r="C89" s="32"/>
+      <c r="D89" s="32"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E90" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G90" s="11"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C84" s="8"/>
-      <c r="D84" s="9" t="str">
-        <f>IF(B84="String", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"', ",C84,");"), IF(B84="Integer", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"')-&gt;unsigned()-&gt;default(0);"), IF(B84="Text", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"');"), IF(B84="Date", CONCATENATE("$table-&gt;","timestamp","('",A84,"');")) )))</f>
-        <v>$table-&gt;timestamp('end_time');</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B87" s="22"/>
-      <c r="C87" s="22"/>
-      <c r="D87" s="22"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="22"/>
-      <c r="B88" s="22"/>
-      <c r="C88" s="22"/>
-      <c r="D88" s="22"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G89" s="12"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C90" s="8">
-        <v>250</v>
-      </c>
-      <c r="D90" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="10" t="s">
-        <v>81</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C91" s="8"/>
-      <c r="D91" s="10" t="s">
-        <v>82</v>
+      <c r="C91" s="8">
+        <v>250</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E91" s="25" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="10" t="s">
-        <v>73</v>
+      <c r="A92" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C92" s="8"/>
-      <c r="D92" s="14" t="s">
+      <c r="D92" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E92" s="25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E93" s="22"/>
+      <c r="G93" s="12"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" s="9">
+        <v>255</v>
+      </c>
+      <c r="D94" s="13" t="str">
+        <f>IF(B94="String", CONCATENATE("$table-&gt;",LOWER(B94),"('",A94,"', ",C94,");"), IF(B94="Integer", CONCATENATE("$table-&gt;",LOWER(B94),"('",A94,"')-&gt;unsigned()-&gt;default(0);"), IF(B94="Text", CONCATENATE("$table-&gt;",LOWER(B94),"('",A94,"');"), IF(B94="Date", CONCATENATE("$table-&gt;","timestamp","('",A94,"');")) )))</f>
+        <v>$table-&gt;string('first_name', 255);</v>
+      </c>
+      <c r="E94" s="22"/>
+      <c r="G94" s="12"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" s="9">
+        <v>255</v>
+      </c>
+      <c r="D95" s="13" t="str">
+        <f>IF(B95="String", CONCATENATE("$table-&gt;",LOWER(B95),"('",A95,"', ",C95,");"), IF(B95="Integer", CONCATENATE("$table-&gt;",LOWER(B95),"('",A95,"')-&gt;unsigned()-&gt;default(0);"), IF(B95="Text", CONCATENATE("$table-&gt;",LOWER(B95),"('",A95,"');"), IF(B95="Date", CONCATENATE("$table-&gt;","timestamp","('",A95,"');")) )))</f>
+        <v>$table-&gt;string('last_name', 255);</v>
+      </c>
+      <c r="E95" s="22"/>
+      <c r="G95" s="12"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C96" s="8">
+        <v>200</v>
+      </c>
+      <c r="D96" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G92" s="13"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C93" s="10">
+      <c r="E96" s="22"/>
+      <c r="G96" s="12"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" s="22">
         <v>255</v>
       </c>
-      <c r="D93" s="14" t="str">
-        <f>IF(B93="String", CONCATENATE("$table-&gt;",LOWER(B93),"('",A93,"', ",C93,");"), IF(B93="Integer", CONCATENATE("$table-&gt;",LOWER(B93),"('",A93,"')-&gt;unsigned()-&gt;default(0);"), IF(B93="Text", CONCATENATE("$table-&gt;",LOWER(B93),"('",A93,"');"), IF(B93="Date", CONCATENATE("$table-&gt;","timestamp","('",A93,"');")) )))</f>
-        <v>$table-&gt;string('first_name', 255);</v>
-      </c>
-      <c r="G93" s="13"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B94" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C94" s="10">
-        <v>255</v>
-      </c>
-      <c r="D94" s="14" t="str">
-        <f>IF(B94="String", CONCATENATE("$table-&gt;",LOWER(B94),"('",A94,"', ",C94,");"), IF(B94="Integer", CONCATENATE("$table-&gt;",LOWER(B94),"('",A94,"')-&gt;unsigned()-&gt;default(0);"), IF(B94="Text", CONCATENATE("$table-&gt;",LOWER(B94),"('",A94,"');"), IF(B94="Date", CONCATENATE("$table-&gt;","timestamp","('",A94,"');")) )))</f>
-        <v>$table-&gt;string('last_name', 255);</v>
-      </c>
-      <c r="G94" s="13"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B95" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C95" s="8">
-        <v>200</v>
-      </c>
-      <c r="D95" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G95" s="13"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B96" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C96" s="23">
-        <v>255</v>
-      </c>
-      <c r="D96" s="14" t="str">
-        <f>IF(B96="String", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"', ",C96,");"), IF(B96="Integer", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"')-&gt;unsigned()-&gt;default(0);"), IF(B96="Text", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"');"), IF(B96="Date", CONCATENATE("$table-&gt;","timestamp","('",A96,"');")) )))</f>
+      <c r="D97" s="13" t="str">
+        <f>IF(B97="String", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"', ",C97,");"), IF(B97="Integer", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"')-&gt;unsigned()-&gt;default(0);"), IF(B97="Text", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"');"), IF(B97="Date", CONCATENATE("$table-&gt;","timestamp","('",A97,"');")) )))</f>
         <v>$table-&gt;string('address', 255);</v>
       </c>
-      <c r="G96" s="13"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B97" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C97" s="8">
-        <v>50</v>
-      </c>
-      <c r="D97" s="14" t="str">
-        <f>IF(B97="String", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"', ",C97,");"), IF(B97="Integer", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"')-&gt;unsigned()-&gt;default(0);"), IF(B97="Text", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"');"), IF(B97="Date", CONCATENATE("$table-&gt;","timestamp","('",A97,"');")) )))</f>
-        <v>$table-&gt;string('phone', 50);</v>
-      </c>
-      <c r="G97" s="13"/>
+      <c r="E97" s="22"/>
+      <c r="G97" s="12"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B98" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B98" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C98" s="8">
+        <v>50</v>
+      </c>
+      <c r="D98" s="13" t="str">
+        <f>IF(B98="String", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"', ",C98,");"), IF(B98="Integer", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"')-&gt;unsigned()-&gt;default(0);"), IF(B98="Text", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"');"), IF(B98="Date", CONCATENATE("$table-&gt;","timestamp","('",A98,"');")) )))</f>
+        <v>$table-&gt;string('phone', 50);</v>
+      </c>
+      <c r="E98" s="22"/>
+      <c r="G98" s="12"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="8">
         <v>255</v>
       </c>
-      <c r="D98" s="14" t="str">
-        <f>IF(B98="String", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"', ",C98,");"), IF(B98="Integer", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"')-&gt;unsigned()-&gt;default(0);"), IF(B98="Text", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"');"), IF(B98="Date", CONCATENATE("$table-&gt;","timestamp","('",A98,"');")) )))</f>
+      <c r="D99" s="13" t="str">
+        <f>IF(B99="String", CONCATENATE("$table-&gt;",LOWER(B99),"('",A99,"', ",C99,");"), IF(B99="Integer", CONCATENATE("$table-&gt;",LOWER(B99),"('",A99,"')-&gt;unsigned()-&gt;default(0);"), IF(B99="Text", CONCATENATE("$table-&gt;",LOWER(B99),"('",A99,"');"), IF(B99="Date", CONCATENATE("$table-&gt;","timestamp","('",A99,"');")) )))</f>
         <v>$table-&gt;string('password', 255);</v>
       </c>
-      <c r="G98" s="13"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="15" t="s">
+      <c r="E99" s="22"/>
+      <c r="G99" s="12"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B99" s="7" t="s">
+      <c r="B100" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C99" s="15"/>
-      <c r="D99" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="G99" s="13"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="22" t="s">
+      <c r="C100" s="14"/>
+      <c r="D100" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E100" s="22"/>
+      <c r="G100" s="12"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B103" s="32"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="32"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="32"/>
+      <c r="B104" s="32"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="32"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D105" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B102" s="22"/>
-      <c r="C102" s="22"/>
-      <c r="D102" s="22"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="22"/>
-      <c r="B103" s="22"/>
-      <c r="C103" s="22"/>
-      <c r="D103" s="22"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B104" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C104" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D104" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C105" s="8">
+      <c r="B106" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C106" s="8">
         <v>255</v>
       </c>
-      <c r="D105" s="14" t="str">
-        <f>IF(B105="String", CONCATENATE("$table-&gt;",LOWER(B105),"('",A105,"', ",C105,");"), IF(B105="Integer", CONCATENATE("$table-&gt;",LOWER(B105),"('",A105,"')-&gt;unsigned()-&gt;default(0);"), IF(B105="Text", CONCATENATE("$table-&gt;",LOWER(B105),"('",A105,"');"), IF(B105="Date", CONCATENATE("$table-&gt;","timestamp","('",A105,"');")) )))</f>
+      <c r="D106" s="13" t="str">
+        <f>IF(B106="String", CONCATENATE("$table-&gt;",LOWER(B106),"('",A106,"', ",C106,");"), IF(B106="Integer", CONCATENATE("$table-&gt;",LOWER(B106),"('",A106,"')-&gt;unsigned()-&gt;default(0);"), IF(B106="Text", CONCATENATE("$table-&gt;",LOWER(B106),"('",A106,"');"), IF(B106="Date", CONCATENATE("$table-&gt;","timestamp","('",A106,"');")) )))</f>
         <v>$table-&gt;string('status', 255);</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="15"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="15"/>
-      <c r="D106" s="16"/>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="14"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="14"/>
+      <c r="D107" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A102:D103"/>
-    <mergeCell ref="A87:D88"/>
+    <mergeCell ref="A103:D104"/>
+    <mergeCell ref="A88:D89"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A53:D54"/>
     <mergeCell ref="A61:D62"/>

</xml_diff>

<commit_message>
#5 Created the models: Category and Job
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="113">
   <si>
     <t>PATIENT</t>
   </si>
@@ -311,6 +311,72 @@
   </si>
   <si>
     <t>Added as column because the meccanism created can't retrieve the path by id, we are using Ajax style</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t>id_invoice</t>
+  </si>
+  <si>
+    <t>$table-&gt;integer('id_dentist')-&gt;unsigned();</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>id_category</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>prize2</t>
+  </si>
+  <si>
+    <t>currency2</t>
+  </si>
+  <si>
+    <t>prize1</t>
+  </si>
+  <si>
+    <t>currency1</t>
+  </si>
+  <si>
+    <t>currency3</t>
+  </si>
+  <si>
+    <t>prize3</t>
+  </si>
+  <si>
+    <t>currency4</t>
+  </si>
+  <si>
+    <t>prize4</t>
+  </si>
+  <si>
+    <t>vat</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('vat', 5, 2);</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>type_operation</t>
+  </si>
+  <si>
+    <t>short_detail</t>
   </si>
 </sst>
 </file>
@@ -475,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,11 +643,260 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1219,7 +1534,7 @@
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="29">
+    <tableColumn id="4" name="Code generated" dataDxfId="41">
       <calculatedColumnFormula>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"')-&gt;unsigned()-&gt;default(0);"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5),"('",Table1[[#This Row],[Column name]],"');")) )))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Type Column"/>
@@ -1229,13 +1544,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A57:D61" totalsRowShown="0" headerRowDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A57:D61" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A57:D61"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="27"/>
+    <tableColumn id="2" name="Type" dataDxfId="39"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="26">
+    <tableColumn id="4" name="Code generated" dataDxfId="38">
       <calculatedColumnFormula>IF(B58="String", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"', ",C58,");"), IF(B58="Integer", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"')-&gt;unsigned()-&gt;default(0);"), IF(B58="Text", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');"), IF(B58="Date", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1244,13 +1559,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A65:D70" totalsRowShown="0" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A65:D70" totalsRowShown="0" headerRowDxfId="37">
   <autoFilter ref="A65:D70"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="24"/>
+    <tableColumn id="2" name="Type" dataDxfId="36"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="23">
+    <tableColumn id="4" name="Code generated" dataDxfId="35">
       <calculatedColumnFormula>IF(B66="String", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"', ",C66,");"), IF(B66="Integer", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"')-&gt;unsigned()-&gt;default(0);"), IF(B66="Text", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');"), IF(B66="Date", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1259,13 +1574,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A74:D76" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A74:D76" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="A74:D76"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="21"/>
+    <tableColumn id="2" name="Type" dataDxfId="33"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="20">
+    <tableColumn id="4" name="Code generated" dataDxfId="32">
       <calculatedColumnFormula>IF(B75="String", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"', ",C75,");"), IF(B75="Integer", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"')-&gt;unsigned()-&gt;default(0);"), IF(B75="Text", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');"), IF(B75="Date", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1274,43 +1589,73 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A82:E88" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A82:E88" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A82:E88"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column name" dataDxfId="17"/>
-    <tableColumn id="2" name="Type" dataDxfId="16"/>
-    <tableColumn id="3" name="Length" dataDxfId="15"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="14">
+    <tableColumn id="1" name="Column name" dataDxfId="29"/>
+    <tableColumn id="2" name="Type" dataDxfId="28"/>
+    <tableColumn id="3" name="Length" dataDxfId="27"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="26">
       <calculatedColumnFormula>IF(B83="String", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"', ",C83,");"), IF(B83="Integer", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"')-&gt;unsigned()-&gt;default(0);"), IF(B83="Text", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"');"), IF(B83="Date", CONCATENATE("$table-&gt;","timestamp","('",A83,"');")) )))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Type Column" dataDxfId="13"/>
+    <tableColumn id="5" name="Type Column" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A92:E102" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A92:E102" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A92:E102"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column name" dataDxfId="10"/>
-    <tableColumn id="2" name="Type" dataDxfId="9"/>
-    <tableColumn id="3" name="Length" dataDxfId="8"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="7"/>
-    <tableColumn id="5" name="Type Column" dataDxfId="6"/>
+    <tableColumn id="1" name="Column name" dataDxfId="22"/>
+    <tableColumn id="2" name="Type" dataDxfId="21"/>
+    <tableColumn id="3" name="Length" dataDxfId="20"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="19"/>
+    <tableColumn id="5" name="Type Column" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A107:D109" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A107:D109" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A107:D109"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Column name" dataDxfId="15"/>
+    <tableColumn id="2" name="Type" dataDxfId="14"/>
+    <tableColumn id="3" name="Length" dataDxfId="13"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table2546879" displayName="Table2546879" ref="A113:D131" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A113:D131"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Column name" dataDxfId="9"/>
+    <tableColumn id="2" name="Type" dataDxfId="8"/>
+    <tableColumn id="3" name="Length" dataDxfId="7"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="6">
+      <calculatedColumnFormula>IF(B114="String", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"', ",C114,");"), IF(B114="Integer", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"')-&gt;unsigned()-&gt;default(0);"), IF(B114="Text", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"');"), IF(B114="Date", CONCATENATE("$table-&gt;","timestamp","('",A114,"');")) )))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table254687910" displayName="Table254687910" ref="A135:D137" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A135:D137"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="3"/>
     <tableColumn id="2" name="Type" dataDxfId="2"/>
     <tableColumn id="3" name="Length" dataDxfId="1"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="0"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="0">
+      <calculatedColumnFormula>IF(B136="String", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"', ",C136,");"), IF(B136="Integer", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"')-&gt;unsigned()-&gt;default(0);"), IF(B136="Text", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"');"), IF(B136="Date", CONCATENATE("$table-&gt;","timestamp","('",A136,"');")) )))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1359,7 +1704,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1394,7 +1739,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1603,10 +1948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114:D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,22 +1964,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2343,18 +2688,18 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="39"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
+      <c r="B55" s="41"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="39"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39"/>
+      <c r="A56" s="41"/>
+      <c r="B56" s="41"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -2431,18 +2776,18 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="39" t="s">
+      <c r="A63" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="39"/>
-      <c r="C63" s="39"/>
-      <c r="D63" s="39"/>
+      <c r="B63" s="41"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="41"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="39"/>
-      <c r="B64" s="39"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
+      <c r="A64" s="41"/>
+      <c r="B64" s="41"/>
+      <c r="C64" s="41"/>
+      <c r="D64" s="41"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
@@ -2528,18 +2873,18 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="39" t="s">
+      <c r="A72" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="39"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
+      <c r="B72" s="41"/>
+      <c r="C72" s="41"/>
+      <c r="D72" s="41"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="39"/>
-      <c r="B73" s="39"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
+      <c r="A73" s="41"/>
+      <c r="B73" s="41"/>
+      <c r="C73" s="41"/>
+      <c r="D73" s="41"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
@@ -2578,18 +2923,18 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="39" t="s">
+      <c r="A80" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B80" s="39"/>
-      <c r="C80" s="39"/>
-      <c r="D80" s="39"/>
+      <c r="B80" s="41"/>
+      <c r="C80" s="41"/>
+      <c r="D80" s="41"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="39"/>
-      <c r="B81" s="39"/>
-      <c r="C81" s="39"/>
-      <c r="D81" s="39"/>
+      <c r="A81" s="41"/>
+      <c r="B81" s="41"/>
+      <c r="C81" s="41"/>
+      <c r="D81" s="41"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
@@ -2693,18 +3038,18 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="39" t="s">
+      <c r="A90" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="B90" s="39"/>
-      <c r="C90" s="39"/>
-      <c r="D90" s="39"/>
+      <c r="B90" s="41"/>
+      <c r="C90" s="41"/>
+      <c r="D90" s="41"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="39"/>
-      <c r="B91" s="39"/>
-      <c r="C91" s="39"/>
-      <c r="D91" s="39"/>
+      <c r="A91" s="41"/>
+      <c r="B91" s="41"/>
+      <c r="C91" s="41"/>
+      <c r="D91" s="41"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
@@ -2886,18 +3231,18 @@
       <c r="G102" s="12"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="39" t="s">
+      <c r="A105" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="B105" s="39"/>
-      <c r="C105" s="39"/>
-      <c r="D105" s="39"/>
+      <c r="B105" s="41"/>
+      <c r="C105" s="41"/>
+      <c r="D105" s="41"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="39"/>
-      <c r="B106" s="39"/>
-      <c r="C106" s="39"/>
-      <c r="D106" s="39"/>
+      <c r="A106" s="41"/>
+      <c r="B106" s="41"/>
+      <c r="C106" s="41"/>
+      <c r="D106" s="41"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
@@ -2934,8 +3279,327 @@
       <c r="C109" s="14"/>
       <c r="D109" s="15"/>
     </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B111" s="41"/>
+      <c r="C111" s="41"/>
+      <c r="D111" s="41"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="41"/>
+      <c r="B112" s="41"/>
+      <c r="C112" s="41"/>
+      <c r="D112" s="41"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B113" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C113" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D113" s="39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C114" s="8">
+        <v>50</v>
+      </c>
+      <c r="D114" s="13" t="str">
+        <f>IF(B114="String", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"', ",C114,");"), IF(B114="Integer", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"')-&gt;unsigned()-&gt;default(0);"), IF(B114="Text", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"');"), IF(B114="Date", CONCATENATE("$table-&gt;","timestamp","('",A114,"');")) )))</f>
+        <v>$table-&gt;string('id_invoice', 50);</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C115" s="14"/>
+      <c r="D115" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="B116" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C116" s="44"/>
+      <c r="D116" s="45" t="str">
+        <f>IF(B116="String", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"', ",C116,");"), IF(B116="Integer", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"')-&gt;unsigned()-&gt;default(0);"), IF(B116="Text", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"');"), IF(B116="Date", CONCATENATE("$table-&gt;","timestamp","('",A116,"');")) )))</f>
+        <v>$table-&gt;integer('id_category')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B117" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117" s="44">
+        <v>250</v>
+      </c>
+      <c r="D117" s="45" t="str">
+        <f>IF(B117="String", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"', ",C117,");"), IF(B117="Integer", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"')-&gt;unsigned()-&gt;default(0);"), IF(B117="Text", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"');"), IF(B117="Date", CONCATENATE("$table-&gt;","timestamp","('",A117,"');")) )))</f>
+        <v>$table-&gt;string('detail', 250);</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="B118" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C118" s="44">
+        <v>100</v>
+      </c>
+      <c r="D118" s="43" t="str">
+        <f>IF(B118="String", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"', ",C118,");"), IF(B118="Integer", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"')-&gt;unsigned()-&gt;default(0);"), IF(B118="Text", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"');"), IF(B118="Date", CONCATENATE("$table-&gt;","timestamp","('",A118,"');")) )))</f>
+        <v>$table-&gt;string('short_detail', 100);</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="B119" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C119" s="44"/>
+      <c r="D119" s="45" t="str">
+        <f>IF(B119="String", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"', ",C119,");"), IF(B119="Integer", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"')-&gt;unsigned()-&gt;default(0);"), IF(B119="Text", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"');"), IF(B119="Date", CONCATENATE("$table-&gt;","timestamp","('",A119,"');")) )))</f>
+        <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B120" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C120" s="44"/>
+      <c r="D120" s="45" t="str">
+        <f>IF(B120="String", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"', ",C120,");"), IF(B120="Integer", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"')-&gt;unsigned()-&gt;default(0);"), IF(B120="Text", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"');"), IF(B120="Date", CONCATENATE("$table-&gt;","timestamp","('",A120,"');")) )))</f>
+        <v>$table-&gt;integer('prize1')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="B121" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C121" s="44"/>
+      <c r="D121" s="43" t="str">
+        <f t="shared" ref="D121:D122" si="4">IF(B121="String", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"', ",C121,");"), IF(B121="Integer", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"')-&gt;unsigned()-&gt;default(0);"), IF(B121="Text", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"');"), IF(B121="Date", CONCATENATE("$table-&gt;","timestamp","('",A121,"');")) )))</f>
+        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B122" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C122" s="44"/>
+      <c r="D122" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>$table-&gt;integer('prize2')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="B123" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C123" s="44"/>
+      <c r="D123" s="43" t="str">
+        <f t="shared" ref="D123:D126" si="5">IF(B123="String", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"', ",C123,");"), IF(B123="Integer", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"')-&gt;unsigned()-&gt;default(0);"), IF(B123="Text", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"');"), IF(B123="Date", CONCATENATE("$table-&gt;","timestamp","('",A123,"');")) )))</f>
+        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="B124" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C124" s="44"/>
+      <c r="D124" s="43" t="str">
+        <f t="shared" si="5"/>
+        <v>$table-&gt;integer('prize3')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B125" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C125" s="44"/>
+      <c r="D125" s="43" t="str">
+        <f t="shared" si="5"/>
+        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B126" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C126" s="44"/>
+      <c r="D126" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>$table-&gt;integer('prize4')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B127" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="C127" s="44"/>
+      <c r="D127" s="45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="B128" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C128" s="44">
+        <v>255</v>
+      </c>
+      <c r="D128" s="45" t="str">
+        <f>IF(B128="String", CONCATENATE("$table-&gt;",LOWER(B128),"('",A128,"', ",C128,");"), IF(B128="Integer", CONCATENATE("$table-&gt;",LOWER(B128),"('",A128,"')-&gt;unsigned()-&gt;default(0);"), IF(B128="Text", CONCATENATE("$table-&gt;",LOWER(B128),"('",A128,"');"), IF(B128="Date", CONCATENATE("$table-&gt;","timestamp","('",A128,"');")) )))</f>
+        <v>$table-&gt;string('position', 255);</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="B129" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C129" s="44"/>
+      <c r="D129" s="45" t="str">
+        <f>IF(B129="String", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"', ",C129,");"), IF(B129="Integer", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"')-&gt;unsigned()-&gt;default(0);"), IF(B129="Text", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"');"), IF(B129="Date", CONCATENATE("$table-&gt;","timestamp","('",A129,"');")) )))</f>
+        <v>$table-&gt;integer('object')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="B130" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C130" s="44"/>
+      <c r="D130" s="45" t="str">
+        <f>IF(B130="String", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"', ",C130,");"), IF(B130="Integer", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"')-&gt;unsigned()-&gt;default(0);"), IF(B130="Text", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"');"), IF(B130="Date", CONCATENATE("$table-&gt;","timestamp","('",A130,"');")) )))</f>
+        <v>$table-&gt;integer('type_operation')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B131" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C131" s="44"/>
+      <c r="D131" s="45" t="str">
+        <f>IF(B131="String", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"', ",C131,");"), IF(B131="Integer", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"')-&gt;unsigned()-&gt;default(0);"), IF(B131="Text", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"');"), IF(B131="Date", CONCATENATE("$table-&gt;","timestamp","('",A131,"');")) )))</f>
+        <v>$table-&gt;text('note');</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="44"/>
+      <c r="B132" s="46"/>
+      <c r="C132" s="44"/>
+      <c r="D132" s="47"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B133" s="41"/>
+      <c r="C133" s="41"/>
+      <c r="D133" s="41"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="41"/>
+      <c r="B134" s="41"/>
+      <c r="C134" s="41"/>
+      <c r="D134" s="41"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B135" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C135" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D135" s="39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C136" s="8">
+        <v>255</v>
+      </c>
+      <c r="D136" s="13" t="str">
+        <f>IF(B136="String", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"', ",C136,");"), IF(B136="Integer", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"')-&gt;unsigned()-&gt;default(0);"), IF(B136="Text", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"');"), IF(B136="Date", CONCATENATE("$table-&gt;","timestamp","('",A136,"');")) )))</f>
+        <v>$table-&gt;string('category', 255);</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A111:D112"/>
+    <mergeCell ref="A133:D134"/>
     <mergeCell ref="A105:D106"/>
     <mergeCell ref="A90:D91"/>
     <mergeCell ref="A1:F2"/>
@@ -2946,7 +3610,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <tableParts count="7">
+  <tableParts count="9">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -2954,6 +3618,8 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#5 Minor fixes ( Back from vacation )
:construction:
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="125">
   <si>
     <t>PATIENT</t>
   </si>
@@ -319,9 +319,6 @@
     <t>id_invoice</t>
   </si>
   <si>
-    <t>$table-&gt;integer('id_dentist')-&gt;unsigned();</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
     <t>Categories</t>
   </si>
   <si>
-    <t>detail</t>
-  </si>
-  <si>
     <t>prize2</t>
   </si>
   <si>
@@ -376,7 +370,49 @@
     <t>type_operation</t>
   </si>
   <si>
-    <t>short_detail</t>
+    <t>JobsDetail</t>
+  </si>
+  <si>
+    <t>id_job</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>teeth_no</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('price', 7, 2);</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('discount', 5, 2);</t>
+  </si>
+  <si>
+    <t>clicnic_note</t>
+  </si>
+  <si>
+    <t>general_note</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('price4', 7, 2);</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('price3', 7, 2);</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('price2', 7, 2);</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('price1', 7, 2);</t>
   </si>
 </sst>
 </file>
@@ -541,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -658,11 +694,131 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1534,7 +1690,7 @@
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="41">
+    <tableColumn id="4" name="Code generated" dataDxfId="47">
       <calculatedColumnFormula>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"')-&gt;unsigned()-&gt;default(0);"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5),"('",Table1[[#This Row],[Column name]],"');")) )))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Type Column"/>
@@ -1543,14 +1699,29 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table254687911" displayName="Table254687911" ref="A142:D159" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A142:D159"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Column name" dataDxfId="3"/>
+    <tableColumn id="2" name="Type" dataDxfId="2"/>
+    <tableColumn id="3" name="Length" dataDxfId="1"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="0">
+      <calculatedColumnFormula>IF(B143="String", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"', ",C143,");"), IF(B143="Integer", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"')-&gt;unsigned()-&gt;default(0);"), IF(B143="Text", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"');"), IF(B143="Date", CONCATENATE("$table-&gt;","timestamp","('",A143,"');")) )))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A57:D61" totalsRowShown="0" headerRowDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A57:D61" totalsRowShown="0" headerRowDxfId="46">
   <autoFilter ref="A57:D61"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="39"/>
+    <tableColumn id="2" name="Type" dataDxfId="45"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="38">
+    <tableColumn id="4" name="Code generated" dataDxfId="44">
       <calculatedColumnFormula>IF(B58="String", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"', ",C58,");"), IF(B58="Integer", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"')-&gt;unsigned()-&gt;default(0);"), IF(B58="Text", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');"), IF(B58="Date", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1559,13 +1730,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A65:D70" totalsRowShown="0" headerRowDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A65:D70" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="A65:D70"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="36"/>
+    <tableColumn id="2" name="Type" dataDxfId="42"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="35">
+    <tableColumn id="4" name="Code generated" dataDxfId="41">
       <calculatedColumnFormula>IF(B66="String", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"', ",C66,");"), IF(B66="Integer", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"')-&gt;unsigned()-&gt;default(0);"), IF(B66="Text", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');"), IF(B66="Date", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1574,13 +1745,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A74:D76" totalsRowShown="0" headerRowDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A74:D76" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A74:D76"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="33"/>
+    <tableColumn id="2" name="Type" dataDxfId="39"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="32">
+    <tableColumn id="4" name="Code generated" dataDxfId="38">
       <calculatedColumnFormula>IF(B75="String", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"', ",C75,");"), IF(B75="Integer", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"')-&gt;unsigned()-&gt;default(0);"), IF(B75="Text", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');"), IF(B75="Date", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1589,56 +1760,56 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A82:E88" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A82:E88" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="A82:E88"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column name" dataDxfId="29"/>
-    <tableColumn id="2" name="Type" dataDxfId="28"/>
-    <tableColumn id="3" name="Length" dataDxfId="27"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="26">
+    <tableColumn id="1" name="Column name" dataDxfId="35"/>
+    <tableColumn id="2" name="Type" dataDxfId="34"/>
+    <tableColumn id="3" name="Length" dataDxfId="33"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="32">
       <calculatedColumnFormula>IF(B83="String", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"', ",C83,");"), IF(B83="Integer", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"')-&gt;unsigned()-&gt;default(0);"), IF(B83="Text", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"');"), IF(B83="Date", CONCATENATE("$table-&gt;","timestamp","('",A83,"');")) )))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Type Column" dataDxfId="25"/>
+    <tableColumn id="5" name="Type Column" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A92:E102" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A92:E102" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A92:E102"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column name" dataDxfId="22"/>
-    <tableColumn id="2" name="Type" dataDxfId="21"/>
-    <tableColumn id="3" name="Length" dataDxfId="20"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="19"/>
-    <tableColumn id="5" name="Type Column" dataDxfId="18"/>
+    <tableColumn id="1" name="Column name" dataDxfId="28"/>
+    <tableColumn id="2" name="Type" dataDxfId="27"/>
+    <tableColumn id="3" name="Length" dataDxfId="26"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="25"/>
+    <tableColumn id="5" name="Type Column" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A107:D109" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A107:D109" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A107:D109"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Column name" dataDxfId="15"/>
-    <tableColumn id="2" name="Type" dataDxfId="14"/>
-    <tableColumn id="3" name="Length" dataDxfId="13"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="12"/>
+    <tableColumn id="1" name="Column name" dataDxfId="21"/>
+    <tableColumn id="2" name="Type" dataDxfId="20"/>
+    <tableColumn id="3" name="Length" dataDxfId="19"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table2546879" displayName="Table2546879" ref="A113:D131" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table2546879" displayName="Table2546879" ref="A113:D131" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A113:D131"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Column name" dataDxfId="9"/>
-    <tableColumn id="2" name="Type" dataDxfId="8"/>
-    <tableColumn id="3" name="Length" dataDxfId="7"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="6">
+    <tableColumn id="1" name="Column name" dataDxfId="15"/>
+    <tableColumn id="2" name="Type" dataDxfId="14"/>
+    <tableColumn id="3" name="Length" dataDxfId="13"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="12">
       <calculatedColumnFormula>IF(B114="String", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"', ",C114,");"), IF(B114="Integer", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"')-&gt;unsigned()-&gt;default(0);"), IF(B114="Text", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"');"), IF(B114="Date", CONCATENATE("$table-&gt;","timestamp","('",A114,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1647,13 +1818,13 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table254687910" displayName="Table254687910" ref="A135:D137" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table254687910" displayName="Table254687910" ref="A135:D137" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A135:D137"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Column name" dataDxfId="3"/>
-    <tableColumn id="2" name="Type" dataDxfId="2"/>
-    <tableColumn id="3" name="Length" dataDxfId="1"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="0">
+    <tableColumn id="1" name="Column name" dataDxfId="9"/>
+    <tableColumn id="2" name="Type" dataDxfId="8"/>
+    <tableColumn id="3" name="Length" dataDxfId="7"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="6">
       <calculatedColumnFormula>IF(B136="String", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"', ",C136,");"), IF(B136="Integer", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"')-&gt;unsigned()-&gt;default(0);"), IF(B136="Text", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"');"), IF(B136="Date", CONCATENATE("$table-&gt;","timestamp","('",A136,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1704,7 +1875,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1739,7 +1910,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1948,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114:D131"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A161" sqref="A161:D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,22 +2135,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2688,18 +2859,18 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="41" t="s">
+      <c r="A55" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="41"/>
-      <c r="B56" s="41"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="41"/>
+      <c r="A56" s="48"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="48"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -2776,18 +2947,18 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="41" t="s">
+      <c r="A63" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="41"/>
-      <c r="C63" s="41"/>
-      <c r="D63" s="41"/>
+      <c r="B63" s="48"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="48"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="41"/>
-      <c r="B64" s="41"/>
-      <c r="C64" s="41"/>
-      <c r="D64" s="41"/>
+      <c r="A64" s="48"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="48"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
@@ -2873,18 +3044,18 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="41" t="s">
+      <c r="A72" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="41"/>
-      <c r="C72" s="41"/>
-      <c r="D72" s="41"/>
+      <c r="B72" s="48"/>
+      <c r="C72" s="48"/>
+      <c r="D72" s="48"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="41"/>
-      <c r="B73" s="41"/>
-      <c r="C73" s="41"/>
-      <c r="D73" s="41"/>
+      <c r="A73" s="48"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="48"/>
+      <c r="D73" s="48"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
@@ -2923,18 +3094,18 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="41" t="s">
+      <c r="A80" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="B80" s="41"/>
-      <c r="C80" s="41"/>
-      <c r="D80" s="41"/>
+      <c r="B80" s="48"/>
+      <c r="C80" s="48"/>
+      <c r="D80" s="48"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="41"/>
-      <c r="B81" s="41"/>
-      <c r="C81" s="41"/>
-      <c r="D81" s="41"/>
+      <c r="A81" s="48"/>
+      <c r="B81" s="48"/>
+      <c r="C81" s="48"/>
+      <c r="D81" s="48"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
@@ -3038,18 +3209,18 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="41" t="s">
+      <c r="A90" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="B90" s="41"/>
-      <c r="C90" s="41"/>
-      <c r="D90" s="41"/>
+      <c r="B90" s="48"/>
+      <c r="C90" s="48"/>
+      <c r="D90" s="48"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="41"/>
-      <c r="B91" s="41"/>
-      <c r="C91" s="41"/>
-      <c r="D91" s="41"/>
+      <c r="A91" s="48"/>
+      <c r="B91" s="48"/>
+      <c r="C91" s="48"/>
+      <c r="D91" s="48"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
@@ -3154,7 +3325,7 @@
         <v>16</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C98" s="8">
         <v>200</v>
@@ -3231,18 +3402,18 @@
       <c r="G102" s="12"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="41" t="s">
+      <c r="A105" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="B105" s="41"/>
-      <c r="C105" s="41"/>
-      <c r="D105" s="41"/>
+      <c r="B105" s="48"/>
+      <c r="C105" s="48"/>
+      <c r="D105" s="48"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="41"/>
-      <c r="B106" s="41"/>
-      <c r="C106" s="41"/>
-      <c r="D106" s="41"/>
+      <c r="A106" s="48"/>
+      <c r="B106" s="48"/>
+      <c r="C106" s="48"/>
+      <c r="D106" s="48"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
@@ -3280,18 +3451,18 @@
       <c r="D109" s="15"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="41" t="s">
+      <c r="A111" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B111" s="41"/>
-      <c r="C111" s="41"/>
-      <c r="D111" s="41"/>
+      <c r="B111" s="48"/>
+      <c r="C111" s="48"/>
+      <c r="D111" s="48"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="41"/>
-      <c r="B112" s="41"/>
-      <c r="C112" s="41"/>
-      <c r="D112" s="41"/>
+      <c r="A112" s="48"/>
+      <c r="B112" s="48"/>
+      <c r="C112" s="48"/>
+      <c r="D112" s="48"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="39" t="s">
@@ -3327,16 +3498,19 @@
         <v>7</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C115" s="14"/>
-      <c r="D115" s="13" t="s">
-        <v>93</v>
+        <v>6</v>
+      </c>
+      <c r="C115" s="14">
+        <v>50</v>
+      </c>
+      <c r="D115" s="13" t="str">
+        <f>IF(B115="String", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"', ",C115,");"), IF(B115="Integer", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"')-&gt;unsigned()-&gt;default(0);"), IF(B115="Text", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"');"), IF(B115="Date", CONCATENATE("$table-&gt;","timestamp","('",A115,"');")) )))</f>
+        <v>$table-&gt;string('id_dentist', 50);</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B116" s="42" t="s">
         <v>25</v>
@@ -3349,37 +3523,33 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="44" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="B117" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="C117" s="44">
-        <v>250</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C117" s="44"/>
       <c r="D117" s="45" t="str">
         <f>IF(B117="String", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"', ",C117,");"), IF(B117="Integer", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"')-&gt;unsigned()-&gt;default(0);"), IF(B117="Text", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"');"), IF(B117="Date", CONCATENATE("$table-&gt;","timestamp","('",A117,"');")) )))</f>
-        <v>$table-&gt;string('detail', 250);</v>
+        <v>$table-&gt;timestamp('date');</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B118" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="C118" s="44">
-        <v>100</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C118" s="44"/>
       <c r="D118" s="43" t="str">
         <f>IF(B118="String", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"', ",C118,");"), IF(B118="Integer", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"')-&gt;unsigned()-&gt;default(0);"), IF(B118="Text", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"');"), IF(B118="Date", CONCATENATE("$table-&gt;","timestamp","('",A118,"');")) )))</f>
-        <v>$table-&gt;string('short_detail', 100);</v>
+        <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B119" s="42" t="s">
         <v>25</v>
@@ -3392,72 +3562,69 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B120" s="42" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="C120" s="44"/>
-      <c r="D120" s="45" t="str">
-        <f>IF(B120="String", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"', ",C120,");"), IF(B120="Integer", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"')-&gt;unsigned()-&gt;default(0);"), IF(B120="Text", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"');"), IF(B120="Date", CONCATENATE("$table-&gt;","timestamp","('",A120,"');")) )))</f>
-        <v>$table-&gt;integer('prize1')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D120" s="45" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="44" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B121" s="42" t="s">
         <v>25</v>
       </c>
       <c r="C121" s="44"/>
       <c r="D121" s="43" t="str">
-        <f t="shared" ref="D121:D122" si="4">IF(B121="String", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"', ",C121,");"), IF(B121="Integer", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"')-&gt;unsigned()-&gt;default(0);"), IF(B121="Text", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"');"), IF(B121="Date", CONCATENATE("$table-&gt;","timestamp","('",A121,"');")) )))</f>
+        <f t="shared" ref="D121" si="4">IF(B121="String", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"', ",C121,");"), IF(B121="Integer", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"')-&gt;unsigned()-&gt;default(0);"), IF(B121="Text", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"');"), IF(B121="Date", CONCATENATE("$table-&gt;","timestamp","('",A121,"');")) )))</f>
         <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="44" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B122" s="42" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="C122" s="44"/>
-      <c r="D122" s="45" t="str">
-        <f t="shared" si="4"/>
-        <v>$table-&gt;integer('prize2')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D122" s="45" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="44" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B123" s="42" t="s">
         <v>25</v>
       </c>
       <c r="C123" s="44"/>
       <c r="D123" s="43" t="str">
-        <f t="shared" ref="D123:D126" si="5">IF(B123="String", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"', ",C123,");"), IF(B123="Integer", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"')-&gt;unsigned()-&gt;default(0);"), IF(B123="Text", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"');"), IF(B123="Date", CONCATENATE("$table-&gt;","timestamp","('",A123,"');")) )))</f>
+        <f t="shared" ref="D123:D125" si="5">IF(B123="String", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"', ",C123,");"), IF(B123="Integer", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"')-&gt;unsigned()-&gt;default(0);"), IF(B123="Text", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"');"), IF(B123="Date", CONCATENATE("$table-&gt;","timestamp","('",A123,"');")) )))</f>
         <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B124" s="42" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="C124" s="44"/>
-      <c r="D124" s="43" t="str">
-        <f t="shared" si="5"/>
-        <v>$table-&gt;integer('prize3')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D124" s="45" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B125" s="42" t="s">
         <v>25</v>
@@ -3470,32 +3637,31 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="B126" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="B126" s="42" t="s">
-        <v>25</v>
-      </c>
       <c r="C126" s="44"/>
-      <c r="D126" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v>$table-&gt;integer('prize4')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D126" s="45" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="44" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B127" s="42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C127" s="44"/>
       <c r="D127" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="44" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B128" s="42" t="s">
         <v>6</v>
@@ -3510,7 +3676,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="44" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B129" s="42" t="s">
         <v>25</v>
@@ -3523,7 +3689,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B130" s="42" t="s">
         <v>25</v>
@@ -3554,18 +3720,18 @@
       <c r="D132" s="47"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="B133" s="41"/>
-      <c r="C133" s="41"/>
-      <c r="D133" s="41"/>
+      <c r="A133" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B133" s="48"/>
+      <c r="C133" s="48"/>
+      <c r="D133" s="48"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="41"/>
-      <c r="B134" s="41"/>
-      <c r="C134" s="41"/>
-      <c r="D134" s="41"/>
+      <c r="A134" s="48"/>
+      <c r="B134" s="48"/>
+      <c r="C134" s="48"/>
+      <c r="D134" s="48"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="39" t="s">
@@ -3583,7 +3749,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B136" s="7" t="s">
         <v>6</v>
@@ -3596,8 +3762,228 @@
         <v>$table-&gt;string('category', 255);</v>
       </c>
     </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="B140" s="48"/>
+      <c r="C140" s="48"/>
+      <c r="D140" s="48"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="48"/>
+      <c r="B141" s="48"/>
+      <c r="C141" s="48"/>
+      <c r="D141" s="48"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B142" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C142" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D142" s="41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C143" s="8"/>
+      <c r="D143" s="13" t="str">
+        <f>IF(B143="String", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"', ",C143,");"), IF(B143="Integer", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"')-&gt;unsigned()-&gt;default(0);"), IF(B143="Text", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"');"), IF(B143="Date", CONCATENATE("$table-&gt;","timestamp","('",A143,"');")) )))</f>
+        <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B144" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C144" s="44"/>
+      <c r="D144" s="45" t="str">
+        <f>IF(B144="String", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"', ",C144,");"), IF(B144="Integer", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"')-&gt;unsigned()-&gt;default(0);"), IF(B144="Text", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"');"), IF(B144="Date", CONCATENATE("$table-&gt;","timestamp","('",A144,"');")) )))</f>
+        <v>$table-&gt;integer('id_category')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B145" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C145" s="44">
+        <v>50</v>
+      </c>
+      <c r="D145" s="45" t="str">
+        <f>IF(B145="String", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"', ",C145,");"), IF(B145="Integer", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"')-&gt;unsigned()-&gt;default(0);"), IF(B145="Text", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"');"), IF(B145="Date", CONCATENATE("$table-&gt;","timestamp","('",A145,"');")) )))</f>
+        <v>$table-&gt;string('id_dentist', 50);</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="B146" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146" s="44"/>
+      <c r="D146" s="43" t="str">
+        <f>IF(B146="String", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"', ",C146,");"), IF(B146="Integer", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"')-&gt;unsigned()-&gt;default(0);"), IF(B146="Text", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"');"), IF(B146="Date", CONCATENATE("$table-&gt;","timestamp","('",A146,"');")) )))</f>
+        <v>$table-&gt;timestamp('date');</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B147" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C147" s="44"/>
+      <c r="D147" s="45" t="str">
+        <f>IF(B147="String", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"', ",C147,");"), IF(B147="Integer", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"')-&gt;unsigned()-&gt;default(0);"), IF(B147="Text", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"');"), IF(B147="Date", CONCATENATE("$table-&gt;","timestamp","('",A147,"');")) )))</f>
+        <v>$table-&gt;integer('teeth_no')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B148" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C148" s="44"/>
+      <c r="D148" s="45" t="str">
+        <f>IF(B148="String", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"', ",C148,");"), IF(B148="Integer", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"')-&gt;unsigned()-&gt;default(0);"), IF(B148="Text", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"');"), IF(B148="Date", CONCATENATE("$table-&gt;","timestamp","('",A148,"');")) )))</f>
+        <v>$table-&gt;text('description');</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B149" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C149" s="44"/>
+      <c r="D149" s="43" t="str">
+        <f t="shared" ref="D149:D154" si="6">IF(B149="String", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"', ",C149,");"), IF(B149="Integer", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"')-&gt;unsigned()-&gt;default(0);"), IF(B149="Text", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"');"), IF(B149="Date", CONCATENATE("$table-&gt;","timestamp","('",A149,"');")) )))</f>
+        <v>$table-&gt;integer('currency')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B150" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C150" s="44"/>
+      <c r="D150" s="45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="B151" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C151" s="44"/>
+      <c r="D151" s="43" t="str">
+        <f t="shared" si="6"/>
+        <v>$table-&gt;integer('quantity')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B152" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C152" s="44"/>
+      <c r="D152" s="45" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B153" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C153" s="44"/>
+      <c r="D153" s="45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B154" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C154" s="44"/>
+      <c r="D154" s="45" t="str">
+        <f t="shared" si="6"/>
+        <v>$table-&gt;text('clicnic_note');</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B155" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C155" s="44"/>
+      <c r="D155" s="45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="44"/>
+      <c r="B156" s="42"/>
+      <c r="C156" s="44"/>
+      <c r="D156" s="45"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="44"/>
+      <c r="B157" s="42"/>
+      <c r="C157" s="44"/>
+      <c r="D157" s="45"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="44"/>
+      <c r="B158" s="42"/>
+      <c r="C158" s="44"/>
+      <c r="D158" s="45"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="44"/>
+      <c r="B159" s="42"/>
+      <c r="C159" s="44"/>
+      <c r="D159" s="45"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A140:D141"/>
     <mergeCell ref="A111:D112"/>
     <mergeCell ref="A133:D134"/>
     <mergeCell ref="A105:D106"/>
@@ -3610,7 +3996,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <tableParts count="9">
+  <tableParts count="10">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -3620,6 +4006,7 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#5 Minor fixes ( Added new table, teeth_prize, which contain the default prize of teeth, fixed the jsTree of categories ) :squirrel:
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="132">
   <si>
     <t>PATIENT</t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t>$table-&gt;integer('is_active')-&gt;default(0);</t>
-  </si>
-  <si>
-    <t>$table-&gt;string('email', 200)-&gt;unique();</t>
   </si>
   <si>
     <t>phone</t>
@@ -413,6 +410,30 @@
   </si>
   <si>
     <t>$table-&gt;decimal('price1', 7, 2);</t>
+  </si>
+  <si>
+    <t>$table-&gt;integer('category_id')-&gt;index()-&gt;unsigned();</t>
+  </si>
+  <si>
+    <t>TeethsPrize</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('vat', 5, 2)-&gt;nullable();</t>
+  </si>
+  <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('price1', 10, 2);</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('price2', 10, 2)-&gt;nullable();</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('price3', 10, 2)-&gt;nullable();</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('price4', 10, 2)-&gt;nullable();</t>
   </si>
 </sst>
 </file>
@@ -480,10 +501,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -577,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -672,13 +692,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -697,11 +713,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="54">
     <dxf>
       <font>
         <b val="0"/>
@@ -1078,6 +1103,123 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0"/>
         </left>
@@ -1690,7 +1832,7 @@
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="47">
+    <tableColumn id="4" name="Code generated" dataDxfId="53">
       <calculatedColumnFormula>IF(B5="String", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"', ",C5,");"), IF(B5="Integer", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"')-&gt;unsigned()-&gt;default(0);"), IF(B5="Text", CONCATENATE("$table-&gt;",LOWER(B5),"('",A5,"');"), IF(B5="Date", CONCATENATE("$table-&gt;",LOWER(B5),"('",Table1[[#This Row],[Column name]],"');")) )))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Type Column"/>
@@ -1700,14 +1842,29 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table254687911" displayName="Table254687911" ref="A142:D159" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A142:D159"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table254687911" displayName="Table254687911" ref="A143:D160" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A143:D160"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Column name" dataDxfId="9"/>
+    <tableColumn id="2" name="Type" dataDxfId="8"/>
+    <tableColumn id="3" name="Length" dataDxfId="7"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="6">
+      <calculatedColumnFormula>IF(B144="String", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"', ",C144,");"), IF(B144="Integer", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"')-&gt;unsigned()-&gt;default(0);"), IF(B144="Text", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"');"), IF(B144="Date", CONCATENATE("$table-&gt;","timestamp","('",A144,"');")) )))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table254687912" displayName="Table254687912" ref="A165:D180" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A165:D180"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="3"/>
     <tableColumn id="2" name="Type" dataDxfId="2"/>
     <tableColumn id="3" name="Length" dataDxfId="1"/>
     <tableColumn id="4" name="Code generated" dataDxfId="0">
-      <calculatedColumnFormula>IF(B143="String", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"', ",C143,");"), IF(B143="Integer", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"')-&gt;unsigned()-&gt;default(0);"), IF(B143="Text", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"');"), IF(B143="Date", CONCATENATE("$table-&gt;","timestamp","('",A143,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B166="String", CONCATENATE("$table-&gt;",LOWER(B166),"('",A166,"', ",C166,");"), IF(B166="Integer", CONCATENATE("$table-&gt;",LOWER(B166),"('",A166,"')-&gt;unsigned()-&gt;default(0);"), IF(B166="Text", CONCATENATE("$table-&gt;",LOWER(B166),"('",A166,"');"), IF(B166="Date", CONCATENATE("$table-&gt;","timestamp","('",A166,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1715,14 +1872,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A57:D61" totalsRowShown="0" headerRowDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A57:D61" totalsRowShown="0" headerRowDxfId="52">
   <autoFilter ref="A57:D61"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="45"/>
+    <tableColumn id="2" name="Type" dataDxfId="51"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="44">
-      <calculatedColumnFormula>IF(B58="String", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"', ",C58,");"), IF(B58="Integer", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"')-&gt;unsigned()-&gt;default(0);"), IF(B58="Text", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');"), IF(B58="Date", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');")) )))</calculatedColumnFormula>
+    <tableColumn id="4" name="Code generated" dataDxfId="50">
+      <calculatedColumnFormula>IF(B58="String", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"', ",C58,")-&gt;nullable();"), IF(B58="Integer", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"')-&gt;unsigned()-&gt;default(0);"), IF(B58="Text", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');"), IF(B58="Date", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1730,14 +1887,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A65:D70" totalsRowShown="0" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A65:D70" totalsRowShown="0" headerRowDxfId="49">
   <autoFilter ref="A65:D70"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="42"/>
+    <tableColumn id="2" name="Type" dataDxfId="48"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="41">
-      <calculatedColumnFormula>IF(B66="String", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"', ",C66,");"), IF(B66="Integer", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"')-&gt;unsigned()-&gt;default(0);"), IF(B66="Text", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');"), IF(B66="Date", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');")) )))</calculatedColumnFormula>
+    <tableColumn id="4" name="Code generated" dataDxfId="47">
+      <calculatedColumnFormula>IF(B66="String", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"', ",C66,")-&gt;nullable();"), IF(B66="Integer", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"')-&gt;unsigned()-&gt;default(0);"), IF(B66="Text", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');"), IF(B66="Date", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1745,14 +1902,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A74:D76" totalsRowShown="0" headerRowDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A74:D76" totalsRowShown="0" headerRowDxfId="46">
   <autoFilter ref="A74:D76"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
-    <tableColumn id="2" name="Type" dataDxfId="39"/>
+    <tableColumn id="2" name="Type" dataDxfId="45"/>
     <tableColumn id="3" name="Length"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="38">
-      <calculatedColumnFormula>IF(B75="String", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"', ",C75,");"), IF(B75="Integer", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"')-&gt;unsigned()-&gt;default(0);"), IF(B75="Text", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');"), IF(B75="Date", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');")) )))</calculatedColumnFormula>
+    <tableColumn id="4" name="Code generated" dataDxfId="44">
+      <calculatedColumnFormula>IF(B75="String", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"', ",C75,")-&gt;nullable();"), IF(B75="Integer", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"')-&gt;unsigned()-&gt;default(0);"), IF(B75="Text", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');"), IF(B75="Date", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1760,56 +1917,58 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A82:E88" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A82:E88" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A82:E88"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column name" dataDxfId="35"/>
-    <tableColumn id="2" name="Type" dataDxfId="34"/>
-    <tableColumn id="3" name="Length" dataDxfId="33"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="32">
+    <tableColumn id="1" name="Column name" dataDxfId="41"/>
+    <tableColumn id="2" name="Type" dataDxfId="40"/>
+    <tableColumn id="3" name="Length" dataDxfId="39"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="38">
       <calculatedColumnFormula>IF(B83="String", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"', ",C83,");"), IF(B83="Integer", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"')-&gt;unsigned()-&gt;default(0);"), IF(B83="Text", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"');"), IF(B83="Date", CONCATENATE("$table-&gt;","timestamp","('",A83,"');")) )))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Type Column" dataDxfId="31"/>
+    <tableColumn id="5" name="Type Column" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A92:E102" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A92:E102" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A92:E102"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column name" dataDxfId="28"/>
-    <tableColumn id="2" name="Type" dataDxfId="27"/>
-    <tableColumn id="3" name="Length" dataDxfId="26"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="25"/>
-    <tableColumn id="5" name="Type Column" dataDxfId="24"/>
+    <tableColumn id="1" name="Column name" dataDxfId="34"/>
+    <tableColumn id="2" name="Type" dataDxfId="33"/>
+    <tableColumn id="3" name="Length" dataDxfId="32"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="31"/>
+    <tableColumn id="5" name="Type Column" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A107:D109" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A107:D109" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A107:D109"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Column name" dataDxfId="21"/>
-    <tableColumn id="2" name="Type" dataDxfId="20"/>
-    <tableColumn id="3" name="Length" dataDxfId="19"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="18"/>
+    <tableColumn id="1" name="Column name" dataDxfId="27"/>
+    <tableColumn id="2" name="Type" dataDxfId="26"/>
+    <tableColumn id="3" name="Length" dataDxfId="25"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="24">
+      <calculatedColumnFormula>IF(B108="String", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"', ",C108,")-&gt;nullable();"), IF(B108="Integer", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"')-&gt;unsigned()-&gt;default(0);"), IF(B108="Text", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"');"), IF(B108="Date", CONCATENATE("$table-&gt;","timestamp","('",A108,"');")) )))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table2546879" displayName="Table2546879" ref="A113:D131" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A113:D131"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table2546879" displayName="Table2546879" ref="A113:D132" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A113:D132"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Column name" dataDxfId="15"/>
-    <tableColumn id="2" name="Type" dataDxfId="14"/>
-    <tableColumn id="3" name="Length" dataDxfId="13"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="12">
+    <tableColumn id="1" name="Column name" dataDxfId="21"/>
+    <tableColumn id="2" name="Type" dataDxfId="20"/>
+    <tableColumn id="3" name="Length" dataDxfId="19"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="18">
       <calculatedColumnFormula>IF(B114="String", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"', ",C114,");"), IF(B114="Integer", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"')-&gt;unsigned()-&gt;default(0);"), IF(B114="Text", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"');"), IF(B114="Date", CONCATENATE("$table-&gt;","timestamp","('",A114,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1818,14 +1977,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table254687910" displayName="Table254687910" ref="A135:D137" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A135:D137"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table254687910" displayName="Table254687910" ref="A136:D138" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A136:D138"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Column name" dataDxfId="9"/>
-    <tableColumn id="2" name="Type" dataDxfId="8"/>
-    <tableColumn id="3" name="Length" dataDxfId="7"/>
-    <tableColumn id="4" name="Code generated" dataDxfId="6">
-      <calculatedColumnFormula>IF(B136="String", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"', ",C136,");"), IF(B136="Integer", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"')-&gt;unsigned()-&gt;default(0);"), IF(B136="Text", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"');"), IF(B136="Date", CONCATENATE("$table-&gt;","timestamp","('",A136,"');")) )))</calculatedColumnFormula>
+    <tableColumn id="1" name="Column name" dataDxfId="15"/>
+    <tableColumn id="2" name="Type" dataDxfId="14"/>
+    <tableColumn id="3" name="Length" dataDxfId="13"/>
+    <tableColumn id="4" name="Code generated" dataDxfId="12">
+      <calculatedColumnFormula>IF(B137="String", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"', ",C137,");"), IF(B137="Integer", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"')-&gt;unsigned()-&gt;default(0);"), IF(B137="Text", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"');"), IF(B137="Date", CONCATENATE("$table-&gt;","timestamp","('",A137,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1875,7 +2034,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1910,7 +2069,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2119,10 +2278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G159"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161:D165"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="D178" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2135,22 +2294,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2166,7 +2325,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2184,7 +2343,7 @@
         <v>$table-&gt;string('id_patient', 50);</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2198,8 +2357,8 @@
         <v>50</v>
       </c>
       <c r="D6" t="str">
-        <f>IF(B6="String", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"', ",C6,");"), IF(B6="Integer", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"')-&gt;unsigned()-&gt;default(0);"), IF(B6="Text", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"');"), IF(B6="Date", CONCATENATE("$table-&gt;",LOWER(B6),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('id_dentist', 50);</v>
+        <f>IF(B6="String", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"', ",C6,")-&gt;nullable();"), IF(B6="Integer", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"')-&gt;unsigned()-&gt;default(0);"), IF(B6="Text", CONCATENATE("$table-&gt;",LOWER(B6),"('",A6,"')-&gt;nullable();"), IF(B6="Date", CONCATENATE("$table-&gt;",LOWER(B6),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('id_dentist', 50)-&gt;nullable();</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2213,8 +2372,8 @@
         <v>50</v>
       </c>
       <c r="D7" t="str">
-        <f>IF(B7="String", CONCATENATE("$table-&gt;",LOWER(B7),"('",A7,"', ",C7,");"), IF(B7="Integer", CONCATENATE("$table-&gt;",LOWER(B7),"('",A7,"')-&gt;unsigned()-&gt;default(0);"), IF(B7="Text", CONCATENATE("$table-&gt;",LOWER(B7),"('",A7,"');"), IF(B7="Date", CONCATENATE("$table-&gt;",LOWER(B7),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('proffession', 50);</v>
+        <f>IF(B7="String", CONCATENATE("$table-&gt;",LOWER(B7),"('",A7,"', ",C7,")-&gt;nullable();"), IF(B7="Integer", CONCATENATE("$table-&gt;",LOWER(B7),"('",A7,"')-&gt;unsigned()-&gt;default(0);"), IF(B7="Text", CONCATENATE("$table-&gt;",LOWER(B7),"('",A7,"')-&gt;nullable();"), IF(B7="Date", CONCATENATE("$table-&gt;",LOWER(B7),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('proffession', 50)-&gt;nullable();</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2228,8 +2387,8 @@
         <v>255</v>
       </c>
       <c r="D8" t="str">
-        <f>IF(B8="String", CONCATENATE("$table-&gt;",LOWER(B8),"('",A8,"', ",C8,");"), IF(B8="Integer", CONCATENATE("$table-&gt;",LOWER(B8),"('",A8,"')-&gt;unsigned()-&gt;default(0);"), IF(B8="Text", CONCATENATE("$table-&gt;",LOWER(B8),"('",A8,"');"), IF(B8="Date", CONCATENATE("$table-&gt;",LOWER(B8),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('company_name', 255);</v>
+        <f>IF(B8="String", CONCATENATE("$table-&gt;",LOWER(B8),"('",A8,"', ",C8,")-&gt;nullable();"), IF(B8="Integer", CONCATENATE("$table-&gt;",LOWER(B8),"('",A8,"')-&gt;unsigned()-&gt;default(0);"), IF(B8="Text", CONCATENATE("$table-&gt;",LOWER(B8),"('",A8,"')-&gt;nullable();"), IF(B8="Date", CONCATENATE("$table-&gt;",LOWER(B8),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('company_name', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2243,8 +2402,8 @@
         <v>255</v>
       </c>
       <c r="D9" t="str">
-        <f>IF(B9="String", CONCATENATE("$table-&gt;",LOWER(B9),"('",A9,"', ",C9,");"), IF(B9="Integer", CONCATENATE("$table-&gt;",LOWER(B9),"('",A9,"')-&gt;unsigned()-&gt;default(0);"), IF(B9="Text", CONCATENATE("$table-&gt;",LOWER(B9),"('",A9,"');"), IF(B9="Date", CONCATENATE("$table-&gt;",LOWER(B9),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('last_name', 255);</v>
+        <f>IF(B9="String", CONCATENATE("$table-&gt;",LOWER(B9),"('",A9,"', ",C9,")-&gt;nullable();"), IF(B9="Integer", CONCATENATE("$table-&gt;",LOWER(B9),"('",A9,"')-&gt;unsigned()-&gt;default(0);"), IF(B9="Text", CONCATENATE("$table-&gt;",LOWER(B9),"('",A9,"')-&gt;nullable();"), IF(B9="Date", CONCATENATE("$table-&gt;",LOWER(B9),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('last_name', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2258,8 +2417,8 @@
         <v>255</v>
       </c>
       <c r="D10" t="str">
-        <f>IF(B10="String", CONCATENATE("$table-&gt;",LOWER(B10),"('",A10,"', ",C10,");"), IF(B10="Integer", CONCATENATE("$table-&gt;",LOWER(B10),"('",A10,"')-&gt;unsigned()-&gt;default(0);"), IF(B10="Text", CONCATENATE("$table-&gt;",LOWER(B10),"('",A10,"');"), IF(B10="Date", CONCATENATE("$table-&gt;",LOWER(B10),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('first_name', 255);</v>
+        <f>IF(B10="String", CONCATENATE("$table-&gt;",LOWER(B10),"('",A10,"', ",C10,")-&gt;nullable();"), IF(B10="Integer", CONCATENATE("$table-&gt;",LOWER(B10),"('",A10,"')-&gt;unsigned()-&gt;default(0);"), IF(B10="Text", CONCATENATE("$table-&gt;",LOWER(B10),"('",A10,"')-&gt;nullable();"), IF(B10="Date", CONCATENATE("$table-&gt;",LOWER(B10),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('first_name', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2273,8 +2432,8 @@
         <v>255</v>
       </c>
       <c r="D11" t="str">
-        <f>IF(B11="String", CONCATENATE("$table-&gt;",LOWER(B11),"('",A11,"', ",C11,");"), IF(B11="Integer", CONCATENATE("$table-&gt;",LOWER(B11),"('",A11,"')-&gt;unsigned()-&gt;default(0);"), IF(B11="Text", CONCATENATE("$table-&gt;",LOWER(B11),"('",A11,"');"), IF(B11="Date", CONCATENATE("$table-&gt;",LOWER(B11),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('address', 255);</v>
+        <f>IF(B11="String", CONCATENATE("$table-&gt;",LOWER(B11),"('",A11,"', ",C11,")-&gt;nullable();"), IF(B11="Integer", CONCATENATE("$table-&gt;",LOWER(B11),"('",A11,"')-&gt;unsigned()-&gt;default(0);"), IF(B11="Text", CONCATENATE("$table-&gt;",LOWER(B11),"('",A11,"')-&gt;nullable();"), IF(B11="Date", CONCATENATE("$table-&gt;",LOWER(B11),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('address', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2288,8 +2447,8 @@
         <v>100</v>
       </c>
       <c r="D12" t="str">
-        <f>IF(B12="String", CONCATENATE("$table-&gt;",LOWER(B12),"('",A12,"', ",C12,");"), IF(B12="Integer", CONCATENATE("$table-&gt;",LOWER(B12),"('",A12,"')-&gt;unsigned()-&gt;default(0);"), IF(B12="Text", CONCATENATE("$table-&gt;",LOWER(B12),"('",A12,"');"), IF(B12="Date", CONCATENATE("$table-&gt;",LOWER(B12),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('city', 100);</v>
+        <f>IF(B12="String", CONCATENATE("$table-&gt;",LOWER(B12),"('",A12,"', ",C12,")-&gt;nullable();"), IF(B12="Integer", CONCATENATE("$table-&gt;",LOWER(B12),"('",A12,"')-&gt;unsigned()-&gt;default(0);"), IF(B12="Text", CONCATENATE("$table-&gt;",LOWER(B12),"('",A12,"')-&gt;nullable();"), IF(B12="Date", CONCATENATE("$table-&gt;",LOWER(B12),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('city', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2300,7 +2459,7 @@
         <v>15</v>
       </c>
       <c r="D13" t="str">
-        <f>IF(B13="String", CONCATENATE("$table-&gt;",LOWER(B13),"('",A13,"', ",C13,");"), IF(B13="Integer", CONCATENATE("$table-&gt;",LOWER(B13),"('",A13,"')-&gt;unsigned()-&gt;default(0);"), IF(B13="Text", CONCATENATE("$table-&gt;",LOWER(B13),"('",A13,"');"), IF(B13="Date", CONCATENATE("$table-&gt;",LOWER(B13),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <f>IF(B13="String", CONCATENATE("$table-&gt;",LOWER(B13),"('",A13,"', ",C13,")-&gt;nullable();"), IF(B13="Integer", CONCATENATE("$table-&gt;",LOWER(B13),"('",A13,"')-&gt;unsigned()-&gt;default(0);"), IF(B13="Text", CONCATENATE("$table-&gt;",LOWER(B13),"('",A13,"')-&gt;nullable();"), IF(B13="Date", CONCATENATE("$table-&gt;",LOWER(B13),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;date('date_birth');</v>
       </c>
     </row>
@@ -2315,8 +2474,8 @@
         <v>20</v>
       </c>
       <c r="D14" t="str">
-        <f>IF(B14="String", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"', ",C14,");"), IF(B14="Integer", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"')-&gt;unsigned()-&gt;default(0);"), IF(B14="Text", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"');"), IF(B14="Date", CONCATENATE("$table-&gt;",LOWER(B14),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('marital_status', 20);</v>
+        <f>IF(B14="String", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"', ",C14,")-&gt;nullable();"), IF(B14="Integer", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"')-&gt;unsigned()-&gt;default(0);"), IF(B14="Text", CONCATENATE("$table-&gt;",LOWER(B14),"('",A14,"')-&gt;nullable();"), IF(B14="Date", CONCATENATE("$table-&gt;",LOWER(B14),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('marital_status', 20)-&gt;nullable();</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2330,8 +2489,8 @@
         <v>100</v>
       </c>
       <c r="D15" t="str">
-        <f>IF(B15="String", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"', ",C15,");"), IF(B15="Integer", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"')-&gt;unsigned()-&gt;default(0);"), IF(B15="Text", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"');"), IF(B15="Date", CONCATENATE("$table-&gt;",LOWER(B15),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('language', 100);</v>
+        <f>IF(B15="String", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"', ",C15,")-&gt;nullable();"), IF(B15="Integer", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"')-&gt;unsigned()-&gt;default(0);"), IF(B15="Text", CONCATENATE("$table-&gt;",LOWER(B15),"('",A15,"')-&gt;nullable();"), IF(B15="Date", CONCATENATE("$table-&gt;",LOWER(B15),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('language', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2345,8 +2504,8 @@
         <v>50</v>
       </c>
       <c r="D16" t="str">
-        <f>IF(B16="String", CONCATENATE("$table-&gt;",LOWER(B16),"('",A16,"', ",C16,");"), IF(B16="Integer", CONCATENATE("$table-&gt;",LOWER(B16),"('",A16,"')-&gt;unsigned()-&gt;default(0);"), IF(B16="Text", CONCATENATE("$table-&gt;",LOWER(B16),"('",A16,"');"), IF(B16="Date", CONCATENATE("$table-&gt;",LOWER(B16),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('sex', 50);</v>
+        <f>IF(B16="String", CONCATENATE("$table-&gt;",LOWER(B16),"('",A16,"', ",C16,")-&gt;nullable();"), IF(B16="Integer", CONCATENATE("$table-&gt;",LOWER(B16),"('",A16,"')-&gt;unsigned()-&gt;default(0);"), IF(B16="Text", CONCATENATE("$table-&gt;",LOWER(B16),"('",A16,"')-&gt;nullable();"), IF(B16="Date", CONCATENATE("$table-&gt;",LOWER(B16),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('sex', 50)-&gt;nullable();</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2360,8 +2519,8 @@
         <v>255</v>
       </c>
       <c r="D17" t="str">
-        <f>IF(B17="String", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"', ",C17,");"), IF(B17="Integer", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"')-&gt;unsigned()-&gt;default(0);"), IF(B17="Text", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"');"), IF(B17="Date", CONCATENATE("$table-&gt;",LOWER(B17),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('email', 255);</v>
+        <f>IF(B17="String", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"', ",C17,")-&gt;nullable();"), IF(B17="Integer", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"')-&gt;unsigned()-&gt;default(0);"), IF(B17="Text", CONCATENATE("$table-&gt;",LOWER(B17),"('",A17,"')-&gt;nullable();"), IF(B17="Date", CONCATENATE("$table-&gt;",LOWER(B17),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('email', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2375,8 +2534,8 @@
         <v>100</v>
       </c>
       <c r="D18" t="str">
-        <f>IF(B18="String", CONCATENATE("$table-&gt;",LOWER(B18),"('",A18,"', ",C18,");"), IF(B18="Integer", CONCATENATE("$table-&gt;",LOWER(B18),"('",A18,"')-&gt;unsigned()-&gt;default(0);"), IF(B18="Text", CONCATENATE("$table-&gt;",LOWER(B18),"('",A18,"');"), IF(B18="Date", CONCATENATE("$table-&gt;",LOWER(B18),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('zip_code', 100);</v>
+        <f>IF(B18="String", CONCATENATE("$table-&gt;",LOWER(B18),"('",A18,"', ",C18,")-&gt;nullable();"), IF(B18="Integer", CONCATENATE("$table-&gt;",LOWER(B18),"('",A18,"')-&gt;unsigned()-&gt;default(0);"), IF(B18="Text", CONCATENATE("$table-&gt;",LOWER(B18),"('",A18,"')-&gt;nullable();"), IF(B18="Date", CONCATENATE("$table-&gt;",LOWER(B18),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('zip_code', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2390,8 +2549,8 @@
         <v>200</v>
       </c>
       <c r="D19" t="str">
-        <f>IF(B19="String", CONCATENATE("$table-&gt;",LOWER(B19),"('",A19,"', ",C19,");"), IF(B19="Integer", CONCATENATE("$table-&gt;",LOWER(B19),"('",A19,"')-&gt;unsigned()-&gt;default(0);"), IF(B19="Text", CONCATENATE("$table-&gt;",LOWER(B19),"('",A19,"');"), IF(B19="Date", CONCATENATE("$table-&gt;",LOWER(B19),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('birth_place', 200);</v>
+        <f>IF(B19="String", CONCATENATE("$table-&gt;",LOWER(B19),"('",A19,"', ",C19,")-&gt;nullable();"), IF(B19="Integer", CONCATENATE("$table-&gt;",LOWER(B19),"('",A19,"')-&gt;unsigned()-&gt;default(0);"), IF(B19="Text", CONCATENATE("$table-&gt;",LOWER(B19),"('",A19,"')-&gt;nullable();"), IF(B19="Date", CONCATENATE("$table-&gt;",LOWER(B19),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('birth_place', 200)-&gt;nullable();</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2405,8 +2564,8 @@
         <v>30</v>
       </c>
       <c r="D20" t="str">
-        <f>IF(B20="String", CONCATENATE("$table-&gt;",LOWER(B20),"('",A20,"', ",C20,");"), IF(B20="Integer", CONCATENATE("$table-&gt;",LOWER(B20),"('",A20,"')-&gt;unsigned()-&gt;default(0);"), IF(B20="Text", CONCATENATE("$table-&gt;",LOWER(B20),"('",A20,"');"), IF(B20="Date", CONCATENATE("$table-&gt;",LOWER(B20),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('personal_phone', 30);</v>
+        <f>IF(B20="String", CONCATENATE("$table-&gt;",LOWER(B20),"('",A20,"', ",C20,")-&gt;nullable();"), IF(B20="Integer", CONCATENATE("$table-&gt;",LOWER(B20),"('",A20,"')-&gt;unsigned()-&gt;default(0);"), IF(B20="Text", CONCATENATE("$table-&gt;",LOWER(B20),"('",A20,"')-&gt;nullable();"), IF(B20="Date", CONCATENATE("$table-&gt;",LOWER(B20),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('personal_phone', 30)-&gt;nullable();</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2420,8 +2579,8 @@
         <v>30</v>
       </c>
       <c r="D21" t="str">
-        <f>IF(B21="String", CONCATENATE("$table-&gt;",LOWER(B21),"('",A21,"', ",C21,");"), IF(B21="Integer", CONCATENATE("$table-&gt;",LOWER(B21),"('",A21,"')-&gt;unsigned()-&gt;default(0);"), IF(B21="Text", CONCATENATE("$table-&gt;",LOWER(B21),"('",A21,"');"), IF(B21="Date", CONCATENATE("$table-&gt;",LOWER(B21),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('office_phone', 30);</v>
+        <f>IF(B21="String", CONCATENATE("$table-&gt;",LOWER(B21),"('",A21,"', ",C21,")-&gt;nullable();"), IF(B21="Integer", CONCATENATE("$table-&gt;",LOWER(B21),"('",A21,"')-&gt;unsigned()-&gt;default(0);"), IF(B21="Text", CONCATENATE("$table-&gt;",LOWER(B21),"('",A21,"')-&gt;nullable();"), IF(B21="Date", CONCATENATE("$table-&gt;",LOWER(B21),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('office_phone', 30)-&gt;nullable();</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2435,8 +2594,8 @@
         <v>30</v>
       </c>
       <c r="D22" t="str">
-        <f>IF(B22="String", CONCATENATE("$table-&gt;",LOWER(B22),"('",A22,"', ",C22,");"), IF(B22="Integer", CONCATENATE("$table-&gt;",LOWER(B22),"('",A22,"')-&gt;unsigned()-&gt;default(0);"), IF(B22="Text", CONCATENATE("$table-&gt;",LOWER(B22),"('",A22,"');"), IF(B22="Date", CONCATENATE("$table-&gt;",LOWER(B22),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('fax', 30);</v>
+        <f>IF(B22="String", CONCATENATE("$table-&gt;",LOWER(B22),"('",A22,"', ",C22,")-&gt;nullable();"), IF(B22="Integer", CONCATENATE("$table-&gt;",LOWER(B22),"('",A22,"')-&gt;unsigned()-&gt;default(0);"), IF(B22="Text", CONCATENATE("$table-&gt;",LOWER(B22),"('",A22,"')-&gt;nullable();"), IF(B22="Date", CONCATENATE("$table-&gt;",LOWER(B22),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('fax', 30)-&gt;nullable();</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2450,8 +2609,8 @@
         <v>255</v>
       </c>
       <c r="D23" t="str">
-        <f>IF(B23="String", CONCATENATE("$table-&gt;",LOWER(B23),"('",A23,"', ",C23,");"), IF(B23="Integer", CONCATENATE("$table-&gt;",LOWER(B23),"('",A23,"')-&gt;unsigned()-&gt;default(0);"), IF(B23="Text", CONCATENATE("$table-&gt;",LOWER(B23),"('",A23,"');"), IF(B23="Date", CONCATENATE("$table-&gt;",LOWER(B23),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('tax_code', 255);</v>
+        <f>IF(B23="String", CONCATENATE("$table-&gt;",LOWER(B23),"('",A23,"', ",C23,")-&gt;nullable();"), IF(B23="Integer", CONCATENATE("$table-&gt;",LOWER(B23),"('",A23,"')-&gt;unsigned()-&gt;default(0);"), IF(B23="Text", CONCATENATE("$table-&gt;",LOWER(B23),"('",A23,"')-&gt;nullable();"), IF(B23="Date", CONCATENATE("$table-&gt;",LOWER(B23),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('tax_code', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2465,13 +2624,13 @@
         <v>255</v>
       </c>
       <c r="D24" t="str">
-        <f>IF(B24="String", CONCATENATE("$table-&gt;",LOWER(B24),"('",A24,"', ",C24,");"), IF(B24="Integer", CONCATENATE("$table-&gt;",LOWER(B24),"('",A24,"')-&gt;unsigned()-&gt;default(0);"), IF(B24="Text", CONCATENATE("$table-&gt;",LOWER(B24),"('",A24,"');"), IF(B24="Date", CONCATENATE("$table-&gt;",LOWER(B24),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('photo', 255);</v>
+        <f>IF(B24="String", CONCATENATE("$table-&gt;",LOWER(B24),"('",A24,"', ",C24,")-&gt;nullable();"), IF(B24="Integer", CONCATENATE("$table-&gt;",LOWER(B24),"('",A24,"')-&gt;unsigned()-&gt;default(0);"), IF(B24="Text", CONCATENATE("$table-&gt;",LOWER(B24),"('",A24,"')-&gt;nullable();"), IF(B24="Date", CONCATENATE("$table-&gt;",LOWER(B24),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('photo', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -2479,23 +2638,24 @@
       <c r="C25">
         <v>255</v>
       </c>
-      <c r="D25" s="40" t="str">
-        <f>IF(B25="String", CONCATENATE("$table-&gt;",LOWER(B25),"('",A25,"', ",C25,");"), IF(B25="Integer", CONCATENATE("$table-&gt;",LOWER(B25),"('",A25,"')-&gt;unsigned()-&gt;default(0);"), IF(B25="Text", CONCATENATE("$table-&gt;",LOWER(B25),"('",A25,"');"), IF(B25="Date", CONCATENATE("$table-&gt;",LOWER(B25),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('image_path', 255);</v>
+      <c r="D25" t="str">
+        <f>IF(B25="String", CONCATENATE("$table-&gt;",LOWER(B25),"('",A25,"', ",C25,")-&gt;nullable();"), IF(B25="Integer", CONCATENATE("$table-&gt;",LOWER(B25),"('",A25,"')-&gt;unsigned()-&gt;default(0);"), IF(B25="Text", CONCATENATE("$table-&gt;",LOWER(B25),"('",A25,"')-&gt;nullable();"), IF(B25="Date", CONCATENATE("$table-&gt;",LOWER(B25),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('image_path', 255)-&gt;nullable();</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="38" t="s">
-        <v>81</v>
+      <c r="D26" t="str">
+        <f>IF(B26="String", CONCATENATE("$table-&gt;",LOWER(B26),"('",A26,"', ",C26,")-&gt;nullable();"), IF(B26="Integer", CONCATENATE("$table-&gt;",LOWER(B26),"('",A26,"')-&gt;unsigned()-&gt;default(0);"), IF(B26="Text", CONCATENATE("$table-&gt;",LOWER(B26),"('",A26,"')-&gt;nullable();"), IF(B26="Date", CONCATENATE("$table-&gt;",LOWER(B26),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;integer('image_id')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2506,7 +2666,7 @@
         <v>25</v>
       </c>
       <c r="D27" t="str">
-        <f>IF(B27="String", CONCATENATE("$table-&gt;",LOWER(B27),"('",A27,"', ",C27,");"), IF(B27="Integer", CONCATENATE("$table-&gt;",LOWER(B27),"('",A27,"')-&gt;unsigned()-&gt;default(0);"), IF(B27="Text", CONCATENATE("$table-&gt;",LOWER(B27),"('",A27,"');"), IF(B27="Date", CONCATENATE("$table-&gt;",LOWER(B27),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <f>IF(B27="String", CONCATENATE("$table-&gt;",LOWER(B27),"('",A27,"', ",C27,")-&gt;nullable();"), IF(B27="Integer", CONCATENATE("$table-&gt;",LOWER(B27),"('",A27,"')-&gt;unsigned()-&gt;default(0);"), IF(B27="Text", CONCATENATE("$table-&gt;",LOWER(B27),"('",A27,"')-&gt;nullable();"), IF(B27="Date", CONCATENATE("$table-&gt;",LOWER(B27),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;integer('type_photo')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
@@ -2518,7 +2678,7 @@
         <v>15</v>
       </c>
       <c r="D28" t="str">
-        <f>IF(B28="String", CONCATENATE("$table-&gt;",LOWER(B28),"('",A28,"', ",C28,");"), IF(B28="Integer", CONCATENATE("$table-&gt;",LOWER(B28),"('",A28,"')-&gt;unsigned()-&gt;default(0);"), IF(B28="Text", CONCATENATE("$table-&gt;",LOWER(B28),"('",A28,"');"), IF(B28="Date", CONCATENATE("$table-&gt;",LOWER(B28),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <f>IF(B28="String", CONCATENATE("$table-&gt;",LOWER(B28),"('",A28,"', ",C28,")-&gt;nullable();"), IF(B28="Integer", CONCATENATE("$table-&gt;",LOWER(B28),"('",A28,"')-&gt;unsigned()-&gt;default(0);"), IF(B28="Text", CONCATENATE("$table-&gt;",LOWER(B28),"('",A28,"')-&gt;nullable();"), IF(B28="Date", CONCATENATE("$table-&gt;",LOWER(B28),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;date('date_last_visit');</v>
       </c>
     </row>
@@ -2530,7 +2690,7 @@
         <v>15</v>
       </c>
       <c r="D29" t="str">
-        <f>IF(B29="String", CONCATENATE("$table-&gt;",LOWER(B29),"('",A29,"', ",C29,");"), IF(B29="Integer", CONCATENATE("$table-&gt;",LOWER(B29),"('",A29,"')-&gt;unsigned()-&gt;default(0);"), IF(B29="Text", CONCATENATE("$table-&gt;",LOWER(B29),"('",A29,"');"), IF(B29="Date", CONCATENATE("$table-&gt;",LOWER(B29),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <f>IF(B29="String", CONCATENATE("$table-&gt;",LOWER(B29),"('",A29,"', ",C29,")-&gt;nullable();"), IF(B29="Integer", CONCATENATE("$table-&gt;",LOWER(B29),"('",A29,"')-&gt;unsigned()-&gt;default(0);"), IF(B29="Text", CONCATENATE("$table-&gt;",LOWER(B29),"('",A29,"')-&gt;nullable();"), IF(B29="Date", CONCATENATE("$table-&gt;",LOWER(B29),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;date('date_next_visit');</v>
       </c>
     </row>
@@ -2542,7 +2702,7 @@
         <v>15</v>
       </c>
       <c r="D30" t="str">
-        <f>IF(B30="String", CONCATENATE("$table-&gt;",LOWER(B30),"('",A30,"', ",C30,");"), IF(B30="Integer", CONCATENATE("$table-&gt;",LOWER(B30),"('",A30,"')-&gt;unsigned()-&gt;default(0);"), IF(B30="Text", CONCATENATE("$table-&gt;",LOWER(B30),"('",A30,"');"), IF(B30="Date", CONCATENATE("$table-&gt;",LOWER(B30),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <f>IF(B30="String", CONCATENATE("$table-&gt;",LOWER(B30),"('",A30,"', ",C30,")-&gt;nullable();"), IF(B30="Integer", CONCATENATE("$table-&gt;",LOWER(B30),"('",A30,"')-&gt;unsigned()-&gt;default(0);"), IF(B30="Text", CONCATENATE("$table-&gt;",LOWER(B30),"('",A30,"')-&gt;nullable();"), IF(B30="Date", CONCATENATE("$table-&gt;",LOWER(B30),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;date('date_first_visit');</v>
       </c>
     </row>
@@ -2554,7 +2714,7 @@
         <v>15</v>
       </c>
       <c r="D31" t="str">
-        <f>IF(B31="String", CONCATENATE("$table-&gt;",LOWER(B31),"('",A31,"', ",C31,");"), IF(B31="Integer", CONCATENATE("$table-&gt;",LOWER(B31),"('",A31,"')-&gt;unsigned()-&gt;default(0);"), IF(B31="Text", CONCATENATE("$table-&gt;",LOWER(B31),"('",A31,"');"), IF(B31="Date", CONCATENATE("$table-&gt;",LOWER(B31),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <f>IF(B31="String", CONCATENATE("$table-&gt;",LOWER(B31),"('",A31,"', ",C31,")-&gt;nullable();"), IF(B31="Integer", CONCATENATE("$table-&gt;",LOWER(B31),"('",A31,"')-&gt;unsigned()-&gt;default(0);"), IF(B31="Text", CONCATENATE("$table-&gt;",LOWER(B31),"('",A31,"')-&gt;nullable();"), IF(B31="Date", CONCATENATE("$table-&gt;",LOWER(B31),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;date('date_last_pay');</v>
       </c>
     </row>
@@ -2566,8 +2726,8 @@
         <v>31</v>
       </c>
       <c r="D32" t="str">
-        <f>IF(B32="String", CONCATENATE("$table-&gt;",LOWER(B32),"('",A32,"', ",C32,");"), IF(B32="Integer", CONCATENATE("$table-&gt;",LOWER(B32),"('",A32,"')-&gt;unsigned()-&gt;default(0);"), IF(B32="Text", CONCATENATE("$table-&gt;",LOWER(B32),"('",A32,"');"), IF(B32="Date", CONCATENATE("$table-&gt;",LOWER(B32),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;text('note');</v>
+        <f>IF(B32="String", CONCATENATE("$table-&gt;",LOWER(B32),"('",A32,"', ",C32,")-&gt;nullable();"), IF(B32="Integer", CONCATENATE("$table-&gt;",LOWER(B32),"('",A32,"')-&gt;unsigned()-&gt;default(0);"), IF(B32="Text", CONCATENATE("$table-&gt;",LOWER(B32),"('",A32,"')-&gt;nullable();"), IF(B32="Date", CONCATENATE("$table-&gt;",LOWER(B32),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note')-&gt;nullable();</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2578,7 +2738,7 @@
         <v>25</v>
       </c>
       <c r="D33" t="str">
-        <f>IF(B33="String", CONCATENATE("$table-&gt;",LOWER(B33),"('",A33,"', ",C33,");"), IF(B33="Integer", CONCATENATE("$table-&gt;",LOWER(B33),"('",A33,"')-&gt;unsigned()-&gt;default(0);"), IF(B33="Text", CONCATENATE("$table-&gt;",LOWER(B33),"('",A33,"');"), IF(B33="Date", CONCATENATE("$table-&gt;",LOWER(B33),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <f>IF(B33="String", CONCATENATE("$table-&gt;",LOWER(B33),"('",A33,"', ",C33,")-&gt;nullable();"), IF(B33="Integer", CONCATENATE("$table-&gt;",LOWER(B33),"('",A33,"')-&gt;unsigned()-&gt;default(0);"), IF(B33="Text", CONCATENATE("$table-&gt;",LOWER(B33),"('",A33,"')-&gt;nullable();"), IF(B33="Date", CONCATENATE("$table-&gt;",LOWER(B33),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;integer('discount')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
@@ -2593,8 +2753,8 @@
         <v>100</v>
       </c>
       <c r="D34" t="str">
-        <f>IF(B34="String", CONCATENATE("$table-&gt;",LOWER(B34),"('",A34,"', ",C34,");"), IF(B34="Integer", CONCATENATE("$table-&gt;",LOWER(B34),"('",A34,"')-&gt;unsigned()-&gt;default(0);"), IF(B34="Text", CONCATENATE("$table-&gt;",LOWER(B34),"('",A34,"');"), IF(B34="Date", CONCATENATE("$table-&gt;",LOWER(B34),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('insurance', 100);</v>
+        <f>IF(B34="String", CONCATENATE("$table-&gt;",LOWER(B34),"('",A34,"', ",C34,")-&gt;nullable();"), IF(B34="Integer", CONCATENATE("$table-&gt;",LOWER(B34),"('",A34,"')-&gt;unsigned()-&gt;default(0);"), IF(B34="Text", CONCATENATE("$table-&gt;",LOWER(B34),"('",A34,"')-&gt;nullable();"), IF(B34="Date", CONCATENATE("$table-&gt;",LOWER(B34),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('insurance', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2605,7 +2765,7 @@
         <v>25</v>
       </c>
       <c r="D35" t="str">
-        <f>IF(B35="String", CONCATENATE("$table-&gt;",LOWER(B35),"('",A35,"', ",C35,");"), IF(B35="Integer", CONCATENATE("$table-&gt;",LOWER(B35),"('",A35,"')-&gt;unsigned()-&gt;default(0);"), IF(B35="Text", CONCATENATE("$table-&gt;",LOWER(B35),"('",A35,"');"), IF(B35="Date", CONCATENATE("$table-&gt;",LOWER(B35),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <f>IF(B35="String", CONCATENATE("$table-&gt;",LOWER(B35),"('",A35,"', ",C35,")-&gt;nullable();"), IF(B35="Integer", CONCATENATE("$table-&gt;",LOWER(B35),"('",A35,"')-&gt;unsigned()-&gt;default(0);"), IF(B35="Text", CONCATENATE("$table-&gt;",LOWER(B35),"('",A35,"')-&gt;nullable();"), IF(B35="Date", CONCATENATE("$table-&gt;",LOWER(B35),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;integer('user_update')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
@@ -2620,8 +2780,8 @@
         <v>100</v>
       </c>
       <c r="D36" t="str">
-        <f>IF(B36="String", CONCATENATE("$table-&gt;",LOWER(B36),"('",A36,"', ",C36,");"), IF(B36="Integer", CONCATENATE("$table-&gt;",LOWER(B36),"('",A36,"')-&gt;unsigned()-&gt;default(0);"), IF(B36="Text", CONCATENATE("$table-&gt;",LOWER(B36),"('",A36,"');"), IF(B36="Date", CONCATENATE("$table-&gt;",LOWER(B36),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('doctor_name', 100);</v>
+        <f>IF(B36="String", CONCATENATE("$table-&gt;",LOWER(B36),"('",A36,"', ",C36,")-&gt;nullable();"), IF(B36="Integer", CONCATENATE("$table-&gt;",LOWER(B36),"('",A36,"')-&gt;unsigned()-&gt;default(0);"), IF(B36="Text", CONCATENATE("$table-&gt;",LOWER(B36),"('",A36,"')-&gt;nullable();"), IF(B36="Date", CONCATENATE("$table-&gt;",LOWER(B36),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('doctor_name', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2635,8 +2795,8 @@
         <v>50</v>
       </c>
       <c r="D37" t="str">
-        <f>IF(B37="String", CONCATENATE("$table-&gt;",LOWER(B37),"('",A37,"', ",C37,");"), IF(B37="Integer", CONCATENATE("$table-&gt;",LOWER(B37),"('",A37,"')-&gt;unsigned()-&gt;default(0);"), IF(B37="Text", CONCATENATE("$table-&gt;",LOWER(B37),"('",A37,"');"), IF(B37="Date", CONCATENATE("$table-&gt;",LOWER(B37),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('phone_doctor', 50);</v>
+        <f>IF(B37="String", CONCATENATE("$table-&gt;",LOWER(B37),"('",A37,"', ",C37,")-&gt;nullable();"), IF(B37="Integer", CONCATENATE("$table-&gt;",LOWER(B37),"('",A37,"')-&gt;unsigned()-&gt;default(0);"), IF(B37="Text", CONCATENATE("$table-&gt;",LOWER(B37),"('",A37,"')-&gt;nullable();"), IF(B37="Date", CONCATENATE("$table-&gt;",LOWER(B37),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('phone_doctor', 50)-&gt;nullable();</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2650,8 +2810,8 @@
         <v>10</v>
       </c>
       <c r="D38" t="str">
-        <f>IF(B38="String", CONCATENATE("$table-&gt;",LOWER(B38),"('",A38,"', ",C38,");"), IF(B38="Integer", CONCATENATE("$table-&gt;",LOWER(B38),"('",A38,"')-&gt;unsigned()-&gt;default(0);"), IF(B38="Text", CONCATENATE("$table-&gt;",LOWER(B38),"('",A38,"');"), IF(B38="Date", CONCATENATE("$table-&gt;",LOWER(B38),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('adult_child', 10);</v>
+        <f>IF(B38="String", CONCATENATE("$table-&gt;",LOWER(B38),"('",A38,"', ",C38,")-&gt;nullable();"), IF(B38="Integer", CONCATENATE("$table-&gt;",LOWER(B38),"('",A38,"')-&gt;unsigned()-&gt;default(0);"), IF(B38="Text", CONCATENATE("$table-&gt;",LOWER(B38),"('",A38,"')-&gt;nullable();"), IF(B38="Date", CONCATENATE("$table-&gt;",LOWER(B38),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('adult_child', 10)-&gt;nullable();</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2662,7 +2822,7 @@
         <v>25</v>
       </c>
       <c r="D39" t="str">
-        <f>IF(B39="String", CONCATENATE("$table-&gt;",LOWER(B39),"('",A39,"', ",C39,");"), IF(B39="Integer", CONCATENATE("$table-&gt;",LOWER(B39),"('",A39,"')-&gt;unsigned()-&gt;default(0);"), IF(B39="Text", CONCATENATE("$table-&gt;",LOWER(B39),"('",A39,"');"), IF(B39="Date", CONCATENATE("$table-&gt;",LOWER(B39),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <f>IF(B39="String", CONCATENATE("$table-&gt;",LOWER(B39),"('",A39,"', ",C39,")-&gt;nullable();"), IF(B39="Integer", CONCATENATE("$table-&gt;",LOWER(B39),"('",A39,"')-&gt;unsigned()-&gt;default(0);"), IF(B39="Text", CONCATENATE("$table-&gt;",LOWER(B39),"('",A39,"')-&gt;nullable();"), IF(B39="Date", CONCATENATE("$table-&gt;",LOWER(B39),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;integer('age')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
@@ -2677,8 +2837,8 @@
         <v>20</v>
       </c>
       <c r="D40" t="str">
-        <f>IF(B40="String", CONCATENATE("$table-&gt;",LOWER(B40),"('",A40,"', ",C40,");"), IF(B40="Integer", CONCATENATE("$table-&gt;",LOWER(B40),"('",A40,"')-&gt;unsigned()-&gt;default(0);"), IF(B40="Text", CONCATENATE("$table-&gt;",LOWER(B40),"('",A40,"');"), IF(B40="Date", CONCATENATE("$table-&gt;",LOWER(B40),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('barcode', 20);</v>
+        <f>IF(B40="String", CONCATENATE("$table-&gt;",LOWER(B40),"('",A40,"', ",C40,")-&gt;nullable();"), IF(B40="Integer", CONCATENATE("$table-&gt;",LOWER(B40),"('",A40,"')-&gt;unsigned()-&gt;default(0);"), IF(B40="Text", CONCATENATE("$table-&gt;",LOWER(B40),"('",A40,"')-&gt;nullable();"), IF(B40="Date", CONCATENATE("$table-&gt;",LOWER(B40),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('barcode', 20)-&gt;nullable();</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2692,8 +2852,8 @@
         <v>50</v>
       </c>
       <c r="D41" t="str">
-        <f>IF(B41="String", CONCATENATE("$table-&gt;",LOWER(B41),"('",A41,"', ",C41,");"), IF(B41="Integer", CONCATENATE("$table-&gt;",LOWER(B41),"('",A41,"')-&gt;unsigned()-&gt;default(0);"), IF(B41="Text", CONCATENATE("$table-&gt;",LOWER(B41),"('",A41,"');"), IF(B41="Date", CONCATENATE("$table-&gt;",LOWER(B41),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('province', 50);</v>
+        <f>IF(B41="String", CONCATENATE("$table-&gt;",LOWER(B41),"('",A41,"', ",C41,")-&gt;nullable();"), IF(B41="Integer", CONCATENATE("$table-&gt;",LOWER(B41),"('",A41,"')-&gt;unsigned()-&gt;default(0);"), IF(B41="Text", CONCATENATE("$table-&gt;",LOWER(B41),"('",A41,"')-&gt;nullable();"), IF(B41="Date", CONCATENATE("$table-&gt;",LOWER(B41),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('province', 50)-&gt;nullable();</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2707,8 +2867,8 @@
         <v>50</v>
       </c>
       <c r="D42" t="str">
-        <f>IF(B42="String", CONCATENATE("$table-&gt;",LOWER(B42),"('",A42,"', ",C42,");"), IF(B42="Integer", CONCATENATE("$table-&gt;",LOWER(B42),"('",A42,"')-&gt;unsigned()-&gt;default(0);"), IF(B42="Text", CONCATENATE("$table-&gt;",LOWER(B42),"('",A42,"');"), IF(B42="Date", CONCATENATE("$table-&gt;",LOWER(B42),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('id_family', 50);</v>
+        <f>IF(B42="String", CONCATENATE("$table-&gt;",LOWER(B42),"('",A42,"', ",C42,")-&gt;nullable();"), IF(B42="Integer", CONCATENATE("$table-&gt;",LOWER(B42),"('",A42,"')-&gt;unsigned()-&gt;default(0);"), IF(B42="Text", CONCATENATE("$table-&gt;",LOWER(B42),"('",A42,"')-&gt;nullable();"), IF(B42="Date", CONCATENATE("$table-&gt;",LOWER(B42),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('id_family', 50)-&gt;nullable();</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2719,7 +2879,7 @@
         <v>25</v>
       </c>
       <c r="D43" t="str">
-        <f>IF(B43="String", CONCATENATE("$table-&gt;",LOWER(B43),"('",A43,"', ",C43,");"), IF(B43="Integer", CONCATENATE("$table-&gt;",LOWER(B43),"('",A43,"')-&gt;unsigned()-&gt;default(0);"), IF(B43="Text", CONCATENATE("$table-&gt;",LOWER(B43),"('",A43,"');"), IF(B43="Date", CONCATENATE("$table-&gt;",LOWER(B43),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <f>IF(B43="String", CONCATENATE("$table-&gt;",LOWER(B43),"('",A43,"', ",C43,")-&gt;nullable();"), IF(B43="Integer", CONCATENATE("$table-&gt;",LOWER(B43),"('",A43,"')-&gt;unsigned()-&gt;default(0);"), IF(B43="Text", CONCATENATE("$table-&gt;",LOWER(B43),"('",A43,"')-&gt;nullable();"), IF(B43="Date", CONCATENATE("$table-&gt;",LOWER(B43),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;integer('family_type')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
@@ -2734,8 +2894,8 @@
         <v>255</v>
       </c>
       <c r="D44" t="str">
-        <f>IF(B44="String", CONCATENATE("$table-&gt;",LOWER(B44),"('",A44,"', ",C44,");"), IF(B44="Integer", CONCATENATE("$table-&gt;",LOWER(B44),"('",A44,"')-&gt;unsigned()-&gt;default(0);"), IF(B44="Text", CONCATENATE("$table-&gt;",LOWER(B44),"('",A44,"');"), IF(B44="Date", CONCATENATE("$table-&gt;",LOWER(B44),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('nation', 255);</v>
+        <f>IF(B44="String", CONCATENATE("$table-&gt;",LOWER(B44),"('",A44,"', ",C44,")-&gt;nullable();"), IF(B44="Integer", CONCATENATE("$table-&gt;",LOWER(B44),"('",A44,"')-&gt;unsigned()-&gt;default(0);"), IF(B44="Text", CONCATENATE("$table-&gt;",LOWER(B44),"('",A44,"')-&gt;nullable();"), IF(B44="Date", CONCATENATE("$table-&gt;",LOWER(B44),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('nation', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2749,8 +2909,8 @@
         <v>255</v>
       </c>
       <c r="D45" t="str">
-        <f>IF(B45="String", CONCATENATE("$table-&gt;",LOWER(B45),"('",A45,"', ",C45,");"), IF(B45="Integer", CONCATENATE("$table-&gt;",LOWER(B45),"('",A45,"')-&gt;unsigned()-&gt;default(0);"), IF(B45="Text", CONCATENATE("$table-&gt;",LOWER(B45),"('",A45,"');"), IF(B45="Date", CONCATENATE("$table-&gt;",LOWER(B45),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('site', 255);</v>
+        <f>IF(B45="String", CONCATENATE("$table-&gt;",LOWER(B45),"('",A45,"', ",C45,")-&gt;nullable();"), IF(B45="Integer", CONCATENATE("$table-&gt;",LOWER(B45),"('",A45,"')-&gt;unsigned()-&gt;default(0);"), IF(B45="Text", CONCATENATE("$table-&gt;",LOWER(B45),"('",A45,"')-&gt;nullable();"), IF(B45="Date", CONCATENATE("$table-&gt;",LOWER(B45),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('site', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2761,8 +2921,8 @@
         <v>31</v>
       </c>
       <c r="D46" t="str">
-        <f>IF(B46="String", CONCATENATE("$table-&gt;",LOWER(B46),"('",A46,"', ",C46,");"), IF(B46="Integer", CONCATENATE("$table-&gt;",LOWER(B46),"('",A46,"')-&gt;unsigned()-&gt;default(0);"), IF(B46="Text", CONCATENATE("$table-&gt;",LOWER(B46),"('",A46,"');"), IF(B46="Date", CONCATENATE("$table-&gt;",LOWER(B46),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;text('note1');</v>
+        <f>IF(B46="String", CONCATENATE("$table-&gt;",LOWER(B46),"('",A46,"', ",C46,")-&gt;nullable();"), IF(B46="Integer", CONCATENATE("$table-&gt;",LOWER(B46),"('",A46,"')-&gt;unsigned()-&gt;default(0);"), IF(B46="Text", CONCATENATE("$table-&gt;",LOWER(B46),"('",A46,"')-&gt;nullable();"), IF(B46="Date", CONCATENATE("$table-&gt;",LOWER(B46),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note1')-&gt;nullable();</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2773,8 +2933,8 @@
         <v>31</v>
       </c>
       <c r="D47" t="str">
-        <f>IF(B47="String", CONCATENATE("$table-&gt;",LOWER(B47),"('",A47,"', ",C47,");"), IF(B47="Integer", CONCATENATE("$table-&gt;",LOWER(B47),"('",A47,"')-&gt;unsigned()-&gt;default(0);"), IF(B47="Text", CONCATENATE("$table-&gt;",LOWER(B47),"('",A47,"');"), IF(B47="Date", CONCATENATE("$table-&gt;",LOWER(B47),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;text('note2');</v>
+        <f>IF(B47="String", CONCATENATE("$table-&gt;",LOWER(B47),"('",A47,"', ",C47,")-&gt;nullable();"), IF(B47="Integer", CONCATENATE("$table-&gt;",LOWER(B47),"('",A47,"')-&gt;unsigned()-&gt;default(0);"), IF(B47="Text", CONCATENATE("$table-&gt;",LOWER(B47),"('",A47,"')-&gt;nullable();"), IF(B47="Date", CONCATENATE("$table-&gt;",LOWER(B47),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note2')-&gt;nullable();</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2785,8 +2945,8 @@
         <v>31</v>
       </c>
       <c r="D48" t="str">
-        <f>IF(B48="String", CONCATENATE("$table-&gt;",LOWER(B48),"('",A48,"', ",C48,");"), IF(B48="Integer", CONCATENATE("$table-&gt;",LOWER(B48),"('",A48,"')-&gt;unsigned()-&gt;default(0);"), IF(B48="Text", CONCATENATE("$table-&gt;",LOWER(B48),"('",A48,"');"), IF(B48="Date", CONCATENATE("$table-&gt;",LOWER(B48),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;text('note3');</v>
+        <f>IF(B48="String", CONCATENATE("$table-&gt;",LOWER(B48),"('",A48,"', ",C48,")-&gt;nullable();"), IF(B48="Integer", CONCATENATE("$table-&gt;",LOWER(B48),"('",A48,"')-&gt;unsigned()-&gt;default(0);"), IF(B48="Text", CONCATENATE("$table-&gt;",LOWER(B48),"('",A48,"')-&gt;nullable();"), IF(B48="Date", CONCATENATE("$table-&gt;",LOWER(B48),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note3')-&gt;nullable();</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2797,8 +2957,8 @@
         <v>31</v>
       </c>
       <c r="D49" t="str">
-        <f>IF(B49="String", CONCATENATE("$table-&gt;",LOWER(B49),"('",A49,"', ",C49,");"), IF(B49="Integer", CONCATENATE("$table-&gt;",LOWER(B49),"('",A49,"')-&gt;unsigned()-&gt;default(0);"), IF(B49="Text", CONCATENATE("$table-&gt;",LOWER(B49),"('",A49,"');"), IF(B49="Date", CONCATENATE("$table-&gt;",LOWER(B49),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;text('note4');</v>
+        <f>IF(B49="String", CONCATENATE("$table-&gt;",LOWER(B49),"('",A49,"', ",C49,")-&gt;nullable();"), IF(B49="Integer", CONCATENATE("$table-&gt;",LOWER(B49),"('",A49,"')-&gt;unsigned()-&gt;default(0);"), IF(B49="Text", CONCATENATE("$table-&gt;",LOWER(B49),"('",A49,"')-&gt;nullable();"), IF(B49="Date", CONCATENATE("$table-&gt;",LOWER(B49),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note4')-&gt;nullable();</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2809,8 +2969,8 @@
         <v>31</v>
       </c>
       <c r="D50" t="str">
-        <f>IF(B50="String", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"', ",C50,");"), IF(B50="Integer", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"')-&gt;unsigned()-&gt;default(0);"), IF(B50="Text", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"');"), IF(B50="Date", CONCATENATE("$table-&gt;",LOWER(B50),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;text('note5');</v>
+        <f>IF(B50="String", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"', ",C50,")-&gt;nullable();"), IF(B50="Integer", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"')-&gt;unsigned()-&gt;default(0);"), IF(B50="Text", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"')-&gt;nullable();"), IF(B50="Date", CONCATENATE("$table-&gt;",LOWER(B50),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;text('note5')-&gt;nullable();</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2824,8 +2984,8 @@
         <v>1</v>
       </c>
       <c r="D51" t="str">
-        <f>IF(B51="String", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"', ",C51,");"), IF(B51="Integer", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"')-&gt;unsigned()-&gt;default(0);"), IF(B51="Text", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"');"), IF(B51="Date", CONCATENATE("$table-&gt;",LOWER(B51),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('sms_notify_news', 1);</v>
+        <f>IF(B51="String", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"', ",C51,")-&gt;nullable();"), IF(B51="Integer", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"')-&gt;unsigned()-&gt;default(0);"), IF(B51="Text", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"')-&gt;nullable();"), IF(B51="Date", CONCATENATE("$table-&gt;",LOWER(B51),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('sms_notify_news', 1)-&gt;nullable();</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2839,8 +2999,8 @@
         <v>30</v>
       </c>
       <c r="D52" t="str">
-        <f>IF(B52="String", CONCATENATE("$table-&gt;",LOWER(B52),"('",A52,"', ",C52,");"), IF(B52="Integer", CONCATENATE("$table-&gt;",LOWER(B52),"('",A52,"')-&gt;unsigned()-&gt;default(0);"), IF(B52="Text", CONCATENATE("$table-&gt;",LOWER(B52),"('",A52,"');"), IF(B52="Date", CONCATENATE("$table-&gt;",LOWER(B52),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('patient_status', 30);</v>
+        <f>IF(B52="String", CONCATENATE("$table-&gt;",LOWER(B52),"('",A52,"', ",C52,")-&gt;nullable();"), IF(B52="Integer", CONCATENATE("$table-&gt;",LOWER(B52),"('",A52,"')-&gt;unsigned()-&gt;default(0);"), IF(B52="Text", CONCATENATE("$table-&gt;",LOWER(B52),"('",A52,"')-&gt;nullable();"), IF(B52="Date", CONCATENATE("$table-&gt;",LOWER(B52),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('patient_status', 30)-&gt;nullable();</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2854,23 +3014,23 @@
         <v>1</v>
       </c>
       <c r="D53" t="str">
-        <f>IF(B53="String", CONCATENATE("$table-&gt;",LOWER(B53),"('",A53,"', ",C53,");"), IF(B53="Integer", CONCATENATE("$table-&gt;",LOWER(B53),"('",A53,"')-&gt;unsigned()-&gt;default(0);"), IF(B53="Text", CONCATENATE("$table-&gt;",LOWER(B53),"('",A53,"');"), IF(B53="Date", CONCATENATE("$table-&gt;",LOWER(B53),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('head_household', 1);</v>
+        <f>IF(B53="String", CONCATENATE("$table-&gt;",LOWER(B53),"('",A53,"', ",C53,")-&gt;nullable();"), IF(B53="Integer", CONCATENATE("$table-&gt;",LOWER(B53),"('",A53,"')-&gt;unsigned()-&gt;default(0);"), IF(B53="Text", CONCATENATE("$table-&gt;",LOWER(B53),"('",A53,"')-&gt;nullable();"), IF(B53="Date", CONCATENATE("$table-&gt;",LOWER(B53),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
+        <v>$table-&gt;string('head_household', 1)-&gt;nullable();</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="48" t="s">
+      <c r="A55" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="48"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
+      <c r="B55" s="47"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="48"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
+      <c r="A56" s="47"/>
+      <c r="B56" s="47"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -2897,8 +3057,8 @@
         <v>100</v>
       </c>
       <c r="D58" s="3" t="str">
-        <f t="shared" ref="D58:D61" si="0">IF(B58="String", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"', ",C58,");"), IF(B58="Integer", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"')-&gt;unsigned()-&gt;default(0);"), IF(B58="Text", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');"), IF(B58="Date", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');")) )))</f>
-        <v>$table-&gt;string('option', 100);</v>
+        <f t="shared" ref="D58:D61" si="0">IF(B58="String", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"', ",C58,")-&gt;nullable();"), IF(B58="Integer", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"')-&gt;unsigned()-&gt;default(0);"), IF(B58="Text", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');"), IF(B58="Date", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');")) )))</f>
+        <v>$table-&gt;string('option', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2913,7 +3073,7 @@
       </c>
       <c r="D59" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>$table-&gt;string('section', 100);</v>
+        <v>$table-&gt;string('section', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2928,7 +3088,7 @@
       </c>
       <c r="D60" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>$table-&gt;string('description', 100);</v>
+        <v>$table-&gt;string('description', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2943,22 +3103,22 @@
       </c>
       <c r="D61" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>$table-&gt;string('value', 100);</v>
+        <v>$table-&gt;string('value', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="48" t="s">
+      <c r="A63" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="48"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
+      <c r="B63" s="47"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="47"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="48"/>
-      <c r="B64" s="48"/>
-      <c r="C64" s="48"/>
-      <c r="D64" s="48"/>
+      <c r="A64" s="47"/>
+      <c r="B64" s="47"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
@@ -2985,8 +3145,8 @@
         <v>100</v>
       </c>
       <c r="D66" s="3" t="str">
-        <f t="shared" ref="D66:D68" si="1">IF(B66="String", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"', ",C66,");"), IF(B66="Integer", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"')-&gt;unsigned()-&gt;default(0);"), IF(B66="Text", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');"), IF(B66="Date", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');")) )))</f>
-        <v>$table-&gt;string('des_dom', 100);</v>
+        <f t="shared" ref="D66:D70" si="1">IF(B66="String", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"', ",C66,")-&gt;nullable();"), IF(B66="Integer", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"')-&gt;unsigned()-&gt;default(0);"), IF(B66="Text", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');"), IF(B66="Date", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');")) )))</f>
+        <v>$table-&gt;string('des_dom', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3016,7 +3176,7 @@
       </c>
       <c r="D68" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>$table-&gt;string('description', 100);</v>
+        <v>$table-&gt;string('description', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3030,8 +3190,8 @@
         <v>100</v>
       </c>
       <c r="D69" s="3" t="str">
-        <f>IF(B69="String", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"', ",C69,");"), IF(B69="Integer", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"')-&gt;unsigned()-&gt;default(0);"), IF(B69="Text", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"');"), IF(B69="Date", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"');")) )))</f>
-        <v>$table-&gt;string('value', 100);</v>
+        <f t="shared" si="1"/>
+        <v>$table-&gt;string('value', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3039,23 +3199,23 @@
       <c r="B70" s="17"/>
       <c r="C70" s="18"/>
       <c r="D70" s="19" t="b">
-        <f>IF(B70="String", CONCATENATE("$table-&gt;",LOWER(B70),"('",A70,"', ",C70,");"), IF(B70="Integer", CONCATENATE("$table-&gt;",LOWER(B70),"('",A70,"')-&gt;unsigned()-&gt;default(0);"), IF(B70="Text", CONCATENATE("$table-&gt;",LOWER(B70),"('",A70,"');"), IF(B70="Date", CONCATENATE("$table-&gt;",LOWER(B70),"('",A70,"');")) )))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="48" t="s">
+      <c r="A72" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="48"/>
-      <c r="C72" s="48"/>
-      <c r="D72" s="48"/>
+      <c r="B72" s="47"/>
+      <c r="C72" s="47"/>
+      <c r="D72" s="47"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="48"/>
-      <c r="B73" s="48"/>
-      <c r="C73" s="48"/>
-      <c r="D73" s="48"/>
+      <c r="A73" s="47"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="47"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
@@ -3082,8 +3242,8 @@
         <v>255</v>
       </c>
       <c r="D75" s="3" t="str">
-        <f t="shared" ref="D75:D76" si="2">IF(B75="String", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"', ",C75,");"), IF(B75="Integer", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"')-&gt;unsigned()-&gt;default(0);"), IF(B75="Text", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');"), IF(B75="Date", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');")) )))</f>
-        <v>$table-&gt;string('path', 255);</v>
+        <f t="shared" ref="D75:D76" si="2">IF(B75="String", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"', ",C75,")-&gt;nullable();"), IF(B75="Integer", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"')-&gt;unsigned()-&gt;default(0);"), IF(B75="Text", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');"), IF(B75="Date", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');")) )))</f>
+        <v>$table-&gt;string('path', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3094,18 +3254,18 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="48" t="s">
+      <c r="A80" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B80" s="48"/>
-      <c r="C80" s="48"/>
-      <c r="D80" s="48"/>
+      <c r="B80" s="47"/>
+      <c r="C80" s="47"/>
+      <c r="D80" s="47"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="48"/>
-      <c r="B81" s="48"/>
-      <c r="C81" s="48"/>
-      <c r="D81" s="48"/>
+      <c r="A81" s="47"/>
+      <c r="B81" s="47"/>
+      <c r="C81" s="47"/>
+      <c r="D81" s="47"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
@@ -3121,7 +3281,7 @@
         <v>4</v>
       </c>
       <c r="E82" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3135,10 +3295,10 @@
         <v>255</v>
       </c>
       <c r="D83" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E83" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3152,21 +3312,21 @@
         <v>250</v>
       </c>
       <c r="D84" s="28" t="str">
-        <f t="shared" ref="D84:D86" si="3">IF(B84="String", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"', ",C84,");"), IF(B84="Integer", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"')-&gt;unsigned()-&gt;default(0);"), IF(B84="Text", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"');"), IF(B84="Date", CONCATENATE("$table-&gt;","timestamp","('",A84,"');")) )))</f>
-        <v>$table-&gt;string('title', 250);</v>
+        <f>IF(B84="String", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"', ",C84,")-&gt;nullable();"), IF(B84="Integer", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"')-&gt;unsigned()-&gt;default(0);"), IF(B84="Text", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"');"), IF(B84="Date", CONCATENATE("$table-&gt;","timestamp","('",A84,"');")) )))</f>
+        <v>$table-&gt;string('title', 250)-&gt;nullable();</v>
       </c>
       <c r="E84" s="25"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" s="27" t="s">
         <v>31</v>
       </c>
       <c r="C85" s="30"/>
       <c r="D85" s="28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D85:D86" si="3">IF(B85="String", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"', ",C85,");"), IF(B85="Integer", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"')-&gt;unsigned()-&gt;default(0);"), IF(B85="Text", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"');"), IF(B85="Date", CONCATENATE("$table-&gt;","timestamp","('",A85,"');")) )))</f>
         <v>$table-&gt;text('content');</v>
       </c>
       <c r="E85" s="25"/>
@@ -3205,22 +3365,22 @@
       <c r="C88" s="35"/>
       <c r="D88" s="36"/>
       <c r="E88" s="37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="B90" s="48"/>
-      <c r="C90" s="48"/>
-      <c r="D90" s="48"/>
+      <c r="A90" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B90" s="47"/>
+      <c r="C90" s="47"/>
+      <c r="D90" s="47"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="48"/>
-      <c r="B91" s="48"/>
-      <c r="C91" s="48"/>
-      <c r="D91" s="48"/>
+      <c r="A91" s="47"/>
+      <c r="B91" s="47"/>
+      <c r="C91" s="47"/>
+      <c r="D91" s="47"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
@@ -3236,7 +3396,7 @@
         <v>4</v>
       </c>
       <c r="E92" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G92" s="11"/>
     </row>
@@ -3254,22 +3414,22 @@
         <v>73</v>
       </c>
       <c r="E93" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E94" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3297,8 +3457,8 @@
         <v>255</v>
       </c>
       <c r="D96" s="13" t="str">
-        <f>IF(B96="String", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"', ",C96,");"), IF(B96="Integer", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"')-&gt;unsigned()-&gt;default(0);"), IF(B96="Text", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"');"), IF(B96="Date", CONCATENATE("$table-&gt;","timestamp","('",A96,"');")) )))</f>
-        <v>$table-&gt;string('first_name', 255);</v>
+        <f>IF(B96="String", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"', ",C96,")-&gt;nullable();"), IF(B96="Integer", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"')-&gt;unsigned()-&gt;default(0);"), IF(B96="Text", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"');"), IF(B96="Date", CONCATENATE("$table-&gt;","timestamp","('",A96,"');")) )))</f>
+        <v>$table-&gt;string('first_name', 255)-&gt;nullable();</v>
       </c>
       <c r="E96" s="22"/>
       <c r="G96" s="12"/>
@@ -3314,8 +3474,8 @@
         <v>255</v>
       </c>
       <c r="D97" s="13" t="str">
-        <f>IF(B97="String", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"', ",C97,");"), IF(B97="Integer", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"')-&gt;unsigned()-&gt;default(0);"), IF(B97="Text", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"');"), IF(B97="Date", CONCATENATE("$table-&gt;","timestamp","('",A97,"');")) )))</f>
-        <v>$table-&gt;string('last_name', 255);</v>
+        <f t="shared" ref="D97:D101" si="4">IF(B97="String", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"', ",C97,")-&gt;nullable();"), IF(B97="Integer", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"')-&gt;unsigned()-&gt;default(0);"), IF(B97="Text", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"');"), IF(B97="Date", CONCATENATE("$table-&gt;","timestamp","('",A97,"');")) )))</f>
+        <v>$table-&gt;string('last_name', 255)-&gt;nullable();</v>
       </c>
       <c r="E97" s="22"/>
       <c r="G97" s="12"/>
@@ -3330,8 +3490,9 @@
       <c r="C98" s="8">
         <v>200</v>
       </c>
-      <c r="D98" s="13" t="s">
-        <v>75</v>
+      <c r="D98" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>$table-&gt;string('email', 200)-&gt;nullable();</v>
       </c>
       <c r="E98" s="22"/>
       <c r="G98" s="12"/>
@@ -3347,15 +3508,15 @@
         <v>255</v>
       </c>
       <c r="D99" s="13" t="str">
-        <f>IF(B99="String", CONCATENATE("$table-&gt;",LOWER(B99),"('",A99,"', ",C99,");"), IF(B99="Integer", CONCATENATE("$table-&gt;",LOWER(B99),"('",A99,"')-&gt;unsigned()-&gt;default(0);"), IF(B99="Text", CONCATENATE("$table-&gt;",LOWER(B99),"('",A99,"');"), IF(B99="Date", CONCATENATE("$table-&gt;","timestamp","('",A99,"');")) )))</f>
-        <v>$table-&gt;string('address', 255);</v>
+        <f t="shared" si="4"/>
+        <v>$table-&gt;string('address', 255)-&gt;nullable();</v>
       </c>
       <c r="E99" s="22"/>
       <c r="G99" s="12"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B100" s="16" t="s">
         <v>6</v>
@@ -3364,8 +3525,8 @@
         <v>50</v>
       </c>
       <c r="D100" s="13" t="str">
-        <f>IF(B100="String", CONCATENATE("$table-&gt;",LOWER(B100),"('",A100,"', ",C100,");"), IF(B100="Integer", CONCATENATE("$table-&gt;",LOWER(B100),"('",A100,"')-&gt;unsigned()-&gt;default(0);"), IF(B100="Text", CONCATENATE("$table-&gt;",LOWER(B100),"('",A100,"');"), IF(B100="Date", CONCATENATE("$table-&gt;","timestamp","('",A100,"');")) )))</f>
-        <v>$table-&gt;string('phone', 50);</v>
+        <f t="shared" si="4"/>
+        <v>$table-&gt;string('phone', 50)-&gt;nullable();</v>
       </c>
       <c r="E100" s="22"/>
       <c r="G100" s="12"/>
@@ -3381,8 +3542,8 @@
         <v>255</v>
       </c>
       <c r="D101" s="13" t="str">
-        <f>IF(B101="String", CONCATENATE("$table-&gt;",LOWER(B101),"('",A101,"', ",C101,");"), IF(B101="Integer", CONCATENATE("$table-&gt;",LOWER(B101),"('",A101,"')-&gt;unsigned()-&gt;default(0);"), IF(B101="Text", CONCATENATE("$table-&gt;",LOWER(B101),"('",A101,"');"), IF(B101="Date", CONCATENATE("$table-&gt;","timestamp","('",A101,"');")) )))</f>
-        <v>$table-&gt;string('password', 255);</v>
+        <f t="shared" si="4"/>
+        <v>$table-&gt;string('password', 255)-&gt;nullable();</v>
       </c>
       <c r="E101" s="22"/>
       <c r="G101" s="12"/>
@@ -3396,24 +3557,24 @@
       </c>
       <c r="C102" s="14"/>
       <c r="D102" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E102" s="22"/>
       <c r="G102" s="12"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="B105" s="48"/>
-      <c r="C105" s="48"/>
-      <c r="D105" s="48"/>
+      <c r="A105" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B105" s="47"/>
+      <c r="C105" s="47"/>
+      <c r="D105" s="47"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="48"/>
-      <c r="B106" s="48"/>
-      <c r="C106" s="48"/>
-      <c r="D106" s="48"/>
+      <c r="A106" s="47"/>
+      <c r="B106" s="47"/>
+      <c r="C106" s="47"/>
+      <c r="D106" s="47"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
@@ -3431,7 +3592,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>6</v>
@@ -3440,47 +3601,50 @@
         <v>255</v>
       </c>
       <c r="D108" s="13" t="str">
-        <f>IF(B108="String", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"', ",C108,");"), IF(B108="Integer", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"')-&gt;unsigned()-&gt;default(0);"), IF(B108="Text", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"');"), IF(B108="Date", CONCATENATE("$table-&gt;","timestamp","('",A108,"');")) )))</f>
-        <v>$table-&gt;string('status', 255);</v>
+        <f t="shared" ref="D108:D109" si="5">IF(B108="String", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"', ",C108,")-&gt;nullable();"), IF(B108="Integer", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"')-&gt;unsigned()-&gt;default(0);"), IF(B108="Text", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"');"), IF(B108="Date", CONCATENATE("$table-&gt;","timestamp","('",A108,"');")) )))</f>
+        <v>$table-&gt;string('status', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="14"/>
       <c r="B109" s="7"/>
       <c r="C109" s="14"/>
-      <c r="D109" s="15"/>
+      <c r="D109" s="15" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="B111" s="48"/>
-      <c r="C111" s="48"/>
-      <c r="D111" s="48"/>
+      <c r="A111" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="B111" s="47"/>
+      <c r="C111" s="47"/>
+      <c r="D111" s="47"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="48"/>
-      <c r="B112" s="48"/>
-      <c r="C112" s="48"/>
-      <c r="D112" s="48"/>
+      <c r="A112" s="47"/>
+      <c r="B112" s="47"/>
+      <c r="C112" s="47"/>
+      <c r="D112" s="47"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="39" t="s">
+      <c r="A113" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B113" s="39" t="s">
+      <c r="B113" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C113" s="39" t="s">
+      <c r="C113" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D113" s="39" t="s">
+      <c r="D113" s="38" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>6</v>
@@ -3489,8 +3653,8 @@
         <v>50</v>
       </c>
       <c r="D114" s="13" t="str">
-        <f>IF(B114="String", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"', ",C114,");"), IF(B114="Integer", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"')-&gt;unsigned()-&gt;default(0);"), IF(B114="Text", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"');"), IF(B114="Date", CONCATENATE("$table-&gt;","timestamp","('",A114,"');")) )))</f>
-        <v>$table-&gt;string('id_invoice', 50);</v>
+        <f>IF(B114="String", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"', ",C114,")-nullable();"), IF(B114="Integer", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"')-&gt;unsigned()-&gt;default(0);"), IF(B114="Text", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"');"), IF(B114="Date", CONCATENATE("$table-&gt;","timestamp","('",A114,"');")) )))</f>
+        <v>$table-&gt;string('id_invoice', 50)-nullable();</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3504,488 +3668,726 @@
         <v>50</v>
       </c>
       <c r="D115" s="13" t="str">
-        <f>IF(B115="String", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"', ",C115,");"), IF(B115="Integer", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"')-&gt;unsigned()-&gt;default(0);"), IF(B115="Text", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"');"), IF(B115="Date", CONCATENATE("$table-&gt;","timestamp","('",A115,"');")) )))</f>
+        <f t="shared" ref="D115:D120" si="6">IF(B115="String", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"', ",C115,");"), IF(B115="Integer", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"')-&gt;unsigned()-&gt;default(0);"), IF(B115="Text", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"');"), IF(B115="Date", CONCATENATE("$table-&gt;","timestamp","('",A115,"');")) )))</f>
         <v>$table-&gt;string('id_dentist', 50);</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="44" t="s">
+      <c r="A116" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B116" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C116" s="42"/>
+      <c r="D116" s="49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117" s="42">
+        <v>255</v>
+      </c>
+      <c r="D117" s="43" t="str">
+        <f t="shared" ref="D117" si="7">IF(B117="String", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"', ",C117,");"), IF(B117="Integer", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"')-&gt;unsigned()-&gt;default(0);"), IF(B117="Text", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"');"), IF(B117="Date", CONCATENATE("$table-&gt;","timestamp","('",A117,"');")) )))</f>
+        <v>$table-&gt;string('detail', 255);</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B118" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C118" s="42"/>
+      <c r="D118" s="43" t="str">
+        <f t="shared" si="6"/>
+        <v>$table-&gt;timestamp('date');</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="B119" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C119" s="42"/>
+      <c r="D119" s="41" t="str">
+        <f t="shared" si="6"/>
+        <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B120" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C120" s="42"/>
+      <c r="D120" s="43" t="str">
+        <f t="shared" si="6"/>
+        <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B121" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C121" s="42"/>
+      <c r="D121" s="43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B122" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C122" s="42"/>
+      <c r="D122" s="41" t="str">
+        <f t="shared" ref="D122" si="8">IF(B122="String", CONCATENATE("$table-&gt;",LOWER(B122),"('",A122,"', ",C122,");"), IF(B122="Integer", CONCATENATE("$table-&gt;",LOWER(B122),"('",A122,"')-&gt;unsigned()-&gt;default(0);"), IF(B122="Text", CONCATENATE("$table-&gt;",LOWER(B122),"('",A122,"');"), IF(B122="Date", CONCATENATE("$table-&gt;","timestamp","('",A122,"');")) )))</f>
+        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B123" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C123" s="42"/>
+      <c r="D123" s="43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B124" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C124" s="42"/>
+      <c r="D124" s="41" t="str">
+        <f t="shared" ref="D124:D126" si="9">IF(B124="String", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"', ",C124,");"), IF(B124="Integer", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"')-&gt;unsigned()-&gt;default(0);"), IF(B124="Text", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"');"), IF(B124="Date", CONCATENATE("$table-&gt;","timestamp","('",A124,"');")) )))</f>
+        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B125" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C125" s="42"/>
+      <c r="D125" s="43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B126" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C126" s="42"/>
+      <c r="D126" s="41" t="str">
+        <f t="shared" si="9"/>
+        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B127" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C127" s="42"/>
+      <c r="D127" s="43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B128" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C128" s="42"/>
+      <c r="D128" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B129" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129" s="42">
+        <v>255</v>
+      </c>
+      <c r="D129" s="43" t="str">
+        <f>IF(B129="String", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"', ",C129,");"), IF(B129="Integer", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"')-&gt;unsigned()-&gt;default(0);"), IF(B129="Text", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"');"), IF(B129="Date", CONCATENATE("$table-&gt;","timestamp","('",A129,"');")) )))</f>
+        <v>$table-&gt;string('position', 255);</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B130" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C130" s="42"/>
+      <c r="D130" s="43" t="str">
+        <f>IF(B130="String", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"', ",C130,");"), IF(B130="Integer", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"')-&gt;unsigned()-&gt;default(0);"), IF(B130="Text", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"');"), IF(B130="Date", CONCATENATE("$table-&gt;","timestamp","('",A130,"');")) )))</f>
+        <v>$table-&gt;integer('object')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="B131" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C131" s="42"/>
+      <c r="D131" s="43" t="str">
+        <f>IF(B131="String", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"', ",C131,");"), IF(B131="Integer", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"')-&gt;unsigned()-&gt;default(0);"), IF(B131="Text", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"');"), IF(B131="Date", CONCATENATE("$table-&gt;","timestamp","('",A131,"');")) )))</f>
+        <v>$table-&gt;integer('type_operation')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B132" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C132" s="42"/>
+      <c r="D132" s="43" t="str">
+        <f>IF(B132="String", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"', ",C132,");"), IF(B132="Integer", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"')-&gt;unsigned()-&gt;default(0);"), IF(B132="Text", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"');"), IF(B132="Date", CONCATENATE("$table-&gt;","timestamp","('",A132,"');")) )))</f>
+        <v>$table-&gt;text('note');</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="42"/>
+      <c r="B133" s="44"/>
+      <c r="C133" s="42"/>
+      <c r="D133" s="45"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="B116" s="42" t="s">
+      <c r="B134" s="47"/>
+      <c r="C134" s="47"/>
+      <c r="D134" s="47"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="47"/>
+      <c r="B135" s="47"/>
+      <c r="C135" s="47"/>
+      <c r="D135" s="47"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B136" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D136" s="38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C137" s="8">
+        <v>255</v>
+      </c>
+      <c r="D137" s="13" t="str">
+        <f>IF(B137="String", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"', ",C137,");"), IF(B137="Integer", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"')-&gt;unsigned()-&gt;default(0);"), IF(B137="Text", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"');"), IF(B137="Date", CONCATENATE("$table-&gt;","timestamp","('",A137,"');")) )))</f>
+        <v>$table-&gt;string('category', 255);</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B141" s="47"/>
+      <c r="C141" s="47"/>
+      <c r="D141" s="47"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="47"/>
+      <c r="B142" s="47"/>
+      <c r="C142" s="47"/>
+      <c r="D142" s="47"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B143" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C143" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D143" s="39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B144" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C116" s="44"/>
-      <c r="D116" s="45" t="str">
-        <f>IF(B116="String", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"', ",C116,");"), IF(B116="Integer", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"')-&gt;unsigned()-&gt;default(0);"), IF(B116="Text", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"');"), IF(B116="Date", CONCATENATE("$table-&gt;","timestamp","('",A116,"');")) )))</f>
+      <c r="C144" s="8"/>
+      <c r="D144" s="13" t="str">
+        <f t="shared" ref="D144:D149" si="10">IF(B144="String", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"', ",C144,");"), IF(B144="Integer", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"')-&gt;unsigned()-&gt;default(0);"), IF(B144="Text", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"');"), IF(B144="Date", CONCATENATE("$table-&gt;","timestamp","('",A144,"');")) )))</f>
+        <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B145" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C145" s="42"/>
+      <c r="D145" s="43" t="str">
+        <f t="shared" si="10"/>
         <v>$table-&gt;integer('id_category')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="44" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B146" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C146" s="42">
+        <v>50</v>
+      </c>
+      <c r="D146" s="43" t="str">
+        <f t="shared" si="10"/>
+        <v>$table-&gt;string('id_dentist', 50);</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B147" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C147" s="42"/>
+      <c r="D147" s="41" t="str">
+        <f t="shared" si="10"/>
+        <v>$table-&gt;timestamp('date');</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="B117" s="42" t="s">
+      <c r="B148" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C148" s="42"/>
+      <c r="D148" s="43" t="str">
+        <f t="shared" si="10"/>
+        <v>$table-&gt;integer('teeth_no')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B149" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C149" s="42"/>
+      <c r="D149" s="43" t="str">
+        <f t="shared" si="10"/>
+        <v>$table-&gt;text('description');</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="B150" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C150" s="42"/>
+      <c r="D150" s="41" t="str">
+        <f t="shared" ref="D150:D155" si="11">IF(B150="String", CONCATENATE("$table-&gt;",LOWER(B150),"('",A150,"', ",C150,");"), IF(B150="Integer", CONCATENATE("$table-&gt;",LOWER(B150),"('",A150,"')-&gt;unsigned()-&gt;default(0);"), IF(B150="Text", CONCATENATE("$table-&gt;",LOWER(B150),"('",A150,"');"), IF(B150="Date", CONCATENATE("$table-&gt;","timestamp","('",A150,"');")) )))</f>
+        <v>$table-&gt;integer('currency')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B151" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C151" s="42"/>
+      <c r="D151" s="43" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B152" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C152" s="42"/>
+      <c r="D152" s="41" t="str">
+        <f t="shared" si="11"/>
+        <v>$table-&gt;integer('quantity')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B153" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C153" s="42"/>
+      <c r="D153" s="43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B154" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C154" s="42"/>
+      <c r="D154" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B155" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C155" s="42"/>
+      <c r="D155" s="43" t="str">
+        <f t="shared" si="11"/>
+        <v>$table-&gt;text('clicnic_note');</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B156" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C156" s="42"/>
+      <c r="D156" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="42"/>
+      <c r="B157" s="40"/>
+      <c r="C157" s="42"/>
+      <c r="D157" s="43"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="42"/>
+      <c r="B158" s="40"/>
+      <c r="C158" s="42"/>
+      <c r="D158" s="43"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="42"/>
+      <c r="B159" s="40"/>
+      <c r="C159" s="42"/>
+      <c r="D159" s="43"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="42"/>
+      <c r="B160" s="40"/>
+      <c r="C160" s="42"/>
+      <c r="D160" s="43"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="B163" s="47"/>
+      <c r="C163" s="47"/>
+      <c r="D163" s="47"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="47"/>
+      <c r="B164" s="47"/>
+      <c r="C164" s="47"/>
+      <c r="D164" s="47"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B165" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C165" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D165" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B166" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C166" s="42"/>
+      <c r="D166" s="49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B167" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C167" s="14">
+        <v>255</v>
+      </c>
+      <c r="D167" s="48" t="str">
+        <f>IF(B167="String", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"', ",C167,")-&gt;nullable();"), IF(B167="Integer", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"')-&gt;unsigned()-&gt;default(0);"), IF(B167="Text", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"');"), IF(B167="Date", CONCATENATE("$table-&gt;","timestamp","('",A167,"');")) )))</f>
+        <v>$table-&gt;string('category', 255)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B168" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168" s="42">
+        <v>255</v>
+      </c>
+      <c r="D168" s="43" t="str">
+        <f t="shared" ref="D168" si="12">IF(B168="String", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"', ",C168,");"), IF(B168="Integer", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"')-&gt;unsigned()-&gt;default(0);"), IF(B168="Text", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"');"), IF(B168="Date", CONCATENATE("$table-&gt;","timestamp","('",A168,"');")) )))</f>
+        <v>$table-&gt;string('detail', 255);</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B169" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C117" s="44"/>
-      <c r="D117" s="45" t="str">
-        <f>IF(B117="String", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"', ",C117,");"), IF(B117="Integer", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"')-&gt;unsigned()-&gt;default(0);"), IF(B117="Text", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"');"), IF(B117="Date", CONCATENATE("$table-&gt;","timestamp","('",A117,"');")) )))</f>
+      <c r="C169" s="42"/>
+      <c r="D169" s="43" t="str">
+        <f t="shared" ref="D169:D170" si="13">IF(B169="String", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"', ",C169,");"), IF(B169="Integer", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"')-&gt;unsigned()-&gt;default(0);"), IF(B169="Text", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"');"), IF(B169="Date", CONCATENATE("$table-&gt;","timestamp","('",A169,"');")) )))</f>
         <v>$table-&gt;timestamp('date');</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B118" s="42" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B170" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C118" s="44"/>
-      <c r="D118" s="43" t="str">
-        <f>IF(B118="String", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"', ",C118,");"), IF(B118="Integer", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"')-&gt;unsigned()-&gt;default(0);"), IF(B118="Text", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"');"), IF(B118="Date", CONCATENATE("$table-&gt;","timestamp","('",A118,"');")) )))</f>
-        <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="44" t="s">
+      <c r="C170" s="42"/>
+      <c r="D170" s="43" t="str">
+        <f t="shared" si="13"/>
+        <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B171" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C171" s="42"/>
+      <c r="D171" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B172" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C172" s="42"/>
+      <c r="D172" s="41" t="str">
+        <f t="shared" ref="D172" si="14">IF(B172="String", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"', ",C172,");"), IF(B172="Integer", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"')-&gt;unsigned()-&gt;default(0);"), IF(B172="Text", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"');"), IF(B172="Date", CONCATENATE("$table-&gt;","timestamp","('",A172,"');")) )))</f>
+        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B173" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C173" s="42"/>
+      <c r="D173" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="B119" s="42" t="s">
+      <c r="B174" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C119" s="44"/>
-      <c r="D119" s="45" t="str">
-        <f>IF(B119="String", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"', ",C119,");"), IF(B119="Integer", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"')-&gt;unsigned()-&gt;default(0);"), IF(B119="Text", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"');"), IF(B119="Date", CONCATENATE("$table-&gt;","timestamp","('",A119,"');")) )))</f>
-        <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="B120" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="C120" s="44"/>
-      <c r="D120" s="45" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="B121" s="42" t="s">
+      <c r="C174" s="42"/>
+      <c r="D174" s="41" t="str">
+        <f t="shared" ref="D174" si="15">IF(B174="String", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"', ",C174,");"), IF(B174="Integer", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"')-&gt;unsigned()-&gt;default(0);"), IF(B174="Text", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"');"), IF(B174="Date", CONCATENATE("$table-&gt;","timestamp","('",A174,"');")) )))</f>
+        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B175" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C175" s="42"/>
+      <c r="D175" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B176" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C121" s="44"/>
-      <c r="D121" s="43" t="str">
-        <f t="shared" ref="D121" si="4">IF(B121="String", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"', ",C121,");"), IF(B121="Integer", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"')-&gt;unsigned()-&gt;default(0);"), IF(B121="Text", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"');"), IF(B121="Date", CONCATENATE("$table-&gt;","timestamp","('",A121,"');")) )))</f>
-        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="B122" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="C122" s="44"/>
-      <c r="D122" s="45" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="B123" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C123" s="44"/>
-      <c r="D123" s="43" t="str">
-        <f t="shared" ref="D123:D125" si="5">IF(B123="String", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"', ",C123,");"), IF(B123="Integer", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"')-&gt;unsigned()-&gt;default(0);"), IF(B123="Text", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"');"), IF(B123="Date", CONCATENATE("$table-&gt;","timestamp","('",A123,"');")) )))</f>
-        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="B124" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="C124" s="44"/>
-      <c r="D124" s="45" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="44" t="s">
+      <c r="C176" s="42"/>
+      <c r="D176" s="41" t="str">
+        <f t="shared" ref="D176" si="16">IF(B176="String", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"', ",C176,");"), IF(B176="Integer", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"')-&gt;unsigned()-&gt;default(0);"), IF(B176="Text", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"');"), IF(B176="Date", CONCATENATE("$table-&gt;","timestamp","('",A176,"');")) )))</f>
+        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="B125" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C125" s="44"/>
-      <c r="D125" s="43" t="str">
-        <f t="shared" si="5"/>
-        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="44" t="s">
+      <c r="B177" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C177" s="42"/>
+      <c r="D177" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="B126" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="C126" s="44"/>
-      <c r="D126" s="45" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="44" t="s">
+      <c r="B178" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="B127" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="C127" s="44"/>
-      <c r="D127" s="45" t="s">
+      <c r="C178" s="42"/>
+      <c r="D178" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="42" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="B128" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="C128" s="44">
+      <c r="B179" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179" s="42">
         <v>255</v>
       </c>
-      <c r="D128" s="45" t="str">
-        <f>IF(B128="String", CONCATENATE("$table-&gt;",LOWER(B128),"('",A128,"', ",C128,");"), IF(B128="Integer", CONCATENATE("$table-&gt;",LOWER(B128),"('",A128,"')-&gt;unsigned()-&gt;default(0);"), IF(B128="Text", CONCATENATE("$table-&gt;",LOWER(B128),"('",A128,"');"), IF(B128="Date", CONCATENATE("$table-&gt;","timestamp","('",A128,"');")) )))</f>
-        <v>$table-&gt;string('position', 255);</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="B129" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C129" s="44"/>
-      <c r="D129" s="45" t="str">
-        <f>IF(B129="String", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"', ",C129,");"), IF(B129="Integer", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"')-&gt;unsigned()-&gt;default(0);"), IF(B129="Text", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"');"), IF(B129="Date", CONCATENATE("$table-&gt;","timestamp","('",A129,"');")) )))</f>
-        <v>$table-&gt;integer('object')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="B130" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C130" s="44"/>
-      <c r="D130" s="45" t="str">
-        <f>IF(B130="String", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"', ",C130,");"), IF(B130="Integer", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"')-&gt;unsigned()-&gt;default(0);"), IF(B130="Text", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"');"), IF(B130="Date", CONCATENATE("$table-&gt;","timestamp","('",A130,"');")) )))</f>
-        <v>$table-&gt;integer('type_operation')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="44" t="s">
+      <c r="D179" s="43" t="str">
+        <f>IF(B179="String", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"', ",C179,")-&gt;nullable();"), IF(B179="Integer", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"')-&gt;unsigned()-&gt;default(0);"), IF(B179="Text", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"');"), IF(B179="Date", CONCATENATE("$table-&gt;","timestamp","('",A179,"');")) )))</f>
+        <v>$table-&gt;string('position', 255)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B131" s="42" t="s">
+      <c r="B180" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C131" s="44"/>
-      <c r="D131" s="45" t="str">
-        <f>IF(B131="String", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"', ",C131,");"), IF(B131="Integer", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"')-&gt;unsigned()-&gt;default(0);"), IF(B131="Text", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"');"), IF(B131="Date", CONCATENATE("$table-&gt;","timestamp","('",A131,"');")) )))</f>
-        <v>$table-&gt;text('note');</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="44"/>
-      <c r="B132" s="46"/>
-      <c r="C132" s="44"/>
-      <c r="D132" s="47"/>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="B133" s="48"/>
-      <c r="C133" s="48"/>
-      <c r="D133" s="48"/>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="48"/>
-      <c r="B134" s="48"/>
-      <c r="C134" s="48"/>
-      <c r="D134" s="48"/>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B135" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="C135" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="D135" s="39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B136" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C136" s="8">
-        <v>255</v>
-      </c>
-      <c r="D136" s="13" t="str">
-        <f>IF(B136="String", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"', ",C136,");"), IF(B136="Integer", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"')-&gt;unsigned()-&gt;default(0);"), IF(B136="Text", CONCATENATE("$table-&gt;",LOWER(B136),"('",A136,"');"), IF(B136="Date", CONCATENATE("$table-&gt;","timestamp","('",A136,"');")) )))</f>
-        <v>$table-&gt;string('category', 255);</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="B140" s="48"/>
-      <c r="C140" s="48"/>
-      <c r="D140" s="48"/>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="48"/>
-      <c r="B141" s="48"/>
-      <c r="C141" s="48"/>
-      <c r="D141" s="48"/>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B142" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="C142" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="D142" s="41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B143" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C143" s="8"/>
-      <c r="D143" s="13" t="str">
-        <f>IF(B143="String", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"', ",C143,");"), IF(B143="Integer", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"')-&gt;unsigned()-&gt;default(0);"), IF(B143="Text", CONCATENATE("$table-&gt;",LOWER(B143),"('",A143,"');"), IF(B143="Date", CONCATENATE("$table-&gt;","timestamp","('",A143,"');")) )))</f>
-        <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="B144" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C144" s="44"/>
-      <c r="D144" s="45" t="str">
-        <f>IF(B144="String", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"', ",C144,");"), IF(B144="Integer", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"')-&gt;unsigned()-&gt;default(0);"), IF(B144="Text", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"');"), IF(B144="Date", CONCATENATE("$table-&gt;","timestamp","('",A144,"');")) )))</f>
-        <v>$table-&gt;integer('id_category')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="B145" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="C145" s="44">
-        <v>50</v>
-      </c>
-      <c r="D145" s="45" t="str">
-        <f>IF(B145="String", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"', ",C145,");"), IF(B145="Integer", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"')-&gt;unsigned()-&gt;default(0);"), IF(B145="Text", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"');"), IF(B145="Date", CONCATENATE("$table-&gt;","timestamp","('",A145,"');")) )))</f>
-        <v>$table-&gt;string('id_dentist', 50);</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="B146" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C146" s="44"/>
-      <c r="D146" s="43" t="str">
-        <f>IF(B146="String", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"', ",C146,");"), IF(B146="Integer", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"')-&gt;unsigned()-&gt;default(0);"), IF(B146="Text", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"');"), IF(B146="Date", CONCATENATE("$table-&gt;","timestamp","('",A146,"');")) )))</f>
-        <v>$table-&gt;timestamp('date');</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="B147" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C147" s="44"/>
-      <c r="D147" s="45" t="str">
-        <f>IF(B147="String", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"', ",C147,");"), IF(B147="Integer", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"')-&gt;unsigned()-&gt;default(0);"), IF(B147="Text", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"');"), IF(B147="Date", CONCATENATE("$table-&gt;","timestamp","('",A147,"');")) )))</f>
-        <v>$table-&gt;integer('teeth_no')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="B148" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C148" s="44"/>
-      <c r="D148" s="45" t="str">
-        <f>IF(B148="String", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"', ",C148,");"), IF(B148="Integer", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"')-&gt;unsigned()-&gt;default(0);"), IF(B148="Text", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"');"), IF(B148="Date", CONCATENATE("$table-&gt;","timestamp","('",A148,"');")) )))</f>
-        <v>$table-&gt;text('description');</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="B149" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C149" s="44"/>
-      <c r="D149" s="43" t="str">
-        <f t="shared" ref="D149:D154" si="6">IF(B149="String", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"', ",C149,");"), IF(B149="Integer", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"')-&gt;unsigned()-&gt;default(0);"), IF(B149="Text", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"');"), IF(B149="Date", CONCATENATE("$table-&gt;","timestamp","('",A149,"');")) )))</f>
-        <v>$table-&gt;integer('currency')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="B150" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="C150" s="44"/>
-      <c r="D150" s="45" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="B151" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C151" s="44"/>
-      <c r="D151" s="43" t="str">
-        <f t="shared" si="6"/>
-        <v>$table-&gt;integer('quantity')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="B152" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="C152" s="44"/>
-      <c r="D152" s="45" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="B153" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="C153" s="44"/>
-      <c r="D153" s="45" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B154" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C154" s="44"/>
-      <c r="D154" s="45" t="str">
-        <f t="shared" si="6"/>
-        <v>$table-&gt;text('clicnic_note');</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B155" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C155" s="44"/>
-      <c r="D155" s="45" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="44"/>
-      <c r="B156" s="42"/>
-      <c r="C156" s="44"/>
-      <c r="D156" s="45"/>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="44"/>
-      <c r="B157" s="42"/>
-      <c r="C157" s="44"/>
-      <c r="D157" s="45"/>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="44"/>
-      <c r="B158" s="42"/>
-      <c r="C158" s="44"/>
-      <c r="D158" s="45"/>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="44"/>
-      <c r="B159" s="42"/>
-      <c r="C159" s="44"/>
-      <c r="D159" s="45"/>
+      <c r="C180" s="42"/>
+      <c r="D180" s="43" t="str">
+        <f>IF(B180="String", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"', ",C180,");"), IF(B180="Integer", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"')-&gt;unsigned()-&gt;default(0);"), IF(B180="Text", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"')-&gt;nullable();"), IF(B180="Date", CONCATENATE("$table-&gt;","timestamp","('",A180,"');")) )))</f>
+        <v>$table-&gt;text('note')-&gt;nullable();</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A140:D141"/>
+  <mergeCells count="11">
+    <mergeCell ref="A163:D164"/>
+    <mergeCell ref="A141:D142"/>
     <mergeCell ref="A111:D112"/>
-    <mergeCell ref="A133:D134"/>
+    <mergeCell ref="A134:D135"/>
     <mergeCell ref="A105:D106"/>
     <mergeCell ref="A90:D91"/>
     <mergeCell ref="A1:F2"/>
@@ -3996,7 +4398,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <tableParts count="10">
+  <tableParts count="11">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -4007,6 +4409,7 @@
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#5 Minor fixes (added new field at Cure Modal ) :squirrel:
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -713,14 +713,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2280,8 +2280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="D178" sqref="D178"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,22 +2294,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3019,18 +3019,18 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="47" t="s">
+      <c r="A55" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="47"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="49"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="47"/>
-      <c r="B56" s="47"/>
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
+      <c r="A56" s="49"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -3107,18 +3107,18 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="47" t="s">
+      <c r="A63" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="47"/>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="47"/>
-      <c r="B64" s="47"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
+      <c r="A64" s="49"/>
+      <c r="B64" s="49"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="49"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
@@ -3184,14 +3184,11 @@
         <v>58</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C69">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="D69" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>$table-&gt;string('value', 100)-&gt;nullable();</v>
+        <v>$table-&gt;text('value');</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3204,18 +3201,18 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="47" t="s">
+      <c r="A72" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="47"/>
-      <c r="C72" s="47"/>
-      <c r="D72" s="47"/>
+      <c r="B72" s="49"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="49"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="47"/>
-      <c r="B73" s="47"/>
-      <c r="C73" s="47"/>
-      <c r="D73" s="47"/>
+      <c r="A73" s="49"/>
+      <c r="B73" s="49"/>
+      <c r="C73" s="49"/>
+      <c r="D73" s="49"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
@@ -3254,18 +3251,18 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="47" t="s">
+      <c r="A80" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="B80" s="47"/>
-      <c r="C80" s="47"/>
-      <c r="D80" s="47"/>
+      <c r="B80" s="49"/>
+      <c r="C80" s="49"/>
+      <c r="D80" s="49"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="47"/>
-      <c r="B81" s="47"/>
-      <c r="C81" s="47"/>
-      <c r="D81" s="47"/>
+      <c r="A81" s="49"/>
+      <c r="B81" s="49"/>
+      <c r="C81" s="49"/>
+      <c r="D81" s="49"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
@@ -3369,18 +3366,18 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="47" t="s">
+      <c r="A90" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B90" s="47"/>
-      <c r="C90" s="47"/>
-      <c r="D90" s="47"/>
+      <c r="B90" s="49"/>
+      <c r="C90" s="49"/>
+      <c r="D90" s="49"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="47"/>
-      <c r="B91" s="47"/>
-      <c r="C91" s="47"/>
-      <c r="D91" s="47"/>
+      <c r="A91" s="49"/>
+      <c r="B91" s="49"/>
+      <c r="C91" s="49"/>
+      <c r="D91" s="49"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
@@ -3563,18 +3560,18 @@
       <c r="G102" s="12"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="47" t="s">
+      <c r="A105" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="B105" s="47"/>
-      <c r="C105" s="47"/>
-      <c r="D105" s="47"/>
+      <c r="B105" s="49"/>
+      <c r="C105" s="49"/>
+      <c r="D105" s="49"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="47"/>
-      <c r="B106" s="47"/>
-      <c r="C106" s="47"/>
-      <c r="D106" s="47"/>
+      <c r="A106" s="49"/>
+      <c r="B106" s="49"/>
+      <c r="C106" s="49"/>
+      <c r="D106" s="49"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
@@ -3615,18 +3612,18 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="47" t="s">
+      <c r="A111" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="B111" s="47"/>
-      <c r="C111" s="47"/>
-      <c r="D111" s="47"/>
+      <c r="B111" s="49"/>
+      <c r="C111" s="49"/>
+      <c r="D111" s="49"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="47"/>
-      <c r="B112" s="47"/>
-      <c r="C112" s="47"/>
-      <c r="D112" s="47"/>
+      <c r="A112" s="49"/>
+      <c r="B112" s="49"/>
+      <c r="C112" s="49"/>
+      <c r="D112" s="49"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="38" t="s">
@@ -3680,7 +3677,7 @@
         <v>25</v>
       </c>
       <c r="C116" s="42"/>
-      <c r="D116" s="49" t="s">
+      <c r="D116" s="48" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3898,18 +3895,18 @@
       <c r="D133" s="45"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="47" t="s">
+      <c r="A134" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="B134" s="47"/>
-      <c r="C134" s="47"/>
-      <c r="D134" s="47"/>
+      <c r="B134" s="49"/>
+      <c r="C134" s="49"/>
+      <c r="D134" s="49"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="47"/>
-      <c r="B135" s="47"/>
-      <c r="C135" s="47"/>
-      <c r="D135" s="47"/>
+      <c r="A135" s="49"/>
+      <c r="B135" s="49"/>
+      <c r="C135" s="49"/>
+      <c r="D135" s="49"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="38" t="s">
@@ -3941,18 +3938,18 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="47" t="s">
+      <c r="A141" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="B141" s="47"/>
-      <c r="C141" s="47"/>
-      <c r="D141" s="47"/>
+      <c r="B141" s="49"/>
+      <c r="C141" s="49"/>
+      <c r="D141" s="49"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="47"/>
-      <c r="B142" s="47"/>
-      <c r="C142" s="47"/>
-      <c r="D142" s="47"/>
+      <c r="A142" s="49"/>
+      <c r="B142" s="49"/>
+      <c r="C142" s="49"/>
+      <c r="D142" s="49"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="39" t="s">
@@ -4160,18 +4157,18 @@
       <c r="D160" s="43"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="47" t="s">
+      <c r="A163" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="B163" s="47"/>
-      <c r="C163" s="47"/>
-      <c r="D163" s="47"/>
+      <c r="B163" s="49"/>
+      <c r="C163" s="49"/>
+      <c r="D163" s="49"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="47"/>
-      <c r="B164" s="47"/>
-      <c r="C164" s="47"/>
-      <c r="D164" s="47"/>
+      <c r="A164" s="49"/>
+      <c r="B164" s="49"/>
+      <c r="C164" s="49"/>
+      <c r="D164" s="49"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="46" t="s">
@@ -4195,7 +4192,7 @@
         <v>25</v>
       </c>
       <c r="C166" s="42"/>
-      <c r="D166" s="49" t="s">
+      <c r="D166" s="48" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4209,7 +4206,7 @@
       <c r="C167" s="14">
         <v>255</v>
       </c>
-      <c r="D167" s="48" t="str">
+      <c r="D167" s="47" t="str">
         <f>IF(B167="String", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"', ",C167,")-&gt;nullable();"), IF(B167="Integer", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"')-&gt;unsigned()-&gt;default(0);"), IF(B167="Text", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"');"), IF(B167="Date", CONCATENATE("$table-&gt;","timestamp","('",A167,"');")) )))</f>
         <v>$table-&gt;string('category', 255)-&gt;nullable();</v>
       </c>
@@ -4384,17 +4381,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A163:D164"/>
-    <mergeCell ref="A141:D142"/>
-    <mergeCell ref="A111:D112"/>
-    <mergeCell ref="A134:D135"/>
-    <mergeCell ref="A105:D106"/>
     <mergeCell ref="A90:D91"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A55:D56"/>
     <mergeCell ref="A63:D64"/>
     <mergeCell ref="A72:D73"/>
     <mergeCell ref="A80:D81"/>
+    <mergeCell ref="A163:D164"/>
+    <mergeCell ref="A141:D142"/>
+    <mergeCell ref="A111:D112"/>
+    <mergeCell ref="A134:D135"/>
+    <mergeCell ref="A105:D106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
#5 Minor fixes ( ... ) :star:
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="133">
   <si>
     <t>PATIENT</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>$table-&gt;decimal('price4', 10, 2)-&gt;nullable();</t>
+  </si>
+  <si>
+    <t>shortDesc</t>
   </si>
 </sst>
 </file>
@@ -597,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -722,6 +725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1842,14 +1846,14 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table254687911" displayName="Table254687911" ref="A143:D160" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A143:D160"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table254687911" displayName="Table254687911" ref="A144:D161" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A144:D161"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="9"/>
     <tableColumn id="2" name="Type" dataDxfId="8"/>
     <tableColumn id="3" name="Length" dataDxfId="7"/>
     <tableColumn id="4" name="Code generated" dataDxfId="6">
-      <calculatedColumnFormula>IF(B144="String", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"', ",C144,");"), IF(B144="Integer", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"')-&gt;unsigned()-&gt;default(0);"), IF(B144="Text", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"');"), IF(B144="Date", CONCATENATE("$table-&gt;","timestamp","('",A144,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B145="String", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"', ",C145,");"), IF(B145="Integer", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"')-&gt;unsigned()-&gt;default(0);"), IF(B145="Text", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"');"), IF(B145="Date", CONCATENATE("$table-&gt;","timestamp","('",A145,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1857,14 +1861,14 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table254687912" displayName="Table254687912" ref="A165:D180" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A165:D180"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table254687912" displayName="Table254687912" ref="A166:D181" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A166:D181"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="3"/>
     <tableColumn id="2" name="Type" dataDxfId="2"/>
     <tableColumn id="3" name="Length" dataDxfId="1"/>
     <tableColumn id="4" name="Code generated" dataDxfId="0">
-      <calculatedColumnFormula>IF(B166="String", CONCATENATE("$table-&gt;",LOWER(B166),"('",A166,"', ",C166,");"), IF(B166="Integer", CONCATENATE("$table-&gt;",LOWER(B166),"('",A166,"')-&gt;unsigned()-&gt;default(0);"), IF(B166="Text", CONCATENATE("$table-&gt;",LOWER(B166),"('",A166,"');"), IF(B166="Date", CONCATENATE("$table-&gt;","timestamp","('",A166,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B167="String", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"', ",C167,");"), IF(B167="Integer", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"')-&gt;unsigned()-&gt;default(0);"), IF(B167="Text", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"');"), IF(B167="Date", CONCATENATE("$table-&gt;","timestamp","('",A167,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1887,8 +1891,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A65:D70" totalsRowShown="0" headerRowDxfId="49">
-  <autoFilter ref="A65:D70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A65:D71" totalsRowShown="0" headerRowDxfId="49">
+  <autoFilter ref="A65:D71"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type" dataDxfId="48"/>
@@ -1902,14 +1906,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A74:D76" totalsRowShown="0" headerRowDxfId="46">
-  <autoFilter ref="A74:D76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A75:D77" totalsRowShown="0" headerRowDxfId="46">
+  <autoFilter ref="A75:D77"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type" dataDxfId="45"/>
     <tableColumn id="3" name="Length"/>
     <tableColumn id="4" name="Code generated" dataDxfId="44">
-      <calculatedColumnFormula>IF(B75="String", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"', ",C75,")-&gt;nullable();"), IF(B75="Integer", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"')-&gt;unsigned()-&gt;default(0);"), IF(B75="Text", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');"), IF(B75="Date", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B76="String", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"', ",C76,")-&gt;nullable();"), IF(B76="Integer", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"')-&gt;unsigned()-&gt;default(0);"), IF(B76="Text", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"');"), IF(B76="Date", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1917,14 +1921,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A82:E88" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A82:E88"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A83:E89" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A83:E89"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Column name" dataDxfId="41"/>
     <tableColumn id="2" name="Type" dataDxfId="40"/>
     <tableColumn id="3" name="Length" dataDxfId="39"/>
     <tableColumn id="4" name="Code generated" dataDxfId="38">
-      <calculatedColumnFormula>IF(B83="String", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"', ",C83,");"), IF(B83="Integer", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"')-&gt;unsigned()-&gt;default(0);"), IF(B83="Text", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"');"), IF(B83="Date", CONCATENATE("$table-&gt;","timestamp","('",A83,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B84="String", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"', ",C84,");"), IF(B84="Integer", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"')-&gt;unsigned()-&gt;default(0);"), IF(B84="Text", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"');"), IF(B84="Date", CONCATENATE("$table-&gt;","timestamp","('",A84,"');")) )))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Type Column" dataDxfId="37"/>
   </tableColumns>
@@ -1933,8 +1937,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A92:E102" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A92:E102"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A93:E103" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A93:E103"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Column name" dataDxfId="34"/>
     <tableColumn id="2" name="Type" dataDxfId="33"/>
@@ -1947,14 +1951,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A107:D109" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A107:D109"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A108:D110" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A108:D110"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="27"/>
     <tableColumn id="2" name="Type" dataDxfId="26"/>
     <tableColumn id="3" name="Length" dataDxfId="25"/>
     <tableColumn id="4" name="Code generated" dataDxfId="24">
-      <calculatedColumnFormula>IF(B108="String", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"', ",C108,")-&gt;nullable();"), IF(B108="Integer", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"')-&gt;unsigned()-&gt;default(0);"), IF(B108="Text", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"');"), IF(B108="Date", CONCATENATE("$table-&gt;","timestamp","('",A108,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B109="String", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"', ",C109,")-&gt;nullable();"), IF(B109="Integer", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"')-&gt;unsigned()-&gt;default(0);"), IF(B109="Text", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"');"), IF(B109="Date", CONCATENATE("$table-&gt;","timestamp","('",A109,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1962,14 +1966,14 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table2546879" displayName="Table2546879" ref="A113:D132" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A113:D132"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table2546879" displayName="Table2546879" ref="A114:D133" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A114:D133"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="21"/>
     <tableColumn id="2" name="Type" dataDxfId="20"/>
     <tableColumn id="3" name="Length" dataDxfId="19"/>
     <tableColumn id="4" name="Code generated" dataDxfId="18">
-      <calculatedColumnFormula>IF(B114="String", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"', ",C114,");"), IF(B114="Integer", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"')-&gt;unsigned()-&gt;default(0);"), IF(B114="Text", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"');"), IF(B114="Date", CONCATENATE("$table-&gt;","timestamp","('",A114,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B115="String", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"', ",C115,");"), IF(B115="Integer", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"')-&gt;unsigned()-&gt;default(0);"), IF(B115="Text", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"');"), IF(B115="Date", CONCATENATE("$table-&gt;","timestamp","('",A115,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1977,14 +1981,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table254687910" displayName="Table254687910" ref="A136:D138" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A136:D138"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table254687910" displayName="Table254687910" ref="A137:D139" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A137:D139"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="15"/>
     <tableColumn id="2" name="Type" dataDxfId="14"/>
     <tableColumn id="3" name="Length" dataDxfId="13"/>
     <tableColumn id="4" name="Code generated" dataDxfId="12">
-      <calculatedColumnFormula>IF(B137="String", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"', ",C137,");"), IF(B137="Integer", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"')-&gt;unsigned()-&gt;default(0);"), IF(B137="Text", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"');"), IF(B137="Date", CONCATENATE("$table-&gt;","timestamp","('",A137,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B138="String", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"', ",C138,");"), IF(B138="Integer", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"')-&gt;unsigned()-&gt;default(0);"), IF(B138="Text", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"');"), IF(B138="Date", CONCATENATE("$table-&gt;","timestamp","('",A138,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2278,10 +2282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G180"/>
+  <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3145,7 +3149,7 @@
         <v>100</v>
       </c>
       <c r="D66" s="3" t="str">
-        <f t="shared" ref="D66:D70" si="1">IF(B66="String", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"', ",C66,")-&gt;nullable();"), IF(B66="Integer", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"')-&gt;unsigned()-&gt;default(0);"), IF(B66="Text", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');"), IF(B66="Date", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');")) )))</f>
+        <f t="shared" ref="D66:D71" si="1">IF(B66="String", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"', ",C66,")-&gt;nullable();"), IF(B66="Integer", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"')-&gt;unsigned()-&gt;default(0);"), IF(B66="Text", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');"), IF(B66="Date", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');")) )))</f>
         <v>$table-&gt;string('des_dom', 100)-&gt;nullable();</v>
       </c>
     </row>
@@ -3181,249 +3185,249 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69">
+        <v>100</v>
+      </c>
+      <c r="D69" s="50" t="str">
+        <f>IF(B69="String", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"', ",C69,")-&gt;nullable();"), IF(B69="Integer", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"')-&gt;unsigned()-&gt;default(0);"), IF(B69="Text", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"');"), IF(B69="Date", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"');")) )))</f>
+        <v>$table-&gt;string('shortDesc', 100)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>58</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D69" s="3" t="str">
+      <c r="D70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>$table-&gt;text('value');</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="18"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="19" t="b">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="18"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="19" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="49" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="49"/>
-      <c r="C72" s="49"/>
-      <c r="D72" s="49"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="49"/>
       <c r="B73" s="49"/>
       <c r="C73" s="49"/>
       <c r="D73" s="49"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="49"/>
+      <c r="B74" s="49"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="49"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C75" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D75" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>63</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C75">
+      <c r="B76" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76">
         <v>255</v>
       </c>
-      <c r="D75" s="3" t="str">
-        <f t="shared" ref="D75:D76" si="2">IF(B75="String", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"', ",C75,")-&gt;nullable();"), IF(B75="Integer", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"')-&gt;unsigned()-&gt;default(0);"), IF(B75="Text", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');"), IF(B75="Date", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');")) )))</f>
+      <c r="D76" s="3" t="str">
+        <f t="shared" ref="D76:D77" si="2">IF(B76="String", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"', ",C76,")-&gt;nullable();"), IF(B76="Integer", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"')-&gt;unsigned()-&gt;default(0);"), IF(B76="Text", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"');"), IF(B76="Date", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"');")) )))</f>
         <v>$table-&gt;string('path', 255)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="2"/>
-      <c r="D76" s="3" t="b">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="2"/>
+      <c r="D77" s="3" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="49" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="B80" s="49"/>
-      <c r="C80" s="49"/>
-      <c r="D80" s="49"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="49"/>
       <c r="B81" s="49"/>
       <c r="C81" s="49"/>
       <c r="D81" s="49"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="49"/>
+      <c r="B82" s="49"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="49"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B83" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C83" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D83" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E82" s="21" t="s">
+      <c r="E83" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="25" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B83" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C83" s="29">
+      <c r="B84" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" s="29">
         <v>255</v>
       </c>
-      <c r="D83" s="32" t="s">
+      <c r="D84" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="E83" s="25" t="s">
+      <c r="E84" s="25" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B84" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" s="30">
-        <v>250</v>
-      </c>
-      <c r="D84" s="28" t="str">
-        <f>IF(B84="String", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"', ",C84,")-&gt;nullable();"), IF(B84="Integer", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"')-&gt;unsigned()-&gt;default(0);"), IF(B84="Text", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"');"), IF(B84="Date", CONCATENATE("$table-&gt;","timestamp","('",A84,"');")) )))</f>
-        <v>$table-&gt;string('title', 250)-&gt;nullable();</v>
-      </c>
-      <c r="E84" s="25"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C85" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="C85" s="30">
+        <v>250</v>
+      </c>
       <c r="D85" s="28" t="str">
-        <f t="shared" ref="D85:D86" si="3">IF(B85="String", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"', ",C85,");"), IF(B85="Integer", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"')-&gt;unsigned()-&gt;default(0);"), IF(B85="Text", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"');"), IF(B85="Date", CONCATENATE("$table-&gt;","timestamp","('",A85,"');")) )))</f>
-        <v>$table-&gt;text('content');</v>
+        <f>IF(B85="String", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"', ",C85,")-&gt;nullable();"), IF(B85="Integer", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"')-&gt;unsigned()-&gt;default(0);"), IF(B85="Text", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"');"), IF(B85="Date", CONCATENATE("$table-&gt;","timestamp","('",A85,"');")) )))</f>
+        <v>$table-&gt;string('title', 250)-&gt;nullable();</v>
       </c>
       <c r="E85" s="25"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B86" s="24" t="s">
-        <v>15</v>
+        <v>82</v>
+      </c>
+      <c r="B86" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="C86" s="30"/>
       <c r="D86" s="28" t="str">
+        <f t="shared" ref="D86:D87" si="3">IF(B86="String", CONCATENATE("$table-&gt;",LOWER(B86),"('",A86,"', ",C86,");"), IF(B86="Integer", CONCATENATE("$table-&gt;",LOWER(B86),"('",A86,"')-&gt;unsigned()-&gt;default(0);"), IF(B86="Text", CONCATENATE("$table-&gt;",LOWER(B86),"('",A86,"');"), IF(B86="Date", CONCATENATE("$table-&gt;","timestamp","('",A86,"');")) )))</f>
+        <v>$table-&gt;text('content');</v>
+      </c>
+      <c r="E86" s="25"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B87" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="30"/>
+      <c r="D87" s="28" t="str">
         <f t="shared" si="3"/>
         <v>$table-&gt;timestamp('start_time');</v>
       </c>
-      <c r="E86" s="25"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="24" t="s">
+      <c r="E87" s="25"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="B87" s="24" t="s">
+      <c r="B88" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C87" s="30"/>
-      <c r="D87" s="31" t="str">
-        <f>IF(B87="String", CONCATENATE("$table-&gt;",LOWER(B87),"('",A87,"', ",C87,");"), IF(B87="Integer", CONCATENATE("$table-&gt;",LOWER(B87),"('",A87,"')-&gt;unsigned()-&gt;default(0);"), IF(B87="Text", CONCATENATE("$table-&gt;",LOWER(B87),"('",A87,"');"), IF(B87="Date", CONCATENATE("$table-&gt;","timestamp","('",A87,"');")) )))</f>
+      <c r="C88" s="30"/>
+      <c r="D88" s="31" t="str">
+        <f>IF(B88="String", CONCATENATE("$table-&gt;",LOWER(B88),"('",A88,"', ",C88,");"), IF(B88="Integer", CONCATENATE("$table-&gt;",LOWER(B88),"('",A88,"')-&gt;unsigned()-&gt;default(0);"), IF(B88="Text", CONCATENATE("$table-&gt;",LOWER(B88),"('",A88,"');"), IF(B88="Date", CONCATENATE("$table-&gt;","timestamp","('",A88,"');")) )))</f>
         <v>$table-&gt;timestamp('end_time');</v>
       </c>
-      <c r="E87" s="25"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
-      <c r="B88" s="33"/>
-      <c r="C88" s="35"/>
-      <c r="D88" s="36"/>
-      <c r="E88" s="37" t="s">
+      <c r="E88" s="25"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="34"/>
+      <c r="B89" s="33"/>
+      <c r="C89" s="35"/>
+      <c r="D89" s="36"/>
+      <c r="E89" s="37" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="49" t="s">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B90" s="49"/>
-      <c r="C90" s="49"/>
-      <c r="D90" s="49"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="49"/>
       <c r="B91" s="49"/>
       <c r="C91" s="49"/>
       <c r="D91" s="49"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+      <c r="A92" s="49"/>
+      <c r="B92" s="49"/>
+      <c r="C92" s="49"/>
+      <c r="D92" s="49"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B93" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C93" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D92" s="6" t="s">
+      <c r="D93" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E92" s="21" t="s">
+      <c r="E93" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="G92" s="11"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C93" s="8">
-        <v>250</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E93" s="25" t="s">
-        <v>83</v>
-      </c>
+      <c r="G93" s="11"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C94" s="8"/>
-      <c r="D94" s="9" t="s">
-        <v>80</v>
+      <c r="C94" s="8">
+        <v>250</v>
+      </c>
+      <c r="D94" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="E94" s="25" t="s">
         <v>83</v>
@@ -3431,440 +3435,442 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C95" s="8"/>
-      <c r="D95" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E95" s="22"/>
-      <c r="G95" s="12"/>
+      <c r="D95" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E95" s="25" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C96" s="9">
-        <v>255</v>
-      </c>
-      <c r="D96" s="13" t="str">
-        <f>IF(B96="String", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"', ",C96,")-&gt;nullable();"), IF(B96="Integer", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"')-&gt;unsigned()-&gt;default(0);"), IF(B96="Text", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"');"), IF(B96="Date", CONCATENATE("$table-&gt;","timestamp","('",A96,"');")) )))</f>
-        <v>$table-&gt;string('first_name', 255)-&gt;nullable();</v>
+        <v>72</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C96" s="8"/>
+      <c r="D96" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="E96" s="22"/>
       <c r="G96" s="12"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B97" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B97" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C97" s="9">
         <v>255</v>
       </c>
       <c r="D97" s="13" t="str">
-        <f t="shared" ref="D97:D101" si="4">IF(B97="String", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"', ",C97,")-&gt;nullable();"), IF(B97="Integer", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"')-&gt;unsigned()-&gt;default(0);"), IF(B97="Text", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"');"), IF(B97="Date", CONCATENATE("$table-&gt;","timestamp","('",A97,"');")) )))</f>
-        <v>$table-&gt;string('last_name', 255)-&gt;nullable();</v>
+        <f>IF(B97="String", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"', ",C97,")-&gt;nullable();"), IF(B97="Integer", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"')-&gt;unsigned()-&gt;default(0);"), IF(B97="Text", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"');"), IF(B97="Date", CONCATENATE("$table-&gt;","timestamp","('",A97,"');")) )))</f>
+        <v>$table-&gt;string('first_name', 255)-&gt;nullable();</v>
       </c>
       <c r="E97" s="22"/>
       <c r="G97" s="12"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
+      <c r="A98" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98" s="9">
+        <v>255</v>
+      </c>
+      <c r="D98" s="13" t="str">
+        <f t="shared" ref="D98:D102" si="4">IF(B98="String", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"', ",C98,")-&gt;nullable();"), IF(B98="Integer", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"')-&gt;unsigned()-&gt;default(0);"), IF(B98="Text", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"');"), IF(B98="Date", CONCATENATE("$table-&gt;","timestamp","('",A98,"');")) )))</f>
+        <v>$table-&gt;string('last_name', 255)-&gt;nullable();</v>
+      </c>
+      <c r="E98" s="22"/>
+      <c r="G98" s="12"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B98" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C98" s="8">
+      <c r="B99" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="8">
         <v>200</v>
       </c>
-      <c r="D98" s="13" t="str">
+      <c r="D99" s="13" t="str">
         <f t="shared" si="4"/>
         <v>$table-&gt;string('email', 200)-&gt;nullable();</v>
       </c>
-      <c r="E98" s="22"/>
-      <c r="G98" s="12"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="22" t="s">
+      <c r="E99" s="22"/>
+      <c r="G99" s="12"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B99" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C99" s="22">
+      <c r="B100" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" s="22">
         <v>255</v>
       </c>
-      <c r="D99" s="13" t="str">
+      <c r="D100" s="13" t="str">
         <f t="shared" si="4"/>
         <v>$table-&gt;string('address', 255)-&gt;nullable();</v>
       </c>
-      <c r="E99" s="22"/>
-      <c r="G99" s="12"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
+      <c r="E100" s="22"/>
+      <c r="G100" s="12"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B100" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C100" s="8">
+      <c r="B101" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101" s="8">
         <v>50</v>
       </c>
-      <c r="D100" s="13" t="str">
+      <c r="D101" s="13" t="str">
         <f t="shared" si="4"/>
         <v>$table-&gt;string('phone', 50)-&gt;nullable();</v>
       </c>
-      <c r="E100" s="22"/>
-      <c r="G100" s="12"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
+      <c r="E101" s="22"/>
+      <c r="G101" s="12"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B101" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C101" s="8">
+      <c r="B102" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C102" s="8">
         <v>255</v>
       </c>
-      <c r="D101" s="13" t="str">
+      <c r="D102" s="13" t="str">
         <f t="shared" si="4"/>
         <v>$table-&gt;string('password', 255)-&gt;nullable();</v>
       </c>
-      <c r="E101" s="22"/>
-      <c r="G101" s="12"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C102" s="14"/>
-      <c r="D102" s="20" t="s">
-        <v>81</v>
-      </c>
       <c r="E102" s="22"/>
       <c r="G102" s="12"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="49" t="s">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C103" s="14"/>
+      <c r="D103" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E103" s="22"/>
+      <c r="G103" s="12"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="B105" s="49"/>
-      <c r="C105" s="49"/>
-      <c r="D105" s="49"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="49"/>
       <c r="B106" s="49"/>
       <c r="C106" s="49"/>
       <c r="D106" s="49"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="10" t="s">
+      <c r="A107" s="49"/>
+      <c r="B107" s="49"/>
+      <c r="C107" s="49"/>
+      <c r="D107" s="49"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B107" s="10" t="s">
+      <c r="B108" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C107" s="10" t="s">
+      <c r="C108" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D107" s="10" t="s">
+      <c r="D108" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B108" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C108" s="8">
+      <c r="B109" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" s="8">
         <v>255</v>
       </c>
-      <c r="D108" s="13" t="str">
-        <f t="shared" ref="D108:D109" si="5">IF(B108="String", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"', ",C108,")-&gt;nullable();"), IF(B108="Integer", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"')-&gt;unsigned()-&gt;default(0);"), IF(B108="Text", CONCATENATE("$table-&gt;",LOWER(B108),"('",A108,"');"), IF(B108="Date", CONCATENATE("$table-&gt;","timestamp","('",A108,"');")) )))</f>
+      <c r="D109" s="13" t="str">
+        <f t="shared" ref="D109:D110" si="5">IF(B109="String", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"', ",C109,")-&gt;nullable();"), IF(B109="Integer", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"')-&gt;unsigned()-&gt;default(0);"), IF(B109="Text", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"');"), IF(B109="Date", CONCATENATE("$table-&gt;","timestamp","('",A109,"');")) )))</f>
         <v>$table-&gt;string('status', 255)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="14"/>
-      <c r="B109" s="7"/>
-      <c r="C109" s="14"/>
-      <c r="D109" s="15" t="b">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="14"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="14"/>
+      <c r="D110" s="15" t="b">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="49" t="s">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="B111" s="49"/>
-      <c r="C111" s="49"/>
-      <c r="D111" s="49"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="49"/>
       <c r="B112" s="49"/>
       <c r="C112" s="49"/>
       <c r="D112" s="49"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="38" t="s">
+      <c r="A113" s="49"/>
+      <c r="B113" s="49"/>
+      <c r="C113" s="49"/>
+      <c r="D113" s="49"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B113" s="38" t="s">
+      <c r="B114" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C113" s="38" t="s">
+      <c r="C114" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D113" s="38" t="s">
+      <c r="D114" s="38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="8" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B114" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C114" s="8">
+      <c r="B115" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C115" s="8">
         <v>50</v>
       </c>
-      <c r="D114" s="13" t="str">
-        <f>IF(B114="String", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"', ",C114,")-nullable();"), IF(B114="Integer", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"')-&gt;unsigned()-&gt;default(0);"), IF(B114="Text", CONCATENATE("$table-&gt;",LOWER(B114),"('",A114,"');"), IF(B114="Date", CONCATENATE("$table-&gt;","timestamp","('",A114,"');")) )))</f>
+      <c r="D115" s="13" t="str">
+        <f>IF(B115="String", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"', ",C115,")-nullable();"), IF(B115="Integer", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"')-&gt;unsigned()-&gt;default(0);"), IF(B115="Text", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"');"), IF(B115="Date", CONCATENATE("$table-&gt;","timestamp","('",A115,"');")) )))</f>
         <v>$table-&gt;string('id_invoice', 50)-nullable();</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="14" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B115" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C115" s="14">
+      <c r="B116" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116" s="14">
         <v>50</v>
       </c>
-      <c r="D115" s="13" t="str">
-        <f t="shared" ref="D115:D120" si="6">IF(B115="String", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"', ",C115,");"), IF(B115="Integer", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"')-&gt;unsigned()-&gt;default(0);"), IF(B115="Text", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"');"), IF(B115="Date", CONCATENATE("$table-&gt;","timestamp","('",A115,"');")) )))</f>
+      <c r="D116" s="13" t="str">
+        <f t="shared" ref="D116:D121" si="6">IF(B116="String", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"', ",C116,");"), IF(B116="Integer", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"')-&gt;unsigned()-&gt;default(0);"), IF(B116="Text", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"');"), IF(B116="Date", CONCATENATE("$table-&gt;","timestamp","('",A116,"');")) )))</f>
         <v>$table-&gt;string('id_dentist', 50);</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="42" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B116" s="40" t="s">
+      <c r="B117" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C116" s="42"/>
-      <c r="D116" s="48" t="s">
+      <c r="C117" s="42"/>
+      <c r="D117" s="48" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="14" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B117" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C117" s="42">
+      <c r="B118" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C118" s="42">
         <v>255</v>
       </c>
-      <c r="D117" s="43" t="str">
-        <f t="shared" ref="D117" si="7">IF(B117="String", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"', ",C117,");"), IF(B117="Integer", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"')-&gt;unsigned()-&gt;default(0);"), IF(B117="Text", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"');"), IF(B117="Date", CONCATENATE("$table-&gt;","timestamp","('",A117,"');")) )))</f>
+      <c r="D118" s="43" t="str">
+        <f t="shared" ref="D118" si="7">IF(B118="String", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"', ",C118,");"), IF(B118="Integer", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"')-&gt;unsigned()-&gt;default(0);"), IF(B118="Text", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"');"), IF(B118="Date", CONCATENATE("$table-&gt;","timestamp","('",A118,"');")) )))</f>
         <v>$table-&gt;string('detail', 255);</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="42" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B118" s="40" t="s">
+      <c r="B119" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C118" s="42"/>
-      <c r="D118" s="43" t="str">
+      <c r="C119" s="42"/>
+      <c r="D119" s="43" t="str">
         <f t="shared" si="6"/>
         <v>$table-&gt;timestamp('date');</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="42" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="B119" s="40" t="s">
+      <c r="B120" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C119" s="42"/>
-      <c r="D119" s="41" t="str">
+      <c r="C120" s="42"/>
+      <c r="D120" s="41" t="str">
         <f t="shared" si="6"/>
         <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="42" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="B120" s="40" t="s">
+      <c r="B121" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C120" s="42"/>
-      <c r="D120" s="43" t="str">
+      <c r="C121" s="42"/>
+      <c r="D121" s="43" t="str">
         <f t="shared" si="6"/>
         <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="B121" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C121" s="42"/>
-      <c r="D121" s="43" t="s">
-        <v>123</v>
-      </c>
-    </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="42" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B122" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C122" s="42"/>
-      <c r="D122" s="41" t="str">
-        <f t="shared" ref="D122" si="8">IF(B122="String", CONCATENATE("$table-&gt;",LOWER(B122),"('",A122,"', ",C122,");"), IF(B122="Integer", CONCATENATE("$table-&gt;",LOWER(B122),"('",A122,"')-&gt;unsigned()-&gt;default(0);"), IF(B122="Text", CONCATENATE("$table-&gt;",LOWER(B122),"('",A122,"');"), IF(B122="Date", CONCATENATE("$table-&gt;","timestamp","('",A122,"');")) )))</f>
-        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D122" s="43" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="42" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C123" s="42"/>
-      <c r="D123" s="43" t="s">
-        <v>122</v>
+      <c r="D123" s="41" t="str">
+        <f t="shared" ref="D123" si="8">IF(B123="String", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"', ",C123,");"), IF(B123="Integer", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"')-&gt;unsigned()-&gt;default(0);"), IF(B123="Text", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"');"), IF(B123="Date", CONCATENATE("$table-&gt;","timestamp","('",A123,"');")) )))</f>
+        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="42" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B124" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C124" s="42"/>
-      <c r="D124" s="41" t="str">
-        <f t="shared" ref="D124:D126" si="9">IF(B124="String", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"', ",C124,");"), IF(B124="Integer", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"')-&gt;unsigned()-&gt;default(0);"), IF(B124="Text", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"');"), IF(B124="Date", CONCATENATE("$table-&gt;","timestamp","('",A124,"');")) )))</f>
-        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D124" s="43" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B125" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C125" s="42"/>
-      <c r="D125" s="43" t="s">
-        <v>121</v>
+      <c r="D125" s="41" t="str">
+        <f t="shared" ref="D125:D127" si="9">IF(B125="String", CONCATENATE("$table-&gt;",LOWER(B125),"('",A125,"', ",C125,");"), IF(B125="Integer", CONCATENATE("$table-&gt;",LOWER(B125),"('",A125,"')-&gt;unsigned()-&gt;default(0);"), IF(B125="Text", CONCATENATE("$table-&gt;",LOWER(B125),"('",A125,"');"), IF(B125="Date", CONCATENATE("$table-&gt;","timestamp","('",A125,"');")) )))</f>
+        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B126" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C126" s="42"/>
+      <c r="D126" s="43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="B126" s="40" t="s">
+      <c r="B127" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C126" s="42"/>
-      <c r="D126" s="41" t="str">
+      <c r="C127" s="42"/>
+      <c r="D127" s="41" t="str">
         <f t="shared" si="9"/>
         <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="B127" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C127" s="42"/>
-      <c r="D127" s="43" t="s">
-        <v>120</v>
-      </c>
-    </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B128" s="40" t="s">
         <v>104</v>
       </c>
       <c r="C128" s="42"/>
       <c r="D128" s="43" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="42" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C129" s="42">
-        <v>255</v>
-      </c>
-      <c r="D129" s="43" t="str">
-        <f>IF(B129="String", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"', ",C129,");"), IF(B129="Integer", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"')-&gt;unsigned()-&gt;default(0);"), IF(B129="Text", CONCATENATE("$table-&gt;",LOWER(B129),"('",A129,"');"), IF(B129="Date", CONCATENATE("$table-&gt;","timestamp","('",A129,"');")) )))</f>
-        <v>$table-&gt;string('position', 255);</v>
+        <v>104</v>
+      </c>
+      <c r="C129" s="42"/>
+      <c r="D129" s="43" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B130" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C130" s="42"/>
+        <v>6</v>
+      </c>
+      <c r="C130" s="42">
+        <v>255</v>
+      </c>
       <c r="D130" s="43" t="str">
         <f>IF(B130="String", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"', ",C130,");"), IF(B130="Integer", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"')-&gt;unsigned()-&gt;default(0);"), IF(B130="Text", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"');"), IF(B130="Date", CONCATENATE("$table-&gt;","timestamp","('",A130,"');")) )))</f>
-        <v>$table-&gt;integer('object')-&gt;unsigned()-&gt;default(0);</v>
+        <v>$table-&gt;string('position', 255);</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B131" s="40" t="s">
         <v>25</v>
@@ -3872,271 +3878,278 @@
       <c r="C131" s="42"/>
       <c r="D131" s="43" t="str">
         <f>IF(B131="String", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"', ",C131,");"), IF(B131="Integer", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"')-&gt;unsigned()-&gt;default(0);"), IF(B131="Text", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"');"), IF(B131="Date", CONCATENATE("$table-&gt;","timestamp","('",A131,"');")) )))</f>
-        <v>$table-&gt;integer('type_operation')-&gt;unsigned()-&gt;default(0);</v>
+        <v>$table-&gt;integer('object')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="42" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C132" s="42"/>
       <c r="D132" s="43" t="str">
         <f>IF(B132="String", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"', ",C132,");"), IF(B132="Integer", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"')-&gt;unsigned()-&gt;default(0);"), IF(B132="Text", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"');"), IF(B132="Date", CONCATENATE("$table-&gt;","timestamp","('",A132,"');")) )))</f>
+        <v>$table-&gt;integer('type_operation')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B133" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C133" s="42"/>
+      <c r="D133" s="43" t="str">
+        <f>IF(B133="String", CONCATENATE("$table-&gt;",LOWER(B133),"('",A133,"', ",C133,");"), IF(B133="Integer", CONCATENATE("$table-&gt;",LOWER(B133),"('",A133,"')-&gt;unsigned()-&gt;default(0);"), IF(B133="Text", CONCATENATE("$table-&gt;",LOWER(B133),"('",A133,"');"), IF(B133="Date", CONCATENATE("$table-&gt;","timestamp","('",A133,"');")) )))</f>
         <v>$table-&gt;text('note');</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="42"/>
-      <c r="B133" s="44"/>
-      <c r="C133" s="42"/>
-      <c r="D133" s="45"/>
-    </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="49" t="s">
+      <c r="A134" s="42"/>
+      <c r="B134" s="44"/>
+      <c r="C134" s="42"/>
+      <c r="D134" s="45"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="B134" s="49"/>
-      <c r="C134" s="49"/>
-      <c r="D134" s="49"/>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="49"/>
       <c r="B135" s="49"/>
       <c r="C135" s="49"/>
       <c r="D135" s="49"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="38" t="s">
+      <c r="A136" s="49"/>
+      <c r="B136" s="49"/>
+      <c r="C136" s="49"/>
+      <c r="D136" s="49"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B136" s="38" t="s">
+      <c r="B137" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C136" s="38" t="s">
+      <c r="C137" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D136" s="38" t="s">
+      <c r="D137" s="38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="8" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B137" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C137" s="8">
+      <c r="B138" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138" s="8">
         <v>255</v>
       </c>
-      <c r="D137" s="13" t="str">
-        <f>IF(B137="String", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"', ",C137,");"), IF(B137="Integer", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"')-&gt;unsigned()-&gt;default(0);"), IF(B137="Text", CONCATENATE("$table-&gt;",LOWER(B137),"('",A137,"');"), IF(B137="Date", CONCATENATE("$table-&gt;","timestamp","('",A137,"');")) )))</f>
+      <c r="D138" s="13" t="str">
+        <f>IF(B138="String", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"', ",C138,");"), IF(B138="Integer", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"')-&gt;unsigned()-&gt;default(0);"), IF(B138="Text", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"');"), IF(B138="Date", CONCATENATE("$table-&gt;","timestamp","('",A138,"');")) )))</f>
         <v>$table-&gt;string('category', 255);</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="49" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="B141" s="49"/>
-      <c r="C141" s="49"/>
-      <c r="D141" s="49"/>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="49"/>
       <c r="B142" s="49"/>
       <c r="C142" s="49"/>
       <c r="D142" s="49"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="39" t="s">
+      <c r="A143" s="49"/>
+      <c r="B143" s="49"/>
+      <c r="C143" s="49"/>
+      <c r="D143" s="49"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B143" s="39" t="s">
+      <c r="B144" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C143" s="39" t="s">
+      <c r="C144" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D143" s="39" t="s">
+      <c r="D144" s="39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="8" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B144" s="7" t="s">
+      <c r="B145" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C144" s="8"/>
-      <c r="D144" s="13" t="str">
-        <f t="shared" ref="D144:D149" si="10">IF(B144="String", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"', ",C144,");"), IF(B144="Integer", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"')-&gt;unsigned()-&gt;default(0);"), IF(B144="Text", CONCATENATE("$table-&gt;",LOWER(B144),"('",A144,"');"), IF(B144="Date", CONCATENATE("$table-&gt;","timestamp","('",A144,"');")) )))</f>
+      <c r="C145" s="8"/>
+      <c r="D145" s="13" t="str">
+        <f t="shared" ref="D145:D150" si="10">IF(B145="String", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"', ",C145,");"), IF(B145="Integer", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"')-&gt;unsigned()-&gt;default(0);"), IF(B145="Text", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"');"), IF(B145="Date", CONCATENATE("$table-&gt;","timestamp","('",A145,"');")) )))</f>
         <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="42" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B145" s="40" t="s">
+      <c r="B146" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C145" s="42"/>
-      <c r="D145" s="43" t="str">
+      <c r="C146" s="42"/>
+      <c r="D146" s="43" t="str">
         <f t="shared" si="10"/>
         <v>$table-&gt;integer('id_category')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="42" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B146" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C146" s="42">
+      <c r="B147" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C147" s="42">
         <v>50</v>
       </c>
-      <c r="D146" s="43" t="str">
+      <c r="D147" s="43" t="str">
         <f t="shared" si="10"/>
         <v>$table-&gt;string('id_dentist', 50);</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="42" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B147" s="40" t="s">
+      <c r="B148" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C147" s="42"/>
-      <c r="D147" s="41" t="str">
+      <c r="C148" s="42"/>
+      <c r="D148" s="41" t="str">
         <f t="shared" si="10"/>
         <v>$table-&gt;timestamp('date');</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="B148" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C148" s="42"/>
-      <c r="D148" s="43" t="str">
-        <f t="shared" si="10"/>
-        <v>$table-&gt;integer('teeth_no')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="42" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="B149" s="40" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C149" s="42"/>
       <c r="D149" s="43" t="str">
         <f t="shared" si="10"/>
-        <v>$table-&gt;text('description');</v>
+        <v>$table-&gt;integer('teeth_no')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="42" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C150" s="42"/>
-      <c r="D150" s="41" t="str">
-        <f t="shared" ref="D150:D155" si="11">IF(B150="String", CONCATENATE("$table-&gt;",LOWER(B150),"('",A150,"', ",C150,");"), IF(B150="Integer", CONCATENATE("$table-&gt;",LOWER(B150),"('",A150,"')-&gt;unsigned()-&gt;default(0);"), IF(B150="Text", CONCATENATE("$table-&gt;",LOWER(B150),"('",A150,"');"), IF(B150="Date", CONCATENATE("$table-&gt;","timestamp","('",A150,"');")) )))</f>
-        <v>$table-&gt;integer('currency')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D150" s="43" t="str">
+        <f t="shared" si="10"/>
+        <v>$table-&gt;text('description');</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B151" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C151" s="42"/>
-      <c r="D151" s="43" t="s">
-        <v>115</v>
+      <c r="D151" s="41" t="str">
+        <f t="shared" ref="D151:D156" si="11">IF(B151="String", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"', ",C151,");"), IF(B151="Integer", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"')-&gt;unsigned()-&gt;default(0);"), IF(B151="Text", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"');"), IF(B151="Date", CONCATENATE("$table-&gt;","timestamp","('",A151,"');")) )))</f>
+        <v>$table-&gt;integer('currency')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B152" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C152" s="42"/>
+      <c r="D152" s="43" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="B152" s="40" t="s">
+      <c r="B153" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C152" s="42"/>
-      <c r="D152" s="41" t="str">
+      <c r="C153" s="42"/>
+      <c r="D153" s="41" t="str">
         <f t="shared" si="11"/>
         <v>$table-&gt;integer('quantity')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B153" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C153" s="42"/>
-      <c r="D153" s="43" t="s">
-        <v>117</v>
-      </c>
-    </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="42" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="B154" s="40" t="s">
         <v>104</v>
       </c>
       <c r="C154" s="42"/>
       <c r="D154" s="43" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B155" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C155" s="42"/>
+      <c r="D155" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="B155" s="40" t="s">
+      <c r="B156" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C155" s="42"/>
-      <c r="D155" s="43" t="str">
+      <c r="C156" s="42"/>
+      <c r="D156" s="43" t="str">
         <f t="shared" si="11"/>
         <v>$table-&gt;text('clicnic_note');</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="42" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="B156" s="40" t="s">
+      <c r="B157" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C156" s="42"/>
-      <c r="D156" s="43" t="s">
+      <c r="C157" s="42"/>
+      <c r="D157" s="43" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="42"/>
-      <c r="B157" s="40"/>
-      <c r="C157" s="42"/>
-      <c r="D157" s="43"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="42"/>
@@ -4156,242 +4169,248 @@
       <c r="C160" s="42"/>
       <c r="D160" s="43"/>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="49" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="42"/>
+      <c r="B161" s="40"/>
+      <c r="C161" s="42"/>
+      <c r="D161" s="43"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="B163" s="49"/>
-      <c r="C163" s="49"/>
-      <c r="D163" s="49"/>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="49"/>
       <c r="B164" s="49"/>
       <c r="C164" s="49"/>
       <c r="D164" s="49"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="46" t="s">
+      <c r="A165" s="49"/>
+      <c r="B165" s="49"/>
+      <c r="C165" s="49"/>
+      <c r="D165" s="49"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B165" s="46" t="s">
+      <c r="B166" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C165" s="46" t="s">
+      <c r="C166" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D165" s="46" t="s">
+      <c r="D166" s="46" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="42" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B166" s="40" t="s">
+      <c r="B167" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C166" s="42"/>
-      <c r="D166" s="48" t="s">
+      <c r="C167" s="42"/>
+      <c r="D167" s="48" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B167" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C167" s="14">
-        <v>255</v>
-      </c>
-      <c r="D167" s="47" t="str">
-        <f>IF(B167="String", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"', ",C167,")-&gt;nullable();"), IF(B167="Integer", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"')-&gt;unsigned()-&gt;default(0);"), IF(B167="Text", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"');"), IF(B167="Date", CONCATENATE("$table-&gt;","timestamp","('",A167,"');")) )))</f>
-        <v>$table-&gt;string('category', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B168" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168" s="14">
+        <v>255</v>
+      </c>
+      <c r="D168" s="47" t="str">
+        <f>IF(B168="String", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"', ",C168,")-&gt;nullable();"), IF(B168="Integer", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"')-&gt;unsigned()-&gt;default(0);"), IF(B168="Text", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"');"), IF(B168="Date", CONCATENATE("$table-&gt;","timestamp","('",A168,"');")) )))</f>
+        <v>$table-&gt;string('category', 255)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B168" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C168" s="42">
+      <c r="B169" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C169" s="42">
         <v>255</v>
       </c>
-      <c r="D168" s="43" t="str">
-        <f t="shared" ref="D168" si="12">IF(B168="String", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"', ",C168,");"), IF(B168="Integer", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"')-&gt;unsigned()-&gt;default(0);"), IF(B168="Text", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"');"), IF(B168="Date", CONCATENATE("$table-&gt;","timestamp","('",A168,"');")) )))</f>
+      <c r="D169" s="43" t="str">
+        <f t="shared" ref="D169" si="12">IF(B169="String", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"', ",C169,");"), IF(B169="Integer", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"')-&gt;unsigned()-&gt;default(0);"), IF(B169="Text", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"');"), IF(B169="Date", CONCATENATE("$table-&gt;","timestamp","('",A169,"');")) )))</f>
         <v>$table-&gt;string('detail', 255);</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="B169" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C169" s="42"/>
-      <c r="D169" s="43" t="str">
-        <f t="shared" ref="D169:D170" si="13">IF(B169="String", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"', ",C169,");"), IF(B169="Integer", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"')-&gt;unsigned()-&gt;default(0);"), IF(B169="Text", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"');"), IF(B169="Date", CONCATENATE("$table-&gt;","timestamp","('",A169,"');")) )))</f>
-        <v>$table-&gt;timestamp('date');</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="42" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B170" s="40" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C170" s="42"/>
       <c r="D170" s="43" t="str">
+        <f t="shared" ref="D170:D171" si="13">IF(B170="String", CONCATENATE("$table-&gt;",LOWER(B170),"('",A170,"', ",C170,");"), IF(B170="Integer", CONCATENATE("$table-&gt;",LOWER(B170),"('",A170,"')-&gt;unsigned()-&gt;default(0);"), IF(B170="Text", CONCATENATE("$table-&gt;",LOWER(B170),"('",A170,"');"), IF(B170="Date", CONCATENATE("$table-&gt;","timestamp","('",A170,"');")) )))</f>
+        <v>$table-&gt;timestamp('date');</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B171" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C171" s="42"/>
+      <c r="D171" s="43" t="str">
         <f t="shared" si="13"/>
         <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="B171" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C171" s="42"/>
-      <c r="D171" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="42" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B172" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C172" s="42"/>
-      <c r="D172" s="41" t="str">
-        <f t="shared" ref="D172" si="14">IF(B172="String", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"', ",C172,");"), IF(B172="Integer", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"')-&gt;unsigned()-&gt;default(0);"), IF(B172="Text", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"');"), IF(B172="Date", CONCATENATE("$table-&gt;","timestamp","('",A172,"');")) )))</f>
-        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D172" s="15" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="42" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B173" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C173" s="42"/>
-      <c r="D173" s="15" t="s">
-        <v>129</v>
+      <c r="D173" s="41" t="str">
+        <f t="shared" ref="D173" si="14">IF(B173="String", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"', ",C173,");"), IF(B173="Integer", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"')-&gt;unsigned()-&gt;default(0);"), IF(B173="Text", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"');"), IF(B173="Date", CONCATENATE("$table-&gt;","timestamp","('",A173,"');")) )))</f>
+        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="42" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B174" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C174" s="42"/>
-      <c r="D174" s="41" t="str">
-        <f t="shared" ref="D174" si="15">IF(B174="String", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"', ",C174,");"), IF(B174="Integer", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"')-&gt;unsigned()-&gt;default(0);"), IF(B174="Text", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"');"), IF(B174="Date", CONCATENATE("$table-&gt;","timestamp","('",A174,"');")) )))</f>
-        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D174" s="15" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B175" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C175" s="42"/>
-      <c r="D175" s="15" t="s">
-        <v>130</v>
+      <c r="D175" s="41" t="str">
+        <f t="shared" ref="D175" si="15">IF(B175="String", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"', ",C175,");"), IF(B175="Integer", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"')-&gt;unsigned()-&gt;default(0);"), IF(B175="Text", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"');"), IF(B175="Date", CONCATENATE("$table-&gt;","timestamp","('",A175,"');")) )))</f>
+        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B176" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C176" s="42"/>
-      <c r="D176" s="41" t="str">
-        <f t="shared" ref="D176" si="16">IF(B176="String", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"', ",C176,");"), IF(B176="Integer", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"')-&gt;unsigned()-&gt;default(0);"), IF(B176="Text", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"');"), IF(B176="Date", CONCATENATE("$table-&gt;","timestamp","('",A176,"');")) )))</f>
-        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D176" s="15" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B177" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C177" s="42"/>
-      <c r="D177" s="15" t="s">
-        <v>131</v>
+      <c r="D177" s="41" t="str">
+        <f t="shared" ref="D177" si="16">IF(B177="String", CONCATENATE("$table-&gt;",LOWER(B177),"('",A177,"', ",C177,");"), IF(B177="Integer", CONCATENATE("$table-&gt;",LOWER(B177),"('",A177,"')-&gt;unsigned()-&gt;default(0);"), IF(B177="Text", CONCATENATE("$table-&gt;",LOWER(B177),"('",A177,"');"), IF(B177="Date", CONCATENATE("$table-&gt;","timestamp","('",A177,"');")) )))</f>
+        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B178" s="40" t="s">
         <v>104</v>
       </c>
       <c r="C178" s="42"/>
       <c r="D178" s="15" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="42" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B179" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C179" s="42">
-        <v>255</v>
-      </c>
-      <c r="D179" s="43" t="str">
-        <f>IF(B179="String", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"', ",C179,")-&gt;nullable();"), IF(B179="Integer", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"')-&gt;unsigned()-&gt;default(0);"), IF(B179="Text", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"');"), IF(B179="Date", CONCATENATE("$table-&gt;","timestamp","('",A179,"');")) )))</f>
-        <v>$table-&gt;string('position', 255)-&gt;nullable();</v>
+        <v>104</v>
+      </c>
+      <c r="C179" s="42"/>
+      <c r="D179" s="15" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B180" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180" s="42">
+        <v>255</v>
+      </c>
+      <c r="D180" s="43" t="str">
+        <f>IF(B180="String", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"', ",C180,")-&gt;nullable();"), IF(B180="Integer", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"')-&gt;unsigned()-&gt;default(0);"), IF(B180="Text", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"');"), IF(B180="Date", CONCATENATE("$table-&gt;","timestamp","('",A180,"');")) )))</f>
+        <v>$table-&gt;string('position', 255)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B180" s="40" t="s">
+      <c r="B181" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C180" s="42"/>
-      <c r="D180" s="43" t="str">
-        <f>IF(B180="String", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"', ",C180,");"), IF(B180="Integer", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"')-&gt;unsigned()-&gt;default(0);"), IF(B180="Text", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"')-&gt;nullable();"), IF(B180="Date", CONCATENATE("$table-&gt;","timestamp","('",A180,"');")) )))</f>
+      <c r="C181" s="42"/>
+      <c r="D181" s="43" t="str">
+        <f>IF(B181="String", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"', ",C181,");"), IF(B181="Integer", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"')-&gt;unsigned()-&gt;default(0);"), IF(B181="Text", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"')-&gt;nullable();"), IF(B181="Date", CONCATENATE("$table-&gt;","timestamp","('",A181,"');")) )))</f>
         <v>$table-&gt;text('note')-&gt;nullable();</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A90:D91"/>
+    <mergeCell ref="A164:D165"/>
+    <mergeCell ref="A142:D143"/>
+    <mergeCell ref="A112:D113"/>
+    <mergeCell ref="A135:D136"/>
+    <mergeCell ref="A106:D107"/>
+    <mergeCell ref="A91:D92"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A55:D56"/>
     <mergeCell ref="A63:D64"/>
-    <mergeCell ref="A72:D73"/>
-    <mergeCell ref="A80:D81"/>
-    <mergeCell ref="A163:D164"/>
-    <mergeCell ref="A141:D142"/>
-    <mergeCell ref="A111:D112"/>
-    <mergeCell ref="A134:D135"/>
-    <mergeCell ref="A105:D106"/>
+    <mergeCell ref="A73:D74"/>
+    <mergeCell ref="A81:D82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
#5 Minor fixes ( Cure Modal: Added amount, calculator, and can be saved at jobs ) :progress:
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="140">
   <si>
     <t>PATIENT</t>
   </si>
@@ -437,6 +437,27 @@
   </si>
   <si>
     <t>shortDesc</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>$table-&gt;decimal('amount', 7, 2);</t>
+  </si>
+  <si>
+    <t>id_teeth_prizes</t>
+  </si>
+  <si>
+    <t>shortCode</t>
+  </si>
+  <si>
+    <t>type_cure</t>
+  </si>
+  <si>
+    <t>status_cure</t>
+  </si>
+  <si>
+    <t>desc_client</t>
   </si>
 </sst>
 </file>
@@ -722,10 +743,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1846,8 +1867,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table254687911" displayName="Table254687911" ref="A144:D161" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A144:D161"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table254687911" displayName="Table254687911" ref="A144:D166" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A144:D166"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="9"/>
     <tableColumn id="2" name="Type" dataDxfId="8"/>
@@ -1861,14 +1882,14 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table254687912" displayName="Table254687912" ref="A166:D181" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A166:D181"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table254687912" displayName="Table254687912" ref="A171:D187" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A171:D187"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="3"/>
     <tableColumn id="2" name="Type" dataDxfId="2"/>
     <tableColumn id="3" name="Length" dataDxfId="1"/>
     <tableColumn id="4" name="Code generated" dataDxfId="0">
-      <calculatedColumnFormula>IF(B167="String", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"', ",C167,");"), IF(B167="Integer", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"')-&gt;unsigned()-&gt;default(0);"), IF(B167="Text", CONCATENATE("$table-&gt;",LOWER(B167),"('",A167,"');"), IF(B167="Date", CONCATENATE("$table-&gt;","timestamp","('",A167,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B172="String", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"', ",C172,");"), IF(B172="Integer", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"')-&gt;unsigned()-&gt;default(0);"), IF(B172="Text", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"');"), IF(B172="Date", CONCATENATE("$table-&gt;","timestamp","('",A172,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2282,10 +2303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G181"/>
+  <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2298,22 +2319,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3023,18 +3044,18 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="49" t="s">
+      <c r="A55" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="49"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="49"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="49"/>
-      <c r="B56" s="49"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="49"/>
+      <c r="A56" s="50"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -3111,18 +3132,18 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="49" t="s">
+      <c r="A63" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="49"/>
-      <c r="C63" s="49"/>
-      <c r="D63" s="49"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="49"/>
-      <c r="B64" s="49"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="49"/>
+      <c r="A64" s="50"/>
+      <c r="B64" s="50"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
@@ -3193,7 +3214,7 @@
       <c r="C69">
         <v>100</v>
       </c>
-      <c r="D69" s="50" t="str">
+      <c r="D69" s="49" t="str">
         <f>IF(B69="String", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"', ",C69,")-&gt;nullable();"), IF(B69="Integer", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"')-&gt;unsigned()-&gt;default(0);"), IF(B69="Text", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"');"), IF(B69="Date", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"');")) )))</f>
         <v>$table-&gt;string('shortDesc', 100)-&gt;nullable();</v>
       </c>
@@ -3220,18 +3241,18 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="49" t="s">
+      <c r="A73" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="B73" s="49"/>
-      <c r="C73" s="49"/>
-      <c r="D73" s="49"/>
+      <c r="B73" s="50"/>
+      <c r="C73" s="50"/>
+      <c r="D73" s="50"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="49"/>
-      <c r="B74" s="49"/>
-      <c r="C74" s="49"/>
-      <c r="D74" s="49"/>
+      <c r="A74" s="50"/>
+      <c r="B74" s="50"/>
+      <c r="C74" s="50"/>
+      <c r="D74" s="50"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
@@ -3270,18 +3291,18 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="49" t="s">
+      <c r="A81" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B81" s="49"/>
-      <c r="C81" s="49"/>
-      <c r="D81" s="49"/>
+      <c r="B81" s="50"/>
+      <c r="C81" s="50"/>
+      <c r="D81" s="50"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="49"/>
-      <c r="B82" s="49"/>
-      <c r="C82" s="49"/>
-      <c r="D82" s="49"/>
+      <c r="A82" s="50"/>
+      <c r="B82" s="50"/>
+      <c r="C82" s="50"/>
+      <c r="D82" s="50"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
@@ -3385,18 +3406,18 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="49" t="s">
+      <c r="A91" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="B91" s="49"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="49"/>
-      <c r="B92" s="49"/>
-      <c r="C92" s="49"/>
-      <c r="D92" s="49"/>
+      <c r="A92" s="50"/>
+      <c r="B92" s="50"/>
+      <c r="C92" s="50"/>
+      <c r="D92" s="50"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
@@ -3579,18 +3600,18 @@
       <c r="G103" s="12"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="49" t="s">
+      <c r="A106" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="B106" s="49"/>
-      <c r="C106" s="49"/>
-      <c r="D106" s="49"/>
+      <c r="B106" s="50"/>
+      <c r="C106" s="50"/>
+      <c r="D106" s="50"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="49"/>
-      <c r="B107" s="49"/>
-      <c r="C107" s="49"/>
-      <c r="D107" s="49"/>
+      <c r="A107" s="50"/>
+      <c r="B107" s="50"/>
+      <c r="C107" s="50"/>
+      <c r="D107" s="50"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="s">
@@ -3631,18 +3652,18 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="49" t="s">
+      <c r="A112" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="B112" s="49"/>
-      <c r="C112" s="49"/>
-      <c r="D112" s="49"/>
+      <c r="B112" s="50"/>
+      <c r="C112" s="50"/>
+      <c r="D112" s="50"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="49"/>
-      <c r="B113" s="49"/>
-      <c r="C113" s="49"/>
-      <c r="D113" s="49"/>
+      <c r="A113" s="50"/>
+      <c r="B113" s="50"/>
+      <c r="C113" s="50"/>
+      <c r="D113" s="50"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="38" t="s">
@@ -3914,18 +3935,18 @@
       <c r="D134" s="45"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="49" t="s">
+      <c r="A135" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="B135" s="49"/>
-      <c r="C135" s="49"/>
-      <c r="D135" s="49"/>
+      <c r="B135" s="50"/>
+      <c r="C135" s="50"/>
+      <c r="D135" s="50"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="49"/>
-      <c r="B136" s="49"/>
-      <c r="C136" s="49"/>
-      <c r="D136" s="49"/>
+      <c r="A136" s="50"/>
+      <c r="B136" s="50"/>
+      <c r="C136" s="50"/>
+      <c r="D136" s="50"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="38" t="s">
@@ -3957,18 +3978,18 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="49" t="s">
+      <c r="A142" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="B142" s="49"/>
-      <c r="C142" s="49"/>
-      <c r="D142" s="49"/>
+      <c r="B142" s="50"/>
+      <c r="C142" s="50"/>
+      <c r="D142" s="50"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="49"/>
-      <c r="B143" s="49"/>
-      <c r="C143" s="49"/>
-      <c r="D143" s="49"/>
+      <c r="A143" s="50"/>
+      <c r="B143" s="50"/>
+      <c r="C143" s="50"/>
+      <c r="D143" s="50"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="39" t="s">
@@ -3999,15 +4020,15 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="42" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="B146" s="40" t="s">
         <v>25</v>
       </c>
       <c r="C146" s="42"/>
       <c r="D146" s="43" t="str">
-        <f t="shared" si="10"/>
-        <v>$table-&gt;integer('id_category')-&gt;unsigned()-&gt;default(0);</v>
+        <f>IF(B146="String", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"', ",C146,");"), IF(B146="Integer", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"')-&gt;unsigned()-&gt;default(0);"), IF(B146="Text", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"');"), IF(B146="Date", CONCATENATE("$table-&gt;","timestamp","('",A146,"');")) )))</f>
+        <v>$table-&gt;integer('id_teeth_prizes')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -4043,12 +4064,14 @@
         <v>112</v>
       </c>
       <c r="B149" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C149" s="42"/>
+        <v>6</v>
+      </c>
+      <c r="C149" s="42">
+        <v>255</v>
+      </c>
       <c r="D149" s="43" t="str">
         <f t="shared" si="10"/>
-        <v>$table-&gt;integer('teeth_no')-&gt;unsigned()-&gt;default(0);</v>
+        <v>$table-&gt;string('teeth_no', 255);</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -4066,85 +4089,88 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="42" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="B151" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C151" s="42"/>
+        <v>6</v>
+      </c>
+      <c r="C151" s="42">
+        <v>255</v>
+      </c>
       <c r="D151" s="41" t="str">
-        <f t="shared" ref="D151:D156" si="11">IF(B151="String", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"', ",C151,");"), IF(B151="Integer", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"')-&gt;unsigned()-&gt;default(0);"), IF(B151="Text", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"');"), IF(B151="Date", CONCATENATE("$table-&gt;","timestamp","('",A151,"');")) )))</f>
-        <v>$table-&gt;integer('currency')-&gt;unsigned()-&gt;default(0);</v>
+        <f>IF(B151="String", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"', ",C151,");"), IF(B151="Integer", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"')-&gt;unsigned()-&gt;default(0);"), IF(B151="Text", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"');"), IF(B151="Date", CONCATENATE("$table-&gt;","timestamp","('",A151,"');")) )))</f>
+        <v>$table-&gt;string('shortCode', 255);</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="42" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="B152" s="40" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="C152" s="42"/>
-      <c r="D152" s="43" t="s">
-        <v>115</v>
+      <c r="D152" s="41" t="str">
+        <f>IF(B152="String", CONCATENATE("$table-&gt;",LOWER(B152),"('",A152,"', ",C152,");"), IF(B152="Integer", CONCATENATE("$table-&gt;",LOWER(B152),"('",A152,"')-&gt;unsigned()-&gt;default(0);"), IF(B152="Text", CONCATENATE("$table-&gt;",LOWER(B152),"('",A152,"');"), IF(B152="Date", CONCATENATE("$table-&gt;","timestamp","('",A152,"');")) )))</f>
+        <v>$table-&gt;text('desc_client');</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="42" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B153" s="40" t="s">
         <v>25</v>
       </c>
       <c r="C153" s="42"/>
       <c r="D153" s="41" t="str">
+        <f t="shared" ref="D153:D161" si="11">IF(B153="String", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"', ",C153,");"), IF(B153="Integer", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"')-&gt;unsigned()-&gt;default(0);"), IF(B153="Text", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"');"), IF(B153="Date", CONCATENATE("$table-&gt;","timestamp","('",A153,"');")) )))</f>
+        <v>$table-&gt;integer('currency')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B154" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C154" s="42"/>
+      <c r="D154" s="43" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B155" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C155" s="42"/>
+      <c r="D155" s="41" t="str">
         <f t="shared" si="11"/>
         <v>$table-&gt;integer('quantity')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B154" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C154" s="42"/>
-      <c r="D154" s="43" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="B155" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C155" s="42"/>
-      <c r="D155" s="43" t="s">
-        <v>105</v>
-      </c>
-    </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="42" t="s">
-        <v>118</v>
+        <v>32</v>
       </c>
       <c r="B156" s="40" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="C156" s="42"/>
-      <c r="D156" s="43" t="str">
-        <f t="shared" si="11"/>
-        <v>$table-&gt;text('clicnic_note');</v>
+      <c r="D156" s="43" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="42" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B157" s="40" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="C157" s="42"/>
       <c r="D157" s="43" t="s">
@@ -4152,255 +4178,335 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="42"/>
-      <c r="B158" s="40"/>
+      <c r="A158" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B158" s="40" t="s">
+        <v>104</v>
+      </c>
       <c r="C158" s="42"/>
-      <c r="D158" s="43"/>
+      <c r="D158" s="43" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="42"/>
-      <c r="B159" s="40"/>
-      <c r="C159" s="42"/>
-      <c r="D159" s="43"/>
+      <c r="A159" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B159" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C159" s="42">
+        <v>255</v>
+      </c>
+      <c r="D159" s="41" t="str">
+        <f>IF(B159="String", CONCATENATE("$table-&gt;",LOWER(B159),"('",A159,"', ",C159,");"), IF(B159="Integer", CONCATENATE("$table-&gt;",LOWER(B159),"('",A159,"')-&gt;unsigned()-&gt;default(0);"), IF(B159="Text", CONCATENATE("$table-&gt;",LOWER(B159),"('",A159,"');"), IF(B159="Date", CONCATENATE("$table-&gt;","timestamp","('",A159,"');")) )))</f>
+        <v>$table-&gt;string('type_cure', 255);</v>
+      </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="42"/>
-      <c r="B160" s="40"/>
-      <c r="C160" s="42"/>
-      <c r="D160" s="43"/>
+      <c r="A160" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B160" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C160" s="42">
+        <v>255</v>
+      </c>
+      <c r="D160" s="41" t="str">
+        <f>IF(B160="String", CONCATENATE("$table-&gt;",LOWER(B160),"('",A160,"', ",C160,");"), IF(B160="Integer", CONCATENATE("$table-&gt;",LOWER(B160),"('",A160,"')-&gt;unsigned()-&gt;default(0);"), IF(B160="Text", CONCATENATE("$table-&gt;",LOWER(B160),"('",A160,"');"), IF(B160="Date", CONCATENATE("$table-&gt;","timestamp","('",A160,"');")) )))</f>
+        <v>$table-&gt;string('status_cure', 255);</v>
+      </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="42"/>
-      <c r="B161" s="40"/>
+      <c r="A161" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B161" s="40" t="s">
+        <v>31</v>
+      </c>
       <c r="C161" s="42"/>
-      <c r="D161" s="43"/>
+      <c r="D161" s="43" t="str">
+        <f t="shared" si="11"/>
+        <v>$table-&gt;text('clicnic_note');</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B162" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C162" s="42"/>
+      <c r="D162" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="42"/>
+      <c r="B163" s="40"/>
+      <c r="C163" s="42"/>
+      <c r="D163" s="43"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="49" t="s">
+      <c r="A164" s="42"/>
+      <c r="B164" s="40"/>
+      <c r="C164" s="42"/>
+      <c r="D164" s="43"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="42"/>
+      <c r="B165" s="40"/>
+      <c r="C165" s="42"/>
+      <c r="D165" s="43"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="42"/>
+      <c r="B166" s="40"/>
+      <c r="C166" s="42"/>
+      <c r="D166" s="43"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="B164" s="49"/>
-      <c r="C164" s="49"/>
-      <c r="D164" s="49"/>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="49"/>
-      <c r="B165" s="49"/>
-      <c r="C165" s="49"/>
-      <c r="D165" s="49"/>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="46" t="s">
+      <c r="B169" s="50"/>
+      <c r="C169" s="50"/>
+      <c r="D169" s="50"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="50"/>
+      <c r="B170" s="50"/>
+      <c r="C170" s="50"/>
+      <c r="D170" s="50"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B166" s="46" t="s">
+      <c r="B171" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C166" s="46" t="s">
+      <c r="C171" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D166" s="46" t="s">
+      <c r="D171" s="46" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="42" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B167" s="40" t="s">
+      <c r="B172" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C167" s="42"/>
-      <c r="D167" s="48" t="s">
+      <c r="C172" s="42"/>
+      <c r="D172" s="48" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="14" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B168" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C168" s="14">
+      <c r="B173" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173" s="14">
         <v>255</v>
       </c>
-      <c r="D168" s="47" t="str">
-        <f>IF(B168="String", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"', ",C168,")-&gt;nullable();"), IF(B168="Integer", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"')-&gt;unsigned()-&gt;default(0);"), IF(B168="Text", CONCATENATE("$table-&gt;",LOWER(B168),"('",A168,"');"), IF(B168="Date", CONCATENATE("$table-&gt;","timestamp","('",A168,"');")) )))</f>
+      <c r="D173" s="47" t="str">
+        <f>IF(B173="String", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"', ",C173,")-&gt;nullable();"), IF(B173="Integer", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"')-&gt;unsigned()-&gt;default(0);"), IF(B173="Text", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"');"), IF(B173="Date", CONCATENATE("$table-&gt;","timestamp","('",A173,"');")) )))</f>
         <v>$table-&gt;string('category', 255)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="14" t="s">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B169" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C169" s="42">
+      <c r="B174" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174" s="42">
         <v>255</v>
       </c>
-      <c r="D169" s="43" t="str">
-        <f t="shared" ref="D169" si="12">IF(B169="String", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"', ",C169,");"), IF(B169="Integer", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"')-&gt;unsigned()-&gt;default(0);"), IF(B169="Text", CONCATENATE("$table-&gt;",LOWER(B169),"('",A169,"');"), IF(B169="Date", CONCATENATE("$table-&gt;","timestamp","('",A169,"');")) )))</f>
+      <c r="D174" s="43" t="str">
+        <f t="shared" ref="D174" si="12">IF(B174="String", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"', ",C174,");"), IF(B174="Integer", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"')-&gt;unsigned()-&gt;default(0);"), IF(B174="Text", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"');"), IF(B174="Date", CONCATENATE("$table-&gt;","timestamp","('",A174,"');")) )))</f>
         <v>$table-&gt;string('detail', 255);</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="42" t="s">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B170" s="40" t="s">
+      <c r="B175" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C170" s="42"/>
-      <c r="D170" s="43" t="str">
-        <f t="shared" ref="D170:D171" si="13">IF(B170="String", CONCATENATE("$table-&gt;",LOWER(B170),"('",A170,"', ",C170,");"), IF(B170="Integer", CONCATENATE("$table-&gt;",LOWER(B170),"('",A170,"')-&gt;unsigned()-&gt;default(0);"), IF(B170="Text", CONCATENATE("$table-&gt;",LOWER(B170),"('",A170,"');"), IF(B170="Date", CONCATENATE("$table-&gt;","timestamp","('",A170,"');")) )))</f>
+      <c r="C175" s="42"/>
+      <c r="D175" s="43" t="str">
+        <f t="shared" ref="D175:D176" si="13">IF(B175="String", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"', ",C175,");"), IF(B175="Integer", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"')-&gt;unsigned()-&gt;default(0);"), IF(B175="Text", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"');"), IF(B175="Date", CONCATENATE("$table-&gt;","timestamp","('",A175,"');")) )))</f>
         <v>$table-&gt;timestamp('date');</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="42" t="s">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="B171" s="40" t="s">
+      <c r="B176" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C171" s="42"/>
-      <c r="D171" s="43" t="str">
+      <c r="C176" s="42"/>
+      <c r="D176" s="43" t="str">
         <f t="shared" si="13"/>
         <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="B172" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C172" s="42"/>
-      <c r="D172" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="B173" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C173" s="42"/>
-      <c r="D173" s="41" t="str">
-        <f t="shared" ref="D173" si="14">IF(B173="String", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"', ",C173,");"), IF(B173="Integer", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"')-&gt;unsigned()-&gt;default(0);"), IF(B173="Text", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"');"), IF(B173="Date", CONCATENATE("$table-&gt;","timestamp","('",A173,"');")) )))</f>
-        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="B174" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C174" s="42"/>
-      <c r="D174" s="15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="B175" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C175" s="42"/>
-      <c r="D175" s="41" t="str">
-        <f t="shared" ref="D175" si="15">IF(B175="String", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"', ",C175,");"), IF(B175="Integer", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"')-&gt;unsigned()-&gt;default(0);"), IF(B175="Text", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"');"), IF(B175="Date", CONCATENATE("$table-&gt;","timestamp","('",A175,"');")) )))</f>
-        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="B176" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C176" s="42"/>
-      <c r="D176" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="42" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B177" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C177" s="42"/>
-      <c r="D177" s="41" t="str">
-        <f t="shared" ref="D177" si="16">IF(B177="String", CONCATENATE("$table-&gt;",LOWER(B177),"('",A177,"', ",C177,");"), IF(B177="Integer", CONCATENATE("$table-&gt;",LOWER(B177),"('",A177,"')-&gt;unsigned()-&gt;default(0);"), IF(B177="Text", CONCATENATE("$table-&gt;",LOWER(B177),"('",A177,"');"), IF(B177="Date", CONCATENATE("$table-&gt;","timestamp","('",A177,"');")) )))</f>
-        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D177" s="15" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="42" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B178" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C178" s="42"/>
-      <c r="D178" s="15" t="s">
-        <v>131</v>
+      <c r="D178" s="41" t="str">
+        <f t="shared" ref="D178" si="14">IF(B178="String", CONCATENATE("$table-&gt;",LOWER(B178),"('",A178,"', ",C178,");"), IF(B178="Integer", CONCATENATE("$table-&gt;",LOWER(B178),"('",A178,"')-&gt;unsigned()-&gt;default(0);"), IF(B178="Text", CONCATENATE("$table-&gt;",LOWER(B178),"('",A178,"');"), IF(B178="Date", CONCATENATE("$table-&gt;","timestamp","('",A178,"');")) )))</f>
+        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="42" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B179" s="40" t="s">
         <v>104</v>
       </c>
       <c r="C179" s="42"/>
       <c r="D179" s="15" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="42" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B180" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C180" s="42">
-        <v>255</v>
-      </c>
-      <c r="D180" s="43" t="str">
-        <f>IF(B180="String", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"', ",C180,")-&gt;nullable();"), IF(B180="Integer", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"')-&gt;unsigned()-&gt;default(0);"), IF(B180="Text", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"');"), IF(B180="Date", CONCATENATE("$table-&gt;","timestamp","('",A180,"');")) )))</f>
-        <v>$table-&gt;string('position', 255)-&gt;nullable();</v>
+        <v>25</v>
+      </c>
+      <c r="C180" s="42"/>
+      <c r="D180" s="41" t="str">
+        <f t="shared" ref="D180" si="15">IF(B180="String", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"', ",C180,");"), IF(B180="Integer", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"')-&gt;unsigned()-&gt;default(0);"), IF(B180="Text", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"');"), IF(B180="Date", CONCATENATE("$table-&gt;","timestamp","('",A180,"');")) )))</f>
+        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B181" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C181" s="42"/>
+      <c r="D181" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B182" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C182" s="42"/>
+      <c r="D182" s="41" t="str">
+        <f t="shared" ref="D182" si="16">IF(B182="String", CONCATENATE("$table-&gt;",LOWER(B182),"('",A182,"', ",C182,");"), IF(B182="Integer", CONCATENATE("$table-&gt;",LOWER(B182),"('",A182,"')-&gt;unsigned()-&gt;default(0);"), IF(B182="Text", CONCATENATE("$table-&gt;",LOWER(B182),"('",A182,"');"), IF(B182="Date", CONCATENATE("$table-&gt;","timestamp","('",A182,"');")) )))</f>
+        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B183" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C183" s="42"/>
+      <c r="D183" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B184" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C184" s="42"/>
+      <c r="D184" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B185" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C185" s="42"/>
+      <c r="D185" s="41" t="str">
+        <f>IF(B185="String", CONCATENATE("$table-&gt;",LOWER(B185),"('",A185,"', ",C185,");"), IF(B185="Integer", CONCATENATE("$table-&gt;",LOWER(B185),"('",A185,"')-&gt;unsigned()-&gt;default(0);"), IF(B185="Text", CONCATENATE("$table-&gt;",LOWER(B185),"('",A185,"');"), IF(B185="Date", CONCATENATE("$table-&gt;","timestamp","('",A185,"');")) )))</f>
+        <v>$table-&gt;integer('discount')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B186" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C186" s="42">
+        <v>255</v>
+      </c>
+      <c r="D186" s="43" t="str">
+        <f>IF(B186="String", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"', ",C186,")-&gt;nullable();"), IF(B186="Integer", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"')-&gt;unsigned()-&gt;default(0);"), IF(B186="Text", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"');"), IF(B186="Date", CONCATENATE("$table-&gt;","timestamp","('",A186,"');")) )))</f>
+        <v>$table-&gt;string('position', 255)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B181" s="40" t="s">
+      <c r="B187" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C181" s="42"/>
-      <c r="D181" s="43" t="str">
-        <f>IF(B181="String", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"', ",C181,");"), IF(B181="Integer", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"')-&gt;unsigned()-&gt;default(0);"), IF(B181="Text", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"')-&gt;nullable();"), IF(B181="Date", CONCATENATE("$table-&gt;","timestamp","('",A181,"');")) )))</f>
+      <c r="C187" s="42"/>
+      <c r="D187" s="43" t="str">
+        <f>IF(B187="String", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"', ",C187,");"), IF(B187="Integer", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"')-&gt;unsigned()-&gt;default(0);"), IF(B187="Text", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"')-&gt;nullable();"), IF(B187="Date", CONCATENATE("$table-&gt;","timestamp","('",A187,"');")) )))</f>
         <v>$table-&gt;text('note')-&gt;nullable();</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A164:D165"/>
+    <mergeCell ref="A169:D170"/>
     <mergeCell ref="A142:D143"/>
     <mergeCell ref="A112:D113"/>
     <mergeCell ref="A135:D136"/>

</xml_diff>

<commit_message>
#5 Minor fixes ( ... )
:horse:
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -2059,7 +2059,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2094,7 +2094,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2305,8 +2305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3745,8 +3745,8 @@
       </c>
       <c r="C119" s="42"/>
       <c r="D119" s="43" t="str">
-        <f t="shared" si="6"/>
-        <v>$table-&gt;timestamp('date');</v>
+        <f>IF(B119="String", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"', ",C119,");"), IF(B119="Integer", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"')-&gt;unsigned()-&gt;default(0);"), IF(B119="Text", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"');"), IF(B119="Date", CONCATENATE("$table-&gt;","date","('",A119,"');")) )))</f>
+        <v>$table-&gt;date('date');</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -4055,8 +4055,8 @@
       </c>
       <c r="C148" s="42"/>
       <c r="D148" s="41" t="str">
-        <f t="shared" si="10"/>
-        <v>$table-&gt;timestamp('date');</v>
+        <f>IF(B148="String", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"', ",C148,");"), IF(B148="Integer", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"')-&gt;unsigned()-&gt;default(0);"), IF(B148="Text", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"');"), IF(B148="Date", CONCATENATE("$table-&gt;","date","('",A148,"');")) )))</f>
+        <v>$table-&gt;date('date');</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed login mechanism with username and password (before was with email)
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="143">
   <si>
     <t>PATIENT</t>
   </si>
@@ -458,6 +458,15 @@
   </si>
   <si>
     <t>desc_client</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>$table-&gt;string('username')-&gt;unique();</t>
+  </si>
+  <si>
+    <t>$table-&gt;string('email')-&gt;unique();</t>
   </si>
 </sst>
 </file>
@@ -621,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -747,6 +756,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1867,14 +1879,14 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table254687911" displayName="Table254687911" ref="A144:D166" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A144:D166"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table254687911" displayName="Table254687911" ref="A145:D167" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A145:D167"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="9"/>
     <tableColumn id="2" name="Type" dataDxfId="8"/>
     <tableColumn id="3" name="Length" dataDxfId="7"/>
     <tableColumn id="4" name="Code generated" dataDxfId="6">
-      <calculatedColumnFormula>IF(B145="String", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"', ",C145,");"), IF(B145="Integer", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"')-&gt;unsigned()-&gt;default(0);"), IF(B145="Text", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"');"), IF(B145="Date", CONCATENATE("$table-&gt;","timestamp","('",A145,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B146="String", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"', ",C146,");"), IF(B146="Integer", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"')-&gt;unsigned()-&gt;default(0);"), IF(B146="Text", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"');"), IF(B146="Date", CONCATENATE("$table-&gt;","timestamp","('",A146,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1882,14 +1894,14 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table254687912" displayName="Table254687912" ref="A171:D187" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A171:D187"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table254687912" displayName="Table254687912" ref="A172:D188" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A172:D188"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="3"/>
     <tableColumn id="2" name="Type" dataDxfId="2"/>
     <tableColumn id="3" name="Length" dataDxfId="1"/>
     <tableColumn id="4" name="Code generated" dataDxfId="0">
-      <calculatedColumnFormula>IF(B172="String", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"', ",C172,");"), IF(B172="Integer", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"')-&gt;unsigned()-&gt;default(0);"), IF(B172="Text", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"');"), IF(B172="Date", CONCATENATE("$table-&gt;","timestamp","('",A172,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B173="String", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"', ",C173,");"), IF(B173="Integer", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"')-&gt;unsigned()-&gt;default(0);"), IF(B173="Text", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"');"), IF(B173="Date", CONCATENATE("$table-&gt;","timestamp","('",A173,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1958,8 +1970,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A93:E103" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A93:E103"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A93:E104" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A93:E104"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Column name" dataDxfId="34"/>
     <tableColumn id="2" name="Type" dataDxfId="33"/>
@@ -1972,14 +1984,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A108:D110" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A108:D110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A109:D111" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A109:D111"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="27"/>
     <tableColumn id="2" name="Type" dataDxfId="26"/>
     <tableColumn id="3" name="Length" dataDxfId="25"/>
     <tableColumn id="4" name="Code generated" dataDxfId="24">
-      <calculatedColumnFormula>IF(B109="String", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"', ",C109,")-&gt;nullable();"), IF(B109="Integer", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"')-&gt;unsigned()-&gt;default(0);"), IF(B109="Text", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"');"), IF(B109="Date", CONCATENATE("$table-&gt;","timestamp","('",A109,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B110="String", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"', ",C110,")-&gt;nullable();"), IF(B110="Integer", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"')-&gt;unsigned()-&gt;default(0);"), IF(B110="Text", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"');"), IF(B110="Date", CONCATENATE("$table-&gt;","timestamp","('",A110,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1987,14 +1999,14 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table2546879" displayName="Table2546879" ref="A114:D133" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A114:D133"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table2546879" displayName="Table2546879" ref="A115:D134" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A115:D134"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="21"/>
     <tableColumn id="2" name="Type" dataDxfId="20"/>
     <tableColumn id="3" name="Length" dataDxfId="19"/>
     <tableColumn id="4" name="Code generated" dataDxfId="18">
-      <calculatedColumnFormula>IF(B115="String", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"', ",C115,");"), IF(B115="Integer", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"')-&gt;unsigned()-&gt;default(0);"), IF(B115="Text", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"');"), IF(B115="Date", CONCATENATE("$table-&gt;","timestamp","('",A115,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B116="String", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"', ",C116,");"), IF(B116="Integer", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"')-&gt;unsigned()-&gt;default(0);"), IF(B116="Text", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"');"), IF(B116="Date", CONCATENATE("$table-&gt;","timestamp","('",A116,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2002,14 +2014,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table254687910" displayName="Table254687910" ref="A137:D139" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A137:D139"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table254687910" displayName="Table254687910" ref="A138:D140" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A138:D140"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="15"/>
     <tableColumn id="2" name="Type" dataDxfId="14"/>
     <tableColumn id="3" name="Length" dataDxfId="13"/>
     <tableColumn id="4" name="Code generated" dataDxfId="12">
-      <calculatedColumnFormula>IF(B138="String", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"', ",C138,");"), IF(B138="Integer", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"')-&gt;unsigned()-&gt;default(0);"), IF(B138="Text", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"');"), IF(B138="Date", CONCATENATE("$table-&gt;","timestamp","('",A138,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B139="String", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"', ",C139,");"), IF(B139="Integer", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"')-&gt;unsigned()-&gt;default(0);"), IF(B139="Text", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"');"), IF(B139="Date", CONCATENATE("$table-&gt;","timestamp","('",A139,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2059,7 +2071,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2094,7 +2106,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2303,10 +2315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G187"/>
+  <dimension ref="A1:G188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="E115" sqref="E115"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3511,400 +3523,402 @@
         <v>255</v>
       </c>
       <c r="D98" s="13" t="str">
-        <f t="shared" ref="D98:D102" si="4">IF(B98="String", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"', ",C98,")-&gt;nullable();"), IF(B98="Integer", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"')-&gt;unsigned()-&gt;default(0);"), IF(B98="Text", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"');"), IF(B98="Date", CONCATENATE("$table-&gt;","timestamp","('",A98,"');")) )))</f>
+        <f t="shared" ref="D98:D103" si="4">IF(B98="String", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"', ",C98,")-&gt;nullable();"), IF(B98="Integer", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"')-&gt;unsigned()-&gt;default(0);"), IF(B98="Text", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"');"), IF(B98="Date", CONCATENATE("$table-&gt;","timestamp","('",A98,"');")) )))</f>
         <v>$table-&gt;string('last_name', 255)-&gt;nullable();</v>
       </c>
       <c r="E98" s="22"/>
       <c r="G98" s="12"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C99" s="8">
+      <c r="A99" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="B99" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="51">
         <v>200</v>
       </c>
-      <c r="D99" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>$table-&gt;string('email', 200)-&gt;nullable();</v>
+      <c r="D99" s="41" t="s">
+        <v>141</v>
       </c>
       <c r="E99" s="22"/>
       <c r="G99" s="12"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="22" t="s">
+      <c r="A100" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" s="8">
+        <v>200</v>
+      </c>
+      <c r="D100" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E100" s="22"/>
+      <c r="G100" s="12"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B100" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C100" s="22">
+      <c r="B101" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101" s="22">
         <v>255</v>
       </c>
-      <c r="D100" s="13" t="str">
+      <c r="D101" s="13" t="str">
         <f t="shared" si="4"/>
         <v>$table-&gt;string('address', 255)-&gt;nullable();</v>
       </c>
-      <c r="E100" s="22"/>
-      <c r="G100" s="12"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
+      <c r="E101" s="22"/>
+      <c r="G101" s="12"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B101" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C101" s="8">
+      <c r="B102" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C102" s="8">
         <v>50</v>
       </c>
-      <c r="D101" s="13" t="str">
+      <c r="D102" s="13" t="str">
         <f t="shared" si="4"/>
         <v>$table-&gt;string('phone', 50)-&gt;nullable();</v>
       </c>
-      <c r="E101" s="22"/>
-      <c r="G101" s="12"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
+      <c r="E102" s="22"/>
+      <c r="G102" s="12"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B102" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C102" s="8">
+      <c r="B103" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" s="8">
         <v>255</v>
       </c>
-      <c r="D102" s="13" t="str">
+      <c r="D103" s="13" t="str">
         <f t="shared" si="4"/>
         <v>$table-&gt;string('password', 255)-&gt;nullable();</v>
       </c>
-      <c r="E102" s="22"/>
-      <c r="G102" s="12"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B103" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C103" s="14"/>
-      <c r="D103" s="20" t="s">
-        <v>81</v>
-      </c>
       <c r="E103" s="22"/>
       <c r="G103" s="12"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="50" t="s">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C104" s="14"/>
+      <c r="D104" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E104" s="22"/>
+      <c r="G104" s="12"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="B106" s="50"/>
-      <c r="C106" s="50"/>
-      <c r="D106" s="50"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="50"/>
       <c r="B107" s="50"/>
       <c r="C107" s="50"/>
       <c r="D107" s="50"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="10" t="s">
+      <c r="A108" s="50"/>
+      <c r="B108" s="50"/>
+      <c r="C108" s="50"/>
+      <c r="D108" s="50"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B108" s="10" t="s">
+      <c r="B109" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C108" s="10" t="s">
+      <c r="C109" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D108" s="10" t="s">
+      <c r="D109" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B109" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C109" s="8">
+      <c r="B110" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110" s="8">
         <v>255</v>
       </c>
-      <c r="D109" s="13" t="str">
-        <f t="shared" ref="D109:D110" si="5">IF(B109="String", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"', ",C109,")-&gt;nullable();"), IF(B109="Integer", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"')-&gt;unsigned()-&gt;default(0);"), IF(B109="Text", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"');"), IF(B109="Date", CONCATENATE("$table-&gt;","timestamp","('",A109,"');")) )))</f>
+      <c r="D110" s="13" t="str">
+        <f t="shared" ref="D110:D111" si="5">IF(B110="String", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"', ",C110,")-&gt;nullable();"), IF(B110="Integer", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"')-&gt;unsigned()-&gt;default(0);"), IF(B110="Text", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"');"), IF(B110="Date", CONCATENATE("$table-&gt;","timestamp","('",A110,"');")) )))</f>
         <v>$table-&gt;string('status', 255)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="14"/>
-      <c r="B110" s="7"/>
-      <c r="C110" s="14"/>
-      <c r="D110" s="15" t="b">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="14"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="14"/>
+      <c r="D111" s="15" t="b">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="50" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="B112" s="50"/>
-      <c r="C112" s="50"/>
-      <c r="D112" s="50"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="50"/>
       <c r="B113" s="50"/>
       <c r="C113" s="50"/>
       <c r="D113" s="50"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="38" t="s">
+      <c r="A114" s="50"/>
+      <c r="B114" s="50"/>
+      <c r="C114" s="50"/>
+      <c r="D114" s="50"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B114" s="38" t="s">
+      <c r="B115" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C114" s="38" t="s">
+      <c r="C115" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D114" s="38" t="s">
+      <c r="D115" s="38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="8" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B115" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C115" s="8">
+      <c r="B116" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116" s="8">
         <v>50</v>
       </c>
-      <c r="D115" s="13" t="str">
-        <f>IF(B115="String", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"', ",C115,")-nullable();"), IF(B115="Integer", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"')-&gt;unsigned()-&gt;default(0);"), IF(B115="Text", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"');"), IF(B115="Date", CONCATENATE("$table-&gt;","timestamp","('",A115,"');")) )))</f>
+      <c r="D116" s="13" t="str">
+        <f>IF(B116="String", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"', ",C116,")-nullable();"), IF(B116="Integer", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"')-&gt;unsigned()-&gt;default(0);"), IF(B116="Text", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"');"), IF(B116="Date", CONCATENATE("$table-&gt;","timestamp","('",A116,"');")) )))</f>
         <v>$table-&gt;string('id_invoice', 50)-nullable();</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="14" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B116" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C116" s="14">
+      <c r="B117" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117" s="14">
         <v>50</v>
       </c>
-      <c r="D116" s="13" t="str">
-        <f t="shared" ref="D116:D121" si="6">IF(B116="String", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"', ",C116,");"), IF(B116="Integer", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"')-&gt;unsigned()-&gt;default(0);"), IF(B116="Text", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"');"), IF(B116="Date", CONCATENATE("$table-&gt;","timestamp","('",A116,"');")) )))</f>
+      <c r="D117" s="13" t="str">
+        <f t="shared" ref="D117:D122" si="6">IF(B117="String", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"', ",C117,");"), IF(B117="Integer", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"')-&gt;unsigned()-&gt;default(0);"), IF(B117="Text", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"');"), IF(B117="Date", CONCATENATE("$table-&gt;","timestamp","('",A117,"');")) )))</f>
         <v>$table-&gt;string('id_dentist', 50);</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="42" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B117" s="40" t="s">
+      <c r="B118" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C117" s="42"/>
-      <c r="D117" s="48" t="s">
+      <c r="C118" s="42"/>
+      <c r="D118" s="48" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="14" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B118" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C118" s="42">
+      <c r="B119" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119" s="42">
         <v>255</v>
       </c>
-      <c r="D118" s="43" t="str">
-        <f t="shared" ref="D118" si="7">IF(B118="String", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"', ",C118,");"), IF(B118="Integer", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"')-&gt;unsigned()-&gt;default(0);"), IF(B118="Text", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"');"), IF(B118="Date", CONCATENATE("$table-&gt;","timestamp","('",A118,"');")) )))</f>
+      <c r="D119" s="43" t="str">
+        <f t="shared" ref="D119" si="7">IF(B119="String", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"', ",C119,");"), IF(B119="Integer", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"')-&gt;unsigned()-&gt;default(0);"), IF(B119="Text", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"');"), IF(B119="Date", CONCATENATE("$table-&gt;","timestamp","('",A119,"');")) )))</f>
         <v>$table-&gt;string('detail', 255);</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="B119" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C119" s="42"/>
-      <c r="D119" s="43" t="str">
-        <f>IF(B119="String", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"', ",C119,");"), IF(B119="Integer", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"')-&gt;unsigned()-&gt;default(0);"), IF(B119="Text", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"');"), IF(B119="Date", CONCATENATE("$table-&gt;","date","('",A119,"');")) )))</f>
-        <v>$table-&gt;date('date');</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B120" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120" s="42"/>
+      <c r="D120" s="43" t="str">
+        <f>IF(B120="String", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"', ",C120,");"), IF(B120="Integer", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"')-&gt;unsigned()-&gt;default(0);"), IF(B120="Text", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"');"), IF(B120="Date", CONCATENATE("$table-&gt;","date","('",A120,"');")) )))</f>
+        <v>$table-&gt;date('date');</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="B120" s="40" t="s">
+      <c r="B121" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C120" s="42"/>
-      <c r="D120" s="41" t="str">
+      <c r="C121" s="42"/>
+      <c r="D121" s="41" t="str">
         <f t="shared" si="6"/>
         <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="42" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="B121" s="40" t="s">
+      <c r="B122" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C121" s="42"/>
-      <c r="D121" s="43" t="str">
+      <c r="C122" s="42"/>
+      <c r="D122" s="43" t="str">
         <f t="shared" si="6"/>
         <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="B122" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C122" s="42"/>
-      <c r="D122" s="43" t="s">
-        <v>123</v>
-      </c>
-    </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="42" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C123" s="42"/>
-      <c r="D123" s="41" t="str">
-        <f t="shared" ref="D123" si="8">IF(B123="String", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"', ",C123,");"), IF(B123="Integer", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"')-&gt;unsigned()-&gt;default(0);"), IF(B123="Text", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"');"), IF(B123="Date", CONCATENATE("$table-&gt;","timestamp","('",A123,"');")) )))</f>
-        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D123" s="43" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="42" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B124" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C124" s="42"/>
-      <c r="D124" s="43" t="s">
-        <v>122</v>
+      <c r="D124" s="41" t="str">
+        <f t="shared" ref="D124" si="8">IF(B124="String", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"', ",C124,");"), IF(B124="Integer", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"')-&gt;unsigned()-&gt;default(0);"), IF(B124="Text", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"');"), IF(B124="Date", CONCATENATE("$table-&gt;","timestamp","('",A124,"');")) )))</f>
+        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="42" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B125" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C125" s="42"/>
-      <c r="D125" s="41" t="str">
-        <f t="shared" ref="D125:D127" si="9">IF(B125="String", CONCATENATE("$table-&gt;",LOWER(B125),"('",A125,"', ",C125,");"), IF(B125="Integer", CONCATENATE("$table-&gt;",LOWER(B125),"('",A125,"')-&gt;unsigned()-&gt;default(0);"), IF(B125="Text", CONCATENATE("$table-&gt;",LOWER(B125),"('",A125,"');"), IF(B125="Date", CONCATENATE("$table-&gt;","timestamp","('",A125,"');")) )))</f>
-        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D125" s="43" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C126" s="42"/>
-      <c r="D126" s="43" t="s">
-        <v>121</v>
+      <c r="D126" s="41" t="str">
+        <f t="shared" ref="D126:D128" si="9">IF(B126="String", CONCATENATE("$table-&gt;",LOWER(B126),"('",A126,"', ",C126,");"), IF(B126="Integer", CONCATENATE("$table-&gt;",LOWER(B126),"('",A126,"')-&gt;unsigned()-&gt;default(0);"), IF(B126="Text", CONCATENATE("$table-&gt;",LOWER(B126),"('",A126,"');"), IF(B126="Date", CONCATENATE("$table-&gt;","timestamp","('",A126,"');")) )))</f>
+        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B127" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C127" s="42"/>
+      <c r="D127" s="43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="B127" s="40" t="s">
+      <c r="B128" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C127" s="42"/>
-      <c r="D127" s="41" t="str">
+      <c r="C128" s="42"/>
+      <c r="D128" s="41" t="str">
         <f t="shared" si="9"/>
         <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="B128" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C128" s="42"/>
-      <c r="D128" s="43" t="s">
-        <v>120</v>
-      </c>
-    </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B129" s="40" t="s">
         <v>104</v>
       </c>
       <c r="C129" s="42"/>
       <c r="D129" s="43" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="42" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B130" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C130" s="42">
-        <v>255</v>
-      </c>
-      <c r="D130" s="43" t="str">
-        <f>IF(B130="String", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"', ",C130,");"), IF(B130="Integer", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"')-&gt;unsigned()-&gt;default(0);"), IF(B130="Text", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"');"), IF(B130="Date", CONCATENATE("$table-&gt;","timestamp","('",A130,"');")) )))</f>
-        <v>$table-&gt;string('position', 255);</v>
+        <v>104</v>
+      </c>
+      <c r="C130" s="42"/>
+      <c r="D130" s="43" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B131" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C131" s="42"/>
+        <v>6</v>
+      </c>
+      <c r="C131" s="42">
+        <v>255</v>
+      </c>
       <c r="D131" s="43" t="str">
         <f>IF(B131="String", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"', ",C131,");"), IF(B131="Integer", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"')-&gt;unsigned()-&gt;default(0);"), IF(B131="Text", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"');"), IF(B131="Date", CONCATENATE("$table-&gt;","timestamp","('",A131,"');")) )))</f>
-        <v>$table-&gt;integer('object')-&gt;unsigned()-&gt;default(0);</v>
+        <v>$table-&gt;string('position', 255);</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B132" s="40" t="s">
         <v>25</v>
@@ -3912,301 +3926,299 @@
       <c r="C132" s="42"/>
       <c r="D132" s="43" t="str">
         <f>IF(B132="String", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"', ",C132,");"), IF(B132="Integer", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"')-&gt;unsigned()-&gt;default(0);"), IF(B132="Text", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"');"), IF(B132="Date", CONCATENATE("$table-&gt;","timestamp","('",A132,"');")) )))</f>
-        <v>$table-&gt;integer('type_operation')-&gt;unsigned()-&gt;default(0);</v>
+        <v>$table-&gt;integer('object')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="42" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="B133" s="40" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C133" s="42"/>
       <c r="D133" s="43" t="str">
         <f>IF(B133="String", CONCATENATE("$table-&gt;",LOWER(B133),"('",A133,"', ",C133,");"), IF(B133="Integer", CONCATENATE("$table-&gt;",LOWER(B133),"('",A133,"')-&gt;unsigned()-&gt;default(0);"), IF(B133="Text", CONCATENATE("$table-&gt;",LOWER(B133),"('",A133,"');"), IF(B133="Date", CONCATENATE("$table-&gt;","timestamp","('",A133,"');")) )))</f>
+        <v>$table-&gt;integer('type_operation')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B134" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C134" s="42"/>
+      <c r="D134" s="43" t="str">
+        <f>IF(B134="String", CONCATENATE("$table-&gt;",LOWER(B134),"('",A134,"', ",C134,");"), IF(B134="Integer", CONCATENATE("$table-&gt;",LOWER(B134),"('",A134,"')-&gt;unsigned()-&gt;default(0);"), IF(B134="Text", CONCATENATE("$table-&gt;",LOWER(B134),"('",A134,"');"), IF(B134="Date", CONCATENATE("$table-&gt;","timestamp","('",A134,"');")) )))</f>
         <v>$table-&gt;text('note');</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="42"/>
-      <c r="B134" s="44"/>
-      <c r="C134" s="42"/>
-      <c r="D134" s="45"/>
-    </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="50" t="s">
+      <c r="A135" s="42"/>
+      <c r="B135" s="44"/>
+      <c r="C135" s="42"/>
+      <c r="D135" s="45"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="B135" s="50"/>
-      <c r="C135" s="50"/>
-      <c r="D135" s="50"/>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="50"/>
       <c r="B136" s="50"/>
       <c r="C136" s="50"/>
       <c r="D136" s="50"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="38" t="s">
+      <c r="A137" s="50"/>
+      <c r="B137" s="50"/>
+      <c r="C137" s="50"/>
+      <c r="D137" s="50"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B137" s="38" t="s">
+      <c r="B138" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C137" s="38" t="s">
+      <c r="C138" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D137" s="38" t="s">
+      <c r="D138" s="38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="8" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B138" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C138" s="8">
+      <c r="B139" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139" s="8">
         <v>255</v>
       </c>
-      <c r="D138" s="13" t="str">
-        <f>IF(B138="String", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"', ",C138,");"), IF(B138="Integer", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"')-&gt;unsigned()-&gt;default(0);"), IF(B138="Text", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"');"), IF(B138="Date", CONCATENATE("$table-&gt;","timestamp","('",A138,"');")) )))</f>
+      <c r="D139" s="13" t="str">
+        <f>IF(B139="String", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"', ",C139,");"), IF(B139="Integer", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"')-&gt;unsigned()-&gt;default(0);"), IF(B139="Text", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"');"), IF(B139="Date", CONCATENATE("$table-&gt;","timestamp","('",A139,"');")) )))</f>
         <v>$table-&gt;string('category', 255);</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="50" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="B142" s="50"/>
-      <c r="C142" s="50"/>
-      <c r="D142" s="50"/>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="50"/>
       <c r="B143" s="50"/>
       <c r="C143" s="50"/>
       <c r="D143" s="50"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="39" t="s">
+      <c r="A144" s="50"/>
+      <c r="B144" s="50"/>
+      <c r="C144" s="50"/>
+      <c r="D144" s="50"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B144" s="39" t="s">
+      <c r="B145" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C144" s="39" t="s">
+      <c r="C145" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D144" s="39" t="s">
+      <c r="D145" s="39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="8" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B145" s="7" t="s">
+      <c r="B146" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C145" s="8"/>
-      <c r="D145" s="13" t="str">
-        <f t="shared" ref="D145:D150" si="10">IF(B145="String", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"', ",C145,");"), IF(B145="Integer", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"')-&gt;unsigned()-&gt;default(0);"), IF(B145="Text", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"');"), IF(B145="Date", CONCATENATE("$table-&gt;","timestamp","('",A145,"');")) )))</f>
+      <c r="C146" s="8"/>
+      <c r="D146" s="13" t="str">
+        <f t="shared" ref="D146:D151" si="10">IF(B146="String", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"', ",C146,");"), IF(B146="Integer", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"')-&gt;unsigned()-&gt;default(0);"), IF(B146="Text", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"');"), IF(B146="Date", CONCATENATE("$table-&gt;","timestamp","('",A146,"');")) )))</f>
         <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B146" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C146" s="42"/>
-      <c r="D146" s="43" t="str">
-        <f>IF(B146="String", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"', ",C146,");"), IF(B146="Integer", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"')-&gt;unsigned()-&gt;default(0);"), IF(B146="Text", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"');"), IF(B146="Date", CONCATENATE("$table-&gt;","timestamp","('",A146,"');")) )))</f>
-        <v>$table-&gt;integer('id_teeth_prizes')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B147" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C147" s="42"/>
+      <c r="D147" s="43" t="str">
+        <f>IF(B147="String", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"', ",C147,");"), IF(B147="Integer", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"')-&gt;unsigned()-&gt;default(0);"), IF(B147="Text", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"');"), IF(B147="Date", CONCATENATE("$table-&gt;","timestamp","('",A147,"');")) )))</f>
+        <v>$table-&gt;integer('id_teeth_prizes')-&gt;unsigned()-&gt;default(0);</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B147" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C147" s="42">
+      <c r="B148" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148" s="42">
         <v>50</v>
       </c>
-      <c r="D147" s="43" t="str">
+      <c r="D148" s="43" t="str">
         <f t="shared" si="10"/>
         <v>$table-&gt;string('id_dentist', 50);</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="B148" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C148" s="42"/>
-      <c r="D148" s="41" t="str">
-        <f>IF(B148="String", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"', ",C148,");"), IF(B148="Integer", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"')-&gt;unsigned()-&gt;default(0);"), IF(B148="Text", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"');"), IF(B148="Date", CONCATENATE("$table-&gt;","date","('",A148,"');")) )))</f>
-        <v>$table-&gt;date('date');</v>
-      </c>
-    </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B149" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C149" s="42"/>
+      <c r="D149" s="41" t="str">
+        <f>IF(B149="String", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"', ",C149,");"), IF(B149="Integer", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"')-&gt;unsigned()-&gt;default(0);"), IF(B149="Text", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"');"), IF(B149="Date", CONCATENATE("$table-&gt;","date","('",A149,"');")) )))</f>
+        <v>$table-&gt;date('date');</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="B149" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C149" s="42">
+      <c r="B150" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150" s="42">
         <v>255</v>
       </c>
-      <c r="D149" s="43" t="str">
+      <c r="D150" s="43" t="str">
         <f t="shared" si="10"/>
         <v>$table-&gt;string('teeth_no', 255);</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="42" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B150" s="40" t="s">
+      <c r="B151" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C150" s="42"/>
-      <c r="D150" s="43" t="str">
+      <c r="C151" s="42"/>
+      <c r="D151" s="43" t="str">
         <f t="shared" si="10"/>
         <v>$table-&gt;text('description');</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="B151" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C151" s="42">
-        <v>255</v>
-      </c>
-      <c r="D151" s="41" t="str">
-        <f>IF(B151="String", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"', ",C151,");"), IF(B151="Integer", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"')-&gt;unsigned()-&gt;default(0);"), IF(B151="Text", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"');"), IF(B151="Date", CONCATENATE("$table-&gt;","timestamp","('",A151,"');")) )))</f>
-        <v>$table-&gt;string('shortCode', 255);</v>
-      </c>
-    </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="42" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B152" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C152" s="42"/>
+        <v>6</v>
+      </c>
+      <c r="C152" s="42">
+        <v>255</v>
+      </c>
       <c r="D152" s="41" t="str">
         <f>IF(B152="String", CONCATENATE("$table-&gt;",LOWER(B152),"('",A152,"', ",C152,");"), IF(B152="Integer", CONCATENATE("$table-&gt;",LOWER(B152),"('",A152,"')-&gt;unsigned()-&gt;default(0);"), IF(B152="Text", CONCATENATE("$table-&gt;",LOWER(B152),"('",A152,"');"), IF(B152="Date", CONCATENATE("$table-&gt;","timestamp","('",A152,"');")) )))</f>
-        <v>$table-&gt;text('desc_client');</v>
+        <v>$table-&gt;string('shortCode', 255);</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="42" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="B153" s="40" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C153" s="42"/>
       <c r="D153" s="41" t="str">
-        <f t="shared" ref="D153:D161" si="11">IF(B153="String", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"', ",C153,");"), IF(B153="Integer", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"')-&gt;unsigned()-&gt;default(0);"), IF(B153="Text", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"');"), IF(B153="Date", CONCATENATE("$table-&gt;","timestamp","('",A153,"');")) )))</f>
-        <v>$table-&gt;integer('currency')-&gt;unsigned()-&gt;default(0);</v>
+        <f>IF(B153="String", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"', ",C153,");"), IF(B153="Integer", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"')-&gt;unsigned()-&gt;default(0);"), IF(B153="Text", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"');"), IF(B153="Date", CONCATENATE("$table-&gt;","timestamp","('",A153,"');")) )))</f>
+        <v>$table-&gt;text('desc_client');</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B154" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C154" s="42"/>
-      <c r="D154" s="43" t="s">
-        <v>115</v>
+      <c r="D154" s="41" t="str">
+        <f t="shared" ref="D154:D162" si="11">IF(B154="String", CONCATENATE("$table-&gt;",LOWER(B154),"('",A154,"', ",C154,");"), IF(B154="Integer", CONCATENATE("$table-&gt;",LOWER(B154),"('",A154,"')-&gt;unsigned()-&gt;default(0);"), IF(B154="Text", CONCATENATE("$table-&gt;",LOWER(B154),"('",A154,"');"), IF(B154="Date", CONCATENATE("$table-&gt;","timestamp","('",A154,"');")) )))</f>
+        <v>$table-&gt;integer('currency')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B155" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C155" s="42"/>
+      <c r="D155" s="43" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="B155" s="40" t="s">
+      <c r="B156" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C155" s="42"/>
-      <c r="D155" s="41" t="str">
+      <c r="C156" s="42"/>
+      <c r="D156" s="41" t="str">
         <f t="shared" si="11"/>
         <v>$table-&gt;integer('quantity')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B156" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C156" s="42"/>
-      <c r="D156" s="43" t="s">
-        <v>117</v>
-      </c>
-    </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="42" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="B157" s="40" t="s">
         <v>104</v>
       </c>
       <c r="C157" s="42"/>
       <c r="D157" s="43" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="42" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="B158" s="40" t="s">
         <v>104</v>
       </c>
       <c r="C158" s="42"/>
       <c r="D158" s="43" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="42" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C159" s="42">
-        <v>255</v>
-      </c>
-      <c r="D159" s="41" t="str">
-        <f>IF(B159="String", CONCATENATE("$table-&gt;",LOWER(B159),"('",A159,"', ",C159,");"), IF(B159="Integer", CONCATENATE("$table-&gt;",LOWER(B159),"('",A159,"')-&gt;unsigned()-&gt;default(0);"), IF(B159="Text", CONCATENATE("$table-&gt;",LOWER(B159),"('",A159,"');"), IF(B159="Date", CONCATENATE("$table-&gt;","timestamp","('",A159,"');")) )))</f>
-        <v>$table-&gt;string('type_cure', 255);</v>
+        <v>104</v>
+      </c>
+      <c r="C159" s="42"/>
+      <c r="D159" s="43" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B160" s="40" t="s">
         <v>6</v>
@@ -4216,39 +4228,48 @@
       </c>
       <c r="D160" s="41" t="str">
         <f>IF(B160="String", CONCATENATE("$table-&gt;",LOWER(B160),"('",A160,"', ",C160,");"), IF(B160="Integer", CONCATENATE("$table-&gt;",LOWER(B160),"('",A160,"')-&gt;unsigned()-&gt;default(0);"), IF(B160="Text", CONCATENATE("$table-&gt;",LOWER(B160),"('",A160,"');"), IF(B160="Date", CONCATENATE("$table-&gt;","timestamp","('",A160,"');")) )))</f>
-        <v>$table-&gt;string('status_cure', 255);</v>
+        <v>$table-&gt;string('type_cure', 255);</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B161" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C161" s="42">
+        <v>255</v>
+      </c>
+      <c r="D161" s="41" t="str">
+        <f>IF(B161="String", CONCATENATE("$table-&gt;",LOWER(B161),"('",A161,"', ",C161,");"), IF(B161="Integer", CONCATENATE("$table-&gt;",LOWER(B161),"('",A161,"')-&gt;unsigned()-&gt;default(0);"), IF(B161="Text", CONCATENATE("$table-&gt;",LOWER(B161),"('",A161,"');"), IF(B161="Date", CONCATENATE("$table-&gt;","timestamp","('",A161,"');")) )))</f>
+        <v>$table-&gt;string('status_cure', 255);</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="B161" s="40" t="s">
+      <c r="B162" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C161" s="42"/>
-      <c r="D161" s="43" t="str">
+      <c r="C162" s="42"/>
+      <c r="D162" s="43" t="str">
         <f t="shared" si="11"/>
         <v>$table-&gt;text('clicnic_note');</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="42" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="B162" s="40" t="s">
+      <c r="B163" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C162" s="42"/>
-      <c r="D162" s="43" t="s">
+      <c r="C163" s="42"/>
+      <c r="D163" s="43" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="42"/>
-      <c r="B163" s="40"/>
-      <c r="C163" s="42"/>
-      <c r="D163" s="43"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="42"/>
@@ -4268,255 +4289,261 @@
       <c r="C166" s="42"/>
       <c r="D166" s="43"/>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="50" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="42"/>
+      <c r="B167" s="40"/>
+      <c r="C167" s="42"/>
+      <c r="D167" s="43"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="B169" s="50"/>
-      <c r="C169" s="50"/>
-      <c r="D169" s="50"/>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="50"/>
       <c r="B170" s="50"/>
       <c r="C170" s="50"/>
       <c r="D170" s="50"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="46" t="s">
+      <c r="A171" s="50"/>
+      <c r="B171" s="50"/>
+      <c r="C171" s="50"/>
+      <c r="D171" s="50"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B171" s="46" t="s">
+      <c r="B172" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C171" s="46" t="s">
+      <c r="C172" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D171" s="46" t="s">
+      <c r="D172" s="46" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="42" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B172" s="40" t="s">
+      <c r="B173" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C172" s="42"/>
-      <c r="D172" s="48" t="s">
+      <c r="C173" s="42"/>
+      <c r="D173" s="48" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B173" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C173" s="14">
-        <v>255</v>
-      </c>
-      <c r="D173" s="47" t="str">
-        <f>IF(B173="String", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"', ",C173,")-&gt;nullable();"), IF(B173="Integer", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"')-&gt;unsigned()-&gt;default(0);"), IF(B173="Text", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"');"), IF(B173="Date", CONCATENATE("$table-&gt;","timestamp","('",A173,"');")) )))</f>
-        <v>$table-&gt;string('category', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174" s="14">
+        <v>255</v>
+      </c>
+      <c r="D174" s="47" t="str">
+        <f>IF(B174="String", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"', ",C174,")-&gt;nullable();"), IF(B174="Integer", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"')-&gt;unsigned()-&gt;default(0);"), IF(B174="Text", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"');"), IF(B174="Date", CONCATENATE("$table-&gt;","timestamp","('",A174,"');")) )))</f>
+        <v>$table-&gt;string('category', 255)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B174" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C174" s="42">
+      <c r="B175" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C175" s="42">
         <v>255</v>
       </c>
-      <c r="D174" s="43" t="str">
-        <f t="shared" ref="D174" si="12">IF(B174="String", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"', ",C174,");"), IF(B174="Integer", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"')-&gt;unsigned()-&gt;default(0);"), IF(B174="Text", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"');"), IF(B174="Date", CONCATENATE("$table-&gt;","timestamp","('",A174,"');")) )))</f>
+      <c r="D175" s="43" t="str">
+        <f t="shared" ref="D175" si="12">IF(B175="String", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"', ",C175,");"), IF(B175="Integer", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"')-&gt;unsigned()-&gt;default(0);"), IF(B175="Text", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"');"), IF(B175="Date", CONCATENATE("$table-&gt;","timestamp","('",A175,"');")) )))</f>
         <v>$table-&gt;string('detail', 255);</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="B175" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C175" s="42"/>
-      <c r="D175" s="43" t="str">
-        <f t="shared" ref="D175:D176" si="13">IF(B175="String", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"', ",C175,");"), IF(B175="Integer", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"')-&gt;unsigned()-&gt;default(0);"), IF(B175="Text", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"');"), IF(B175="Date", CONCATENATE("$table-&gt;","timestamp","('",A175,"');")) )))</f>
-        <v>$table-&gt;timestamp('date');</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="42" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B176" s="40" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C176" s="42"/>
       <c r="D176" s="43" t="str">
+        <f t="shared" ref="D176:D177" si="13">IF(B176="String", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"', ",C176,");"), IF(B176="Integer", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"')-&gt;unsigned()-&gt;default(0);"), IF(B176="Text", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"');"), IF(B176="Date", CONCATENATE("$table-&gt;","timestamp","('",A176,"');")) )))</f>
+        <v>$table-&gt;timestamp('date');</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B177" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C177" s="42"/>
+      <c r="D177" s="43" t="str">
         <f t="shared" si="13"/>
         <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="B177" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C177" s="42"/>
-      <c r="D177" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="42" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B178" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C178" s="42"/>
-      <c r="D178" s="41" t="str">
-        <f t="shared" ref="D178" si="14">IF(B178="String", CONCATENATE("$table-&gt;",LOWER(B178),"('",A178,"', ",C178,");"), IF(B178="Integer", CONCATENATE("$table-&gt;",LOWER(B178),"('",A178,"')-&gt;unsigned()-&gt;default(0);"), IF(B178="Text", CONCATENATE("$table-&gt;",LOWER(B178),"('",A178,"');"), IF(B178="Date", CONCATENATE("$table-&gt;","timestamp","('",A178,"');")) )))</f>
-        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D178" s="15" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="42" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B179" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C179" s="42"/>
-      <c r="D179" s="15" t="s">
-        <v>129</v>
+      <c r="D179" s="41" t="str">
+        <f t="shared" ref="D179" si="14">IF(B179="String", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"', ",C179,");"), IF(B179="Integer", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"')-&gt;unsigned()-&gt;default(0);"), IF(B179="Text", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"');"), IF(B179="Date", CONCATENATE("$table-&gt;","timestamp","('",A179,"');")) )))</f>
+        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="42" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B180" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C180" s="42"/>
-      <c r="D180" s="41" t="str">
-        <f t="shared" ref="D180" si="15">IF(B180="String", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"', ",C180,");"), IF(B180="Integer", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"')-&gt;unsigned()-&gt;default(0);"), IF(B180="Text", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"');"), IF(B180="Date", CONCATENATE("$table-&gt;","timestamp","('",A180,"');")) )))</f>
-        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D180" s="15" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B181" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C181" s="42"/>
-      <c r="D181" s="15" t="s">
-        <v>130</v>
+      <c r="D181" s="41" t="str">
+        <f t="shared" ref="D181" si="15">IF(B181="String", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"', ",C181,");"), IF(B181="Integer", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"')-&gt;unsigned()-&gt;default(0);"), IF(B181="Text", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"');"), IF(B181="Date", CONCATENATE("$table-&gt;","timestamp","('",A181,"');")) )))</f>
+        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B182" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C182" s="42"/>
-      <c r="D182" s="41" t="str">
-        <f t="shared" ref="D182" si="16">IF(B182="String", CONCATENATE("$table-&gt;",LOWER(B182),"('",A182,"', ",C182,");"), IF(B182="Integer", CONCATENATE("$table-&gt;",LOWER(B182),"('",A182,"')-&gt;unsigned()-&gt;default(0);"), IF(B182="Text", CONCATENATE("$table-&gt;",LOWER(B182),"('",A182,"');"), IF(B182="Date", CONCATENATE("$table-&gt;","timestamp","('",A182,"');")) )))</f>
-        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D182" s="15" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B183" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C183" s="42"/>
-      <c r="D183" s="15" t="s">
-        <v>131</v>
+      <c r="D183" s="41" t="str">
+        <f t="shared" ref="D183" si="16">IF(B183="String", CONCATENATE("$table-&gt;",LOWER(B183),"('",A183,"', ",C183,");"), IF(B183="Integer", CONCATENATE("$table-&gt;",LOWER(B183),"('",A183,"')-&gt;unsigned()-&gt;default(0);"), IF(B183="Text", CONCATENATE("$table-&gt;",LOWER(B183),"('",A183,"');"), IF(B183="Date", CONCATENATE("$table-&gt;","timestamp","('",A183,"');")) )))</f>
+        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B184" s="40" t="s">
         <v>104</v>
       </c>
       <c r="C184" s="42"/>
       <c r="D184" s="15" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="42" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="B185" s="40" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C185" s="42"/>
-      <c r="D185" s="41" t="str">
-        <f>IF(B185="String", CONCATENATE("$table-&gt;",LOWER(B185),"('",A185,"', ",C185,");"), IF(B185="Integer", CONCATENATE("$table-&gt;",LOWER(B185),"('",A185,"')-&gt;unsigned()-&gt;default(0);"), IF(B185="Text", CONCATENATE("$table-&gt;",LOWER(B185),"('",A185,"');"), IF(B185="Date", CONCATENATE("$table-&gt;","timestamp","('",A185,"');")) )))</f>
-        <v>$table-&gt;integer('discount')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D185" s="15" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="42" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="B186" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C186" s="42">
-        <v>255</v>
-      </c>
-      <c r="D186" s="43" t="str">
-        <f>IF(B186="String", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"', ",C186,")-&gt;nullable();"), IF(B186="Integer", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"')-&gt;unsigned()-&gt;default(0);"), IF(B186="Text", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"');"), IF(B186="Date", CONCATENATE("$table-&gt;","timestamp","('",A186,"');")) )))</f>
-        <v>$table-&gt;string('position', 255)-&gt;nullable();</v>
+        <v>25</v>
+      </c>
+      <c r="C186" s="42"/>
+      <c r="D186" s="41" t="str">
+        <f>IF(B186="String", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"', ",C186,");"), IF(B186="Integer", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"')-&gt;unsigned()-&gt;default(0);"), IF(B186="Text", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"');"), IF(B186="Date", CONCATENATE("$table-&gt;","timestamp","('",A186,"');")) )))</f>
+        <v>$table-&gt;integer('discount')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B187" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C187" s="42">
+        <v>255</v>
+      </c>
+      <c r="D187" s="43" t="str">
+        <f>IF(B187="String", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"', ",C187,")-&gt;nullable();"), IF(B187="Integer", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"')-&gt;unsigned()-&gt;default(0);"), IF(B187="Text", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"');"), IF(B187="Date", CONCATENATE("$table-&gt;","timestamp","('",A187,"');")) )))</f>
+        <v>$table-&gt;string('position', 255)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B187" s="40" t="s">
+      <c r="B188" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C187" s="42"/>
-      <c r="D187" s="43" t="str">
-        <f>IF(B187="String", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"', ",C187,");"), IF(B187="Integer", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"')-&gt;unsigned()-&gt;default(0);"), IF(B187="Text", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"')-&gt;nullable();"), IF(B187="Date", CONCATENATE("$table-&gt;","timestamp","('",A187,"');")) )))</f>
+      <c r="C188" s="42"/>
+      <c r="D188" s="43" t="str">
+        <f>IF(B188="String", CONCATENATE("$table-&gt;",LOWER(B188),"('",A188,"', ",C188,");"), IF(B188="Integer", CONCATENATE("$table-&gt;",LOWER(B188),"('",A188,"')-&gt;unsigned()-&gt;default(0);"), IF(B188="Text", CONCATENATE("$table-&gt;",LOWER(B188),"('",A188,"')-&gt;nullable();"), IF(B188="Date", CONCATENATE("$table-&gt;","timestamp","('",A188,"');")) )))</f>
         <v>$table-&gt;text('note')-&gt;nullable();</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A169:D170"/>
-    <mergeCell ref="A142:D143"/>
-    <mergeCell ref="A112:D113"/>
-    <mergeCell ref="A135:D136"/>
-    <mergeCell ref="A106:D107"/>
     <mergeCell ref="A91:D92"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A55:D56"/>
     <mergeCell ref="A63:D64"/>
     <mergeCell ref="A73:D74"/>
     <mergeCell ref="A81:D82"/>
+    <mergeCell ref="A170:D171"/>
+    <mergeCell ref="A143:D144"/>
+    <mergeCell ref="A113:D114"/>
+    <mergeCell ref="A136:D137"/>
+    <mergeCell ref="A107:D108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
#7 Done, each patient can have more than one chart, each chart is related with the cures :top:
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="147">
   <si>
     <t>PATIENT</t>
   </si>
@@ -367,9 +367,6 @@
     <t>type_operation</t>
   </si>
   <si>
-    <t>JobsDetail</t>
-  </si>
-  <si>
     <t>id_job</t>
   </si>
   <si>
@@ -467,13 +464,28 @@
   </si>
   <si>
     <t>$table-&gt;string('email')-&gt;unique();</t>
+  </si>
+  <si>
+    <t>id_user</t>
+  </si>
+  <si>
+    <t>Chart</t>
+  </si>
+  <si>
+    <t>$table-&gt;integer('id_user')-&gt;nullable();</t>
+  </si>
+  <si>
+    <t>id_chart</t>
+  </si>
+  <si>
+    <t>$table-&gt;integer('id_chart')-&gt;unsigned();</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,6 +546,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <name val="Courier New"/>
       <family val="3"/>
@@ -630,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -753,11 +771,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2317,8 +2338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,22 +2352,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3056,18 +3077,18 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="50" t="s">
+      <c r="A55" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="52"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="50"/>
-      <c r="B56" s="50"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="50"/>
+      <c r="A56" s="52"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -3144,18 +3165,18 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="50" t="s">
+      <c r="A63" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="50"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="50"/>
+      <c r="B63" s="52"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="52"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="50"/>
-      <c r="B64" s="50"/>
-      <c r="C64" s="50"/>
-      <c r="D64" s="50"/>
+      <c r="A64" s="52"/>
+      <c r="B64" s="52"/>
+      <c r="C64" s="52"/>
+      <c r="D64" s="52"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
@@ -3218,7 +3239,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B69" s="17" t="s">
         <v>6</v>
@@ -3253,18 +3274,18 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="50" t="s">
+      <c r="A73" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="B73" s="50"/>
-      <c r="C73" s="50"/>
-      <c r="D73" s="50"/>
+      <c r="B73" s="52"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="52"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="50"/>
-      <c r="B74" s="50"/>
-      <c r="C74" s="50"/>
-      <c r="D74" s="50"/>
+      <c r="A74" s="52"/>
+      <c r="B74" s="52"/>
+      <c r="C74" s="52"/>
+      <c r="D74" s="52"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
@@ -3303,18 +3324,18 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="50" t="s">
+      <c r="A81" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B81" s="50"/>
-      <c r="C81" s="50"/>
-      <c r="D81" s="50"/>
+      <c r="B81" s="52"/>
+      <c r="C81" s="52"/>
+      <c r="D81" s="52"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="50"/>
-      <c r="B82" s="50"/>
-      <c r="C82" s="50"/>
-      <c r="D82" s="50"/>
+      <c r="A82" s="52"/>
+      <c r="B82" s="52"/>
+      <c r="C82" s="52"/>
+      <c r="D82" s="52"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
@@ -3418,18 +3439,18 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="50" t="s">
+      <c r="A91" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="B91" s="50"/>
-      <c r="C91" s="50"/>
-      <c r="D91" s="50"/>
+      <c r="B91" s="52"/>
+      <c r="C91" s="52"/>
+      <c r="D91" s="52"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="50"/>
-      <c r="B92" s="50"/>
-      <c r="C92" s="50"/>
-      <c r="D92" s="50"/>
+      <c r="A92" s="52"/>
+      <c r="B92" s="52"/>
+      <c r="C92" s="52"/>
+      <c r="D92" s="52"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
@@ -3530,17 +3551,17 @@
       <c r="G98" s="12"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="51" t="s">
+      <c r="A99" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="B99" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="50">
+        <v>200</v>
+      </c>
+      <c r="D99" s="41" t="s">
         <v>140</v>
-      </c>
-      <c r="B99" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C99" s="51">
-        <v>200</v>
-      </c>
-      <c r="D99" s="41" t="s">
-        <v>141</v>
       </c>
       <c r="E99" s="22"/>
       <c r="G99" s="12"/>
@@ -3556,7 +3577,7 @@
         <v>200</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E100" s="22"/>
       <c r="G100" s="12"/>
@@ -3627,18 +3648,18 @@
       <c r="G104" s="12"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="50" t="s">
+      <c r="A107" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="B107" s="50"/>
-      <c r="C107" s="50"/>
-      <c r="D107" s="50"/>
+      <c r="B107" s="52"/>
+      <c r="C107" s="52"/>
+      <c r="D107" s="52"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="50"/>
-      <c r="B108" s="50"/>
-      <c r="C108" s="50"/>
-      <c r="D108" s="50"/>
+      <c r="A108" s="52"/>
+      <c r="B108" s="52"/>
+      <c r="C108" s="52"/>
+      <c r="D108" s="52"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="s">
@@ -3679,18 +3700,18 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="B113" s="50"/>
-      <c r="C113" s="50"/>
-      <c r="D113" s="50"/>
+      <c r="A113" s="52" t="s">
+        <v>143</v>
+      </c>
+      <c r="B113" s="52"/>
+      <c r="C113" s="52"/>
+      <c r="D113" s="52"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="50"/>
-      <c r="B114" s="50"/>
-      <c r="C114" s="50"/>
-      <c r="D114" s="50"/>
+      <c r="A114" s="52"/>
+      <c r="B114" s="52"/>
+      <c r="C114" s="52"/>
+      <c r="D114" s="52"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="38" t="s">
@@ -3723,7 +3744,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>7</v>
+        <v>142</v>
       </c>
       <c r="B117" s="7" t="s">
         <v>6</v>
@@ -3731,9 +3752,8 @@
       <c r="C117" s="14">
         <v>50</v>
       </c>
-      <c r="D117" s="13" t="str">
-        <f t="shared" ref="D117:D122" si="6">IF(B117="String", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"', ",C117,");"), IF(B117="Integer", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"')-&gt;unsigned()-&gt;default(0);"), IF(B117="Text", CONCATENATE("$table-&gt;",LOWER(B117),"('",A117,"');"), IF(B117="Date", CONCATENATE("$table-&gt;","timestamp","('",A117,"');")) )))</f>
-        <v>$table-&gt;string('id_dentist', 50);</v>
+      <c r="D117" s="51" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3745,12 +3765,12 @@
       </c>
       <c r="C118" s="42"/>
       <c r="D118" s="48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B119" s="7" t="s">
         <v>6</v>
@@ -3759,13 +3779,13 @@
         <v>255</v>
       </c>
       <c r="D119" s="43" t="str">
-        <f t="shared" ref="D119" si="7">IF(B119="String", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"', ",C119,");"), IF(B119="Integer", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"')-&gt;unsigned()-&gt;default(0);"), IF(B119="Text", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"');"), IF(B119="Date", CONCATENATE("$table-&gt;","timestamp","('",A119,"');")) )))</f>
+        <f t="shared" ref="D119" si="6">IF(B119="String", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"', ",C119,");"), IF(B119="Integer", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"')-&gt;unsigned()-&gt;default(0);"), IF(B119="Text", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"');"), IF(B119="Date", CONCATENATE("$table-&gt;","timestamp","('",A119,"');")) )))</f>
         <v>$table-&gt;string('detail', 255);</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B120" s="40" t="s">
         <v>15</v>
@@ -3778,14 +3798,14 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B121" s="40" t="s">
         <v>25</v>
       </c>
       <c r="C121" s="42"/>
       <c r="D121" s="41" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D121:D122" si="7">IF(B121="String", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"', ",C121,");"), IF(B121="Integer", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"')-&gt;unsigned()-&gt;default(0);"), IF(B121="Text", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"');"), IF(B121="Date", CONCATENATE("$table-&gt;","timestamp","('",A121,"');")) )))</f>
         <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
@@ -3798,7 +3818,7 @@
       </c>
       <c r="C122" s="42"/>
       <c r="D122" s="43" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
@@ -3811,7 +3831,7 @@
       </c>
       <c r="C123" s="42"/>
       <c r="D123" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3836,7 +3856,7 @@
       </c>
       <c r="C125" s="42"/>
       <c r="D125" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3861,7 +3881,7 @@
       </c>
       <c r="C127" s="42"/>
       <c r="D127" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3886,7 +3906,7 @@
       </c>
       <c r="C129" s="42"/>
       <c r="D129" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3962,18 +3982,18 @@
       <c r="D135" s="45"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="50" t="s">
+      <c r="A136" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="B136" s="50"/>
-      <c r="C136" s="50"/>
-      <c r="D136" s="50"/>
+      <c r="B136" s="52"/>
+      <c r="C136" s="52"/>
+      <c r="D136" s="52"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="50"/>
-      <c r="B137" s="50"/>
-      <c r="C137" s="50"/>
-      <c r="D137" s="50"/>
+      <c r="A137" s="52"/>
+      <c r="B137" s="52"/>
+      <c r="C137" s="52"/>
+      <c r="D137" s="52"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="38" t="s">
@@ -4005,18 +4025,18 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="50" t="s">
+      <c r="A143" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="B143" s="50"/>
-      <c r="C143" s="50"/>
-      <c r="D143" s="50"/>
+      <c r="B143" s="52"/>
+      <c r="C143" s="52"/>
+      <c r="D143" s="52"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="50"/>
-      <c r="B144" s="50"/>
-      <c r="C144" s="50"/>
-      <c r="D144" s="50"/>
+      <c r="A144" s="52"/>
+      <c r="B144" s="52"/>
+      <c r="C144" s="52"/>
+      <c r="D144" s="52"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="39" t="s">
@@ -4034,7 +4054,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B146" s="7" t="s">
         <v>25</v>
@@ -4047,7 +4067,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B147" s="40" t="s">
         <v>25</v>
@@ -4075,7 +4095,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B149" s="40" t="s">
         <v>15</v>
@@ -4088,7 +4108,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B150" s="40" t="s">
         <v>6</v>
@@ -4116,7 +4136,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B152" s="40" t="s">
         <v>6</v>
@@ -4131,7 +4151,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B153" s="40" t="s">
         <v>31</v>
@@ -4144,7 +4164,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B154" s="40" t="s">
         <v>25</v>
@@ -4157,26 +4177,26 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B155" s="40" t="s">
         <v>104</v>
       </c>
       <c r="C155" s="42"/>
       <c r="D155" s="43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B156" s="40" t="s">
         <v>25</v>
       </c>
       <c r="C156" s="42"/>
       <c r="D156" s="41" t="str">
-        <f t="shared" si="11"/>
+        <f>IF(B156="String", CONCATENATE("$table-&gt;",LOWER(B156),"('",A156,"', ",C156,");"), IF(B156="Integer", CONCATENATE("$table-&gt;",LOWER(B156),"('",A156,"')-&gt;unsigned()-&gt;default(0);"), IF(B156="Text", CONCATENATE("$table-&gt;",LOWER(B156),"('",A156,"');"), IF(B156="Date", CONCATENATE("$table-&gt;","timestamp","('",A156,"');")) )))</f>
         <v>$table-&gt;integer('quantity')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
@@ -4189,7 +4209,7 @@
       </c>
       <c r="C157" s="42"/>
       <c r="D157" s="43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -4206,19 +4226,19 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B159" s="40" t="s">
         <v>104</v>
       </c>
       <c r="C159" s="42"/>
       <c r="D159" s="43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B160" s="40" t="s">
         <v>6</v>
@@ -4233,7 +4253,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B161" s="40" t="s">
         <v>6</v>
@@ -4248,7 +4268,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B162" s="40" t="s">
         <v>31</v>
@@ -4261,7 +4281,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B163" s="40" t="s">
         <v>31</v>
@@ -4272,10 +4292,16 @@
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="42"/>
-      <c r="B164" s="40"/>
+      <c r="A164" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="C164" s="42"/>
-      <c r="D164" s="43"/>
+      <c r="D164" s="41" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="42"/>
@@ -4296,18 +4322,18 @@
       <c r="D167" s="43"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="50" t="s">
-        <v>125</v>
-      </c>
-      <c r="B170" s="50"/>
-      <c r="C170" s="50"/>
-      <c r="D170" s="50"/>
+      <c r="A170" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B170" s="52"/>
+      <c r="C170" s="52"/>
+      <c r="D170" s="52"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="50"/>
-      <c r="B171" s="50"/>
-      <c r="C171" s="50"/>
-      <c r="D171" s="50"/>
+      <c r="A171" s="52"/>
+      <c r="B171" s="52"/>
+      <c r="C171" s="52"/>
+      <c r="D171" s="52"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="46" t="s">
@@ -4332,7 +4358,7 @@
       </c>
       <c r="C173" s="42"/>
       <c r="D173" s="48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4352,7 +4378,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B175" s="7" t="s">
         <v>6</v>
@@ -4367,7 +4393,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B176" s="40" t="s">
         <v>15</v>
@@ -4400,7 +4426,7 @@
       </c>
       <c r="C178" s="42"/>
       <c r="D178" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4425,7 +4451,7 @@
       </c>
       <c r="C180" s="42"/>
       <c r="D180" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4450,7 +4476,7 @@
       </c>
       <c r="C182" s="42"/>
       <c r="D182" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4475,7 +4501,7 @@
       </c>
       <c r="C184" s="42"/>
       <c r="D184" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4487,7 +4513,7 @@
       </c>
       <c r="C185" s="42"/>
       <c r="D185" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
#9 & #10 Bless Up :pray:
</commit_message>
<xml_diff>
--- a/todo/database-tables.xlsx
+++ b/todo/database-tables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="146">
   <si>
     <t>PATIENT</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>note4</t>
-  </si>
-  <si>
-    <t>note5</t>
   </si>
   <si>
     <t>sms_notify_news</t>
@@ -1884,8 +1881,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E53" totalsRowShown="0">
-  <autoFilter ref="A4:E53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E52" totalsRowShown="0">
+  <autoFilter ref="A4:E52"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type"/>
@@ -1900,14 +1897,14 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table254687911" displayName="Table254687911" ref="A145:D167" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A145:D167"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table254687911" displayName="Table254687911" ref="A144:D166" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A144:D166"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="9"/>
     <tableColumn id="2" name="Type" dataDxfId="8"/>
     <tableColumn id="3" name="Length" dataDxfId="7"/>
     <tableColumn id="4" name="Code generated" dataDxfId="6">
-      <calculatedColumnFormula>IF(B146="String", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"', ",C146,");"), IF(B146="Integer", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"')-&gt;unsigned()-&gt;default(0);"), IF(B146="Text", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"');"), IF(B146="Date", CONCATENATE("$table-&gt;","timestamp","('",A146,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B145="String", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"', ",C145,");"), IF(B145="Integer", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"')-&gt;unsigned()-&gt;default(0);"), IF(B145="Text", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"');"), IF(B145="Date", CONCATENATE("$table-&gt;","timestamp","('",A145,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1915,14 +1912,14 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table254687912" displayName="Table254687912" ref="A172:D188" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A172:D188"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table254687912" displayName="Table254687912" ref="A171:D187" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A171:D187"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="3"/>
     <tableColumn id="2" name="Type" dataDxfId="2"/>
     <tableColumn id="3" name="Length" dataDxfId="1"/>
     <tableColumn id="4" name="Code generated" dataDxfId="0">
-      <calculatedColumnFormula>IF(B173="String", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"', ",C173,");"), IF(B173="Integer", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"')-&gt;unsigned()-&gt;default(0);"), IF(B173="Text", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"');"), IF(B173="Date", CONCATENATE("$table-&gt;","timestamp","('",A173,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B172="String", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"', ",C172,");"), IF(B172="Integer", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"')-&gt;unsigned()-&gt;default(0);"), IF(B172="Text", CONCATENATE("$table-&gt;",LOWER(B172),"('",A172,"');"), IF(B172="Date", CONCATENATE("$table-&gt;","timestamp","('",A172,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1930,14 +1927,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A57:D61" totalsRowShown="0" headerRowDxfId="52">
-  <autoFilter ref="A57:D61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A56:D60" totalsRowShown="0" headerRowDxfId="52">
+  <autoFilter ref="A56:D60"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type" dataDxfId="51"/>
     <tableColumn id="3" name="Length"/>
     <tableColumn id="4" name="Code generated" dataDxfId="50">
-      <calculatedColumnFormula>IF(B58="String", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"', ",C58,")-&gt;nullable();"), IF(B58="Integer", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"')-&gt;unsigned()-&gt;default(0);"), IF(B58="Text", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');"), IF(B58="Date", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B57="String", CONCATENATE("$table-&gt;",LOWER(B57),"('",A57,"', ",C57,")-&gt;nullable();"), IF(B57="Integer", CONCATENATE("$table-&gt;",LOWER(B57),"('",A57,"')-&gt;unsigned()-&gt;default(0);"), IF(B57="Text", CONCATENATE("$table-&gt;",LOWER(B57),"('",A57,"');"), IF(B57="Date", CONCATENATE("$table-&gt;",LOWER(B57),"('",A57,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1945,14 +1942,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A65:D71" totalsRowShown="0" headerRowDxfId="49">
-  <autoFilter ref="A65:D71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A64:D70" totalsRowShown="0" headerRowDxfId="49">
+  <autoFilter ref="A64:D70"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type" dataDxfId="48"/>
     <tableColumn id="3" name="Length"/>
     <tableColumn id="4" name="Code generated" dataDxfId="47">
-      <calculatedColumnFormula>IF(B66="String", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"', ",C66,")-&gt;nullable();"), IF(B66="Integer", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"')-&gt;unsigned()-&gt;default(0);"), IF(B66="Text", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');"), IF(B66="Date", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B65="String", CONCATENATE("$table-&gt;",LOWER(B65),"('",A65,"', ",C65,")-&gt;nullable();"), IF(B65="Integer", CONCATENATE("$table-&gt;",LOWER(B65),"('",A65,"')-&gt;unsigned()-&gt;default(0);"), IF(B65="Text", CONCATENATE("$table-&gt;",LOWER(B65),"('",A65,"');"), IF(B65="Date", CONCATENATE("$table-&gt;",LOWER(B65),"('",A65,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1960,14 +1957,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A75:D77" totalsRowShown="0" headerRowDxfId="46">
-  <autoFilter ref="A75:D77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table254" displayName="Table254" ref="A74:D76" totalsRowShown="0" headerRowDxfId="46">
+  <autoFilter ref="A74:D76"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Type" dataDxfId="45"/>
     <tableColumn id="3" name="Length"/>
     <tableColumn id="4" name="Code generated" dataDxfId="44">
-      <calculatedColumnFormula>IF(B76="String", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"', ",C76,")-&gt;nullable();"), IF(B76="Integer", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"')-&gt;unsigned()-&gt;default(0);"), IF(B76="Text", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"');"), IF(B76="Date", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B75="String", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"', ",C75,")-&gt;nullable();"), IF(B75="Integer", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"')-&gt;unsigned()-&gt;default(0);"), IF(B75="Text", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');"), IF(B75="Date", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1975,14 +1972,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A83:E89" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A83:E89"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2546" displayName="Table2546" ref="A82:E88" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A82:E88"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Column name" dataDxfId="41"/>
     <tableColumn id="2" name="Type" dataDxfId="40"/>
     <tableColumn id="3" name="Length" dataDxfId="39"/>
     <tableColumn id="4" name="Code generated" dataDxfId="38">
-      <calculatedColumnFormula>IF(B84="String", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"', ",C84,");"), IF(B84="Integer", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"')-&gt;unsigned()-&gt;default(0);"), IF(B84="Text", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"');"), IF(B84="Date", CONCATENATE("$table-&gt;","timestamp","('",A84,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B83="String", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"', ",C83,");"), IF(B83="Integer", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"')-&gt;unsigned()-&gt;default(0);"), IF(B83="Text", CONCATENATE("$table-&gt;",LOWER(B83),"('",A83,"');"), IF(B83="Date", CONCATENATE("$table-&gt;","timestamp","('",A83,"');")) )))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Type Column" dataDxfId="37"/>
   </tableColumns>
@@ -1991,8 +1988,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A93:E104" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A93:E104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table25468" displayName="Table25468" ref="A92:E103" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A92:E103"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Column name" dataDxfId="34"/>
     <tableColumn id="2" name="Type" dataDxfId="33"/>
@@ -2005,14 +2002,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A109:D111" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A109:D111"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table254687" displayName="Table254687" ref="A108:D110" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A108:D110"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="27"/>
     <tableColumn id="2" name="Type" dataDxfId="26"/>
     <tableColumn id="3" name="Length" dataDxfId="25"/>
     <tableColumn id="4" name="Code generated" dataDxfId="24">
-      <calculatedColumnFormula>IF(B110="String", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"', ",C110,")-&gt;nullable();"), IF(B110="Integer", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"')-&gt;unsigned()-&gt;default(0);"), IF(B110="Text", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"');"), IF(B110="Date", CONCATENATE("$table-&gt;","timestamp","('",A110,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B109="String", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"', ",C109,")-&gt;nullable();"), IF(B109="Integer", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"')-&gt;unsigned()-&gt;default(0);"), IF(B109="Text", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"');"), IF(B109="Date", CONCATENATE("$table-&gt;","timestamp","('",A109,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2020,14 +2017,14 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table2546879" displayName="Table2546879" ref="A115:D134" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A115:D134"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table2546879" displayName="Table2546879" ref="A114:D133" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A114:D133"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="21"/>
     <tableColumn id="2" name="Type" dataDxfId="20"/>
     <tableColumn id="3" name="Length" dataDxfId="19"/>
     <tableColumn id="4" name="Code generated" dataDxfId="18">
-      <calculatedColumnFormula>IF(B116="String", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"', ",C116,");"), IF(B116="Integer", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"')-&gt;unsigned()-&gt;default(0);"), IF(B116="Text", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"');"), IF(B116="Date", CONCATENATE("$table-&gt;","timestamp","('",A116,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B115="String", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"', ",C115,");"), IF(B115="Integer", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"')-&gt;unsigned()-&gt;default(0);"), IF(B115="Text", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"');"), IF(B115="Date", CONCATENATE("$table-&gt;","timestamp","('",A115,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2035,14 +2032,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table254687910" displayName="Table254687910" ref="A138:D140" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A138:D140"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table254687910" displayName="Table254687910" ref="A137:D139" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A137:D139"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Column name" dataDxfId="15"/>
     <tableColumn id="2" name="Type" dataDxfId="14"/>
     <tableColumn id="3" name="Length" dataDxfId="13"/>
     <tableColumn id="4" name="Code generated" dataDxfId="12">
-      <calculatedColumnFormula>IF(B139="String", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"', ",C139,");"), IF(B139="Integer", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"')-&gt;unsigned()-&gt;default(0);"), IF(B139="Text", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"');"), IF(B139="Date", CONCATENATE("$table-&gt;","timestamp","('",A139,"');")) )))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(B138="String", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"', ",C138,");"), IF(B138="Integer", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"')-&gt;unsigned()-&gt;default(0);"), IF(B138="Text", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"');"), IF(B138="Date", CONCATENATE("$table-&gt;","timestamp","('",A138,"');")) )))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2336,10 +2333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G188"/>
+  <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="D164" sqref="D164"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,7 +2380,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2401,7 +2398,7 @@
         <v>$table-&gt;string('id_patient', 50);</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2523,7 +2520,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -2538,7 +2535,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -2553,7 +2550,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -2688,7 +2685,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -2701,12 +2698,12 @@
         <v>$table-&gt;string('image_path', 255)-&gt;nullable();</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -2817,7 +2814,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
         <v>25</v>
@@ -3024,11 +3021,14 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>6</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
       </c>
       <c r="D50" t="str">
         <f>IF(B50="String", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"', ",C50,")-&gt;nullable();"), IF(B50="Integer", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"')-&gt;unsigned()-&gt;default(0);"), IF(B50="Text", CONCATENATE("$table-&gt;",LOWER(B50),"('",A50,"')-&gt;nullable();"), IF(B50="Date", CONCATENATE("$table-&gt;",LOWER(B50),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;text('note5')-&gt;nullable();</v>
+        <v>$table-&gt;string('sms_notify_news', 1)-&gt;nullable();</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3039,11 +3039,11 @@
         <v>6</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D51" t="str">
         <f>IF(B51="String", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"', ",C51,")-&gt;nullable();"), IF(B51="Integer", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"')-&gt;unsigned()-&gt;default(0);"), IF(B51="Text", CONCATENATE("$table-&gt;",LOWER(B51),"('",A51,"')-&gt;nullable();"), IF(B51="Date", CONCATENATE("$table-&gt;",LOWER(B51),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('sms_notify_news', 1)-&gt;nullable();</v>
+        <v>$table-&gt;string('patient_status', 30)-&gt;nullable();</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3054,54 +3054,54 @@
         <v>6</v>
       </c>
       <c r="C52">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D52" t="str">
         <f>IF(B52="String", CONCATENATE("$table-&gt;",LOWER(B52),"('",A52,"', ",C52,")-&gt;nullable();"), IF(B52="Integer", CONCATENATE("$table-&gt;",LOWER(B52),"('",A52,"')-&gt;unsigned()-&gt;default(0);"), IF(B52="Text", CONCATENATE("$table-&gt;",LOWER(B52),"('",A52,"')-&gt;nullable();"), IF(B52="Date", CONCATENATE("$table-&gt;",LOWER(B52),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
-        <v>$table-&gt;string('patient_status', 30)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" t="str">
-        <f>IF(B53="String", CONCATENATE("$table-&gt;",LOWER(B53),"('",A53,"', ",C53,")-&gt;nullable();"), IF(B53="Integer", CONCATENATE("$table-&gt;",LOWER(B53),"('",A53,"')-&gt;unsigned()-&gt;default(0);"), IF(B53="Text", CONCATENATE("$table-&gt;",LOWER(B53),"('",A53,"')-&gt;nullable();"), IF(B53="Date", CONCATENATE("$table-&gt;",LOWER(B53),"('",Table1[[#This Row],[Column name]],"');")) )))</f>
         <v>$table-&gt;string('head_household', 1)-&gt;nullable();</v>
       </c>
     </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="52"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="52"/>
+    </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="52" t="s">
-        <v>54</v>
-      </c>
+      <c r="A55" s="52"/>
       <c r="B55" s="52"/>
       <c r="C55" s="52"/>
       <c r="D55" s="52"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="52"/>
-      <c r="B56" s="52"/>
-      <c r="C56" s="52"/>
-      <c r="D56" s="52"/>
+      <c r="A56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>4</v>
+      <c r="A57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57">
+        <v>100</v>
+      </c>
+      <c r="D57" s="3" t="str">
+        <f t="shared" ref="D57:D60" si="0">IF(B57="String", CONCATENATE("$table-&gt;",LOWER(B57),"('",A57,"', ",C57,")-&gt;nullable();"), IF(B57="Integer", CONCATENATE("$table-&gt;",LOWER(B57),"('",A57,"')-&gt;unsigned()-&gt;default(0);"), IF(B57="Text", CONCATENATE("$table-&gt;",LOWER(B57),"('",A57,"');"), IF(B57="Date", CONCATENATE("$table-&gt;",LOWER(B57),"('",A57,"');")) )))</f>
+        <v>$table-&gt;string('option', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3115,8 +3115,8 @@
         <v>100</v>
       </c>
       <c r="D58" s="3" t="str">
-        <f t="shared" ref="D58:D61" si="0">IF(B58="String", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"', ",C58,")-&gt;nullable();"), IF(B58="Integer", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"')-&gt;unsigned()-&gt;default(0);"), IF(B58="Text", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');"), IF(B58="Date", CONCATENATE("$table-&gt;",LOWER(B58),"('",A58,"');")) )))</f>
-        <v>$table-&gt;string('option', 100)-&gt;nullable();</v>
+        <f t="shared" si="0"/>
+        <v>$table-&gt;string('section', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3131,7 +3131,7 @@
       </c>
       <c r="D59" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>$table-&gt;string('section', 100)-&gt;nullable();</v>
+        <v>$table-&gt;string('description', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3146,50 +3146,50 @@
       </c>
       <c r="D60" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>$table-&gt;string('description', 100)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+        <v>$table-&gt;string('value', 100)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61">
-        <v>100</v>
-      </c>
-      <c r="D61" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>$table-&gt;string('value', 100)-&gt;nullable();</v>
-      </c>
+      <c r="B62" s="52"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="52"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="52" t="s">
-        <v>59</v>
-      </c>
+      <c r="A63" s="52"/>
       <c r="B63" s="52"/>
       <c r="C63" s="52"/>
       <c r="D63" s="52"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="52"/>
-      <c r="B64" s="52"/>
-      <c r="C64" s="52"/>
-      <c r="D64" s="52"/>
+      <c r="A64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>4</v>
+      <c r="A65" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65">
+        <v>100</v>
+      </c>
+      <c r="D65" s="3" t="str">
+        <f t="shared" ref="D65:D70" si="1">IF(B65="String", CONCATENATE("$table-&gt;",LOWER(B65),"('",A65,"', ",C65,")-&gt;nullable();"), IF(B65="Integer", CONCATENATE("$table-&gt;",LOWER(B65),"('",A65,"')-&gt;unsigned()-&gt;default(0);"), IF(B65="Text", CONCATENATE("$table-&gt;",LOWER(B65),"('",A65,"');"), IF(B65="Date", CONCATENATE("$table-&gt;",LOWER(B65),"('",A65,"');")) )))</f>
+        <v>$table-&gt;string('des_dom', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3197,207 +3197,206 @@
         <v>60</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C66">
         <v>100</v>
       </c>
       <c r="D66" s="3" t="str">
-        <f t="shared" ref="D66:D71" si="1">IF(B66="String", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"', ",C66,")-&gt;nullable();"), IF(B66="Integer", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"')-&gt;unsigned()-&gt;default(0);"), IF(B66="Text", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');"), IF(B66="Date", CONCATENATE("$table-&gt;",LOWER(B66),"('",A66,"');")) )))</f>
-        <v>$table-&gt;string('des_dom', 100)-&gt;nullable();</v>
+        <f t="shared" si="1"/>
+        <v>$table-&gt;integer('order')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C67">
         <v>100</v>
       </c>
       <c r="D67" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>$table-&gt;integer('order')-&gt;unsigned()-&gt;default(0);</v>
+        <v>$table-&gt;string('description', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>57</v>
-      </c>
-      <c r="B68" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B68" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C68">
         <v>100</v>
       </c>
-      <c r="D68" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>$table-&gt;string('description', 100)-&gt;nullable();</v>
+      <c r="D68" s="49" t="str">
+        <f>IF(B68="String", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"', ",C68,")-&gt;nullable();"), IF(B68="Integer", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"')-&gt;unsigned()-&gt;default(0);"), IF(B68="Text", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"');"), IF(B68="Date", CONCATENATE("$table-&gt;",LOWER(B68),"('",A68,"');")) )))</f>
+        <v>$table-&gt;string('shortDesc', 100)-&gt;nullable();</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>131</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C69">
-        <v>100</v>
-      </c>
-      <c r="D69" s="49" t="str">
-        <f>IF(B69="String", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"', ",C69,")-&gt;nullable();"), IF(B69="Integer", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"')-&gt;unsigned()-&gt;default(0);"), IF(B69="Text", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"');"), IF(B69="Date", CONCATENATE("$table-&gt;",LOWER(B69),"('",A69,"');")) )))</f>
-        <v>$table-&gt;string('shortDesc', 100)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>58</v>
-      </c>
-      <c r="B70" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D70" s="3" t="str">
+      <c r="D69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>$table-&gt;text('value');</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="19" t="b">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="19" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B72" s="52"/>
+      <c r="C72" s="52"/>
+      <c r="D72" s="52"/>
+    </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="52" t="s">
-        <v>62</v>
-      </c>
+      <c r="A73" s="52"/>
       <c r="B73" s="52"/>
       <c r="C73" s="52"/>
       <c r="D73" s="52"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="52"/>
-      <c r="B74" s="52"/>
-      <c r="C74" s="52"/>
-      <c r="D74" s="52"/>
+      <c r="A74" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>4</v>
+      <c r="A75" t="s">
+        <v>62</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75">
+        <v>255</v>
+      </c>
+      <c r="D75" s="3" t="str">
+        <f t="shared" ref="D75:D76" si="2">IF(B75="String", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"', ",C75,")-&gt;nullable();"), IF(B75="Integer", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"')-&gt;unsigned()-&gt;default(0);"), IF(B75="Text", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');"), IF(B75="Date", CONCATENATE("$table-&gt;",LOWER(B75),"('",A75,"');")) )))</f>
+        <v>$table-&gt;string('path', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>63</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C76">
-        <v>255</v>
-      </c>
-      <c r="D76" s="3" t="str">
-        <f t="shared" ref="D76:D77" si="2">IF(B76="String", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"', ",C76,")-&gt;nullable();"), IF(B76="Integer", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"')-&gt;unsigned()-&gt;default(0);"), IF(B76="Text", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"');"), IF(B76="Date", CONCATENATE("$table-&gt;",LOWER(B76),"('",A76,"');")) )))</f>
-        <v>$table-&gt;string('path', 255)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="2"/>
-      <c r="D77" s="3" t="b">
+      <c r="B76" s="2"/>
+      <c r="D76" s="3" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B80" s="52"/>
+      <c r="C80" s="52"/>
+      <c r="D80" s="52"/>
+    </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="52" t="s">
-        <v>66</v>
-      </c>
+      <c r="A81" s="52"/>
       <c r="B81" s="52"/>
       <c r="C81" s="52"/>
       <c r="D81" s="52"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="52"/>
-      <c r="B82" s="52"/>
-      <c r="C82" s="52"/>
-      <c r="D82" s="52"/>
+      <c r="A82" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" s="21" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E83" s="21" t="s">
-        <v>84</v>
+      <c r="A83" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" s="29">
+        <v>255</v>
+      </c>
+      <c r="D83" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E83" s="25" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B84" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" s="29">
-        <v>255</v>
-      </c>
-      <c r="D84" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="E84" s="25" t="s">
-        <v>83</v>
-      </c>
+      <c r="A84" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B84" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" s="30">
+        <v>250</v>
+      </c>
+      <c r="D84" s="28" t="str">
+        <f>IF(B84="String", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"', ",C84,")-&gt;nullable();"), IF(B84="Integer", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"')-&gt;unsigned()-&gt;default(0);"), IF(B84="Text", CONCATENATE("$table-&gt;",LOWER(B84),"('",A84,"');"), IF(B84="Date", CONCATENATE("$table-&gt;","timestamp","('",A84,"');")) )))</f>
+        <v>$table-&gt;string('title', 250)-&gt;nullable();</v>
+      </c>
+      <c r="E84" s="25"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C85" s="30">
-        <v>250</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C85" s="30"/>
       <c r="D85" s="28" t="str">
-        <f>IF(B85="String", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"', ",C85,")-&gt;nullable();"), IF(B85="Integer", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"')-&gt;unsigned()-&gt;default(0);"), IF(B85="Text", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"');"), IF(B85="Date", CONCATENATE("$table-&gt;","timestamp","('",A85,"');")) )))</f>
-        <v>$table-&gt;string('title', 250)-&gt;nullable();</v>
+        <f t="shared" ref="D85:D86" si="3">IF(B85="String", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"', ",C85,");"), IF(B85="Integer", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"')-&gt;unsigned()-&gt;default(0);"), IF(B85="Text", CONCATENATE("$table-&gt;",LOWER(B85),"('",A85,"');"), IF(B85="Date", CONCATENATE("$table-&gt;","timestamp","('",A85,"');")) )))</f>
+        <v>$table-&gt;text('content');</v>
       </c>
       <c r="E85" s="25"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="B86" s="27" t="s">
-        <v>31</v>
+        <v>67</v>
+      </c>
+      <c r="B86" s="24" t="s">
+        <v>15</v>
       </c>
       <c r="C86" s="30"/>
       <c r="D86" s="28" t="str">
-        <f t="shared" ref="D86:D87" si="3">IF(B86="String", CONCATENATE("$table-&gt;",LOWER(B86),"('",A86,"', ",C86,");"), IF(B86="Integer", CONCATENATE("$table-&gt;",LOWER(B86),"('",A86,"')-&gt;unsigned()-&gt;default(0);"), IF(B86="Text", CONCATENATE("$table-&gt;",LOWER(B86),"('",A86,"');"), IF(B86="Date", CONCATENATE("$table-&gt;","timestamp","('",A86,"');")) )))</f>
-        <v>$table-&gt;text('content');</v>
+        <f t="shared" si="3"/>
+        <v>$table-&gt;timestamp('start_time');</v>
       </c>
       <c r="E86" s="25"/>
     </row>
@@ -3409,454 +3408,453 @@
         <v>15</v>
       </c>
       <c r="C87" s="30"/>
-      <c r="D87" s="28" t="str">
-        <f t="shared" si="3"/>
-        <v>$table-&gt;timestamp('start_time');</v>
+      <c r="D87" s="31" t="str">
+        <f>IF(B87="String", CONCATENATE("$table-&gt;",LOWER(B87),"('",A87,"', ",C87,");"), IF(B87="Integer", CONCATENATE("$table-&gt;",LOWER(B87),"('",A87,"')-&gt;unsigned()-&gt;default(0);"), IF(B87="Text", CONCATENATE("$table-&gt;",LOWER(B87),"('",A87,"');"), IF(B87="Date", CONCATENATE("$table-&gt;","timestamp","('",A87,"');")) )))</f>
+        <v>$table-&gt;timestamp('end_time');</v>
       </c>
       <c r="E87" s="25"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B88" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C88" s="30"/>
-      <c r="D88" s="31" t="str">
-        <f>IF(B88="String", CONCATENATE("$table-&gt;",LOWER(B88),"('",A88,"', ",C88,");"), IF(B88="Integer", CONCATENATE("$table-&gt;",LOWER(B88),"('",A88,"')-&gt;unsigned()-&gt;default(0);"), IF(B88="Text", CONCATENATE("$table-&gt;",LOWER(B88),"('",A88,"');"), IF(B88="Date", CONCATENATE("$table-&gt;","timestamp","('",A88,"');")) )))</f>
-        <v>$table-&gt;timestamp('end_time');</v>
-      </c>
-      <c r="E88" s="25"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="34"/>
-      <c r="B89" s="33"/>
-      <c r="C89" s="35"/>
-      <c r="D89" s="36"/>
-      <c r="E89" s="37" t="s">
-        <v>87</v>
-      </c>
+      <c r="A88" s="34"/>
+      <c r="B88" s="33"/>
+      <c r="C88" s="35"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B90" s="52"/>
+      <c r="C90" s="52"/>
+      <c r="D90" s="52"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="52" t="s">
-        <v>76</v>
-      </c>
+      <c r="A91" s="52"/>
       <c r="B91" s="52"/>
       <c r="C91" s="52"/>
       <c r="D91" s="52"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="52"/>
-      <c r="B92" s="52"/>
-      <c r="C92" s="52"/>
-      <c r="D92" s="52"/>
+      <c r="A92" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E92" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G92" s="11"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E93" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="G93" s="11"/>
+      <c r="A93" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C93" s="8">
+        <v>250</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E93" s="25" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C94" s="8">
-        <v>250</v>
-      </c>
-      <c r="D94" s="13" t="s">
-        <v>73</v>
+      <c r="C94" s="8"/>
+      <c r="D94" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="E94" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C95" s="8"/>
-      <c r="D95" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E95" s="25" t="s">
-        <v>83</v>
-      </c>
+      <c r="D95" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E95" s="22"/>
+      <c r="G95" s="12"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B96" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C96" s="8"/>
-      <c r="D96" s="13" t="s">
-        <v>74</v>
+        <v>11</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" s="9">
+        <v>255</v>
+      </c>
+      <c r="D96" s="13" t="str">
+        <f>IF(B96="String", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"', ",C96,")-&gt;nullable();"), IF(B96="Integer", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"')-&gt;unsigned()-&gt;default(0);"), IF(B96="Text", CONCATENATE("$table-&gt;",LOWER(B96),"('",A96,"');"), IF(B96="Date", CONCATENATE("$table-&gt;","timestamp","('",A96,"');")) )))</f>
+        <v>$table-&gt;string('first_name', 255)-&gt;nullable();</v>
       </c>
       <c r="E96" s="22"/>
       <c r="G96" s="12"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B97" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C97" s="9">
         <v>255</v>
       </c>
       <c r="D97" s="13" t="str">
-        <f>IF(B97="String", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"', ",C97,")-&gt;nullable();"), IF(B97="Integer", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"')-&gt;unsigned()-&gt;default(0);"), IF(B97="Text", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"');"), IF(B97="Date", CONCATENATE("$table-&gt;","timestamp","('",A97,"');")) )))</f>
-        <v>$table-&gt;string('first_name', 255)-&gt;nullable();</v>
+        <f t="shared" ref="D97:D102" si="4">IF(B97="String", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"', ",C97,")-&gt;nullable();"), IF(B97="Integer", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"')-&gt;unsigned()-&gt;default(0);"), IF(B97="Text", CONCATENATE("$table-&gt;",LOWER(B97),"('",A97,"');"), IF(B97="Date", CONCATENATE("$table-&gt;","timestamp","('",A97,"');")) )))</f>
+        <v>$table-&gt;string('last_name', 255)-&gt;nullable();</v>
       </c>
       <c r="E97" s="22"/>
       <c r="G97" s="12"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B98" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C98" s="9">
-        <v>255</v>
-      </c>
-      <c r="D98" s="13" t="str">
-        <f t="shared" ref="D98:D103" si="4">IF(B98="String", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"', ",C98,")-&gt;nullable();"), IF(B98="Integer", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"')-&gt;unsigned()-&gt;default(0);"), IF(B98="Text", CONCATENATE("$table-&gt;",LOWER(B98),"('",A98,"');"), IF(B98="Date", CONCATENATE("$table-&gt;","timestamp","('",A98,"');")) )))</f>
-        <v>$table-&gt;string('last_name', 255)-&gt;nullable();</v>
+      <c r="A98" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="B98" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98" s="50">
+        <v>200</v>
+      </c>
+      <c r="D98" s="41" t="s">
+        <v>139</v>
       </c>
       <c r="E98" s="22"/>
       <c r="G98" s="12"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="50" t="s">
-        <v>139</v>
-      </c>
-      <c r="B99" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C99" s="50">
+      <c r="A99" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="8">
         <v>200</v>
       </c>
-      <c r="D99" s="41" t="s">
+      <c r="D99" s="13" t="s">
         <v>140</v>
       </c>
       <c r="E99" s="22"/>
       <c r="G99" s="12"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B100" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C100" s="8">
-        <v>200</v>
-      </c>
-      <c r="D100" s="13" t="s">
-        <v>141</v>
+      <c r="A100" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" s="22">
+        <v>255</v>
+      </c>
+      <c r="D100" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>$table-&gt;string('address', 255)-&gt;nullable();</v>
       </c>
       <c r="E100" s="22"/>
       <c r="G100" s="12"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B101" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C101" s="22">
-        <v>255</v>
+      <c r="A101" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101" s="8">
+        <v>50</v>
       </c>
       <c r="D101" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>$table-&gt;string('address', 255)-&gt;nullable();</v>
+        <v>$table-&gt;string('phone', 50)-&gt;nullable();</v>
       </c>
       <c r="E101" s="22"/>
       <c r="G101" s="12"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B102" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B102" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C102" s="8">
-        <v>50</v>
+        <v>255</v>
       </c>
       <c r="D102" s="13" t="str">
         <f t="shared" si="4"/>
-        <v>$table-&gt;string('phone', 50)-&gt;nullable();</v>
+        <v>$table-&gt;string('password', 255)-&gt;nullable();</v>
       </c>
       <c r="E102" s="22"/>
       <c r="G102" s="12"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="8" t="s">
-        <v>71</v>
+      <c r="A103" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C103" s="8">
-        <v>255</v>
-      </c>
-      <c r="D103" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>$table-&gt;string('password', 255)-&gt;nullable();</v>
+        <v>25</v>
+      </c>
+      <c r="C103" s="14"/>
+      <c r="D103" s="20" t="s">
+        <v>80</v>
       </c>
       <c r="E103" s="22"/>
       <c r="G103" s="12"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C104" s="14"/>
-      <c r="D104" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="E104" s="22"/>
-      <c r="G104" s="12"/>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="B106" s="52"/>
+      <c r="C106" s="52"/>
+      <c r="D106" s="52"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="52" t="s">
-        <v>77</v>
-      </c>
+      <c r="A107" s="52"/>
       <c r="B107" s="52"/>
       <c r="C107" s="52"/>
       <c r="D107" s="52"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="52"/>
-      <c r="B108" s="52"/>
-      <c r="C108" s="52"/>
-      <c r="D108" s="52"/>
+      <c r="A108" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" s="10" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B109" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C109" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D109" s="10" t="s">
-        <v>4</v>
+      <c r="A109" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" s="8">
+        <v>255</v>
+      </c>
+      <c r="D109" s="13" t="str">
+        <f t="shared" ref="D109:D110" si="5">IF(B109="String", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"', ",C109,")-&gt;nullable();"), IF(B109="Integer", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"')-&gt;unsigned()-&gt;default(0);"), IF(B109="Text", CONCATENATE("$table-&gt;",LOWER(B109),"('",A109,"');"), IF(B109="Date", CONCATENATE("$table-&gt;","timestamp","('",A109,"');")) )))</f>
+        <v>$table-&gt;string('status', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C110" s="8">
-        <v>255</v>
-      </c>
-      <c r="D110" s="13" t="str">
-        <f t="shared" ref="D110:D111" si="5">IF(B110="String", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"', ",C110,")-&gt;nullable();"), IF(B110="Integer", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"')-&gt;unsigned()-&gt;default(0);"), IF(B110="Text", CONCATENATE("$table-&gt;",LOWER(B110),"('",A110,"');"), IF(B110="Date", CONCATENATE("$table-&gt;","timestamp","('",A110,"');")) )))</f>
-        <v>$table-&gt;string('status', 255)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="14"/>
-      <c r="B111" s="7"/>
-      <c r="C111" s="14"/>
-      <c r="D111" s="15" t="b">
+      <c r="A110" s="14"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="14"/>
+      <c r="D110" s="15" t="b">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B112" s="52"/>
+      <c r="C112" s="52"/>
+      <c r="D112" s="52"/>
+    </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="52" t="s">
-        <v>143</v>
-      </c>
+      <c r="A113" s="52"/>
       <c r="B113" s="52"/>
       <c r="C113" s="52"/>
       <c r="D113" s="52"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="52"/>
-      <c r="B114" s="52"/>
-      <c r="C114" s="52"/>
-      <c r="D114" s="52"/>
+      <c r="A114" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B114" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C114" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" s="38" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B115" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C115" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="D115" s="38" t="s">
-        <v>4</v>
+      <c r="A115" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C115" s="8">
+        <v>50</v>
+      </c>
+      <c r="D115" s="13" t="str">
+        <f>IF(B115="String", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"', ",C115,")-nullable();"), IF(B115="Integer", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"')-&gt;unsigned()-&gt;default(0);"), IF(B115="Text", CONCATENATE("$table-&gt;",LOWER(B115),"('",A115,"');"), IF(B115="Date", CONCATENATE("$table-&gt;","timestamp","('",A115,"');")) )))</f>
+        <v>$table-&gt;string('id_invoice', 50)-nullable();</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="8" t="s">
-        <v>91</v>
+      <c r="A116" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="B116" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C116" s="8">
+      <c r="C116" s="14">
         <v>50</v>
       </c>
-      <c r="D116" s="13" t="str">
-        <f>IF(B116="String", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"', ",C116,")-nullable();"), IF(B116="Integer", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"')-&gt;unsigned()-&gt;default(0);"), IF(B116="Text", CONCATENATE("$table-&gt;",LOWER(B116),"('",A116,"');"), IF(B116="Date", CONCATENATE("$table-&gt;","timestamp","('",A116,"');")) )))</f>
-        <v>$table-&gt;string('id_invoice', 50)-nullable();</v>
+      <c r="D116" s="51" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="B117" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C117" s="14">
-        <v>50</v>
-      </c>
-      <c r="D117" s="51" t="s">
-        <v>144</v>
+      <c r="A117" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B117" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C117" s="42"/>
+      <c r="D117" s="48" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="B118" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C118" s="42"/>
-      <c r="D118" s="48" t="s">
-        <v>123</v>
+      <c r="A118" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C118" s="42">
+        <v>255</v>
+      </c>
+      <c r="D118" s="43" t="str">
+        <f t="shared" ref="D118" si="6">IF(B118="String", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"', ",C118,");"), IF(B118="Integer", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"')-&gt;unsigned()-&gt;default(0);"), IF(B118="Text", CONCATENATE("$table-&gt;",LOWER(B118),"('",A118,"');"), IF(B118="Date", CONCATENATE("$table-&gt;","timestamp","('",A118,"');")) )))</f>
+        <v>$table-&gt;string('detail', 255);</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C119" s="42">
-        <v>255</v>
-      </c>
+      <c r="A119" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B119" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C119" s="42"/>
       <c r="D119" s="43" t="str">
-        <f t="shared" ref="D119" si="6">IF(B119="String", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"', ",C119,");"), IF(B119="Integer", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"')-&gt;unsigned()-&gt;default(0);"), IF(B119="Text", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"');"), IF(B119="Date", CONCATENATE("$table-&gt;","timestamp","('",A119,"');")) )))</f>
-        <v>$table-&gt;string('detail', 255);</v>
+        <f>IF(B119="String", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"', ",C119,");"), IF(B119="Integer", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"')-&gt;unsigned()-&gt;default(0);"), IF(B119="Text", CONCATENATE("$table-&gt;",LOWER(B119),"('",A119,"');"), IF(B119="Date", CONCATENATE("$table-&gt;","date","('",A119,"');")) )))</f>
+        <v>$table-&gt;date('date');</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C120" s="42"/>
-      <c r="D120" s="43" t="str">
-        <f>IF(B120="String", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"', ",C120,");"), IF(B120="Integer", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"')-&gt;unsigned()-&gt;default(0);"), IF(B120="Text", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"');"), IF(B120="Date", CONCATENATE("$table-&gt;","date","('",A120,"');")) )))</f>
-        <v>$table-&gt;date('date');</v>
+      <c r="D120" s="41" t="str">
+        <f t="shared" ref="D120:D121" si="7">IF(B120="String", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"', ",C120,");"), IF(B120="Integer", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"')-&gt;unsigned()-&gt;default(0);"), IF(B120="Text", CONCATENATE("$table-&gt;",LOWER(B120),"('",A120,"');"), IF(B120="Date", CONCATENATE("$table-&gt;","timestamp","('",A120,"');")) )))</f>
+        <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="42" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B121" s="40" t="s">
         <v>25</v>
       </c>
       <c r="C121" s="42"/>
-      <c r="D121" s="41" t="str">
-        <f t="shared" ref="D121:D122" si="7">IF(B121="String", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"', ",C121,");"), IF(B121="Integer", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"')-&gt;unsigned()-&gt;default(0);"), IF(B121="Text", CONCATENATE("$table-&gt;",LOWER(B121),"('",A121,"');"), IF(B121="Date", CONCATENATE("$table-&gt;","timestamp","('",A121,"');")) )))</f>
-        <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D121" s="43" t="str">
+        <f t="shared" si="7"/>
+        <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="42" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B122" s="40" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C122" s="42"/>
-      <c r="D122" s="43" t="str">
-        <f t="shared" si="7"/>
-        <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D122" s="43" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="42" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C123" s="42"/>
-      <c r="D123" s="43" t="s">
-        <v>122</v>
+      <c r="D123" s="41" t="str">
+        <f t="shared" ref="D123" si="8">IF(B123="String", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"', ",C123,");"), IF(B123="Integer", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"')-&gt;unsigned()-&gt;default(0);"), IF(B123="Text", CONCATENATE("$table-&gt;",LOWER(B123),"('",A123,"');"), IF(B123="Date", CONCATENATE("$table-&gt;","timestamp","('",A123,"');")) )))</f>
+        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B124" s="40" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C124" s="42"/>
-      <c r="D124" s="41" t="str">
-        <f t="shared" ref="D124" si="8">IF(B124="String", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"', ",C124,");"), IF(B124="Integer", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"')-&gt;unsigned()-&gt;default(0);"), IF(B124="Text", CONCATENATE("$table-&gt;",LOWER(B124),"('",A124,"');"), IF(B124="Date", CONCATENATE("$table-&gt;","timestamp","('",A124,"');")) )))</f>
-        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D124" s="43" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="42" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B125" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C125" s="42"/>
-      <c r="D125" s="43" t="s">
-        <v>121</v>
+      <c r="D125" s="41" t="str">
+        <f t="shared" ref="D125:D127" si="9">IF(B125="String", CONCATENATE("$table-&gt;",LOWER(B125),"('",A125,"', ",C125,");"), IF(B125="Integer", CONCATENATE("$table-&gt;",LOWER(B125),"('",A125,"')-&gt;unsigned()-&gt;default(0);"), IF(B125="Text", CONCATENATE("$table-&gt;",LOWER(B125),"('",A125,"');"), IF(B125="Date", CONCATENATE("$table-&gt;","timestamp","('",A125,"');")) )))</f>
+        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3864,12 +3862,11 @@
         <v>99</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C126" s="42"/>
-      <c r="D126" s="41" t="str">
-        <f t="shared" ref="D126:D128" si="9">IF(B126="String", CONCATENATE("$table-&gt;",LOWER(B126),"('",A126,"', ",C126,");"), IF(B126="Integer", CONCATENATE("$table-&gt;",LOWER(B126),"('",A126,"')-&gt;unsigned()-&gt;default(0);"), IF(B126="Text", CONCATENATE("$table-&gt;",LOWER(B126),"('",A126,"');"), IF(B126="Date", CONCATENATE("$table-&gt;","timestamp","('",A126,"');")) )))</f>
-        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D126" s="43" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3877,11 +3874,12 @@
         <v>100</v>
       </c>
       <c r="B127" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C127" s="42"/>
-      <c r="D127" s="43" t="s">
-        <v>120</v>
+      <c r="D127" s="41" t="str">
+        <f t="shared" si="9"/>
+        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3889,12 +3887,11 @@
         <v>101</v>
       </c>
       <c r="B128" s="40" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C128" s="42"/>
-      <c r="D128" s="41" t="str">
-        <f t="shared" si="9"/>
-        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D128" s="43" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3902,23 +3899,26 @@
         <v>102</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C129" s="42"/>
       <c r="D129" s="43" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B130" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C130" s="42"/>
-      <c r="D130" s="43" t="s">
-        <v>105</v>
+        <v>6</v>
+      </c>
+      <c r="C130" s="42">
+        <v>255</v>
+      </c>
+      <c r="D130" s="43" t="str">
+        <f>IF(B130="String", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"', ",C130,");"), IF(B130="Integer", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"')-&gt;unsigned()-&gt;default(0);"), IF(B130="Text", CONCATENATE("$table-&gt;",LOWER(B130),"('",A130,"');"), IF(B130="Date", CONCATENATE("$table-&gt;","timestamp","('",A130,"');")) )))</f>
+        <v>$table-&gt;string('position', 255);</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3926,14 +3926,12 @@
         <v>106</v>
       </c>
       <c r="B131" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C131" s="42">
-        <v>255</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C131" s="42"/>
       <c r="D131" s="43" t="str">
         <f>IF(B131="String", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"', ",C131,");"), IF(B131="Integer", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"')-&gt;unsigned()-&gt;default(0);"), IF(B131="Text", CONCATENATE("$table-&gt;",LOWER(B131),"('",A131,"');"), IF(B131="Date", CONCATENATE("$table-&gt;","timestamp","('",A131,"');")) )))</f>
-        <v>$table-&gt;string('position', 255);</v>
+        <v>$table-&gt;integer('object')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3946,151 +3944,151 @@
       <c r="C132" s="42"/>
       <c r="D132" s="43" t="str">
         <f>IF(B132="String", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"', ",C132,");"), IF(B132="Integer", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"')-&gt;unsigned()-&gt;default(0);"), IF(B132="Text", CONCATENATE("$table-&gt;",LOWER(B132),"('",A132,"');"), IF(B132="Date", CONCATENATE("$table-&gt;","timestamp","('",A132,"');")) )))</f>
-        <v>$table-&gt;integer('object')-&gt;unsigned()-&gt;default(0);</v>
+        <v>$table-&gt;integer('type_operation')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="42" t="s">
-        <v>108</v>
+        <v>30</v>
       </c>
       <c r="B133" s="40" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C133" s="42"/>
       <c r="D133" s="43" t="str">
         <f>IF(B133="String", CONCATENATE("$table-&gt;",LOWER(B133),"('",A133,"', ",C133,");"), IF(B133="Integer", CONCATENATE("$table-&gt;",LOWER(B133),"('",A133,"')-&gt;unsigned()-&gt;default(0);"), IF(B133="Text", CONCATENATE("$table-&gt;",LOWER(B133),"('",A133,"');"), IF(B133="Date", CONCATENATE("$table-&gt;","timestamp","('",A133,"');")) )))</f>
-        <v>$table-&gt;integer('type_operation')-&gt;unsigned()-&gt;default(0);</v>
+        <v>$table-&gt;text('note');</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B134" s="40" t="s">
-        <v>31</v>
-      </c>
+      <c r="A134" s="42"/>
+      <c r="B134" s="44"/>
       <c r="C134" s="42"/>
-      <c r="D134" s="43" t="str">
-        <f>IF(B134="String", CONCATENATE("$table-&gt;",LOWER(B134),"('",A134,"', ",C134,");"), IF(B134="Integer", CONCATENATE("$table-&gt;",LOWER(B134),"('",A134,"')-&gt;unsigned()-&gt;default(0);"), IF(B134="Text", CONCATENATE("$table-&gt;",LOWER(B134),"('",A134,"');"), IF(B134="Date", CONCATENATE("$table-&gt;","timestamp","('",A134,"');")) )))</f>
-        <v>$table-&gt;text('note');</v>
-      </c>
+      <c r="D134" s="45"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="42"/>
-      <c r="B135" s="44"/>
-      <c r="C135" s="42"/>
-      <c r="D135" s="45"/>
+      <c r="A135" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="B135" s="52"/>
+      <c r="C135" s="52"/>
+      <c r="D135" s="52"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="52" t="s">
-        <v>94</v>
-      </c>
+      <c r="A136" s="52"/>
       <c r="B136" s="52"/>
       <c r="C136" s="52"/>
       <c r="D136" s="52"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="52"/>
-      <c r="B137" s="52"/>
-      <c r="C137" s="52"/>
-      <c r="D137" s="52"/>
+      <c r="A137" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B137" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D137" s="38" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B138" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C138" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="D138" s="38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B139" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C139" s="8">
+      <c r="A138" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138" s="8">
         <v>255</v>
       </c>
-      <c r="D139" s="13" t="str">
-        <f>IF(B139="String", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"', ",C139,");"), IF(B139="Integer", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"')-&gt;unsigned()-&gt;default(0);"), IF(B139="Text", CONCATENATE("$table-&gt;",LOWER(B139),"('",A139,"');"), IF(B139="Date", CONCATENATE("$table-&gt;","timestamp","('",A139,"');")) )))</f>
+      <c r="D138" s="13" t="str">
+        <f>IF(B138="String", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"', ",C138,");"), IF(B138="Integer", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"')-&gt;unsigned()-&gt;default(0);"), IF(B138="Text", CONCATENATE("$table-&gt;",LOWER(B138),"('",A138,"');"), IF(B138="Date", CONCATENATE("$table-&gt;","timestamp","('",A138,"');")) )))</f>
         <v>$table-&gt;string('category', 255);</v>
       </c>
     </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="B142" s="52"/>
+      <c r="C142" s="52"/>
+      <c r="D142" s="52"/>
+    </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="52" t="s">
-        <v>90</v>
-      </c>
+      <c r="A143" s="52"/>
       <c r="B143" s="52"/>
       <c r="C143" s="52"/>
       <c r="D143" s="52"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="52"/>
-      <c r="B144" s="52"/>
-      <c r="C144" s="52"/>
-      <c r="D144" s="52"/>
+      <c r="A144" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B144" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C144" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D144" s="39" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B145" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="C145" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="D145" s="39" t="s">
-        <v>4</v>
+      <c r="A145" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C145" s="8"/>
+      <c r="D145" s="13" t="str">
+        <f t="shared" ref="D145:D150" si="10">IF(B145="String", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"', ",C145,");"), IF(B145="Integer", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"')-&gt;unsigned()-&gt;default(0);"), IF(B145="Text", CONCATENATE("$table-&gt;",LOWER(B145),"('",A145,"');"), IF(B145="Date", CONCATENATE("$table-&gt;","timestamp","('",A145,"');")) )))</f>
+        <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B146" s="7" t="s">
+      <c r="A146" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B146" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C146" s="8"/>
-      <c r="D146" s="13" t="str">
-        <f t="shared" ref="D146:D151" si="10">IF(B146="String", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"', ",C146,");"), IF(B146="Integer", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"')-&gt;unsigned()-&gt;default(0);"), IF(B146="Text", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"');"), IF(B146="Date", CONCATENATE("$table-&gt;","timestamp","('",A146,"');")) )))</f>
-        <v>$table-&gt;integer('id_job')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="C146" s="42"/>
+      <c r="D146" s="43" t="str">
+        <f>IF(B146="String", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"', ",C146,");"), IF(B146="Integer", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"')-&gt;unsigned()-&gt;default(0);"), IF(B146="Text", CONCATENATE("$table-&gt;",LOWER(B146),"('",A146,"');"), IF(B146="Date", CONCATENATE("$table-&gt;","timestamp","('",A146,"');")) )))</f>
+        <v>$table-&gt;integer('id_teeth_prizes')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="42" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
       <c r="B147" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C147" s="42"/>
+        <v>6</v>
+      </c>
+      <c r="C147" s="42">
+        <v>50</v>
+      </c>
       <c r="D147" s="43" t="str">
-        <f>IF(B147="String", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"', ",C147,");"), IF(B147="Integer", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"')-&gt;unsigned()-&gt;default(0);"), IF(B147="Text", CONCATENATE("$table-&gt;",LOWER(B147),"('",A147,"');"), IF(B147="Date", CONCATENATE("$table-&gt;","timestamp","('",A147,"');")) )))</f>
-        <v>$table-&gt;integer('id_teeth_prizes')-&gt;unsigned()-&gt;default(0);</v>
+        <f t="shared" si="10"/>
+        <v>$table-&gt;string('id_dentist', 50);</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="42" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="B148" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C148" s="42">
-        <v>50</v>
-      </c>
-      <c r="D148" s="43" t="str">
-        <f t="shared" si="10"/>
-        <v>$table-&gt;string('id_dentist', 50);</v>
+        <v>15</v>
+      </c>
+      <c r="C148" s="42"/>
+      <c r="D148" s="41" t="str">
+        <f>IF(B148="String", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"', ",C148,");"), IF(B148="Integer", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"')-&gt;unsigned()-&gt;default(0);"), IF(B148="Text", CONCATENATE("$table-&gt;",LOWER(B148),"('",A148,"');"), IF(B148="Date", CONCATENATE("$table-&gt;","date","('",A148,"');")) )))</f>
+        <v>$table-&gt;date('date');</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -4098,68 +4096,68 @@
         <v>110</v>
       </c>
       <c r="B149" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C149" s="42"/>
-      <c r="D149" s="41" t="str">
-        <f>IF(B149="String", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"', ",C149,");"), IF(B149="Integer", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"')-&gt;unsigned()-&gt;default(0);"), IF(B149="Text", CONCATENATE("$table-&gt;",LOWER(B149),"('",A149,"');"), IF(B149="Date", CONCATENATE("$table-&gt;","date","('",A149,"');")) )))</f>
-        <v>$table-&gt;date('date');</v>
+        <v>6</v>
+      </c>
+      <c r="C149" s="42">
+        <v>255</v>
+      </c>
+      <c r="D149" s="43" t="str">
+        <f t="shared" si="10"/>
+        <v>$table-&gt;string('teeth_no', 255);</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="42" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C150" s="42">
-        <v>255</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C150" s="42"/>
       <c r="D150" s="43" t="str">
         <f t="shared" si="10"/>
-        <v>$table-&gt;string('teeth_no', 255);</v>
+        <v>$table-&gt;text('description');</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="42" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="B151" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C151" s="42"/>
-      <c r="D151" s="43" t="str">
-        <f t="shared" si="10"/>
-        <v>$table-&gt;text('description');</v>
+        <v>6</v>
+      </c>
+      <c r="C151" s="42">
+        <v>255</v>
+      </c>
+      <c r="D151" s="41" t="str">
+        <f>IF(B151="String", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"', ",C151,");"), IF(B151="Integer", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"')-&gt;unsigned()-&gt;default(0);"), IF(B151="Text", CONCATENATE("$table-&gt;",LOWER(B151),"('",A151,"');"), IF(B151="Date", CONCATENATE("$table-&gt;","timestamp","('",A151,"');")) )))</f>
+        <v>$table-&gt;string('shortCode', 255);</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="42" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B152" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C152" s="42">
-        <v>255</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C152" s="42"/>
       <c r="D152" s="41" t="str">
         <f>IF(B152="String", CONCATENATE("$table-&gt;",LOWER(B152),"('",A152,"', ",C152,");"), IF(B152="Integer", CONCATENATE("$table-&gt;",LOWER(B152),"('",A152,"')-&gt;unsigned()-&gt;default(0);"), IF(B152="Text", CONCATENATE("$table-&gt;",LOWER(B152),"('",A152,"');"), IF(B152="Date", CONCATENATE("$table-&gt;","timestamp","('",A152,"');")) )))</f>
-        <v>$table-&gt;string('shortCode', 255);</v>
+        <v>$table-&gt;text('desc_client');</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="42" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="B153" s="40" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C153" s="42"/>
       <c r="D153" s="41" t="str">
-        <f>IF(B153="String", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"', ",C153,");"), IF(B153="Integer", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"')-&gt;unsigned()-&gt;default(0);"), IF(B153="Text", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"');"), IF(B153="Date", CONCATENATE("$table-&gt;","timestamp","('",A153,"');")) )))</f>
-        <v>$table-&gt;text('desc_client');</v>
+        <f t="shared" ref="D153:D161" si="11">IF(B153="String", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"', ",C153,");"), IF(B153="Integer", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"')-&gt;unsigned()-&gt;default(0);"), IF(B153="Text", CONCATENATE("$table-&gt;",LOWER(B153),"('",A153,"');"), IF(B153="Date", CONCATENATE("$table-&gt;","timestamp","('",A153,"');")) )))</f>
+        <v>$table-&gt;integer('currency')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4167,73 +4165,75 @@
         <v>112</v>
       </c>
       <c r="B154" s="40" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C154" s="42"/>
-      <c r="D154" s="41" t="str">
-        <f t="shared" ref="D154:D162" si="11">IF(B154="String", CONCATENATE("$table-&gt;",LOWER(B154),"('",A154,"', ",C154,");"), IF(B154="Integer", CONCATENATE("$table-&gt;",LOWER(B154),"('",A154,"')-&gt;unsigned()-&gt;default(0);"), IF(B154="Text", CONCATENATE("$table-&gt;",LOWER(B154),"('",A154,"');"), IF(B154="Date", CONCATENATE("$table-&gt;","timestamp","('",A154,"');")) )))</f>
-        <v>$table-&gt;integer('currency')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D154" s="43" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="42" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B155" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C155" s="42"/>
-      <c r="D155" s="43" t="s">
-        <v>114</v>
+      <c r="D155" s="41" t="str">
+        <f>IF(B155="String", CONCATENATE("$table-&gt;",LOWER(B155),"('",A155,"', ",C155,");"), IF(B155="Integer", CONCATENATE("$table-&gt;",LOWER(B155),"('",A155,"')-&gt;unsigned()-&gt;default(0);"), IF(B155="Text", CONCATENATE("$table-&gt;",LOWER(B155),"('",A155,"');"), IF(B155="Date", CONCATENATE("$table-&gt;","timestamp","('",A155,"');")) )))</f>
+        <v>$table-&gt;integer('quantity')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B156" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C156" s="42"/>
+      <c r="D156" s="43" t="s">
         <v>115</v>
-      </c>
-      <c r="B156" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C156" s="42"/>
-      <c r="D156" s="41" t="str">
-        <f>IF(B156="String", CONCATENATE("$table-&gt;",LOWER(B156),"('",A156,"', ",C156,");"), IF(B156="Integer", CONCATENATE("$table-&gt;",LOWER(B156),"('",A156,"')-&gt;unsigned()-&gt;default(0);"), IF(B156="Text", CONCATENATE("$table-&gt;",LOWER(B156),"('",A156,"');"), IF(B156="Date", CONCATENATE("$table-&gt;","timestamp","('",A156,"');")) )))</f>
-        <v>$table-&gt;integer('quantity')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="42" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B157" s="40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C157" s="42"/>
       <c r="D157" s="43" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B158" s="40" t="s">
         <v>103</v>
-      </c>
-      <c r="B158" s="40" t="s">
-        <v>104</v>
       </c>
       <c r="C158" s="42"/>
       <c r="D158" s="43" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="42" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C159" s="42"/>
-      <c r="D159" s="43" t="s">
-        <v>133</v>
+        <v>6</v>
+      </c>
+      <c r="C159" s="42">
+        <v>255</v>
+      </c>
+      <c r="D159" s="41" t="str">
+        <f>IF(B159="String", CONCATENATE("$table-&gt;",LOWER(B159),"('",A159,"', ",C159,");"), IF(B159="Integer", CONCATENATE("$table-&gt;",LOWER(B159),"('",A159,"')-&gt;unsigned()-&gt;default(0);"), IF(B159="Text", CONCATENATE("$table-&gt;",LOWER(B159),"('",A159,"');"), IF(B159="Date", CONCATENATE("$table-&gt;","timestamp","('",A159,"');")) )))</f>
+        <v>$table-&gt;string('type_cure', 255);</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -4248,22 +4248,20 @@
       </c>
       <c r="D160" s="41" t="str">
         <f>IF(B160="String", CONCATENATE("$table-&gt;",LOWER(B160),"('",A160,"', ",C160,");"), IF(B160="Integer", CONCATENATE("$table-&gt;",LOWER(B160),"('",A160,"')-&gt;unsigned()-&gt;default(0);"), IF(B160="Text", CONCATENATE("$table-&gt;",LOWER(B160),"('",A160,"');"), IF(B160="Date", CONCATENATE("$table-&gt;","timestamp","('",A160,"');")) )))</f>
-        <v>$table-&gt;string('type_cure', 255);</v>
+        <v>$table-&gt;string('status_cure', 255);</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="42" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B161" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C161" s="42">
-        <v>255</v>
-      </c>
-      <c r="D161" s="41" t="str">
-        <f>IF(B161="String", CONCATENATE("$table-&gt;",LOWER(B161),"('",A161,"', ",C161,");"), IF(B161="Integer", CONCATENATE("$table-&gt;",LOWER(B161),"('",A161,"')-&gt;unsigned()-&gt;default(0);"), IF(B161="Text", CONCATENATE("$table-&gt;",LOWER(B161),"('",A161,"');"), IF(B161="Date", CONCATENATE("$table-&gt;","timestamp","('",A161,"');")) )))</f>
-        <v>$table-&gt;string('status_cure', 255);</v>
+        <v>31</v>
+      </c>
+      <c r="C161" s="42"/>
+      <c r="D161" s="43" t="str">
+        <f t="shared" si="11"/>
+        <v>$table-&gt;text('clicnic_note');</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4274,34 +4272,27 @@
         <v>31</v>
       </c>
       <c r="C162" s="42"/>
-      <c r="D162" s="43" t="str">
-        <f t="shared" si="11"/>
-        <v>$table-&gt;text('clicnic_note');</v>
+      <c r="D162" s="43" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="B163" s="40" t="s">
-        <v>31</v>
+      <c r="A163" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="B163" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C163" s="42"/>
-      <c r="D163" s="43" t="s">
-        <v>105</v>
+      <c r="D163" s="41" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="B164" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="A164" s="42"/>
+      <c r="B164" s="40"/>
       <c r="C164" s="42"/>
-      <c r="D164" s="41" t="s">
-        <v>146</v>
-      </c>
+      <c r="D164" s="43"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="42"/>
@@ -4315,143 +4306,150 @@
       <c r="C166" s="42"/>
       <c r="D166" s="43"/>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="42"/>
-      <c r="B167" s="40"/>
-      <c r="C167" s="42"/>
-      <c r="D167" s="43"/>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="B169" s="52"/>
+      <c r="C169" s="52"/>
+      <c r="D169" s="52"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="52" t="s">
-        <v>124</v>
-      </c>
+      <c r="A170" s="52"/>
       <c r="B170" s="52"/>
       <c r="C170" s="52"/>
       <c r="D170" s="52"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="52"/>
-      <c r="B171" s="52"/>
-      <c r="C171" s="52"/>
-      <c r="D171" s="52"/>
+      <c r="A171" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B171" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C171" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D171" s="46" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="B172" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="C172" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="D172" s="46" t="s">
-        <v>4</v>
+      <c r="A172" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B172" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C172" s="42"/>
+      <c r="D172" s="48" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="B173" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C173" s="42"/>
-      <c r="D173" s="48" t="s">
-        <v>123</v>
+      <c r="A173" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173" s="14">
+        <v>255</v>
+      </c>
+      <c r="D173" s="47" t="str">
+        <f>IF(B173="String", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"', ",C173,")-&gt;nullable();"), IF(B173="Integer", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"')-&gt;unsigned()-&gt;default(0);"), IF(B173="Text", CONCATENATE("$table-&gt;",LOWER(B173),"('",A173,"');"), IF(B173="Date", CONCATENATE("$table-&gt;","timestamp","('",A173,"');")) )))</f>
+        <v>$table-&gt;string('category', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="B174" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C174" s="14">
+      <c r="C174" s="42">
         <v>255</v>
       </c>
-      <c r="D174" s="47" t="str">
-        <f>IF(B174="String", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"', ",C174,")-&gt;nullable();"), IF(B174="Integer", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"')-&gt;unsigned()-&gt;default(0);"), IF(B174="Text", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"');"), IF(B174="Date", CONCATENATE("$table-&gt;","timestamp","('",A174,"');")) )))</f>
-        <v>$table-&gt;string('category', 255)-&gt;nullable();</v>
+      <c r="D174" s="43" t="str">
+        <f t="shared" ref="D174" si="12">IF(B174="String", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"', ",C174,");"), IF(B174="Integer", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"')-&gt;unsigned()-&gt;default(0);"), IF(B174="Text", CONCATENATE("$table-&gt;",LOWER(B174),"('",A174,"');"), IF(B174="Date", CONCATENATE("$table-&gt;","timestamp","('",A174,"');")) )))</f>
+        <v>$table-&gt;string('detail', 255);</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B175" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C175" s="42">
-        <v>255</v>
-      </c>
+      <c r="A175" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B175" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C175" s="42"/>
       <c r="D175" s="43" t="str">
-        <f t="shared" ref="D175" si="12">IF(B175="String", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"', ",C175,");"), IF(B175="Integer", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"')-&gt;unsigned()-&gt;default(0);"), IF(B175="Text", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"');"), IF(B175="Date", CONCATENATE("$table-&gt;","timestamp","('",A175,"');")) )))</f>
-        <v>$table-&gt;string('detail', 255);</v>
+        <f t="shared" ref="D175:D176" si="13">IF(B175="String", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"', ",C175,");"), IF(B175="Integer", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"')-&gt;unsigned()-&gt;default(0);"), IF(B175="Text", CONCATENATE("$table-&gt;",LOWER(B175),"('",A175,"');"), IF(B175="Date", CONCATENATE("$table-&gt;","timestamp","('",A175,"');")) )))</f>
+        <v>$table-&gt;timestamp('date');</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="42" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B176" s="40" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C176" s="42"/>
       <c r="D176" s="43" t="str">
-        <f t="shared" ref="D176:D177" si="13">IF(B176="String", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"', ",C176,");"), IF(B176="Integer", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"')-&gt;unsigned()-&gt;default(0);"), IF(B176="Text", CONCATENATE("$table-&gt;",LOWER(B176),"('",A176,"');"), IF(B176="Date", CONCATENATE("$table-&gt;","timestamp","('",A176,"');")) )))</f>
-        <v>$table-&gt;timestamp('date');</v>
+        <f t="shared" si="13"/>
+        <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="42" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B177" s="40" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C177" s="42"/>
-      <c r="D177" s="43" t="str">
-        <f t="shared" si="13"/>
-        <v>$table-&gt;integer('currency1')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D177" s="15" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="42" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B178" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C178" s="42"/>
-      <c r="D178" s="15" t="s">
-        <v>127</v>
+      <c r="D178" s="41" t="str">
+        <f t="shared" ref="D178" si="14">IF(B178="String", CONCATENATE("$table-&gt;",LOWER(B178),"('",A178,"', ",C178,");"), IF(B178="Integer", CONCATENATE("$table-&gt;",LOWER(B178),"('",A178,"')-&gt;unsigned()-&gt;default(0);"), IF(B178="Text", CONCATENATE("$table-&gt;",LOWER(B178),"('",A178,"');"), IF(B178="Date", CONCATENATE("$table-&gt;","timestamp","('",A178,"');")) )))</f>
+        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B179" s="40" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C179" s="42"/>
-      <c r="D179" s="41" t="str">
-        <f t="shared" ref="D179" si="14">IF(B179="String", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"', ",C179,");"), IF(B179="Integer", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"')-&gt;unsigned()-&gt;default(0);"), IF(B179="Text", CONCATENATE("$table-&gt;",LOWER(B179),"('",A179,"');"), IF(B179="Date", CONCATENATE("$table-&gt;","timestamp","('",A179,"');")) )))</f>
-        <v>$table-&gt;integer('currency2')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D179" s="15" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="42" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B180" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C180" s="42"/>
-      <c r="D180" s="15" t="s">
-        <v>128</v>
+      <c r="D180" s="41" t="str">
+        <f t="shared" ref="D180" si="15">IF(B180="String", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"', ",C180,");"), IF(B180="Integer", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"')-&gt;unsigned()-&gt;default(0);"), IF(B180="Text", CONCATENATE("$table-&gt;",LOWER(B180),"('",A180,"');"), IF(B180="Date", CONCATENATE("$table-&gt;","timestamp","('",A180,"');")) )))</f>
+        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4459,12 +4457,11 @@
         <v>99</v>
       </c>
       <c r="B181" s="40" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C181" s="42"/>
-      <c r="D181" s="41" t="str">
-        <f t="shared" ref="D181" si="15">IF(B181="String", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"', ",C181,");"), IF(B181="Integer", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"')-&gt;unsigned()-&gt;default(0);"), IF(B181="Text", CONCATENATE("$table-&gt;",LOWER(B181),"('",A181,"');"), IF(B181="Date", CONCATENATE("$table-&gt;","timestamp","('",A181,"');")) )))</f>
-        <v>$table-&gt;integer('currency3')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D181" s="15" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4472,11 +4469,12 @@
         <v>100</v>
       </c>
       <c r="B182" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C182" s="42"/>
-      <c r="D182" s="15" t="s">
-        <v>129</v>
+      <c r="D182" s="41" t="str">
+        <f t="shared" ref="D182" si="16">IF(B182="String", CONCATENATE("$table-&gt;",LOWER(B182),"('",A182,"', ",C182,");"), IF(B182="Integer", CONCATENATE("$table-&gt;",LOWER(B182),"('",A182,"')-&gt;unsigned()-&gt;default(0);"), IF(B182="Text", CONCATENATE("$table-&gt;",LOWER(B182),"('",A182,"');"), IF(B182="Date", CONCATENATE("$table-&gt;","timestamp","('",A182,"');")) )))</f>
+        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4484,12 +4482,11 @@
         <v>101</v>
       </c>
       <c r="B183" s="40" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C183" s="42"/>
-      <c r="D183" s="41" t="str">
-        <f t="shared" ref="D183" si="16">IF(B183="String", CONCATENATE("$table-&gt;",LOWER(B183),"('",A183,"', ",C183,");"), IF(B183="Integer", CONCATENATE("$table-&gt;",LOWER(B183),"('",A183,"')-&gt;unsigned()-&gt;default(0);"), IF(B183="Text", CONCATENATE("$table-&gt;",LOWER(B183),"('",A183,"');"), IF(B183="Date", CONCATENATE("$table-&gt;","timestamp","('",A183,"');")) )))</f>
-        <v>$table-&gt;integer('currency4')-&gt;unsigned()-&gt;default(0);</v>
+      <c r="D183" s="15" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4497,79 +4494,67 @@
         <v>102</v>
       </c>
       <c r="B184" s="40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C184" s="42"/>
       <c r="D184" s="15" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="42" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="B185" s="40" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="C185" s="42"/>
-      <c r="D185" s="15" t="s">
-        <v>125</v>
+      <c r="D185" s="41" t="str">
+        <f>IF(B185="String", CONCATENATE("$table-&gt;",LOWER(B185),"('",A185,"', ",C185,");"), IF(B185="Integer", CONCATENATE("$table-&gt;",LOWER(B185),"('",A185,"')-&gt;unsigned()-&gt;default(0);"), IF(B185="Text", CONCATENATE("$table-&gt;",LOWER(B185),"('",A185,"');"), IF(B185="Date", CONCATENATE("$table-&gt;","timestamp","('",A185,"');")) )))</f>
+        <v>$table-&gt;integer('discount')-&gt;unsigned()-&gt;default(0);</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="42" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="B186" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C186" s="42"/>
-      <c r="D186" s="41" t="str">
-        <f>IF(B186="String", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"', ",C186,");"), IF(B186="Integer", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"')-&gt;unsigned()-&gt;default(0);"), IF(B186="Text", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"');"), IF(B186="Date", CONCATENATE("$table-&gt;","timestamp","('",A186,"');")) )))</f>
-        <v>$table-&gt;integer('discount')-&gt;unsigned()-&gt;default(0);</v>
+        <v>6</v>
+      </c>
+      <c r="C186" s="42">
+        <v>255</v>
+      </c>
+      <c r="D186" s="43" t="str">
+        <f>IF(B186="String", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"', ",C186,")-&gt;nullable();"), IF(B186="Integer", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"')-&gt;unsigned()-&gt;default(0);"), IF(B186="Text", CONCATENATE("$table-&gt;",LOWER(B186),"('",A186,"');"), IF(B186="Date", CONCATENATE("$table-&gt;","timestamp","('",A186,"');")) )))</f>
+        <v>$table-&gt;string('position', 255)-&gt;nullable();</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="42" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="B187" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C187" s="42">
-        <v>255</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C187" s="42"/>
       <c r="D187" s="43" t="str">
-        <f>IF(B187="String", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"', ",C187,")-&gt;nullable();"), IF(B187="Integer", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"')-&gt;unsigned()-&gt;default(0);"), IF(B187="Text", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"');"), IF(B187="Date", CONCATENATE("$table-&gt;","timestamp","('",A187,"');")) )))</f>
-        <v>$table-&gt;string('position', 255)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B188" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C188" s="42"/>
-      <c r="D188" s="43" t="str">
-        <f>IF(B188="String", CONCATENATE("$table-&gt;",LOWER(B188),"('",A188,"', ",C188,");"), IF(B188="Integer", CONCATENATE("$table-&gt;",LOWER(B188),"('",A188,"')-&gt;unsigned()-&gt;default(0);"), IF(B188="Text", CONCATENATE("$table-&gt;",LOWER(B188),"('",A188,"')-&gt;nullable();"), IF(B188="Date", CONCATENATE("$table-&gt;","timestamp","('",A188,"');")) )))</f>
+        <f>IF(B187="String", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"', ",C187,");"), IF(B187="Integer", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"')-&gt;unsigned()-&gt;default(0);"), IF(B187="Text", CONCATENATE("$table-&gt;",LOWER(B187),"('",A187,"')-&gt;nullable();"), IF(B187="Date", CONCATENATE("$table-&gt;","timestamp","('",A187,"');")) )))</f>
         <v>$table-&gt;text('note')-&gt;nullable();</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A91:D92"/>
+    <mergeCell ref="A169:D170"/>
+    <mergeCell ref="A142:D143"/>
+    <mergeCell ref="A112:D113"/>
+    <mergeCell ref="A135:D136"/>
+    <mergeCell ref="A106:D107"/>
+    <mergeCell ref="A90:D91"/>
     <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A55:D56"/>
-    <mergeCell ref="A63:D64"/>
-    <mergeCell ref="A73:D74"/>
-    <mergeCell ref="A81:D82"/>
-    <mergeCell ref="A170:D171"/>
-    <mergeCell ref="A143:D144"/>
-    <mergeCell ref="A113:D114"/>
-    <mergeCell ref="A136:D137"/>
-    <mergeCell ref="A107:D108"/>
+    <mergeCell ref="A54:D55"/>
+    <mergeCell ref="A62:D63"/>
+    <mergeCell ref="A72:D73"/>
+    <mergeCell ref="A80:D81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>